<commit_message>
Fixed a couple errors with team members not saving. Still want to make competitions matches weight a bit heavier than practice matches
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -3415,13 +3415,13 @@
         <v>0.0</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>70.56109725687725</v>
+        <v>70.56109725687728</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>34.60317460335194</v>
+        <v>34.603174603351924</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>22.757936507914348</v>
+        <v>22.75793650791434</v>
       </c>
       <c r="H2" t="n" s="0">
         <v>0.0</v>
@@ -3444,13 +3444,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>81.76704545463811</v>
+        <v>81.7670454546381</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>46.8911564625177</v>
+        <v>46.89115646251769</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>33.44897959201044</v>
+        <v>33.448979592010446</v>
       </c>
       <c r="H3" t="n" s="0">
         <v>0.0</v>
@@ -3473,7 +3473,7 @@
         <v>0.0</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>68.96774193562257</v>
+        <v>68.96774193562256</v>
       </c>
       <c r="F4" t="n" s="0">
         <v>26.5</v>
@@ -3502,13 +3502,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>60.57954545464293</v>
+        <v>60.579545454642926</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>37.83219178093086</v>
+        <v>37.832191780930856</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>22.571917808179144</v>
+        <v>22.57191780817914</v>
       </c>
       <c r="H5" t="n" s="0">
         <v>0.0</v>
@@ -3531,7 +3531,7 @@
         <v>0.0</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>93.22368421041327</v>
+        <v>93.22368421041328</v>
       </c>
       <c r="F6" t="n" s="0">
         <v>48.024691357850564</v>
@@ -3566,7 +3566,7 @@
         <v>26.35869565216829</v>
       </c>
       <c r="G7" t="n" s="0">
-        <v>28.71739130433658</v>
+        <v>28.717391304336573</v>
       </c>
       <c r="H7" t="n" s="0">
         <v>0.0</v>
@@ -3592,7 +3592,7 @@
         <v>61.0</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>38.16666666666667</v>
+        <v>38.166666666666664</v>
       </c>
       <c r="G8" t="n" s="0">
         <v>20.166666666666664</v>
@@ -3618,7 +3618,7 @@
         <v>0.0</v>
       </c>
       <c r="E9" t="n" s="0">
-        <v>89.1728395059614</v>
+        <v>89.17283950596142</v>
       </c>
       <c r="F9" t="n" s="0">
         <v>48.024691357850564</v>
@@ -3647,13 +3647,13 @@
         <v>0.0</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>74.01414141434437</v>
+        <v>74.0141414143444</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>32.973684210591465</v>
+        <v>32.97368421059146</v>
       </c>
       <c r="G10" t="n" s="0">
-        <v>26.69736842111582</v>
+        <v>26.69736842111581</v>
       </c>
       <c r="H10" t="n" s="0">
         <v>0.0</v>

</xml_diff>

<commit_message>
Fixed an issue with drive team data list being null. But WHY ARE THE WEIGHTED NUMBERS 0
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A2227F-1C3A-4C6F-A395-EEE5D6D3CBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37629D0-7909-41A6-940A-77698667DC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3792" yWindow="2400" windowWidth="17280" windowHeight="8880" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
+    <workbookView xWindow="3792" yWindow="2400" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
   <sheets>
     <sheet name="Match Data" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="3" r:id="rId2"/>
     <sheet name="Per Member Data" sheetId="4" r:id="rId3"/>
+    <sheet name="Drive Team Data" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="55">
   <si>
     <t>Cyrus</t>
   </si>
@@ -194,6 +195,15 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>B+M</t>
+  </si>
+  <si>
+    <t>E+Z</t>
+  </si>
+  <si>
+    <t>L+C</t>
   </si>
 </sst>
 </file>
@@ -1662,8 +1672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
   <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="A27:I27"/>
+    <sheetView topLeftCell="A18" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3415,13 +3425,13 @@
         <v>0.0</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>70.56109725687728</v>
+        <v>70.55813953490454</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>34.603174603351924</v>
+        <v>34.57613168743349</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>22.75793650791434</v>
+        <v>22.76131687240414</v>
       </c>
       <c r="H2" t="n" s="0">
         <v>0.0</v>
@@ -3444,13 +3454,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>81.7670454546381</v>
+        <v>81.75294117656986</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>46.89115646251769</v>
+        <v>46.90140845063206</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>33.448979592010446</v>
+        <v>33.42253521145376</v>
       </c>
       <c r="H3" t="n" s="0">
         <v>0.0</v>
@@ -3473,7 +3483,7 @@
         <v>0.0</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>68.96774193562256</v>
+        <v>68.94666666681476</v>
       </c>
       <c r="F4" t="n" s="0">
         <v>26.5</v>
@@ -3502,13 +3512,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>60.579545454642926</v>
+        <v>60.564705882457396</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>37.832191780930856</v>
+        <v>37.815602836996234</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>22.57191780817914</v>
+        <v>22.578014184354227</v>
       </c>
       <c r="H5" t="n" s="0">
         <v>0.0</v>
@@ -3531,13 +3541,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>93.22368421041328</v>
+        <v>93.24090909078771</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>48.024691357850564</v>
+        <v>48.051282051094276</v>
       </c>
       <c r="G6" t="n" s="0">
-        <v>41.148148148110835</v>
+        <v>41.153846153805915</v>
       </c>
       <c r="H6" t="n" s="0">
         <v>0.0</v>
@@ -3560,13 +3570,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" t="n" s="0">
-        <v>71.03289473687948</v>
+        <v>71.02721088439371</v>
       </c>
       <c r="F7" t="n" s="0">
-        <v>26.35869565216829</v>
+        <v>26.35955056179175</v>
       </c>
       <c r="G7" t="n" s="0">
-        <v>28.717391304336573</v>
+        <v>28.71910112358349</v>
       </c>
       <c r="H7" t="n" s="0">
         <v>0.0</v>
@@ -3592,7 +3602,7 @@
         <v>61.0</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>38.166666666666664</v>
+        <v>38.16666666666667</v>
       </c>
       <c r="G8" t="n" s="0">
         <v>20.166666666666664</v>
@@ -3618,13 +3628,13 @@
         <v>0.0</v>
       </c>
       <c r="E9" t="n" s="0">
-        <v>89.17283950596142</v>
+        <v>89.20512820490019</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>48.024691357850564</v>
+        <v>48.051282051094276</v>
       </c>
       <c r="G9" t="n" s="0">
-        <v>41.148148148110835</v>
+        <v>41.153846153805915</v>
       </c>
       <c r="H9" t="n" s="0">
         <v>0.0</v>
@@ -3647,19 +3657,121 @@
         <v>0.0</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>74.0141414143444</v>
+        <v>73.98329853883885</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>32.97368421059146</v>
+        <v>32.9638009050467</v>
       </c>
       <c r="G10" t="n" s="0">
-        <v>26.69736842111581</v>
+        <v>26.687782805497104</v>
       </c>
       <c r="H10" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="M10" t="s" s="0">
         <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A2:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="n" s="0">
+        <v>64.85714285714286</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>37.08666666666666</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>22.06</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="n" s="0">
+        <v>87.63333333333334</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>47.040000000000006</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>38.28</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="n" s="0">
+        <v>71.3075</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>27.790476190476188</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>28.46666666666667</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The weighted numbers are appearing now but they're not correct
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37629D0-7909-41A6-940A-77698667DC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F75982-A1CC-404D-AF8D-1652AB1CDB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3792" yWindow="2400" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="59">
   <si>
     <t>Cyrus</t>
   </si>
@@ -204,13 +204,24 @@
   </si>
   <si>
     <t>L+C</t>
+  </si>
+  <si>
+    <t>wAvgtotal</t>
+  </si>
+  <si>
+    <t>wAvgtele</t>
+  </si>
+  <si>
+    <t>wAvgauto</t>
+  </si>
+  <si>
+    <t>wAvgpen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1672,14 +1683,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
   <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -1712,25 +1723,25 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>45237</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>106</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2">
         <v>0</v>
       </c>
       <c r="M2" s="2"/>
@@ -1743,673 +1754,673 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>45237</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>83</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>45237</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4">
         <v>89</v>
       </c>
-      <c r="I4" s="0">
+      <c r="I4">
         <v>0</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>45238</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s" s="0">
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5">
         <v>71</v>
       </c>
-      <c r="I5" s="0">
+      <c r="I5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>45238</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>88</v>
       </c>
-      <c r="I6" s="0">
+      <c r="I6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>45238</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>111</v>
       </c>
-      <c r="I7" s="0">
+      <c r="I7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>45238</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <v>34</v>
       </c>
-      <c r="I8" s="0">
+      <c r="I8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>45238</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s" s="0">
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>120</v>
       </c>
-      <c r="I9" s="0">
+      <c r="I9">
         <v>0</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>45238</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s" s="0">
+      <c r="E10" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="0">
+      <c r="F10">
         <v>75</v>
       </c>
-      <c r="I10" s="0">
+      <c r="I10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>45237</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>2</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="0">
+      <c r="F11">
         <v>111</v>
       </c>
-      <c r="G11" s="0">
+      <c r="G11">
         <v>66</v>
       </c>
-      <c r="H11" s="0">
+      <c r="H11">
         <v>45</v>
       </c>
-      <c r="I11" s="0">
+      <c r="I11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>45238</v>
       </c>
-      <c r="C12" t="s" s="0">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s" s="0">
+      <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s" s="0">
+      <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="0">
+      <c r="F12">
         <v>107</v>
       </c>
-      <c r="G12" s="0">
+      <c r="G12">
         <v>57</v>
       </c>
-      <c r="H12" s="0">
+      <c r="H12">
         <v>50</v>
       </c>
-      <c r="I12" s="0">
+      <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>45234</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>72</v>
       </c>
-      <c r="G13" s="0">
+      <c r="G13">
         <v>44</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <v>28</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s" s="0">
+      <c r="A14" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="1">
         <v>45234</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>97</v>
       </c>
-      <c r="G14" s="0">
+      <c r="G14">
         <v>51</v>
       </c>
-      <c r="H14" s="0">
+      <c r="H14">
         <v>30</v>
       </c>
-      <c r="I14" s="0">
+      <c r="I14">
         <v>0</v>
       </c>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s" s="0">
+      <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="1">
         <v>45234</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s" s="0">
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>54</v>
       </c>
-      <c r="G15" s="0">
+      <c r="G15">
         <v>26</v>
       </c>
-      <c r="H15" s="0">
+      <c r="H15">
         <v>28</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s" s="0">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>45234</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>82</v>
       </c>
-      <c r="G16" s="0">
+      <c r="G16">
         <v>32</v>
       </c>
-      <c r="H16" s="0">
+      <c r="H16">
         <v>50</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" t="s" s="0">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>45234</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>60</v>
       </c>
-      <c r="G17" s="0">
+      <c r="G17">
         <v>40</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H17">
         <v>20</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" t="s" s="0">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>45234</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s" s="0">
+      <c r="D18" t="s">
         <v>9</v>
       </c>
-      <c r="E18" t="s" s="0">
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>56</v>
       </c>
-      <c r="G18" s="0">
+      <c r="G18">
         <v>48</v>
       </c>
-      <c r="H18" s="0">
+      <c r="H18">
         <v>8</v>
       </c>
-      <c r="I18" s="0">
+      <c r="I18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" t="s" s="0">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>45234</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>60</v>
       </c>
-      <c r="G19" s="0">
+      <c r="G19">
         <v>30</v>
       </c>
-      <c r="H19" s="0">
+      <c r="H19">
         <v>30</v>
       </c>
-      <c r="I19" s="0">
+      <c r="I19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" t="s" s="0">
+      <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>45234</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s" s="0">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>39</v>
       </c>
-      <c r="G20" s="0">
+      <c r="G20">
         <v>34</v>
       </c>
-      <c r="H20" s="0">
+      <c r="H20">
         <v>5</v>
       </c>
-      <c r="I20" s="0">
+      <c r="I20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" t="s" s="0">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>45241</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s" s="0">
+      <c r="E21" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21">
         <v>32</v>
       </c>
-      <c r="G21" s="0">
+      <c r="G21">
         <v>4</v>
       </c>
-      <c r="H21" s="0">
+      <c r="H21">
         <v>28</v>
       </c>
-      <c r="I21" s="0">
-        <v>0</v>
-      </c>
-      <c r="K21" t="s" s="0">
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" t="s" s="0">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>45241</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>4</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>83</v>
       </c>
-      <c r="G22" s="0">
+      <c r="G22">
         <v>55</v>
       </c>
-      <c r="H22" s="0">
+      <c r="H22">
         <v>28</v>
       </c>
-      <c r="I22" s="0">
-        <v>0</v>
-      </c>
-      <c r="K22" t="s" s="0">
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" t="s" s="0">
+      <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>45241</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>3</v>
       </c>
-      <c r="D23" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E23" t="s" s="0">
+      <c r="D23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>56</v>
       </c>
-      <c r="G23" s="0">
+      <c r="G23">
         <v>26</v>
       </c>
-      <c r="H23" s="0">
+      <c r="H23">
         <v>30</v>
       </c>
-      <c r="I23" s="0">
-        <v>0</v>
-      </c>
-      <c r="K23" t="s" s="0">
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" t="s" s="0">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>45241</v>
       </c>
-      <c r="C24" t="s" s="0">
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" t="s" s="0">
+      <c r="D24" t="s">
         <v>9</v>
       </c>
-      <c r="E24" t="s" s="0">
+      <c r="E24" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="0">
+      <c r="F24">
         <v>33</v>
       </c>
-      <c r="G24" s="0">
+      <c r="G24">
         <v>28</v>
       </c>
-      <c r="H24" s="0">
+      <c r="H24">
         <v>5</v>
       </c>
-      <c r="I24" s="0">
-        <v>0</v>
-      </c>
-      <c r="K24" t="s" s="0">
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" t="s" s="0">
+      <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>45241</v>
       </c>
-      <c r="C25" t="s" s="0">
+      <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="D25" t="s" s="0">
+      <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" t="s" s="0">
+      <c r="E25" t="s">
         <v>1</v>
       </c>
-      <c r="F25" s="0">
+      <c r="F25">
         <v>56</v>
       </c>
-      <c r="G25" s="0">
+      <c r="G25">
         <v>36</v>
       </c>
-      <c r="H25" s="0">
+      <c r="H25">
         <v>20</v>
       </c>
-      <c r="I25" s="0">
-        <v>0</v>
-      </c>
-      <c r="K25" t="s" s="0">
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" t="s" s="0">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="1">
         <v>45241</v>
       </c>
-      <c r="C26" t="s" s="0">
+      <c r="C26" t="s">
         <v>3</v>
       </c>
-      <c r="D26" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s" s="0">
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="0">
+      <c r="F26">
         <v>55</v>
       </c>
-      <c r="G26" s="0">
+      <c r="G26">
         <v>27</v>
       </c>
-      <c r="H26" s="0">
+      <c r="H26">
         <v>28</v>
       </c>
-      <c r="I26" s="0">
-        <v>0</v>
-      </c>
-      <c r="K26" t="s" s="0">
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
         <v>50</v>
       </c>
       <c r="T26" s="5"/>
@@ -2426,36 +2437,36 @@
       <c r="W31" s="5"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" t="s" s="0">
+      <c r="A32" t="s">
         <v>51</v>
       </c>
-      <c r="F32" s="0">
+      <c r="F32">
         <v>10</v>
       </c>
-      <c r="G32" s="0">
+      <c r="G32">
         <v>10</v>
       </c>
-      <c r="H32" s="0">
+      <c r="H32">
         <v>56</v>
       </c>
-      <c r="I32" s="0">
+      <c r="I32">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" t="s" s="0">
+      <c r="A33" t="s">
         <v>51</v>
       </c>
-      <c r="F33" s="0">
+      <c r="F33">
         <v>10</v>
       </c>
-      <c r="G33" s="0">
+      <c r="G33">
         <v>10</v>
       </c>
-      <c r="H33" s="0">
+      <c r="H33">
         <v>56</v>
       </c>
-      <c r="I33" s="0">
+      <c r="I33">
         <v>0</v>
       </c>
     </row>
@@ -2479,8 +2490,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -2512,7 +2523,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="V2" t="s" s="0">
+      <c r="V2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2520,16 +2531,16 @@
       <c r="A3" s="1">
         <v>45237</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>106</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2537,25 +2548,25 @@
       <c r="A4" s="1">
         <v>45237</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>83</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" t="s" s="0">
+      <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="O4" t="s" s="0">
+      <c r="O4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2563,26 +2574,26 @@
       <c r="A5" s="1">
         <v>45237</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>89</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="M5" t="s" s="0">
+      <c r="M5" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="0">
+      <c r="N5">
         <f>(SUMIF($C$3:$C$100, M5, $B$3:$B$100)/COUNTIF($C$3:$C$100, M5))</f>
         <v>88.083333333333329</v>
       </c>
-      <c r="O5" s="0">
+      <c r="O5">
         <f>(SUMIF($C$3:$C$100, M5, $F$3:$F$100)/COUNTIF($C$13:$C$100, M5))</f>
         <v>42.428571428571431</v>
       </c>
@@ -2591,26 +2602,26 @@
       <c r="A6" s="1">
         <v>45238</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>71</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s" s="0">
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="M6" t="s" s="0">
+      <c r="M6" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="0">
+      <c r="N6">
         <f>(SUMIF($C$3:$C$100, M6, $B$3:$B$100)/COUNTIF($C$3:$C$100, M6))</f>
         <v>98.5</v>
       </c>
-      <c r="O6" s="0">
+      <c r="O6">
         <f>(SUMIF($C$3:$C$100, M6, $F$3:$F$100)/COUNTIF($C$13:$C$100, M6))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2619,26 +2630,26 @@
       <c r="A7" s="1">
         <v>45238</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>88</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="M7" t="s" s="0">
+      <c r="M7" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="0">
+      <c r="N7">
         <f>(SUMIF($C$3:$C$100, M7, $B$3:$B$100)/COUNTIF($C$3:$C$100, M7))</f>
         <v>86.25</v>
       </c>
-      <c r="O7" s="0">
+      <c r="O7">
         <f>(SUMIF($C$3:$C$100, M7, $F$3:$F$100)/COUNTIF($C$13:$C$100, M7))</f>
         <v>38</v>
       </c>
@@ -2647,16 +2658,16 @@
       <c r="A8" s="1">
         <v>45238</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8">
         <v>111</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>2</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2664,16 +2675,16 @@
       <c r="A9" s="1">
         <v>45238</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9">
         <v>34</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -2684,16 +2695,16 @@
       <c r="A10" s="1">
         <v>45238</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10">
         <v>120</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s" s="0">
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -2702,14 +2713,14 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="M10" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="N10" s="0">
+      <c r="M10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <f>(SUMIF($D$3:$D$100, M10, $B$3:$B$100)/COUNTIF($D$3:$D$100, M10))</f>
         <v>96.666666666666671</v>
       </c>
-      <c r="O10" s="0">
+      <c r="O10">
         <f>(SUMIF($D$3:$D$100, M10, $F$3:$F$100)/COUNTIF($D$13:$D$100, M10))</f>
         <v>26</v>
       </c>
@@ -2718,16 +2729,16 @@
       <c r="A11" s="1">
         <v>45238</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11">
         <v>75</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -2738,14 +2749,14 @@
         <v>22</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="M11" t="s" s="0">
+      <c r="M11" t="s">
         <v>9</v>
       </c>
-      <c r="N11" s="0">
+      <c r="N11">
         <f>(SUMIF($D$3:$D$100, M11, $B$3:$B$100)/COUNTIF($D$3:$D$100, M11))</f>
         <v>77</v>
       </c>
-      <c r="O11" s="0">
+      <c r="O11">
         <f>(SUMIF($D$3:$D$100, M11, $F$3:$F$100)/COUNTIF($D$13:$D$100, M11))</f>
         <v>45.166666666666664</v>
       </c>
@@ -2763,14 +2774,14 @@
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s" s="0">
+      <c r="M12" t="s">
         <v>2</v>
       </c>
-      <c r="N12" s="0">
+      <c r="N12">
         <f>(SUMIF($D$3:$D$100, M12, $B$3:$B$100)/COUNTIF($D$3:$D$100, M12))</f>
         <v>97.75</v>
       </c>
-      <c r="O12" s="0">
+      <c r="O12">
         <f>(SUMIF($D$3:$D$100, M12, $F$3:$F$100)/COUNTIF($D$13:$D$100, M12))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2779,26 +2790,26 @@
       <c r="A13" s="1">
         <v>45237</v>
       </c>
-      <c r="B13" s="0">
+      <c r="B13">
         <v>111</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>66</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <f t="shared" ref="H13:H23" si="0">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12)+SUMIF($M$15:$M$17, $E13, $N$15:$N$17))/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <f t="shared" ref="I13:I23" si="1">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12)+SUMIF($M$15:$M$17, $E13, $O$15:$O$17))/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -2806,7 +2817,7 @@
         <f t="shared" ref="J13:J23" si="2">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12))/2</f>
         <v>98.125</v>
       </c>
-      <c r="K13" s="0">
+      <c r="K13">
         <f t="shared" ref="K13:K23" si="3">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12))/2</f>
         <v>57.333333333333336</v>
       </c>
@@ -2815,26 +2826,26 @@
       <c r="A14" s="1">
         <v>45238</v>
       </c>
-      <c r="B14" s="0">
+      <c r="B14">
         <v>107</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>57</v>
       </c>
-      <c r="H14" s="0">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>84.49444444444444</v>
       </c>
-      <c r="I14" s="0">
+      <c r="I14">
         <f t="shared" si="1"/>
         <v>48.198412698412703</v>
       </c>
@@ -2842,7 +2853,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K14" s="0">
+      <c r="K14">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -2854,26 +2865,26 @@
       <c r="A15" s="1">
         <v>45234</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15">
         <v>108</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s" s="0">
+      <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="s" s="0">
+      <c r="E15" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>38</v>
       </c>
-      <c r="H15" s="0">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>63.166666666666664</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15">
         <f t="shared" si="1"/>
         <v>30.166666666666668</v>
       </c>
@@ -2881,18 +2892,18 @@
         <f t="shared" si="2"/>
         <v>43.125</v>
       </c>
-      <c r="K15" s="0">
+      <c r="K15">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="M15" t="s" s="0">
+      <c r="M15" t="s">
         <v>10</v>
       </c>
-      <c r="N15" s="0">
+      <c r="N15">
         <f>(SUMIF($E$3:$E$100, M15, $B$3:$B$100)/COUNTIF($E$3:$E$100, M15))</f>
         <v>83.166666666666671</v>
       </c>
-      <c r="O15" s="0">
+      <c r="O15">
         <f>(SUMIF($E$3:$E$100, M15, $F$3:$F$100)/COUNTIF($E$13:$E$100, M15))</f>
         <v>40</v>
       </c>
@@ -2901,26 +2912,26 @@
       <c r="A16" s="1">
         <v>45234</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16">
         <v>107</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>74</v>
       </c>
-      <c r="H16" s="0">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -2928,18 +2939,18 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K16" s="0">
+      <c r="K16">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
-      <c r="M16" t="s" s="0">
+      <c r="M16" t="s">
         <v>1</v>
       </c>
-      <c r="N16" s="0">
+      <c r="N16">
         <f>(SUMIF($E$3:$E$100, M16, $B$3:$B$100)/COUNTIF($E$3:$E$100, M16))</f>
         <v>88.4</v>
       </c>
-      <c r="O16" s="0">
+      <c r="O16">
         <f>(SUMIF($E$3:$E$100, M16, $F$3:$F$100)/COUNTIF($E$13:$E$100, M16))</f>
         <v>57</v>
       </c>
@@ -2948,26 +2959,26 @@
       <c r="A17" s="1">
         <v>45234</v>
       </c>
-      <c r="B17" s="0">
+      <c r="B17">
         <v>97</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>62</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I17">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -2975,18 +2986,18 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K17" s="0">
+      <c r="K17">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
-      <c r="M17" t="s" s="0">
+      <c r="M17" t="s">
         <v>5</v>
       </c>
-      <c r="N17" s="0">
+      <c r="N17">
         <f>(SUMIF($E$3:$E$100, M17, $B$3:$B$100)/COUNTIF($E$3:$E$100, M17))</f>
         <v>103.25</v>
       </c>
-      <c r="O17" s="0">
+      <c r="O17">
         <f>(SUMIF($E$3:$E$100, M17, $F$3:$F$100)/COUNTIF($E$13:$E$100, M17))</f>
         <v>52.5</v>
       </c>
@@ -2995,26 +3006,26 @@
       <c r="A18" s="1">
         <v>45234</v>
       </c>
-      <c r="B18" s="0">
+      <c r="B18">
         <v>99</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s" s="0">
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>26</v>
       </c>
-      <c r="H18" s="0">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>89.305555555555557</v>
       </c>
-      <c r="I18" s="0">
+      <c r="I18">
         <f t="shared" si="1"/>
         <v>36.142857142857146</v>
       </c>
@@ -3022,7 +3033,7 @@
         <f t="shared" si="2"/>
         <v>92.375</v>
       </c>
-      <c r="K18" s="0">
+      <c r="K18">
         <f t="shared" si="3"/>
         <v>34.214285714285715</v>
       </c>
@@ -3031,26 +3042,26 @@
       <c r="A19" s="1">
         <v>45234</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19">
         <v>87</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>2</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>32</v>
       </c>
-      <c r="H19" s="0">
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I19" s="0">
+      <c r="I19">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -3058,7 +3069,7 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K19" s="0">
+      <c r="K19">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
@@ -3067,26 +3078,26 @@
       <c r="A20" s="1">
         <v>45234</v>
       </c>
-      <c r="B20" s="0">
+      <c r="B20">
         <v>76</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s" s="0">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>48</v>
       </c>
-      <c r="H20" s="0">
+      <c r="H20">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I20" s="0">
+      <c r="I20">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3094,7 +3105,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K20" s="0">
+      <c r="K20">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3103,26 +3114,26 @@
       <c r="A21" s="1">
         <v>45234</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21">
         <v>93</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s" s="0">
+      <c r="E21" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21">
         <v>40</v>
       </c>
-      <c r="H21" s="0">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I21" s="0">
+      <c r="I21">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3130,7 +3141,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K21" s="0">
+      <c r="K21">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3139,26 +3150,26 @@
       <c r="A22" s="1">
         <v>45234</v>
       </c>
-      <c r="B22" s="0">
+      <c r="B22">
         <v>85</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>30</v>
       </c>
-      <c r="H22" s="0">
+      <c r="H22">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I22" s="0">
+      <c r="I22">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3166,7 +3177,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K22" s="0">
+      <c r="K22">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3175,26 +3186,26 @@
       <c r="A23" s="1">
         <v>45234</v>
       </c>
-      <c r="B23" s="0">
+      <c r="B23">
         <v>49</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>11</v>
       </c>
-      <c r="D23" t="s" s="0">
+      <c r="D23" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s" s="0">
+      <c r="E23" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>34</v>
       </c>
-      <c r="H23" s="0">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I23" s="0">
+      <c r="I23">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3202,7 +3213,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K23" s="0">
+      <c r="K23">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3222,67 +3233,67 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T28" s="0">
+      <c r="T28">
         <v>1</v>
       </c>
-      <c r="U28" t="s" s="0">
+      <c r="U28" t="s">
         <v>3</v>
       </c>
-      <c r="V28" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="W28" t="s" s="0">
+      <c r="V28" t="s">
+        <v>0</v>
+      </c>
+      <c r="W28" t="s">
         <v>1</v>
       </c>
-      <c r="X28" s="0">
+      <c r="X28">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y28" s="0">
+      <c r="Y28">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T29" s="0">
+      <c r="T29">
         <v>2</v>
       </c>
-      <c r="U29" t="s" s="0">
+      <c r="U29" t="s">
         <v>11</v>
       </c>
-      <c r="V29" t="s" s="0">
+      <c r="V29" t="s">
         <v>9</v>
       </c>
-      <c r="W29" t="s" s="0">
+      <c r="W29" t="s">
         <v>1</v>
       </c>
-      <c r="X29" s="0">
+      <c r="X29">
         <f>(N5+N11+N16)/3</f>
         <v>84.49444444444444</v>
       </c>
-      <c r="Y29" s="0">
+      <c r="Y29">
         <f>(O5+O11+O16)/3</f>
         <v>48.198412698412703</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T30" s="0">
+      <c r="T30">
         <v>3</v>
       </c>
-      <c r="U30" t="s" s="0">
+      <c r="U30" t="s">
         <v>4</v>
       </c>
-      <c r="V30" t="s" s="0">
+      <c r="V30" t="s">
         <v>9</v>
       </c>
-      <c r="W30" t="s" s="0">
+      <c r="W30" t="s">
         <v>1</v>
       </c>
-      <c r="X30" s="0">
+      <c r="X30">
         <f>(N6+N11+N16)/3</f>
         <v>87.966666666666654</v>
       </c>
-      <c r="Y30" s="0">
+      <c r="Y30">
         <f>(O6+O11+O16)/3</f>
         <v>53.166666666666664</v>
       </c>
@@ -3296,67 +3307,67 @@
       <c r="W32" s="5"/>
     </row>
     <row r="33" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T33" s="0">
+      <c r="T33">
         <v>1</v>
       </c>
-      <c r="U33" t="s" s="0">
+      <c r="U33" t="s">
         <v>3</v>
       </c>
-      <c r="V33" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="W33" t="s" s="0">
+      <c r="V33" t="s">
+        <v>0</v>
+      </c>
+      <c r="W33" t="s">
         <v>1</v>
       </c>
-      <c r="X33" s="0">
+      <c r="X33">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y33" s="0">
+      <c r="Y33">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="34" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T34" s="0">
+      <c r="T34">
         <v>2</v>
       </c>
-      <c r="U34" t="s" s="0">
+      <c r="U34" t="s">
         <v>11</v>
       </c>
-      <c r="V34" t="s" s="0">
+      <c r="V34" t="s">
         <v>9</v>
       </c>
-      <c r="W34" t="s" s="0">
+      <c r="W34" t="s">
         <v>10</v>
       </c>
-      <c r="X34" s="0">
+      <c r="X34">
         <f>(N5+N11+N15)/3</f>
         <v>82.75</v>
       </c>
-      <c r="Y34" s="0">
+      <c r="Y34">
         <f>(O5+O11+O15)/3</f>
         <v>42.531746031746032</v>
       </c>
     </row>
     <row r="35" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T35" s="0">
+      <c r="T35">
         <v>3</v>
       </c>
-      <c r="U35" t="s" s="0">
+      <c r="U35" t="s">
         <v>4</v>
       </c>
-      <c r="V35" t="s" s="0">
+      <c r="V35" t="s">
         <v>2</v>
       </c>
-      <c r="W35" t="s" s="0">
+      <c r="W35" t="s">
         <v>5</v>
       </c>
-      <c r="X35" s="0">
+      <c r="X35">
         <f>(N6+N12+N17)/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="Y35" s="0">
+      <c r="Y35">
         <f>(O6+O12+O17)/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -3386,289 +3397,289 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="n" s="0">
-        <v>70.64285714285714</v>
-      </c>
-      <c r="B2" t="n" s="0">
+      <c r="A2">
+        <v>70.642857142857139</v>
+      </c>
+      <c r="B2">
         <v>35.333333333333336</v>
       </c>
-      <c r="C2" t="n" s="0">
+      <c r="C2">
         <v>22.666666666666668</v>
       </c>
-      <c r="D2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E2" t="n" s="0">
-        <v>70.55813953490454</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>34.57613168743349</v>
-      </c>
-      <c r="G2" t="n" s="0">
-        <v>22.76131687240414</v>
-      </c>
-      <c r="H2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M2" t="s" s="0">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>70.558139534904555</v>
+      </c>
+      <c r="F2">
+        <v>34.576131687433488</v>
+      </c>
+      <c r="G2">
+        <v>22.761316872404141</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="n" s="0">
-        <v>82.16666666666667</v>
-      </c>
-      <c r="B3" t="n" s="0">
+      <c r="A3">
+        <v>82.166666666666671</v>
+      </c>
+      <c r="B3">
         <v>46.6</v>
       </c>
-      <c r="C3" t="n" s="0">
-        <v>34.2</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E3" t="n" s="0">
-        <v>81.75294117656986</v>
-      </c>
-      <c r="F3" t="n" s="0">
-        <v>46.90140845063206</v>
-      </c>
-      <c r="G3" t="n" s="0">
-        <v>33.42253521145376</v>
-      </c>
-      <c r="H3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M3" t="s" s="0">
+      <c r="C3">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>81.752941176569863</v>
+      </c>
+      <c r="F3">
+        <v>46.901408450632054</v>
+      </c>
+      <c r="G3">
+        <v>33.422535211453756</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="n" s="0">
-        <v>69.6</v>
-      </c>
-      <c r="B4" t="n" s="0">
+      <c r="A4">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="B4">
         <v>26.5</v>
       </c>
-      <c r="C4" t="n" s="0">
-        <v>29.0</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E4" t="n" s="0">
-        <v>68.94666666681476</v>
-      </c>
-      <c r="F4" t="n" s="0">
+      <c r="C4">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>68.946666666814778</v>
+      </c>
+      <c r="F4">
         <v>26.5</v>
       </c>
-      <c r="G4" t="n" s="0">
-        <v>29.0</v>
-      </c>
-      <c r="H4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M4" t="s" s="0">
+      <c r="G4">
+        <v>29</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="n" s="0">
-        <v>61.0</v>
-      </c>
-      <c r="B5" t="n" s="0">
-        <v>38.3</v>
-      </c>
-      <c r="C5" t="n" s="0">
+      <c r="A5">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="C5">
         <v>22.4</v>
       </c>
-      <c r="D5" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E5" t="n" s="0">
-        <v>60.564705882457396</v>
-      </c>
-      <c r="F5" t="n" s="0">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>60.564705882457417</v>
+      </c>
+      <c r="F5">
         <v>37.815602836996234</v>
       </c>
-      <c r="G5" t="n" s="0">
-        <v>22.578014184354227</v>
-      </c>
-      <c r="H5" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M5" t="s" s="0">
+      <c r="G5">
+        <v>22.578014184354231</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="n" s="0">
+      <c r="A6">
         <v>92.75</v>
       </c>
-      <c r="B6" t="n" s="0">
+      <c r="B6">
         <v>47.333333333333336</v>
       </c>
-      <c r="C6" t="n" s="0">
-        <v>41.0</v>
-      </c>
-      <c r="D6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E6" t="n" s="0">
-        <v>93.24090909078771</v>
-      </c>
-      <c r="F6" t="n" s="0">
+      <c r="C6">
+        <v>41</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>93.240909090787696</v>
+      </c>
+      <c r="F6">
         <v>48.051282051094276</v>
       </c>
-      <c r="G6" t="n" s="0">
+      <c r="G6">
         <v>41.153846153805915</v>
       </c>
-      <c r="H6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M6" t="s" s="0">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="n" s="0">
+      <c r="A7">
         <v>71.2</v>
       </c>
-      <c r="B7" t="n" s="0">
+      <c r="B7">
         <v>26.333333333333332</v>
       </c>
-      <c r="C7" t="n" s="0">
+      <c r="C7">
         <v>28.666666666666668</v>
       </c>
-      <c r="D7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E7" t="n" s="0">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>71.02721088439371</v>
       </c>
-      <c r="F7" t="n" s="0">
-        <v>26.35955056179175</v>
-      </c>
-      <c r="G7" t="n" s="0">
-        <v>28.71910112358349</v>
-      </c>
-      <c r="H7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M7" t="s" s="0">
+      <c r="F7">
+        <v>26.359550561791742</v>
+      </c>
+      <c r="G7">
+        <v>28.719101123583485</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="n" s="0">
-        <v>61.0</v>
-      </c>
-      <c r="B8" t="n" s="0">
+      <c r="A8">
+        <v>61</v>
+      </c>
+      <c r="B8">
         <v>38.166666666666664</v>
       </c>
-      <c r="C8" t="n" s="0">
+      <c r="C8">
         <v>20.166666666666668</v>
       </c>
-      <c r="D8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E8" t="n" s="0">
-        <v>61.0</v>
-      </c>
-      <c r="F8" t="n" s="0">
-        <v>38.16666666666667</v>
-      </c>
-      <c r="G8" t="n" s="0">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>60.999999999999979</v>
+      </c>
+      <c r="F8">
+        <v>38.166666666666664</v>
+      </c>
+      <c r="G8">
         <v>20.166666666666664</v>
       </c>
-      <c r="H8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M8" t="s" s="0">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="n" s="0">
-        <v>88.33333333333333</v>
-      </c>
-      <c r="B9" t="n" s="0">
+      <c r="A9">
+        <v>88.333333333333329</v>
+      </c>
+      <c r="B9">
         <v>47.333333333333336</v>
       </c>
-      <c r="C9" t="n" s="0">
-        <v>41.0</v>
-      </c>
-      <c r="D9" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E9" t="n" s="0">
-        <v>89.20512820490019</v>
-      </c>
-      <c r="F9" t="n" s="0">
+      <c r="C9">
+        <v>41</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>89.205128204900205</v>
+      </c>
+      <c r="F9">
         <v>48.051282051094276</v>
       </c>
-      <c r="G9" t="n" s="0">
+      <c r="G9">
         <v>41.153846153805915</v>
       </c>
-      <c r="H9" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M9" t="s" s="0">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="n" s="0">
+      <c r="A10">
         <v>74.9375</v>
       </c>
-      <c r="B10" t="n" s="0">
+      <c r="B10">
         <v>33.285714285714285</v>
       </c>
-      <c r="C10" t="n" s="0">
-        <v>27.0</v>
-      </c>
-      <c r="D10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E10" t="n" s="0">
-        <v>73.98329853883885</v>
-      </c>
-      <c r="F10" t="n" s="0">
-        <v>32.9638009050467</v>
-      </c>
-      <c r="G10" t="n" s="0">
+      <c r="C10">
+        <v>27</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>73.983298538838881</v>
+      </c>
+      <c r="F10">
+        <v>32.963800905046703</v>
+      </c>
+      <c r="G10">
         <v>26.687782805497104</v>
       </c>
-      <c r="H10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M10" t="s" s="0">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3679,98 +3690,124 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A2:K4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="n" s="0">
-        <v>64.85714285714286</v>
-      </c>
-      <c r="B2" t="n" s="0">
-        <v>37.08666666666666</v>
-      </c>
-      <c r="C2" t="n" s="0">
+      <c r="A2">
+        <v>64.857142857142861</v>
+      </c>
+      <c r="B2">
+        <v>37.086666666666659</v>
+      </c>
+      <c r="C2">
         <v>22.06</v>
       </c>
-      <c r="D2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="G2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="H2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K2" t="s" s="0">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>62.787836257309934</v>
+      </c>
+      <c r="F2">
+        <v>35.452438672438674</v>
+      </c>
+      <c r="G2">
+        <v>20.141423761423759</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="n" s="0">
+      <c r="A3">
         <v>87.63333333333334</v>
       </c>
-      <c r="B3" t="n" s="0">
+      <c r="B3">
         <v>47.040000000000006</v>
       </c>
-      <c r="C3" t="n" s="0">
+      <c r="C3">
         <v>38.28</v>
       </c>
-      <c r="D3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="F3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="G3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="H3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K3" t="s" s="0">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>88.277777777777771</v>
+      </c>
+      <c r="F3">
+        <v>50.43333333333333</v>
+      </c>
+      <c r="G3">
+        <v>42.666666666666664</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="n" s="0">
-        <v>71.3075</v>
-      </c>
-      <c r="B4" t="n" s="0">
+      <c r="A4">
+        <v>71.307500000000005</v>
+      </c>
+      <c r="B4">
         <v>27.790476190476188</v>
       </c>
-      <c r="C4" t="n" s="0">
-        <v>28.46666666666667</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="H4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K4" t="s" s="0">
+      <c r="C4">
+        <v>28.466666666666669</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>15.286206896551723</v>
+      </c>
+      <c r="F4">
+        <v>4.4818181818181815</v>
+      </c>
+      <c r="G4">
+        <v>4.3090909090909095</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prep for redoing the weighted averages
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -222,6 +222,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1689,8 +1690,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="10.0"/>
+    <col min="5" max="5" customWidth="true" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -1723,25 +1724,25 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>45237</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>106</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>0</v>
       </c>
       <c r="M2" s="2"/>
@@ -1754,673 +1755,673 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>45237</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>83</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>45237</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>89</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>0</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>45238</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>71</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>45238</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>88</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>45238</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>111</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>45238</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>34</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>45238</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>120</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="0">
         <v>0</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>45238</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="0">
         <v>75</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>45237</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="0">
         <v>111</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="0">
         <v>66</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="0">
         <v>45</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>45238</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="0">
         <v>107</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="0">
         <v>57</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="0">
         <v>50</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="0">
         <v>0</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>45234</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>72</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="0">
         <v>44</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0">
         <v>28</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B14" s="1">
         <v>45234</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0">
         <v>97</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="0">
         <v>51</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="0">
         <v>30</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="0">
         <v>0</v>
       </c>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B15" s="1">
         <v>45234</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>54</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="0">
         <v>26</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="0">
         <v>28</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>45234</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>82</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="0">
         <v>32</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="0">
         <v>50</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>45234</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>60</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="0">
         <v>40</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="0">
         <v>20</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>45234</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>56</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="0">
         <v>48</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0">
         <v>8</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>45234</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>60</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="0">
         <v>30</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0">
         <v>30</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>45234</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>39</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="0">
         <v>34</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0">
         <v>5</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>45241</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="0">
         <v>32</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="0">
         <v>4</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="0">
         <v>28</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="0">
         <v>0</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>45241</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="0">
         <v>83</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="0">
         <v>55</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="0">
         <v>28</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="0">
         <v>0</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>45241</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>56</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="0">
         <v>26</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="0">
         <v>30</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="0">
         <v>0</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>45241</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="0">
         <v>33</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="0">
         <v>28</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="0">
         <v>5</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="0">
         <v>0</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>45241</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="0">
         <v>56</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="0">
         <v>36</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="0">
         <v>20</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="0">
         <v>0</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B26" s="1">
         <v>45241</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="0">
         <v>55</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="0">
         <v>27</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="0">
         <v>28</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="0">
         <v>0</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" t="s" s="0">
         <v>50</v>
       </c>
       <c r="T26" s="5"/>
@@ -2437,36 +2438,36 @@
       <c r="W31" s="5"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="0">
         <v>10</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="0">
         <v>10</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="0">
         <v>56</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="0">
         <v>10</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="0">
         <v>10</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="0">
         <v>56</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2490,8 +2491,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="10.0"/>
+    <col min="5" max="5" customWidth="true" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -2523,7 +2524,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="V2" t="s">
+      <c r="V2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
@@ -2531,16 +2532,16 @@
       <c r="A3" s="1">
         <v>45237</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>106</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -2548,25 +2549,25 @@
       <c r="A4" s="1">
         <v>45237</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>83</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" t="s" s="0">
         <v>24</v>
       </c>
     </row>
@@ -2574,26 +2575,26 @@
       <c r="A5" s="1">
         <v>45237</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>89</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="0">
         <f>(SUMIF($C$3:$C$100, M5, $B$3:$B$100)/COUNTIF($C$3:$C$100, M5))</f>
         <v>88.083333333333329</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="0">
         <f>(SUMIF($C$3:$C$100, M5, $F$3:$F$100)/COUNTIF($C$13:$C$100, M5))</f>
         <v>42.428571428571431</v>
       </c>
@@ -2602,26 +2603,26 @@
       <c r="A6" s="1">
         <v>45238</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>71</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="0">
         <f>(SUMIF($C$3:$C$100, M6, $B$3:$B$100)/COUNTIF($C$3:$C$100, M6))</f>
         <v>98.5</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="0">
         <f>(SUMIF($C$3:$C$100, M6, $F$3:$F$100)/COUNTIF($C$13:$C$100, M6))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2630,26 +2631,26 @@
       <c r="A7" s="1">
         <v>45238</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>88</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="0">
         <f>(SUMIF($C$3:$C$100, M7, $B$3:$B$100)/COUNTIF($C$3:$C$100, M7))</f>
         <v>86.25</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="0">
         <f>(SUMIF($C$3:$C$100, M7, $F$3:$F$100)/COUNTIF($C$13:$C$100, M7))</f>
         <v>38</v>
       </c>
@@ -2658,16 +2659,16 @@
       <c r="A8" s="1">
         <v>45238</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>111</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -2675,16 +2676,16 @@
       <c r="A9" s="1">
         <v>45238</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -2695,16 +2696,16 @@
       <c r="A10" s="1">
         <v>45238</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <v>120</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -2713,14 +2714,14 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="M10" t="s">
+      <c r="M10" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="0">
         <f>(SUMIF($D$3:$D$100, M10, $B$3:$B$100)/COUNTIF($D$3:$D$100, M10))</f>
         <v>96.666666666666671</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="0">
         <f>(SUMIF($D$3:$D$100, M10, $F$3:$F$100)/COUNTIF($D$13:$D$100, M10))</f>
         <v>26</v>
       </c>
@@ -2729,16 +2730,16 @@
       <c r="A11" s="1">
         <v>45238</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0">
         <v>75</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>1</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -2749,14 +2750,14 @@
         <v>22</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="M11" t="s">
+      <c r="M11" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="0">
         <f>(SUMIF($D$3:$D$100, M11, $B$3:$B$100)/COUNTIF($D$3:$D$100, M11))</f>
         <v>77</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="0">
         <f>(SUMIF($D$3:$D$100, M11, $F$3:$F$100)/COUNTIF($D$13:$D$100, M11))</f>
         <v>45.166666666666664</v>
       </c>
@@ -2774,14 +2775,14 @@
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="0">
         <f>(SUMIF($D$3:$D$100, M12, $B$3:$B$100)/COUNTIF($D$3:$D$100, M12))</f>
         <v>97.75</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="0">
         <f>(SUMIF($D$3:$D$100, M12, $F$3:$F$100)/COUNTIF($D$13:$D$100, M12))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2790,26 +2791,26 @@
       <c r="A13" s="1">
         <v>45237</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="0">
         <v>111</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>66</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0">
         <f t="shared" ref="H13:H23" si="0">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12)+SUMIF($M$15:$M$17, $E13, $N$15:$N$17))/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="0">
         <f t="shared" ref="I13:I23" si="1">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12)+SUMIF($M$15:$M$17, $E13, $O$15:$O$17))/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -2817,7 +2818,7 @@
         <f t="shared" ref="J13:J23" si="2">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12))/2</f>
         <v>98.125</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="0">
         <f t="shared" ref="K13:K23" si="3">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12))/2</f>
         <v>57.333333333333336</v>
       </c>
@@ -2826,26 +2827,26 @@
       <c r="A14" s="1">
         <v>45238</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="0">
         <v>107</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0">
         <v>57</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="0">
         <f t="shared" si="0"/>
         <v>84.49444444444444</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="0">
         <f t="shared" si="1"/>
         <v>48.198412698412703</v>
       </c>
@@ -2853,7 +2854,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -2865,26 +2866,26 @@
       <c r="A15" s="1">
         <v>45234</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="0">
         <v>108</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>38</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="0">
         <f t="shared" si="0"/>
         <v>63.166666666666664</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="0">
         <f t="shared" si="1"/>
         <v>30.166666666666668</v>
       </c>
@@ -2892,18 +2893,18 @@
         <f t="shared" si="2"/>
         <v>43.125</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="0">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="0">
         <f>(SUMIF($E$3:$E$100, M15, $B$3:$B$100)/COUNTIF($E$3:$E$100, M15))</f>
         <v>83.166666666666671</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="0">
         <f>(SUMIF($E$3:$E$100, M15, $F$3:$F$100)/COUNTIF($E$13:$E$100, M15))</f>
         <v>40</v>
       </c>
@@ -2912,26 +2913,26 @@
       <c r="A16" s="1">
         <v>45234</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="0">
         <v>107</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>74</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="0">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="0">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -2939,18 +2940,18 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="0">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="0">
         <f>(SUMIF($E$3:$E$100, M16, $B$3:$B$100)/COUNTIF($E$3:$E$100, M16))</f>
         <v>88.4</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="0">
         <f>(SUMIF($E$3:$E$100, M16, $F$3:$F$100)/COUNTIF($E$13:$E$100, M16))</f>
         <v>57</v>
       </c>
@@ -2959,26 +2960,26 @@
       <c r="A17" s="1">
         <v>45234</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="0">
         <v>97</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>62</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -2986,18 +2987,18 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="0">
         <f>(SUMIF($E$3:$E$100, M17, $B$3:$B$100)/COUNTIF($E$3:$E$100, M17))</f>
         <v>103.25</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="0">
         <f>(SUMIF($E$3:$E$100, M17, $F$3:$F$100)/COUNTIF($E$13:$E$100, M17))</f>
         <v>52.5</v>
       </c>
@@ -3006,26 +3007,26 @@
       <c r="A18" s="1">
         <v>45234</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="0">
         <v>99</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>26</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0">
         <f t="shared" si="0"/>
         <v>89.305555555555557</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="0">
         <f t="shared" si="1"/>
         <v>36.142857142857146</v>
       </c>
@@ -3033,7 +3034,7 @@
         <f t="shared" si="2"/>
         <v>92.375</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="0">
         <f t="shared" si="3"/>
         <v>34.214285714285715</v>
       </c>
@@ -3042,26 +3043,26 @@
       <c r="A19" s="1">
         <v>45234</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="0">
         <v>87</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>32</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="0">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -3069,7 +3070,7 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="0">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
@@ -3078,26 +3079,26 @@
       <c r="A20" s="1">
         <v>45234</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="0">
         <v>76</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>48</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3105,7 +3106,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3114,26 +3115,26 @@
       <c r="A21" s="1">
         <v>45234</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="0">
         <v>93</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="0">
         <v>40</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3141,7 +3142,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3150,26 +3151,26 @@
       <c r="A22" s="1">
         <v>45234</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="0">
         <v>85</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="0">
         <v>30</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3177,7 +3178,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3186,26 +3187,26 @@
       <c r="A23" s="1">
         <v>45234</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="0">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>34</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3213,7 +3214,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3233,67 +3234,67 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T28">
+      <c r="T28" s="0">
         <v>1</v>
       </c>
-      <c r="U28" t="s">
+      <c r="U28" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="V28" t="s">
+      <c r="V28" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="W28" t="s">
+      <c r="W28" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X28">
+      <c r="X28" s="0">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y28">
+      <c r="Y28" s="0">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T29">
+      <c r="T29" s="0">
         <v>2</v>
       </c>
-      <c r="U29" t="s">
+      <c r="U29" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="V29" t="s">
+      <c r="V29" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W29" t="s">
+      <c r="W29" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X29">
+      <c r="X29" s="0">
         <f>(N5+N11+N16)/3</f>
         <v>84.49444444444444</v>
       </c>
-      <c r="Y29">
+      <c r="Y29" s="0">
         <f>(O5+O11+O16)/3</f>
         <v>48.198412698412703</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T30">
+      <c r="T30" s="0">
         <v>3</v>
       </c>
-      <c r="U30" t="s">
+      <c r="U30" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="V30" t="s">
+      <c r="V30" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W30" t="s">
+      <c r="W30" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X30">
+      <c r="X30" s="0">
         <f>(N6+N11+N16)/3</f>
         <v>87.966666666666654</v>
       </c>
-      <c r="Y30">
+      <c r="Y30" s="0">
         <f>(O6+O11+O16)/3</f>
         <v>53.166666666666664</v>
       </c>
@@ -3307,67 +3308,67 @@
       <c r="W32" s="5"/>
     </row>
     <row r="33" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T33">
+      <c r="T33" s="0">
         <v>1</v>
       </c>
-      <c r="U33" t="s">
+      <c r="U33" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="V33" t="s">
+      <c r="V33" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="W33" t="s">
+      <c r="W33" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X33">
+      <c r="X33" s="0">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y33">
+      <c r="Y33" s="0">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="34" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T34">
+      <c r="T34" s="0">
         <v>2</v>
       </c>
-      <c r="U34" t="s">
+      <c r="U34" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="V34" t="s">
+      <c r="V34" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W34" t="s">
+      <c r="W34" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="X34">
+      <c r="X34" s="0">
         <f>(N5+N11+N15)/3</f>
         <v>82.75</v>
       </c>
-      <c r="Y34">
+      <c r="Y34" s="0">
         <f>(O5+O11+O15)/3</f>
         <v>42.531746031746032</v>
       </c>
     </row>
     <row r="35" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T35">
+      <c r="T35" s="0">
         <v>3</v>
       </c>
-      <c r="U35" t="s">
+      <c r="U35" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="V35" t="s">
+      <c r="V35" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="W35" t="s">
+      <c r="W35" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="X35">
+      <c r="X35" s="0">
         <f>(N6+N12+N17)/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="Y35">
+      <c r="Y35" s="0">
         <f>(O6+O12+O17)/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -3397,289 +3398,289 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>70.642857142857139</v>
-      </c>
-      <c r="B2">
+      <c r="A2" t="n" s="0">
+        <v>70.64285714285714</v>
+      </c>
+      <c r="B2" t="n" s="0">
         <v>35.333333333333336</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n" s="0">
         <v>22.666666666666668</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>70.558139534904555</v>
-      </c>
-      <c r="F2">
-        <v>34.576131687433488</v>
-      </c>
-      <c r="G2">
-        <v>22.761316872404141</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="D2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>70.55813953490454</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>34.57613168743349</v>
+      </c>
+      <c r="G2" t="n" s="0">
+        <v>22.76131687240414</v>
+      </c>
+      <c r="H2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="s" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>82.166666666666671</v>
-      </c>
-      <c r="B3">
+      <c r="A3" t="n" s="0">
+        <v>82.16666666666667</v>
+      </c>
+      <c r="B3" t="n" s="0">
         <v>46.6</v>
       </c>
-      <c r="C3">
-        <v>34.200000000000003</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>81.752941176569863</v>
-      </c>
-      <c r="F3">
-        <v>46.901408450632054</v>
-      </c>
-      <c r="G3">
-        <v>33.422535211453756</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="C3" t="n" s="0">
+        <v>34.2</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>81.75294117656986</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>46.90140845063206</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>33.42253521145376</v>
+      </c>
+      <c r="H3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M3" t="s" s="0">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>69.599999999999994</v>
-      </c>
-      <c r="B4">
+      <c r="A4" t="n" s="0">
+        <v>69.6</v>
+      </c>
+      <c r="B4" t="n" s="0">
         <v>26.5</v>
       </c>
-      <c r="C4">
-        <v>29</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>68.946666666814778</v>
-      </c>
-      <c r="F4">
+      <c r="C4" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>68.94666666681476</v>
+      </c>
+      <c r="F4" t="n" s="0">
         <v>26.5</v>
       </c>
-      <c r="G4">
-        <v>29</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="G4" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="H4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M4" t="s" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>61</v>
-      </c>
-      <c r="B5">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="C5">
+      <c r="A5" t="n" s="0">
+        <v>61.0</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>38.3</v>
+      </c>
+      <c r="C5" t="n" s="0">
         <v>22.4</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>60.564705882457417</v>
-      </c>
-      <c r="F5">
+      <c r="D5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>60.564705882457396</v>
+      </c>
+      <c r="F5" t="n" s="0">
         <v>37.815602836996234</v>
       </c>
-      <c r="G5">
-        <v>22.578014184354231</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="G5" t="n" s="0">
+        <v>22.578014184354227</v>
+      </c>
+      <c r="H5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M5" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" t="n" s="0">
         <v>92.75</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n" s="0">
         <v>47.333333333333336</v>
       </c>
-      <c r="C6">
-        <v>41</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>93.240909090787696</v>
-      </c>
-      <c r="F6">
+      <c r="C6" t="n" s="0">
+        <v>41.0</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>93.24090909078771</v>
+      </c>
+      <c r="F6" t="n" s="0">
         <v>48.051282051094276</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="n" s="0">
         <v>41.153846153805915</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="H6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M6" t="s" s="0">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" t="n" s="0">
         <v>71.2</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n" s="0">
         <v>26.333333333333332</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n" s="0">
         <v>28.666666666666668</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="D7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E7" t="n" s="0">
         <v>71.02721088439371</v>
       </c>
-      <c r="F7">
-        <v>26.359550561791742</v>
-      </c>
-      <c r="G7">
-        <v>28.719101123583485</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="F7" t="n" s="0">
+        <v>26.35955056179175</v>
+      </c>
+      <c r="G7" t="n" s="0">
+        <v>28.71910112358349</v>
+      </c>
+      <c r="H7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M7" t="s" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>61</v>
-      </c>
-      <c r="B8">
+      <c r="A8" t="n" s="0">
+        <v>61.0</v>
+      </c>
+      <c r="B8" t="n" s="0">
         <v>38.166666666666664</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n" s="0">
         <v>20.166666666666668</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>60.999999999999979</v>
-      </c>
-      <c r="F8">
-        <v>38.166666666666664</v>
-      </c>
-      <c r="G8">
+      <c r="D8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>61.0</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>38.16666666666667</v>
+      </c>
+      <c r="G8" t="n" s="0">
         <v>20.166666666666664</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="H8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M8" t="s" s="0">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>88.333333333333329</v>
-      </c>
-      <c r="B9">
+      <c r="A9" t="n" s="0">
+        <v>88.33333333333333</v>
+      </c>
+      <c r="B9" t="n" s="0">
         <v>47.333333333333336</v>
       </c>
-      <c r="C9">
-        <v>41</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>89.205128204900205</v>
-      </c>
-      <c r="F9">
+      <c r="C9" t="n" s="0">
+        <v>41.0</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <v>89.20512820490019</v>
+      </c>
+      <c r="F9" t="n" s="0">
         <v>48.051282051094276</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="n" s="0">
         <v>41.153846153805915</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="H9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M9" t="s" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" t="n" s="0">
         <v>74.9375</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n" s="0">
         <v>33.285714285714285</v>
       </c>
-      <c r="C10">
-        <v>27</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>73.983298538838881</v>
-      </c>
-      <c r="F10">
-        <v>32.963800905046703</v>
-      </c>
-      <c r="G10">
+      <c r="C10" t="n" s="0">
+        <v>27.0</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E10" t="n" s="0">
+        <v>73.98329853883885</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>32.9638009050467</v>
+      </c>
+      <c r="G10" t="n" s="0">
         <v>26.687782805497104</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="H10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M10" t="s" s="0">
         <v>49</v>
       </c>
     </row>
@@ -3699,115 +3700,115 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>64.857142857142861</v>
-      </c>
-      <c r="B2">
-        <v>37.086666666666659</v>
-      </c>
-      <c r="C2">
+      <c r="A2" t="n" s="0">
+        <v>64.85714285714286</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>37.08666666666666</v>
+      </c>
+      <c r="C2" t="n" s="0">
         <v>22.06</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>62.787836257309934</v>
-      </c>
-      <c r="F2">
-        <v>35.452438672438674</v>
-      </c>
-      <c r="G2">
-        <v>20.141423761423759</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="D2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>63.06444444444444</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>37.840666666666664</v>
+      </c>
+      <c r="G2" t="n" s="0">
+        <v>21.654000000000003</v>
+      </c>
+      <c r="H2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K2" t="s" s="0">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" t="n" s="0">
         <v>87.63333333333334</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n" s="0">
         <v>47.040000000000006</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n" s="0">
         <v>38.28</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>88.277777777777771</v>
-      </c>
-      <c r="F3">
-        <v>50.43333333333333</v>
-      </c>
-      <c r="G3">
-        <v>42.666666666666664</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="D3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>87.83333333333334</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>51.8</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>41.8</v>
+      </c>
+      <c r="H3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K3" t="s" s="0">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>71.307500000000005</v>
-      </c>
-      <c r="B4">
+      <c r="A4" t="n" s="0">
+        <v>71.3075</v>
+      </c>
+      <c r="B4" t="n" s="0">
         <v>27.790476190476188</v>
       </c>
-      <c r="C4">
-        <v>28.466666666666669</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>15.286206896551723</v>
-      </c>
-      <c r="F4">
-        <v>4.4818181818181815</v>
-      </c>
-      <c r="G4">
-        <v>4.3090909090909095</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="C4" t="n" s="0">
+        <v>28.46666666666667</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>15.273076923076923</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>4.8625</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="H4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K4" t="s" s="0">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Weighted stuff still isn't working :(
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F75982-A1CC-404D-AF8D-1652AB1CDB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFDA3BB-591D-425A-9B1F-43A56B362251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3792" yWindow="2400" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
   <sheets>
     <sheet name="Match Data" sheetId="1" r:id="rId1"/>
@@ -1684,8 +1684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
   <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView topLeftCell="A12" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2441,34 +2441,10 @@
       <c r="A32" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="F32" s="0">
-        <v>10</v>
-      </c>
-      <c r="G32" s="0">
-        <v>10</v>
-      </c>
-      <c r="H32" s="0">
-        <v>56</v>
-      </c>
-      <c r="I32" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s" s="0">
         <v>51</v>
-      </c>
-      <c r="F33" s="0">
-        <v>10</v>
-      </c>
-      <c r="G33" s="0">
-        <v>10</v>
-      </c>
-      <c r="H33" s="0">
-        <v>56</v>
-      </c>
-      <c r="I33" s="0">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3391,7 +3367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -3693,7 +3669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -3739,16 +3715,16 @@
         <v>0.0</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>63.06444444444444</v>
+        <v>63.528703703703705</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>37.840666666666664</v>
+        <v>33.41111111111111</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>21.654000000000003</v>
-      </c>
-      <c r="H2" t="n" s="0">
-        <v>0.0</v>
+        <v>20.605555555555554</v>
+      </c>
+      <c r="H2" t="e" s="0">
+        <v>#NUM!</v>
       </c>
       <c r="K2" t="s" s="0">
         <v>52</v>
@@ -3767,17 +3743,17 @@
       <c r="D3" t="n" s="0">
         <v>0.0</v>
       </c>
-      <c r="E3" t="n" s="0">
-        <v>87.83333333333334</v>
+      <c r="E3" t="e" s="0">
+        <v>#DIV/0!</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>51.8</v>
-      </c>
-      <c r="G3" t="n" s="0">
-        <v>41.8</v>
-      </c>
-      <c r="H3" t="n" s="0">
-        <v>0.0</v>
+        <v>26.0</v>
+      </c>
+      <c r="G3" t="e" s="0">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H3" t="e" s="0">
+        <v>#NUM!</v>
       </c>
       <c r="K3" t="s" s="0">
         <v>53</v>
@@ -3797,16 +3773,16 @@
         <v>0.0</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>15.273076923076923</v>
+        <v>70.23412698412699</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>4.8625</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>4.5</v>
-      </c>
-      <c r="H4" t="n" s="0">
-        <v>0.0</v>
+        <v>18.35</v>
+      </c>
+      <c r="G4" t="e" s="0">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H4" t="e" s="0">
+        <v>#NUM!</v>
       </c>
       <c r="K4" t="s" s="0">
         <v>54</v>

</xml_diff>

<commit_message>
Started condensing with arrays and functional interfaces
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -3413,13 +3413,13 @@
         <v>0.0</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>70.55813953490454</v>
+        <v>70.55495978554524</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>34.57613168743349</v>
+        <v>34.54700854721421</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>22.76131687240414</v>
+        <v>22.764957264931564</v>
       </c>
       <c r="H2" t="n" s="0">
         <v>0.0</v>
@@ -3442,13 +3442,13 @@
         <v>0.0</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>81.75294117656986</v>
+        <v>81.73780487815547</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>46.90140845063206</v>
+        <v>46.912408759046556</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>33.42253521145376</v>
+        <v>33.394160584141595</v>
       </c>
       <c r="H3" t="n" s="0">
         <v>0.0</v>
@@ -3471,10 +3471,10 @@
         <v>0.0</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>68.94666666681476</v>
+        <v>68.92413793119296</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>26.5</v>
+        <v>26.499999999999996</v>
       </c>
       <c r="G4" t="n" s="0">
         <v>29.0</v>
@@ -3500,13 +3500,13 @@
         <v>0.0</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>60.564705882457396</v>
+        <v>60.54878048791714</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>37.815602836996234</v>
+        <v>37.79779411777262</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>22.578014184354227</v>
+        <v>22.584558823483277</v>
       </c>
       <c r="H5" t="n" s="0">
         <v>0.0</v>
@@ -3529,13 +3529,13 @@
         <v>0.0</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>93.24090909078771</v>
+        <v>93.25943396213344</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>48.051282051094276</v>
+        <v>48.079999999796904</v>
       </c>
       <c r="G6" t="n" s="0">
-        <v>41.153846153805915</v>
+        <v>41.15999999995648</v>
       </c>
       <c r="H6" t="n" s="0">
         <v>0.0</v>
@@ -3558,13 +3558,13 @@
         <v>0.0</v>
       </c>
       <c r="E7" t="n" s="0">
-        <v>71.02721088439371</v>
+        <v>71.02112676060621</v>
       </c>
       <c r="F7" t="n" s="0">
-        <v>26.35955056179175</v>
+        <v>26.36046511627264</v>
       </c>
       <c r="G7" t="n" s="0">
-        <v>28.71910112358349</v>
+        <v>28.720930232545275</v>
       </c>
       <c r="H7" t="n" s="0">
         <v>0.0</v>
@@ -3587,13 +3587,13 @@
         <v>0.0</v>
       </c>
       <c r="E8" t="n" s="0">
-        <v>61.0</v>
+        <v>61.00000000000001</v>
       </c>
       <c r="F8" t="n" s="0">
         <v>38.16666666666667</v>
       </c>
       <c r="G8" t="n" s="0">
-        <v>20.166666666666664</v>
+        <v>20.16666666666667</v>
       </c>
       <c r="H8" t="n" s="0">
         <v>0.0</v>
@@ -3616,13 +3616,13 @@
         <v>0.0</v>
       </c>
       <c r="E9" t="n" s="0">
-        <v>89.20512820490019</v>
+        <v>89.2399999997534</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>48.051282051094276</v>
+        <v>48.079999999796904</v>
       </c>
       <c r="G9" t="n" s="0">
-        <v>41.153846153805915</v>
+        <v>41.15999999995648</v>
       </c>
       <c r="H9" t="n" s="0">
         <v>0.0</v>
@@ -3645,13 +3645,13 @@
         <v>0.0</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>73.98329853883885</v>
+        <v>73.95032397431406</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>32.9638009050467</v>
+        <v>32.95327102811133</v>
       </c>
       <c r="G10" t="n" s="0">
-        <v>26.687782805497104</v>
+        <v>26.67757009352966</v>
       </c>
       <c r="H10" t="n" s="0">
         <v>0.0</v>
@@ -3703,13 +3703,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="n" s="0">
-        <v>64.85714285714286</v>
+        <v>0.0</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>37.08666666666666</v>
+        <v>0.0</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>22.06</v>
+        <v>0.0</v>
       </c>
       <c r="D2" t="n" s="0">
         <v>0.0</v>
@@ -3732,13 +3732,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="n" s="0">
-        <v>87.63333333333334</v>
+        <v>0.0</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>47.040000000000006</v>
+        <v>0.0</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>38.28</v>
+        <v>0.0</v>
       </c>
       <c r="D3" t="n" s="0">
         <v>0.0</v>
@@ -3761,13 +3761,13 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="n" s="0">
-        <v>71.3075</v>
+        <v>0.0</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>27.790476190476188</v>
+        <v>0.0</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>28.46666666666667</v>
+        <v>0.0</v>
       </c>
       <c r="D4" t="n" s="0">
         <v>0.0</v>

</xml_diff>

<commit_message>
More arrays and functional interfaces
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -3703,28 +3703,28 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="n" s="0">
-        <v>0.0</v>
+        <v>64.85714285714286</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>0.0</v>
+        <v>37.08666666666666</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>0.0</v>
+        <v>22.06</v>
       </c>
       <c r="D2" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>63.528703703703705</v>
+        <v>0.0</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>33.41111111111111</v>
+        <v>0.0</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>20.605555555555554</v>
-      </c>
-      <c r="H2" t="e" s="0">
-        <v>#NUM!</v>
+        <v>0.0</v>
+      </c>
+      <c r="H2" t="n" s="0">
+        <v>0.0</v>
       </c>
       <c r="K2" t="s" s="0">
         <v>52</v>
@@ -3732,28 +3732,28 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="n" s="0">
-        <v>0.0</v>
+        <v>87.63333333333334</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>0.0</v>
+        <v>47.040000000000006</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>0.0</v>
+        <v>38.28</v>
       </c>
       <c r="D3" t="n" s="0">
         <v>0.0</v>
       </c>
-      <c r="E3" t="e" s="0">
-        <v>#DIV/0!</v>
+      <c r="E3" t="n" s="0">
+        <v>0.0</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>26.0</v>
-      </c>
-      <c r="G3" t="e" s="0">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H3" t="e" s="0">
-        <v>#NUM!</v>
+        <v>0.0</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H3" t="n" s="0">
+        <v>0.0</v>
       </c>
       <c r="K3" t="s" s="0">
         <v>53</v>
@@ -3761,28 +3761,28 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="n" s="0">
-        <v>0.0</v>
+        <v>71.3075</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>0.0</v>
+        <v>27.790476190476188</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>0.0</v>
+        <v>28.46666666666667</v>
       </c>
       <c r="D4" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>70.23412698412699</v>
+        <v>0.0</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>18.35</v>
-      </c>
-      <c r="G4" t="e" s="0">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H4" t="e" s="0">
-        <v>#NUM!</v>
+        <v>0.0</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H4" t="n" s="0">
+        <v>0.0</v>
       </c>
       <c r="K4" t="s" s="0">
         <v>54</v>

</xml_diff>

<commit_message>
WEIGHTED AVERAGES WORK!! wooo
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFDA3BB-591D-425A-9B1F-43A56B362251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DA2D45-0CC5-416A-8DE0-6E17EC7C7EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
   <sheets>
     <sheet name="Match Data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="59">
   <si>
     <t>Cyrus</t>
   </si>
@@ -1684,8 +1684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
   <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1742,6 +1742,12 @@
       <c r="F2" s="0">
         <v>106</v>
       </c>
+      <c r="G2" s="0">
+        <v>-1</v>
+      </c>
+      <c r="H2" s="0">
+        <v>-1</v>
+      </c>
       <c r="I2" s="0">
         <v>0</v>
       </c>
@@ -1773,6 +1779,12 @@
       <c r="F3" s="0">
         <v>83</v>
       </c>
+      <c r="G3" s="0">
+        <v>-1</v>
+      </c>
+      <c r="H3" s="0">
+        <v>-1</v>
+      </c>
       <c r="I3" s="0">
         <v>0</v>
       </c>
@@ -1796,6 +1808,12 @@
       <c r="F4" s="0">
         <v>89</v>
       </c>
+      <c r="G4" s="0">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="0">
+        <v>-1</v>
+      </c>
       <c r="I4" s="0">
         <v>0</v>
       </c>
@@ -1820,6 +1838,12 @@
       <c r="F5" s="0">
         <v>71</v>
       </c>
+      <c r="G5" s="0">
+        <v>-1</v>
+      </c>
+      <c r="H5" s="0">
+        <v>-1</v>
+      </c>
       <c r="I5" s="0">
         <v>0</v>
       </c>
@@ -1843,6 +1867,12 @@
       <c r="F6" s="0">
         <v>88</v>
       </c>
+      <c r="G6" s="0">
+        <v>-1</v>
+      </c>
+      <c r="H6" s="0">
+        <v>-1</v>
+      </c>
       <c r="I6" s="0">
         <v>0</v>
       </c>
@@ -1866,6 +1896,12 @@
       <c r="F7" s="0">
         <v>111</v>
       </c>
+      <c r="G7" s="0">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="0">
+        <v>-1</v>
+      </c>
       <c r="I7" s="0">
         <v>0</v>
       </c>
@@ -1889,6 +1925,12 @@
       <c r="F8" s="0">
         <v>34</v>
       </c>
+      <c r="G8" s="0">
+        <v>-1</v>
+      </c>
+      <c r="H8" s="0">
+        <v>-1</v>
+      </c>
       <c r="I8" s="0">
         <v>0</v>
       </c>
@@ -1912,6 +1954,12 @@
       <c r="F9" s="0">
         <v>120</v>
       </c>
+      <c r="G9" s="0">
+        <v>-1</v>
+      </c>
+      <c r="H9" s="0">
+        <v>-1</v>
+      </c>
       <c r="I9" s="0">
         <v>0</v>
       </c>
@@ -1935,6 +1983,12 @@
       </c>
       <c r="F10" s="0">
         <v>75</v>
+      </c>
+      <c r="G10" s="0">
+        <v>-1</v>
+      </c>
+      <c r="H10" s="0">
+        <v>-1</v>
       </c>
       <c r="I10" s="0">
         <v>0</v>
@@ -3367,8 +3421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3670,7 +3724,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3714,17 +3768,20 @@
       <c r="D2" t="n" s="0">
         <v>0.0</v>
       </c>
-      <c r="E2" t="n" s="0">
+      <c r="E2" s="0" t="n">
+        <v>64.13627450980393</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>36.37936507936508</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>22.807936507936507</v>
+      </c>
+      <c r="H2" s="0" t="n">
         <v>0.0</v>
       </c>
-      <c r="F2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="G2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="H2" t="n" s="0">
-        <v>0.0</v>
+      <c r="J2" t="s" s="0">
+        <v>53</v>
       </c>
       <c r="K2" t="s" s="0">
         <v>52</v>
@@ -3734,25 +3791,25 @@
       <c r="A3" t="n" s="0">
         <v>87.63333333333334</v>
       </c>
-      <c r="B3" t="n" s="0">
+      <c r="B3" t="n">
         <v>47.040000000000006</v>
       </c>
-      <c r="C3" t="n" s="0">
+      <c r="C3" t="n">
         <v>38.28</v>
       </c>
-      <c r="D3" t="n" s="0">
+      <c r="D3" t="n">
         <v>0.0</v>
       </c>
-      <c r="E3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="F3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="G3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="H3" t="n" s="0">
+      <c r="E3" t="n">
+        <v>88.47222222222221</v>
+      </c>
+      <c r="F3" t="n">
+        <v>46.875</v>
+      </c>
+      <c r="G3" t="n">
+        <v>36.75</v>
+      </c>
+      <c r="H3" t="n">
         <v>0.0</v>
       </c>
       <c r="K3" t="s" s="0">
@@ -3763,25 +3820,25 @@
       <c r="A4" t="n" s="0">
         <v>71.3075</v>
       </c>
-      <c r="B4" t="n" s="0">
+      <c r="B4" t="n">
         <v>27.790476190476188</v>
       </c>
-      <c r="C4" t="n" s="0">
+      <c r="C4" t="n">
         <v>28.46666666666667</v>
       </c>
-      <c r="D4" t="n" s="0">
+      <c r="D4" t="n">
         <v>0.0</v>
       </c>
-      <c r="E4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="H4" t="n" s="0">
+      <c r="E4" t="n">
+        <v>75.03571428571428</v>
+      </c>
+      <c r="F4" t="n">
+        <v>28.160714285714285</v>
+      </c>
+      <c r="G4" t="n">
+        <v>28.42857142857143</v>
+      </c>
+      <c r="H4" t="n">
         <v>0.0</v>
       </c>
       <c r="K4" t="s" s="0">

</xml_diff>

<commit_message>
Some cleanup and transitioning to having a settings file
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DA2D45-0CC5-416A-8DE0-6E17EC7C7EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7BC124-7F1A-41A4-BD2F-892FE4F4EC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="59">
   <si>
     <t>Cyrus</t>
   </si>
@@ -194,9 +194,6 @@
     <t>*</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>B+M</t>
   </si>
   <si>
@@ -216,13 +213,15 @@
   </si>
   <si>
     <t>wAvgpen</t>
+  </si>
+  <si>
+    <t>&lt;- NEW ROBOT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1682,16 +1681,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
-  <dimension ref="A1:Y33"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -1724,31 +1723,31 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>45237</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>106</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>-1</v>
       </c>
-      <c r="H2" s="0">
+      <c r="H2">
         <v>-1</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2">
         <v>0</v>
       </c>
       <c r="M2" s="2"/>
@@ -1761,721 +1760,721 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>45237</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>83</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>-1</v>
       </c>
-      <c r="H3" s="0">
+      <c r="H3">
         <v>-1</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>45237</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4">
         <v>89</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4">
         <v>-1</v>
       </c>
-      <c r="H4" s="0">
+      <c r="H4">
         <v>-1</v>
       </c>
-      <c r="I4" s="0">
+      <c r="I4">
         <v>0</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>45238</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s" s="0">
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5">
         <v>71</v>
       </c>
-      <c r="G5" s="0">
+      <c r="G5">
         <v>-1</v>
       </c>
-      <c r="H5" s="0">
+      <c r="H5">
         <v>-1</v>
       </c>
-      <c r="I5" s="0">
+      <c r="I5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>45238</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>88</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6">
         <v>-1</v>
       </c>
-      <c r="H6" s="0">
+      <c r="H6">
         <v>-1</v>
       </c>
-      <c r="I6" s="0">
+      <c r="I6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>45238</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>111</v>
       </c>
-      <c r="G7" s="0">
+      <c r="G7">
         <v>-1</v>
       </c>
-      <c r="H7" s="0">
+      <c r="H7">
         <v>-1</v>
       </c>
-      <c r="I7" s="0">
+      <c r="I7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>45238</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <v>34</v>
       </c>
-      <c r="G8" s="0">
+      <c r="G8">
         <v>-1</v>
       </c>
-      <c r="H8" s="0">
+      <c r="H8">
         <v>-1</v>
       </c>
-      <c r="I8" s="0">
+      <c r="I8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>45238</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s" s="0">
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>120</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G9">
         <v>-1</v>
       </c>
-      <c r="H9" s="0">
+      <c r="H9">
         <v>-1</v>
       </c>
-      <c r="I9" s="0">
+      <c r="I9">
         <v>0</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>45238</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s" s="0">
+      <c r="E10" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="0">
+      <c r="F10">
         <v>75</v>
       </c>
-      <c r="G10" s="0">
+      <c r="G10">
         <v>-1</v>
       </c>
-      <c r="H10" s="0">
+      <c r="H10">
         <v>-1</v>
       </c>
-      <c r="I10" s="0">
+      <c r="I10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>45237</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>2</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="0">
+      <c r="F11">
         <v>111</v>
       </c>
-      <c r="G11" s="0">
+      <c r="G11">
         <v>66</v>
       </c>
-      <c r="H11" s="0">
+      <c r="H11">
         <v>45</v>
       </c>
-      <c r="I11" s="0">
+      <c r="I11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>45238</v>
       </c>
-      <c r="C12" t="s" s="0">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s" s="0">
+      <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s" s="0">
+      <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="0">
+      <c r="F12">
         <v>107</v>
       </c>
-      <c r="G12" s="0">
+      <c r="G12">
         <v>57</v>
       </c>
-      <c r="H12" s="0">
+      <c r="H12">
         <v>50</v>
       </c>
-      <c r="I12" s="0">
+      <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>45234</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>72</v>
       </c>
-      <c r="G13" s="0">
+      <c r="G13">
         <v>44</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <v>28</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s" s="0">
+      <c r="A14" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="1">
         <v>45234</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>97</v>
       </c>
-      <c r="G14" s="0">
+      <c r="G14">
         <v>51</v>
       </c>
-      <c r="H14" s="0">
+      <c r="H14">
         <v>30</v>
       </c>
-      <c r="I14" s="0">
+      <c r="I14">
         <v>0</v>
       </c>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s" s="0">
+      <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="1">
         <v>45234</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s" s="0">
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>54</v>
       </c>
-      <c r="G15" s="0">
+      <c r="G15">
         <v>26</v>
       </c>
-      <c r="H15" s="0">
+      <c r="H15">
         <v>28</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s" s="0">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>45234</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>82</v>
       </c>
-      <c r="G16" s="0">
+      <c r="G16">
         <v>32</v>
       </c>
-      <c r="H16" s="0">
+      <c r="H16">
         <v>50</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" t="s" s="0">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>45234</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>60</v>
       </c>
-      <c r="G17" s="0">
+      <c r="G17">
         <v>40</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H17">
         <v>20</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" t="s" s="0">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>45234</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s" s="0">
+      <c r="D18" t="s">
         <v>9</v>
       </c>
-      <c r="E18" t="s" s="0">
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>56</v>
       </c>
-      <c r="G18" s="0">
+      <c r="G18">
         <v>48</v>
       </c>
-      <c r="H18" s="0">
+      <c r="H18">
         <v>8</v>
       </c>
-      <c r="I18" s="0">
+      <c r="I18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" t="s" s="0">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>45234</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>60</v>
       </c>
-      <c r="G19" s="0">
+      <c r="G19">
         <v>30</v>
       </c>
-      <c r="H19" s="0">
+      <c r="H19">
         <v>30</v>
       </c>
-      <c r="I19" s="0">
+      <c r="I19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" t="s" s="0">
+      <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>45234</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s" s="0">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>39</v>
       </c>
-      <c r="G20" s="0">
+      <c r="G20">
         <v>34</v>
       </c>
-      <c r="H20" s="0">
+      <c r="H20">
         <v>5</v>
       </c>
-      <c r="I20" s="0">
+      <c r="I20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" t="s" s="0">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>45241</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s" s="0">
+      <c r="E21" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21">
         <v>32</v>
       </c>
-      <c r="G21" s="0">
+      <c r="G21">
         <v>4</v>
       </c>
-      <c r="H21" s="0">
+      <c r="H21">
         <v>28</v>
       </c>
-      <c r="I21" s="0">
-        <v>0</v>
-      </c>
-      <c r="K21" t="s" s="0">
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" t="s" s="0">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>45241</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>4</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>83</v>
       </c>
-      <c r="G22" s="0">
+      <c r="G22">
         <v>55</v>
       </c>
-      <c r="H22" s="0">
+      <c r="H22">
         <v>28</v>
       </c>
-      <c r="I22" s="0">
-        <v>0</v>
-      </c>
-      <c r="K22" t="s" s="0">
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" t="s" s="0">
+      <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>45241</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>3</v>
       </c>
-      <c r="D23" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E23" t="s" s="0">
+      <c r="D23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>56</v>
       </c>
-      <c r="G23" s="0">
+      <c r="G23">
         <v>26</v>
       </c>
-      <c r="H23" s="0">
+      <c r="H23">
         <v>30</v>
       </c>
-      <c r="I23" s="0">
-        <v>0</v>
-      </c>
-      <c r="K23" t="s" s="0">
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" t="s" s="0">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>45241</v>
       </c>
-      <c r="C24" t="s" s="0">
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" t="s" s="0">
+      <c r="D24" t="s">
         <v>9</v>
       </c>
-      <c r="E24" t="s" s="0">
+      <c r="E24" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="0">
+      <c r="F24">
         <v>33</v>
       </c>
-      <c r="G24" s="0">
+      <c r="G24">
         <v>28</v>
       </c>
-      <c r="H24" s="0">
+      <c r="H24">
         <v>5</v>
       </c>
-      <c r="I24" s="0">
-        <v>0</v>
-      </c>
-      <c r="K24" t="s" s="0">
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" t="s" s="0">
+      <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>45241</v>
       </c>
-      <c r="C25" t="s" s="0">
+      <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="D25" t="s" s="0">
+      <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" t="s" s="0">
+      <c r="E25" t="s">
         <v>1</v>
       </c>
-      <c r="F25" s="0">
+      <c r="F25">
         <v>56</v>
       </c>
-      <c r="G25" s="0">
+      <c r="G25">
         <v>36</v>
       </c>
-      <c r="H25" s="0">
+      <c r="H25">
         <v>20</v>
       </c>
-      <c r="I25" s="0">
-        <v>0</v>
-      </c>
-      <c r="K25" t="s" s="0">
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" t="s" s="0">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="1">
         <v>45241</v>
       </c>
-      <c r="C26" t="s" s="0">
+      <c r="C26" t="s">
         <v>3</v>
       </c>
-      <c r="D26" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s" s="0">
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="0">
+      <c r="F26">
         <v>55</v>
       </c>
-      <c r="G26" s="0">
+      <c r="G26">
         <v>27</v>
       </c>
-      <c r="H26" s="0">
+      <c r="H26">
         <v>28</v>
       </c>
-      <c r="I26" s="0">
-        <v>0</v>
-      </c>
-      <c r="K26" t="s" s="0">
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
         <v>50</v>
       </c>
       <c r="T26" s="5"/>
@@ -2485,21 +2484,16 @@
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
     </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="L27" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
       <c r="V31" s="5"/>
       <c r="W31" s="5"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" t="s" s="0">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s" s="0">
-        <v>51</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2521,8 +2515,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -2554,7 +2548,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="V2" t="s" s="0">
+      <c r="V2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2562,16 +2556,16 @@
       <c r="A3" s="1">
         <v>45237</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>106</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2579,25 +2573,25 @@
       <c r="A4" s="1">
         <v>45237</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>83</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" t="s" s="0">
+      <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="O4" t="s" s="0">
+      <c r="O4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2605,26 +2599,26 @@
       <c r="A5" s="1">
         <v>45237</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>89</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="M5" t="s" s="0">
+      <c r="M5" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="0">
+      <c r="N5">
         <f>(SUMIF($C$3:$C$100, M5, $B$3:$B$100)/COUNTIF($C$3:$C$100, M5))</f>
         <v>88.083333333333329</v>
       </c>
-      <c r="O5" s="0">
+      <c r="O5">
         <f>(SUMIF($C$3:$C$100, M5, $F$3:$F$100)/COUNTIF($C$13:$C$100, M5))</f>
         <v>42.428571428571431</v>
       </c>
@@ -2633,26 +2627,26 @@
       <c r="A6" s="1">
         <v>45238</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>71</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s" s="0">
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="M6" t="s" s="0">
+      <c r="M6" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="0">
+      <c r="N6">
         <f>(SUMIF($C$3:$C$100, M6, $B$3:$B$100)/COUNTIF($C$3:$C$100, M6))</f>
         <v>98.5</v>
       </c>
-      <c r="O6" s="0">
+      <c r="O6">
         <f>(SUMIF($C$3:$C$100, M6, $F$3:$F$100)/COUNTIF($C$13:$C$100, M6))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2661,26 +2655,26 @@
       <c r="A7" s="1">
         <v>45238</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>88</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="M7" t="s" s="0">
+      <c r="M7" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="0">
+      <c r="N7">
         <f>(SUMIF($C$3:$C$100, M7, $B$3:$B$100)/COUNTIF($C$3:$C$100, M7))</f>
         <v>86.25</v>
       </c>
-      <c r="O7" s="0">
+      <c r="O7">
         <f>(SUMIF($C$3:$C$100, M7, $F$3:$F$100)/COUNTIF($C$13:$C$100, M7))</f>
         <v>38</v>
       </c>
@@ -2689,16 +2683,16 @@
       <c r="A8" s="1">
         <v>45238</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8">
         <v>111</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>2</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2706,16 +2700,16 @@
       <c r="A9" s="1">
         <v>45238</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9">
         <v>34</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -2726,16 +2720,16 @@
       <c r="A10" s="1">
         <v>45238</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10">
         <v>120</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s" s="0">
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -2744,14 +2738,14 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="M10" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="N10" s="0">
+      <c r="M10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <f>(SUMIF($D$3:$D$100, M10, $B$3:$B$100)/COUNTIF($D$3:$D$100, M10))</f>
         <v>96.666666666666671</v>
       </c>
-      <c r="O10" s="0">
+      <c r="O10">
         <f>(SUMIF($D$3:$D$100, M10, $F$3:$F$100)/COUNTIF($D$13:$D$100, M10))</f>
         <v>26</v>
       </c>
@@ -2760,16 +2754,16 @@
       <c r="A11" s="1">
         <v>45238</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11">
         <v>75</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -2780,14 +2774,14 @@
         <v>22</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="M11" t="s" s="0">
+      <c r="M11" t="s">
         <v>9</v>
       </c>
-      <c r="N11" s="0">
+      <c r="N11">
         <f>(SUMIF($D$3:$D$100, M11, $B$3:$B$100)/COUNTIF($D$3:$D$100, M11))</f>
         <v>77</v>
       </c>
-      <c r="O11" s="0">
+      <c r="O11">
         <f>(SUMIF($D$3:$D$100, M11, $F$3:$F$100)/COUNTIF($D$13:$D$100, M11))</f>
         <v>45.166666666666664</v>
       </c>
@@ -2805,14 +2799,14 @@
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s" s="0">
+      <c r="M12" t="s">
         <v>2</v>
       </c>
-      <c r="N12" s="0">
+      <c r="N12">
         <f>(SUMIF($D$3:$D$100, M12, $B$3:$B$100)/COUNTIF($D$3:$D$100, M12))</f>
         <v>97.75</v>
       </c>
-      <c r="O12" s="0">
+      <c r="O12">
         <f>(SUMIF($D$3:$D$100, M12, $F$3:$F$100)/COUNTIF($D$13:$D$100, M12))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2821,26 +2815,26 @@
       <c r="A13" s="1">
         <v>45237</v>
       </c>
-      <c r="B13" s="0">
+      <c r="B13">
         <v>111</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>66</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <f t="shared" ref="H13:H23" si="0">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12)+SUMIF($M$15:$M$17, $E13, $N$15:$N$17))/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <f t="shared" ref="I13:I23" si="1">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12)+SUMIF($M$15:$M$17, $E13, $O$15:$O$17))/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -2848,7 +2842,7 @@
         <f t="shared" ref="J13:J23" si="2">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12))/2</f>
         <v>98.125</v>
       </c>
-      <c r="K13" s="0">
+      <c r="K13">
         <f t="shared" ref="K13:K23" si="3">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12))/2</f>
         <v>57.333333333333336</v>
       </c>
@@ -2857,26 +2851,26 @@
       <c r="A14" s="1">
         <v>45238</v>
       </c>
-      <c r="B14" s="0">
+      <c r="B14">
         <v>107</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>57</v>
       </c>
-      <c r="H14" s="0">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>84.49444444444444</v>
       </c>
-      <c r="I14" s="0">
+      <c r="I14">
         <f t="shared" si="1"/>
         <v>48.198412698412703</v>
       </c>
@@ -2884,7 +2878,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K14" s="0">
+      <c r="K14">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -2896,26 +2890,26 @@
       <c r="A15" s="1">
         <v>45234</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15">
         <v>108</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s" s="0">
+      <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="s" s="0">
+      <c r="E15" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>38</v>
       </c>
-      <c r="H15" s="0">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>63.166666666666664</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15">
         <f t="shared" si="1"/>
         <v>30.166666666666668</v>
       </c>
@@ -2923,18 +2917,18 @@
         <f t="shared" si="2"/>
         <v>43.125</v>
       </c>
-      <c r="K15" s="0">
+      <c r="K15">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="M15" t="s" s="0">
+      <c r="M15" t="s">
         <v>10</v>
       </c>
-      <c r="N15" s="0">
+      <c r="N15">
         <f>(SUMIF($E$3:$E$100, M15, $B$3:$B$100)/COUNTIF($E$3:$E$100, M15))</f>
         <v>83.166666666666671</v>
       </c>
-      <c r="O15" s="0">
+      <c r="O15">
         <f>(SUMIF($E$3:$E$100, M15, $F$3:$F$100)/COUNTIF($E$13:$E$100, M15))</f>
         <v>40</v>
       </c>
@@ -2943,26 +2937,26 @@
       <c r="A16" s="1">
         <v>45234</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16">
         <v>107</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>74</v>
       </c>
-      <c r="H16" s="0">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -2970,18 +2964,18 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K16" s="0">
+      <c r="K16">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
-      <c r="M16" t="s" s="0">
+      <c r="M16" t="s">
         <v>1</v>
       </c>
-      <c r="N16" s="0">
+      <c r="N16">
         <f>(SUMIF($E$3:$E$100, M16, $B$3:$B$100)/COUNTIF($E$3:$E$100, M16))</f>
         <v>88.4</v>
       </c>
-      <c r="O16" s="0">
+      <c r="O16">
         <f>(SUMIF($E$3:$E$100, M16, $F$3:$F$100)/COUNTIF($E$13:$E$100, M16))</f>
         <v>57</v>
       </c>
@@ -2990,26 +2984,26 @@
       <c r="A17" s="1">
         <v>45234</v>
       </c>
-      <c r="B17" s="0">
+      <c r="B17">
         <v>97</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>62</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I17">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3017,18 +3011,18 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K17" s="0">
+      <c r="K17">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
-      <c r="M17" t="s" s="0">
+      <c r="M17" t="s">
         <v>5</v>
       </c>
-      <c r="N17" s="0">
+      <c r="N17">
         <f>(SUMIF($E$3:$E$100, M17, $B$3:$B$100)/COUNTIF($E$3:$E$100, M17))</f>
         <v>103.25</v>
       </c>
-      <c r="O17" s="0">
+      <c r="O17">
         <f>(SUMIF($E$3:$E$100, M17, $F$3:$F$100)/COUNTIF($E$13:$E$100, M17))</f>
         <v>52.5</v>
       </c>
@@ -3037,26 +3031,26 @@
       <c r="A18" s="1">
         <v>45234</v>
       </c>
-      <c r="B18" s="0">
+      <c r="B18">
         <v>99</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s" s="0">
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>26</v>
       </c>
-      <c r="H18" s="0">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>89.305555555555557</v>
       </c>
-      <c r="I18" s="0">
+      <c r="I18">
         <f t="shared" si="1"/>
         <v>36.142857142857146</v>
       </c>
@@ -3064,7 +3058,7 @@
         <f t="shared" si="2"/>
         <v>92.375</v>
       </c>
-      <c r="K18" s="0">
+      <c r="K18">
         <f t="shared" si="3"/>
         <v>34.214285714285715</v>
       </c>
@@ -3073,26 +3067,26 @@
       <c r="A19" s="1">
         <v>45234</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19">
         <v>87</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>2</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>32</v>
       </c>
-      <c r="H19" s="0">
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I19" s="0">
+      <c r="I19">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -3100,7 +3094,7 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K19" s="0">
+      <c r="K19">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
@@ -3109,26 +3103,26 @@
       <c r="A20" s="1">
         <v>45234</v>
       </c>
-      <c r="B20" s="0">
+      <c r="B20">
         <v>76</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s" s="0">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>48</v>
       </c>
-      <c r="H20" s="0">
+      <c r="H20">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I20" s="0">
+      <c r="I20">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3136,7 +3130,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K20" s="0">
+      <c r="K20">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3145,26 +3139,26 @@
       <c r="A21" s="1">
         <v>45234</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21">
         <v>93</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s" s="0">
+      <c r="E21" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21">
         <v>40</v>
       </c>
-      <c r="H21" s="0">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I21" s="0">
+      <c r="I21">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3172,7 +3166,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K21" s="0">
+      <c r="K21">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3181,26 +3175,26 @@
       <c r="A22" s="1">
         <v>45234</v>
       </c>
-      <c r="B22" s="0">
+      <c r="B22">
         <v>85</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>30</v>
       </c>
-      <c r="H22" s="0">
+      <c r="H22">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I22" s="0">
+      <c r="I22">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3208,7 +3202,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K22" s="0">
+      <c r="K22">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3217,26 +3211,26 @@
       <c r="A23" s="1">
         <v>45234</v>
       </c>
-      <c r="B23" s="0">
+      <c r="B23">
         <v>49</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>11</v>
       </c>
-      <c r="D23" t="s" s="0">
+      <c r="D23" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s" s="0">
+      <c r="E23" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>34</v>
       </c>
-      <c r="H23" s="0">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I23" s="0">
+      <c r="I23">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3244,7 +3238,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K23" s="0">
+      <c r="K23">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3264,67 +3258,67 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T28" s="0">
+      <c r="T28">
         <v>1</v>
       </c>
-      <c r="U28" t="s" s="0">
+      <c r="U28" t="s">
         <v>3</v>
       </c>
-      <c r="V28" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="W28" t="s" s="0">
+      <c r="V28" t="s">
+        <v>0</v>
+      </c>
+      <c r="W28" t="s">
         <v>1</v>
       </c>
-      <c r="X28" s="0">
+      <c r="X28">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y28" s="0">
+      <c r="Y28">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T29" s="0">
+      <c r="T29">
         <v>2</v>
       </c>
-      <c r="U29" t="s" s="0">
+      <c r="U29" t="s">
         <v>11</v>
       </c>
-      <c r="V29" t="s" s="0">
+      <c r="V29" t="s">
         <v>9</v>
       </c>
-      <c r="W29" t="s" s="0">
+      <c r="W29" t="s">
         <v>1</v>
       </c>
-      <c r="X29" s="0">
+      <c r="X29">
         <f>(N5+N11+N16)/3</f>
         <v>84.49444444444444</v>
       </c>
-      <c r="Y29" s="0">
+      <c r="Y29">
         <f>(O5+O11+O16)/3</f>
         <v>48.198412698412703</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T30" s="0">
+      <c r="T30">
         <v>3</v>
       </c>
-      <c r="U30" t="s" s="0">
+      <c r="U30" t="s">
         <v>4</v>
       </c>
-      <c r="V30" t="s" s="0">
+      <c r="V30" t="s">
         <v>9</v>
       </c>
-      <c r="W30" t="s" s="0">
+      <c r="W30" t="s">
         <v>1</v>
       </c>
-      <c r="X30" s="0">
+      <c r="X30">
         <f>(N6+N11+N16)/3</f>
         <v>87.966666666666654</v>
       </c>
-      <c r="Y30" s="0">
+      <c r="Y30">
         <f>(O6+O11+O16)/3</f>
         <v>53.166666666666664</v>
       </c>
@@ -3338,67 +3332,67 @@
       <c r="W32" s="5"/>
     </row>
     <row r="33" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T33" s="0">
+      <c r="T33">
         <v>1</v>
       </c>
-      <c r="U33" t="s" s="0">
+      <c r="U33" t="s">
         <v>3</v>
       </c>
-      <c r="V33" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="W33" t="s" s="0">
+      <c r="V33" t="s">
+        <v>0</v>
+      </c>
+      <c r="W33" t="s">
         <v>1</v>
       </c>
-      <c r="X33" s="0">
+      <c r="X33">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y33" s="0">
+      <c r="Y33">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="34" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T34" s="0">
+      <c r="T34">
         <v>2</v>
       </c>
-      <c r="U34" t="s" s="0">
+      <c r="U34" t="s">
         <v>11</v>
       </c>
-      <c r="V34" t="s" s="0">
+      <c r="V34" t="s">
         <v>9</v>
       </c>
-      <c r="W34" t="s" s="0">
+      <c r="W34" t="s">
         <v>10</v>
       </c>
-      <c r="X34" s="0">
+      <c r="X34">
         <f>(N5+N11+N15)/3</f>
         <v>82.75</v>
       </c>
-      <c r="Y34" s="0">
+      <c r="Y34">
         <f>(O5+O11+O15)/3</f>
         <v>42.531746031746032</v>
       </c>
     </row>
     <row r="35" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T35" s="0">
+      <c r="T35">
         <v>3</v>
       </c>
-      <c r="U35" t="s" s="0">
+      <c r="U35" t="s">
         <v>4</v>
       </c>
-      <c r="V35" t="s" s="0">
+      <c r="V35" t="s">
         <v>2</v>
       </c>
-      <c r="W35" t="s" s="0">
+      <c r="W35" t="s">
         <v>5</v>
       </c>
-      <c r="X35" s="0">
+      <c r="X35">
         <f>(N6+N12+N17)/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="Y35" s="0">
+      <c r="Y35">
         <f>(O6+O12+O17)/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -3422,295 +3416,295 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="n" s="0">
-        <v>70.64285714285714</v>
-      </c>
-      <c r="B2" t="n" s="0">
+      <c r="A2">
+        <v>70.642857142857139</v>
+      </c>
+      <c r="B2">
         <v>35.333333333333336</v>
       </c>
-      <c r="C2" t="n" s="0">
+      <c r="C2">
         <v>22.666666666666668</v>
       </c>
-      <c r="D2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E2" t="n" s="0">
-        <v>70.55495978554524</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>34.54700854721421</v>
-      </c>
-      <c r="G2" t="n" s="0">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>70.554959785545236</v>
+      </c>
+      <c r="F2">
+        <v>34.547008547214212</v>
+      </c>
+      <c r="G2">
         <v>22.764957264931564</v>
       </c>
-      <c r="H2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M2" t="s" s="0">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="n" s="0">
-        <v>82.16666666666667</v>
-      </c>
-      <c r="B3" t="n" s="0">
+      <c r="A3">
+        <v>82.166666666666671</v>
+      </c>
+      <c r="B3">
         <v>46.6</v>
       </c>
-      <c r="C3" t="n" s="0">
-        <v>34.2</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E3" t="n" s="0">
-        <v>81.73780487815547</v>
-      </c>
-      <c r="F3" t="n" s="0">
+      <c r="C3">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>81.737804878155472</v>
+      </c>
+      <c r="F3">
         <v>46.912408759046556</v>
       </c>
-      <c r="G3" t="n" s="0">
+      <c r="G3">
         <v>33.394160584141595</v>
       </c>
-      <c r="H3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M3" t="s" s="0">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="n" s="0">
-        <v>69.6</v>
-      </c>
-      <c r="B4" t="n" s="0">
+      <c r="A4">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="B4">
         <v>26.5</v>
       </c>
-      <c r="C4" t="n" s="0">
-        <v>29.0</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E4" t="n" s="0">
-        <v>68.92413793119296</v>
-      </c>
-      <c r="F4" t="n" s="0">
+      <c r="C4">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>68.924137931192959</v>
+      </c>
+      <c r="F4">
         <v>26.499999999999996</v>
       </c>
-      <c r="G4" t="n" s="0">
-        <v>29.0</v>
-      </c>
-      <c r="H4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M4" t="s" s="0">
+      <c r="G4">
+        <v>29</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="n" s="0">
-        <v>61.0</v>
-      </c>
-      <c r="B5" t="n" s="0">
-        <v>38.3</v>
-      </c>
-      <c r="C5" t="n" s="0">
+      <c r="A5">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="C5">
         <v>22.4</v>
       </c>
-      <c r="D5" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E5" t="n" s="0">
-        <v>60.54878048791714</v>
-      </c>
-      <c r="F5" t="n" s="0">
-        <v>37.79779411777262</v>
-      </c>
-      <c r="G5" t="n" s="0">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>60.548780487917142</v>
+      </c>
+      <c r="F5">
+        <v>37.797794117772618</v>
+      </c>
+      <c r="G5">
         <v>22.584558823483277</v>
       </c>
-      <c r="H5" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M5" t="s" s="0">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="n" s="0">
+      <c r="A6">
         <v>92.75</v>
       </c>
-      <c r="B6" t="n" s="0">
+      <c r="B6">
         <v>47.333333333333336</v>
       </c>
-      <c r="C6" t="n" s="0">
-        <v>41.0</v>
-      </c>
-      <c r="D6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E6" t="n" s="0">
-        <v>93.25943396213344</v>
-      </c>
-      <c r="F6" t="n" s="0">
+      <c r="C6">
+        <v>41</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>93.259433962133443</v>
+      </c>
+      <c r="F6">
         <v>48.079999999796904</v>
       </c>
-      <c r="G6" t="n" s="0">
-        <v>41.15999999995648</v>
-      </c>
-      <c r="H6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M6" t="s" s="0">
+      <c r="G6">
+        <v>41.159999999956483</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="n" s="0">
+      <c r="A7">
         <v>71.2</v>
       </c>
-      <c r="B7" t="n" s="0">
+      <c r="B7">
         <v>26.333333333333332</v>
       </c>
-      <c r="C7" t="n" s="0">
+      <c r="C7">
         <v>28.666666666666668</v>
       </c>
-      <c r="D7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E7" t="n" s="0">
-        <v>71.02112676060621</v>
-      </c>
-      <c r="F7" t="n" s="0">
-        <v>26.36046511627264</v>
-      </c>
-      <c r="G7" t="n" s="0">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>71.021126760606208</v>
+      </c>
+      <c r="F7">
+        <v>26.360465116272639</v>
+      </c>
+      <c r="G7">
         <v>28.720930232545275</v>
       </c>
-      <c r="H7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M7" t="s" s="0">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="n" s="0">
-        <v>61.0</v>
-      </c>
-      <c r="B8" t="n" s="0">
+      <c r="A8">
+        <v>61</v>
+      </c>
+      <c r="B8">
         <v>38.166666666666664</v>
       </c>
-      <c r="C8" t="n" s="0">
+      <c r="C8">
         <v>20.166666666666668</v>
       </c>
-      <c r="D8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E8" t="n" s="0">
-        <v>61.00000000000001</v>
-      </c>
-      <c r="F8" t="n" s="0">
-        <v>38.16666666666667</v>
-      </c>
-      <c r="G8" t="n" s="0">
-        <v>20.16666666666667</v>
-      </c>
-      <c r="H8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M8" t="s" s="0">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>61.000000000000007</v>
+      </c>
+      <c r="F8">
+        <v>38.166666666666671</v>
+      </c>
+      <c r="G8">
+        <v>20.166666666666671</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="n" s="0">
-        <v>88.33333333333333</v>
-      </c>
-      <c r="B9" t="n" s="0">
+      <c r="A9">
+        <v>88.333333333333329</v>
+      </c>
+      <c r="B9">
         <v>47.333333333333336</v>
       </c>
-      <c r="C9" t="n" s="0">
-        <v>41.0</v>
-      </c>
-      <c r="D9" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E9" t="n" s="0">
-        <v>89.2399999997534</v>
-      </c>
-      <c r="F9" t="n" s="0">
+      <c r="C9">
+        <v>41</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>89.239999999753394</v>
+      </c>
+      <c r="F9">
         <v>48.079999999796904</v>
       </c>
-      <c r="G9" t="n" s="0">
-        <v>41.15999999995648</v>
-      </c>
-      <c r="H9" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M9" t="s" s="0">
+      <c r="G9">
+        <v>41.159999999956483</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="n" s="0">
+      <c r="A10">
         <v>74.9375</v>
       </c>
-      <c r="B10" t="n" s="0">
+      <c r="B10">
         <v>33.285714285714285</v>
       </c>
-      <c r="C10" t="n" s="0">
-        <v>27.0</v>
-      </c>
-      <c r="D10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E10" t="n" s="0">
+      <c r="C10">
+        <v>27</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>73.95032397431406</v>
       </c>
-      <c r="F10" t="n" s="0">
-        <v>32.95327102811133</v>
-      </c>
-      <c r="G10" t="n" s="0">
+      <c r="F10">
+        <v>32.953271028111331</v>
+      </c>
+      <c r="G10">
         <v>26.67757009352966</v>
       </c>
-      <c r="H10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M10" t="s" s="0">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3724,125 +3718,122 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="G1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" t="s" s="0">
-        <v>58</v>
-      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="n" s="0">
-        <v>64.85714285714286</v>
-      </c>
-      <c r="B2" t="n" s="0">
-        <v>37.08666666666666</v>
-      </c>
-      <c r="C2" t="n" s="0">
+      <c r="A2">
+        <v>64.857142857142861</v>
+      </c>
+      <c r="B2">
+        <v>37.086666666666659</v>
+      </c>
+      <c r="C2">
         <v>22.06</v>
       </c>
-      <c r="D2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>64.13627450980393</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>64.136274509803926</v>
+      </c>
+      <c r="F2">
         <v>36.37936507936508</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2">
         <v>22.807936507936507</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J2" t="s" s="0">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>87.63333333333334</v>
+      </c>
+      <c r="B3">
+        <v>47.040000000000006</v>
+      </c>
+      <c r="C3">
+        <v>38.28</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>88.472222222222214</v>
+      </c>
+      <c r="F3">
+        <v>46.875</v>
+      </c>
+      <c r="G3">
+        <v>36.75</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>71.307500000000005</v>
+      </c>
+      <c r="B4">
+        <v>27.790476190476188</v>
+      </c>
+      <c r="C4">
+        <v>28.466666666666669</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>75.035714285714278</v>
+      </c>
+      <c r="F4">
+        <v>28.160714285714285</v>
+      </c>
+      <c r="G4">
+        <v>28.428571428571431</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
         <v>53</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="n" s="0">
-        <v>87.63333333333334</v>
-      </c>
-      <c r="B3" t="n">
-        <v>47.040000000000006</v>
-      </c>
-      <c r="C3" t="n">
-        <v>38.28</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>88.47222222222221</v>
-      </c>
-      <c r="F3" t="n">
-        <v>46.875</v>
-      </c>
-      <c r="G3" t="n">
-        <v>36.75</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="n" s="0">
-        <v>71.3075</v>
-      </c>
-      <c r="B4" t="n">
-        <v>27.790476190476188</v>
-      </c>
-      <c r="C4" t="n">
-        <v>28.46666666666667</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>75.03571428571428</v>
-      </c>
-      <c r="F4" t="n">
-        <v>28.160714285714285</v>
-      </c>
-      <c r="G4" t="n">
-        <v>28.42857142857143</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K4" t="s" s="0">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a new file that I'm messing with for UI
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -222,6 +222,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1689,8 +1690,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="10.0"/>
+    <col min="5" max="5" customWidth="true" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -1723,31 +1724,31 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>45237</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>106</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>-1</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0">
         <v>-1</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>0</v>
       </c>
       <c r="M2" s="2"/>
@@ -1760,721 +1761,721 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>45237</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>83</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>-1</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0">
         <v>-1</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>45237</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>89</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>-1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0">
         <v>-1</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>0</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>45238</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>71</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>-1</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0">
         <v>-1</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>45238</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>88</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>-1</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0">
         <v>-1</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>45238</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>111</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>-1</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0">
         <v>-1</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>45238</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>34</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>-1</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="0">
         <v>-1</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>45238</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>120</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>-1</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="0">
         <v>-1</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="0">
         <v>0</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>45238</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="0">
         <v>75</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="0">
         <v>-1</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="0">
         <v>-1</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>45237</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="0">
         <v>111</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="0">
         <v>66</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="0">
         <v>45</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>45238</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="0">
         <v>107</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="0">
         <v>57</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="0">
         <v>50</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="0">
         <v>0</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>45234</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>72</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="0">
         <v>44</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0">
         <v>28</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B14" s="1">
         <v>45234</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0">
         <v>97</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="0">
         <v>51</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="0">
         <v>30</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="0">
         <v>0</v>
       </c>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B15" s="1">
         <v>45234</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>54</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="0">
         <v>26</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="0">
         <v>28</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>45234</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>82</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="0">
         <v>32</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="0">
         <v>50</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>45234</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>60</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="0">
         <v>40</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="0">
         <v>20</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>45234</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>56</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="0">
         <v>48</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0">
         <v>8</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>45234</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>60</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="0">
         <v>30</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0">
         <v>30</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>45234</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>39</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="0">
         <v>34</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0">
         <v>5</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>45241</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="0">
         <v>32</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="0">
         <v>4</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="0">
         <v>28</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="0">
         <v>0</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>45241</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="0">
         <v>83</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="0">
         <v>55</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="0">
         <v>28</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="0">
         <v>0</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>45241</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>56</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="0">
         <v>26</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="0">
         <v>30</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="0">
         <v>0</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>45241</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="0">
         <v>33</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="0">
         <v>28</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="0">
         <v>5</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="0">
         <v>0</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>45241</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="0">
         <v>56</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="0">
         <v>36</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="0">
         <v>20</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="0">
         <v>0</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B26" s="1">
         <v>45241</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="0">
         <v>55</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="0">
         <v>27</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="0">
         <v>28</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="0">
         <v>0</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" t="s" s="0">
         <v>50</v>
       </c>
       <c r="T26" s="5"/>
@@ -2485,7 +2486,7 @@
       <c r="Y26" s="2"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="L27" t="s">
+      <c r="L27" t="s" s="0">
         <v>58</v>
       </c>
     </row>
@@ -2515,8 +2516,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="10.0"/>
+    <col min="5" max="5" customWidth="true" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -2548,7 +2549,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="V2" t="s">
+      <c r="V2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
@@ -2556,16 +2557,16 @@
       <c r="A3" s="1">
         <v>45237</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>106</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -2573,25 +2574,25 @@
       <c r="A4" s="1">
         <v>45237</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>83</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" t="s" s="0">
         <v>24</v>
       </c>
     </row>
@@ -2599,26 +2600,26 @@
       <c r="A5" s="1">
         <v>45237</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>89</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="0">
         <f>(SUMIF($C$3:$C$100, M5, $B$3:$B$100)/COUNTIF($C$3:$C$100, M5))</f>
         <v>88.083333333333329</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="0">
         <f>(SUMIF($C$3:$C$100, M5, $F$3:$F$100)/COUNTIF($C$13:$C$100, M5))</f>
         <v>42.428571428571431</v>
       </c>
@@ -2627,26 +2628,26 @@
       <c r="A6" s="1">
         <v>45238</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>71</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="0">
         <f>(SUMIF($C$3:$C$100, M6, $B$3:$B$100)/COUNTIF($C$3:$C$100, M6))</f>
         <v>98.5</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="0">
         <f>(SUMIF($C$3:$C$100, M6, $F$3:$F$100)/COUNTIF($C$13:$C$100, M6))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2655,26 +2656,26 @@
       <c r="A7" s="1">
         <v>45238</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>88</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="0">
         <f>(SUMIF($C$3:$C$100, M7, $B$3:$B$100)/COUNTIF($C$3:$C$100, M7))</f>
         <v>86.25</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="0">
         <f>(SUMIF($C$3:$C$100, M7, $F$3:$F$100)/COUNTIF($C$13:$C$100, M7))</f>
         <v>38</v>
       </c>
@@ -2683,16 +2684,16 @@
       <c r="A8" s="1">
         <v>45238</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>111</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -2700,16 +2701,16 @@
       <c r="A9" s="1">
         <v>45238</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -2720,16 +2721,16 @@
       <c r="A10" s="1">
         <v>45238</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <v>120</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -2738,14 +2739,14 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="M10" t="s">
+      <c r="M10" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="0">
         <f>(SUMIF($D$3:$D$100, M10, $B$3:$B$100)/COUNTIF($D$3:$D$100, M10))</f>
         <v>96.666666666666671</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="0">
         <f>(SUMIF($D$3:$D$100, M10, $F$3:$F$100)/COUNTIF($D$13:$D$100, M10))</f>
         <v>26</v>
       </c>
@@ -2754,16 +2755,16 @@
       <c r="A11" s="1">
         <v>45238</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0">
         <v>75</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>1</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -2774,14 +2775,14 @@
         <v>22</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="M11" t="s">
+      <c r="M11" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="0">
         <f>(SUMIF($D$3:$D$100, M11, $B$3:$B$100)/COUNTIF($D$3:$D$100, M11))</f>
         <v>77</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="0">
         <f>(SUMIF($D$3:$D$100, M11, $F$3:$F$100)/COUNTIF($D$13:$D$100, M11))</f>
         <v>45.166666666666664</v>
       </c>
@@ -2799,14 +2800,14 @@
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="0">
         <f>(SUMIF($D$3:$D$100, M12, $B$3:$B$100)/COUNTIF($D$3:$D$100, M12))</f>
         <v>97.75</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="0">
         <f>(SUMIF($D$3:$D$100, M12, $F$3:$F$100)/COUNTIF($D$13:$D$100, M12))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2815,26 +2816,26 @@
       <c r="A13" s="1">
         <v>45237</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="0">
         <v>111</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>66</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0">
         <f t="shared" ref="H13:H23" si="0">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12)+SUMIF($M$15:$M$17, $E13, $N$15:$N$17))/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="0">
         <f t="shared" ref="I13:I23" si="1">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12)+SUMIF($M$15:$M$17, $E13, $O$15:$O$17))/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -2842,7 +2843,7 @@
         <f t="shared" ref="J13:J23" si="2">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12))/2</f>
         <v>98.125</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="0">
         <f t="shared" ref="K13:K23" si="3">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12))/2</f>
         <v>57.333333333333336</v>
       </c>
@@ -2851,26 +2852,26 @@
       <c r="A14" s="1">
         <v>45238</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="0">
         <v>107</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0">
         <v>57</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="0">
         <f t="shared" si="0"/>
         <v>84.49444444444444</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="0">
         <f t="shared" si="1"/>
         <v>48.198412698412703</v>
       </c>
@@ -2878,7 +2879,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -2890,26 +2891,26 @@
       <c r="A15" s="1">
         <v>45234</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="0">
         <v>108</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>38</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="0">
         <f t="shared" si="0"/>
         <v>63.166666666666664</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="0">
         <f t="shared" si="1"/>
         <v>30.166666666666668</v>
       </c>
@@ -2917,18 +2918,18 @@
         <f t="shared" si="2"/>
         <v>43.125</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="0">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="0">
         <f>(SUMIF($E$3:$E$100, M15, $B$3:$B$100)/COUNTIF($E$3:$E$100, M15))</f>
         <v>83.166666666666671</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="0">
         <f>(SUMIF($E$3:$E$100, M15, $F$3:$F$100)/COUNTIF($E$13:$E$100, M15))</f>
         <v>40</v>
       </c>
@@ -2937,26 +2938,26 @@
       <c r="A16" s="1">
         <v>45234</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="0">
         <v>107</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>74</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="0">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="0">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -2964,18 +2965,18 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="0">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="0">
         <f>(SUMIF($E$3:$E$100, M16, $B$3:$B$100)/COUNTIF($E$3:$E$100, M16))</f>
         <v>88.4</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="0">
         <f>(SUMIF($E$3:$E$100, M16, $F$3:$F$100)/COUNTIF($E$13:$E$100, M16))</f>
         <v>57</v>
       </c>
@@ -2984,26 +2985,26 @@
       <c r="A17" s="1">
         <v>45234</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="0">
         <v>97</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>62</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3011,18 +3012,18 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="0">
         <f>(SUMIF($E$3:$E$100, M17, $B$3:$B$100)/COUNTIF($E$3:$E$100, M17))</f>
         <v>103.25</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="0">
         <f>(SUMIF($E$3:$E$100, M17, $F$3:$F$100)/COUNTIF($E$13:$E$100, M17))</f>
         <v>52.5</v>
       </c>
@@ -3031,26 +3032,26 @@
       <c r="A18" s="1">
         <v>45234</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="0">
         <v>99</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>26</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0">
         <f t="shared" si="0"/>
         <v>89.305555555555557</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="0">
         <f t="shared" si="1"/>
         <v>36.142857142857146</v>
       </c>
@@ -3058,7 +3059,7 @@
         <f t="shared" si="2"/>
         <v>92.375</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="0">
         <f t="shared" si="3"/>
         <v>34.214285714285715</v>
       </c>
@@ -3067,26 +3068,26 @@
       <c r="A19" s="1">
         <v>45234</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="0">
         <v>87</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>32</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="0">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -3094,7 +3095,7 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="0">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
@@ -3103,26 +3104,26 @@
       <c r="A20" s="1">
         <v>45234</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="0">
         <v>76</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>48</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3130,7 +3131,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3139,26 +3140,26 @@
       <c r="A21" s="1">
         <v>45234</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="0">
         <v>93</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="0">
         <v>40</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3166,7 +3167,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3175,26 +3176,26 @@
       <c r="A22" s="1">
         <v>45234</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="0">
         <v>85</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="0">
         <v>30</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3202,7 +3203,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3211,26 +3212,26 @@
       <c r="A23" s="1">
         <v>45234</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="0">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>34</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3238,7 +3239,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3258,67 +3259,67 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T28">
+      <c r="T28" s="0">
         <v>1</v>
       </c>
-      <c r="U28" t="s">
+      <c r="U28" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="V28" t="s">
+      <c r="V28" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="W28" t="s">
+      <c r="W28" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X28">
+      <c r="X28" s="0">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y28">
+      <c r="Y28" s="0">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T29">
+      <c r="T29" s="0">
         <v>2</v>
       </c>
-      <c r="U29" t="s">
+      <c r="U29" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="V29" t="s">
+      <c r="V29" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W29" t="s">
+      <c r="W29" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X29">
+      <c r="X29" s="0">
         <f>(N5+N11+N16)/3</f>
         <v>84.49444444444444</v>
       </c>
-      <c r="Y29">
+      <c r="Y29" s="0">
         <f>(O5+O11+O16)/3</f>
         <v>48.198412698412703</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T30">
+      <c r="T30" s="0">
         <v>3</v>
       </c>
-      <c r="U30" t="s">
+      <c r="U30" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="V30" t="s">
+      <c r="V30" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W30" t="s">
+      <c r="W30" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X30">
+      <c r="X30" s="0">
         <f>(N6+N11+N16)/3</f>
         <v>87.966666666666654</v>
       </c>
-      <c r="Y30">
+      <c r="Y30" s="0">
         <f>(O6+O11+O16)/3</f>
         <v>53.166666666666664</v>
       </c>
@@ -3332,67 +3333,67 @@
       <c r="W32" s="5"/>
     </row>
     <row r="33" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T33">
+      <c r="T33" s="0">
         <v>1</v>
       </c>
-      <c r="U33" t="s">
+      <c r="U33" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="V33" t="s">
+      <c r="V33" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="W33" t="s">
+      <c r="W33" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X33">
+      <c r="X33" s="0">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y33">
+      <c r="Y33" s="0">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="34" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T34">
+      <c r="T34" s="0">
         <v>2</v>
       </c>
-      <c r="U34" t="s">
+      <c r="U34" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="V34" t="s">
+      <c r="V34" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W34" t="s">
+      <c r="W34" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="X34">
+      <c r="X34" s="0">
         <f>(N5+N11+N15)/3</f>
         <v>82.75</v>
       </c>
-      <c r="Y34">
+      <c r="Y34" s="0">
         <f>(O5+O11+O15)/3</f>
         <v>42.531746031746032</v>
       </c>
     </row>
     <row r="35" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T35">
+      <c r="T35" s="0">
         <v>3</v>
       </c>
-      <c r="U35" t="s">
+      <c r="U35" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="V35" t="s">
+      <c r="V35" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="W35" t="s">
+      <c r="W35" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="X35">
+      <c r="X35" s="0">
         <f>(N6+N12+N17)/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="Y35">
+      <c r="Y35" s="0">
         <f>(O6+O12+O17)/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -3422,289 +3423,289 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>70.642857142857139</v>
-      </c>
-      <c r="B2">
+      <c r="A2" t="n" s="0">
+        <v>70.64285714285714</v>
+      </c>
+      <c r="B2" t="n" s="0">
         <v>35.333333333333336</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n" s="0">
         <v>22.666666666666668</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>70.554959785545236</v>
-      </c>
-      <c r="F2">
-        <v>34.547008547214212</v>
-      </c>
-      <c r="G2">
-        <v>22.764957264931564</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="D2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>70.5515320334504</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>34.515555555777986</v>
+      </c>
+      <c r="G2" t="n" s="0">
+        <v>22.768888888861085</v>
+      </c>
+      <c r="H2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="s" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>82.166666666666671</v>
-      </c>
-      <c r="B3">
+      <c r="A3" t="n" s="0">
+        <v>82.16666666666667</v>
+      </c>
+      <c r="B3" t="n" s="0">
         <v>46.6</v>
       </c>
-      <c r="C3">
-        <v>34.200000000000003</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>81.737804878155472</v>
-      </c>
-      <c r="F3">
-        <v>46.912408759046556</v>
-      </c>
-      <c r="G3">
-        <v>33.394160584141595</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="C3" t="n" s="0">
+        <v>34.2</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>81.72151898745673</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>46.924242424158905</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>33.36363636385179</v>
+      </c>
+      <c r="H3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M3" t="s" s="0">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>69.599999999999994</v>
-      </c>
-      <c r="B4">
+      <c r="A4" t="n" s="0">
+        <v>69.6</v>
+      </c>
+      <c r="B4" t="n" s="0">
         <v>26.5</v>
       </c>
-      <c r="C4">
-        <v>29</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>68.924137931192959</v>
-      </c>
-      <c r="F4">
-        <v>26.499999999999996</v>
-      </c>
-      <c r="G4">
-        <v>29</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="C4" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>68.90000000017001</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>26.500000000000004</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="H4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M4" t="s" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>61</v>
-      </c>
-      <c r="B5">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="C5">
+      <c r="A5" t="n" s="0">
+        <v>61.0</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>38.3</v>
+      </c>
+      <c r="C5" t="n" s="0">
         <v>22.4</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>60.548780487917142</v>
-      </c>
-      <c r="F5">
-        <v>37.797794117772618</v>
-      </c>
-      <c r="G5">
-        <v>22.584558823483277</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="D5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>60.53164556974118</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>37.7786259543338</v>
+      </c>
+      <c r="G5" t="n" s="0">
+        <v>22.59160305338539</v>
+      </c>
+      <c r="H5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M5" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" t="n" s="0">
         <v>92.75</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n" s="0">
         <v>47.333333333333336</v>
       </c>
-      <c r="C6">
-        <v>41</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>93.259433962133443</v>
-      </c>
-      <c r="F6">
-        <v>48.079999999796904</v>
-      </c>
-      <c r="G6">
-        <v>41.159999999956483</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="C6" t="n" s="0">
+        <v>41.0</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>93.2794117645647</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <v>48.11111111089075</v>
+      </c>
+      <c r="G6" t="n" s="0">
+        <v>41.16666666661944</v>
+      </c>
+      <c r="H6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M6" t="s" s="0">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" t="n" s="0">
         <v>71.2</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n" s="0">
         <v>26.333333333333332</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n" s="0">
         <v>28.666666666666668</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>71.021126760606208</v>
-      </c>
-      <c r="F7">
-        <v>26.360465116272639</v>
-      </c>
-      <c r="G7">
-        <v>28.720930232545275</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="D7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E7" t="n" s="0">
+        <v>71.014598540192</v>
+      </c>
+      <c r="F7" t="n" s="0">
+        <v>26.361445783125625</v>
+      </c>
+      <c r="G7" t="n" s="0">
+        <v>28.722891566251242</v>
+      </c>
+      <c r="H7" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M7" t="s" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>61</v>
-      </c>
-      <c r="B8">
+      <c r="A8" t="n" s="0">
+        <v>61.0</v>
+      </c>
+      <c r="B8" t="n" s="0">
         <v>38.166666666666664</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n" s="0">
         <v>20.166666666666668</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>61.000000000000007</v>
-      </c>
-      <c r="F8">
-        <v>38.166666666666671</v>
-      </c>
-      <c r="G8">
-        <v>20.166666666666671</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="D8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>61.00000000000001</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>38.166666666666664</v>
+      </c>
+      <c r="G8" t="n" s="0">
+        <v>20.16666666666667</v>
+      </c>
+      <c r="H8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M8" t="s" s="0">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>88.333333333333329</v>
-      </c>
-      <c r="B9">
+      <c r="A9" t="n" s="0">
+        <v>88.33333333333333</v>
+      </c>
+      <c r="B9" t="n" s="0">
         <v>47.333333333333336</v>
       </c>
-      <c r="C9">
-        <v>41</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>89.239999999753394</v>
-      </c>
-      <c r="F9">
-        <v>48.079999999796904</v>
-      </c>
-      <c r="G9">
-        <v>41.159999999956483</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="C9" t="n" s="0">
+        <v>41.0</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <v>89.27777777751018</v>
+      </c>
+      <c r="F9" t="n" s="0">
+        <v>48.11111111089075</v>
+      </c>
+      <c r="G9" t="n" s="0">
+        <v>41.16666666661944</v>
+      </c>
+      <c r="H9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M9" t="s" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" t="n" s="0">
         <v>74.9375</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n" s="0">
         <v>33.285714285714285</v>
       </c>
-      <c r="C10">
-        <v>27</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>73.95032397431406</v>
-      </c>
-      <c r="F10">
-        <v>32.953271028111331</v>
-      </c>
-      <c r="G10">
-        <v>26.67757009352966</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="C10" t="n" s="0">
+        <v>27.0</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E10" t="n" s="0">
+        <v>73.91498881456651</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>32.94202898558628</v>
+      </c>
+      <c r="G10" t="n" s="0">
+        <v>26.66666666674332</v>
+      </c>
+      <c r="H10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M10" t="s" s="0">
         <v>49</v>
       </c>
     </row>
@@ -3724,115 +3725,115 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>64.857142857142861</v>
-      </c>
-      <c r="B2">
-        <v>37.086666666666659</v>
-      </c>
-      <c r="C2">
+      <c r="A2" t="n" s="0">
+        <v>64.85714285714286</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>37.08666666666666</v>
+      </c>
+      <c r="C2" t="n" s="0">
         <v>22.06</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>64.136274509803926</v>
-      </c>
-      <c r="F2">
+      <c r="D2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>64.13627450980393</v>
+      </c>
+      <c r="F2" t="n" s="0">
         <v>36.37936507936508</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n" s="0">
         <v>22.807936507936507</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="H2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K2" t="s" s="0">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" t="n" s="0">
         <v>87.63333333333334</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n" s="0">
         <v>47.040000000000006</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n" s="0">
         <v>38.28</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>88.472222222222214</v>
-      </c>
-      <c r="F3">
+      <c r="D3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>88.47222222222221</v>
+      </c>
+      <c r="F3" t="n" s="0">
         <v>46.875</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n" s="0">
         <v>36.75</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="H3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K3" t="s" s="0">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>71.307500000000005</v>
-      </c>
-      <c r="B4">
+      <c r="A4" t="n" s="0">
+        <v>71.3075</v>
+      </c>
+      <c r="B4" t="n" s="0">
         <v>27.790476190476188</v>
       </c>
-      <c r="C4">
-        <v>28.466666666666669</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>75.035714285714278</v>
-      </c>
-      <c r="F4">
+      <c r="C4" t="n" s="0">
+        <v>28.46666666666667</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>75.03571428571428</v>
+      </c>
+      <c r="F4" t="n" s="0">
         <v>28.160714285714285</v>
       </c>
-      <c r="G4">
-        <v>28.428571428571431</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="G4" t="n" s="0">
+        <v>28.42857142857143</v>
+      </c>
+      <c r="H4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K4" t="s" s="0">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Calculates drive team standard deviations because why not
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7BC124-7F1A-41A4-BD2F-892FE4F4EC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DB050F-5286-4607-9F36-905B71E39763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
   <sheets>
     <sheet name="Match Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="61">
   <si>
     <t>Cyrus</t>
   </si>
@@ -140,30 +140,6 @@
     <t>Driver Penalties</t>
   </si>
   <si>
-    <t>avgtotal</t>
-  </si>
-  <si>
-    <t>avgtele</t>
-  </si>
-  <si>
-    <t>avgauto</t>
-  </si>
-  <si>
-    <t>avgpen</t>
-  </si>
-  <si>
-    <t>Wavgtele</t>
-  </si>
-  <si>
-    <t>Wavgauto</t>
-  </si>
-  <si>
-    <t>Wavgpen</t>
-  </si>
-  <si>
-    <t>Wavgtot</t>
-  </si>
-  <si>
     <t>bredan</t>
   </si>
   <si>
@@ -194,6 +170,48 @@
     <t>*</t>
   </si>
   <si>
+    <t>&lt;- NEW ROBOT</t>
+  </si>
+  <si>
+    <t>stddev</t>
+  </si>
+  <si>
+    <t>Basic Averages</t>
+  </si>
+  <si>
+    <t>Weighted Averages</t>
+  </si>
+  <si>
+    <t>Duo Total</t>
+  </si>
+  <si>
+    <t>Duo Teleop</t>
+  </si>
+  <si>
+    <t>Duo Autos</t>
+  </si>
+  <si>
+    <t>Duo Penalties</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>teleop</t>
+  </si>
+  <si>
+    <t>auton</t>
+  </si>
+  <si>
+    <t>penalties</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
     <t>B+M</t>
   </si>
   <si>
@@ -203,26 +221,13 @@
     <t>L+C</t>
   </si>
   <si>
-    <t>wAvgtotal</t>
-  </si>
-  <si>
-    <t>wAvgtele</t>
-  </si>
-  <si>
-    <t>wAvgauto</t>
-  </si>
-  <si>
-    <t>wAvgpen</t>
-  </si>
-  <si>
-    <t>&lt;- NEW ROBOT</t>
+    <t>Date-Weighted Averages</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -248,7 +253,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -265,22 +270,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1684,14 +1712,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView topLeftCell="A3" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -1724,31 +1752,31 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>45237</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>106</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>-1</v>
       </c>
-      <c r="H2" s="0">
+      <c r="H2">
         <v>-1</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2">
         <v>0</v>
       </c>
       <c r="M2" s="2"/>
@@ -1761,740 +1789,740 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>45237</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>83</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>-1</v>
       </c>
-      <c r="H3" s="0">
+      <c r="H3">
         <v>-1</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>45237</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4">
         <v>89</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4">
         <v>-1</v>
       </c>
-      <c r="H4" s="0">
+      <c r="H4">
         <v>-1</v>
       </c>
-      <c r="I4" s="0">
+      <c r="I4">
         <v>0</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>45238</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s" s="0">
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5">
         <v>71</v>
       </c>
-      <c r="G5" s="0">
+      <c r="G5">
         <v>-1</v>
       </c>
-      <c r="H5" s="0">
+      <c r="H5">
         <v>-1</v>
       </c>
-      <c r="I5" s="0">
+      <c r="I5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>45238</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>88</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6">
         <v>-1</v>
       </c>
-      <c r="H6" s="0">
+      <c r="H6">
         <v>-1</v>
       </c>
-      <c r="I6" s="0">
+      <c r="I6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>45238</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>111</v>
       </c>
-      <c r="G7" s="0">
+      <c r="G7">
         <v>-1</v>
       </c>
-      <c r="H7" s="0">
+      <c r="H7">
         <v>-1</v>
       </c>
-      <c r="I7" s="0">
+      <c r="I7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>45238</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <v>34</v>
       </c>
-      <c r="G8" s="0">
+      <c r="G8">
         <v>-1</v>
       </c>
-      <c r="H8" s="0">
+      <c r="H8">
         <v>-1</v>
       </c>
-      <c r="I8" s="0">
+      <c r="I8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>45238</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s" s="0">
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>120</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G9">
         <v>-1</v>
       </c>
-      <c r="H9" s="0">
+      <c r="H9">
         <v>-1</v>
       </c>
-      <c r="I9" s="0">
+      <c r="I9">
         <v>0</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>45238</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s" s="0">
+      <c r="E10" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="0">
+      <c r="F10">
         <v>75</v>
       </c>
-      <c r="G10" s="0">
+      <c r="G10">
         <v>-1</v>
       </c>
-      <c r="H10" s="0">
+      <c r="H10">
         <v>-1</v>
       </c>
-      <c r="I10" s="0">
+      <c r="I10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>45237</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>2</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="0">
+      <c r="F11">
         <v>111</v>
       </c>
-      <c r="G11" s="0">
+      <c r="G11">
         <v>66</v>
       </c>
-      <c r="H11" s="0">
+      <c r="H11">
         <v>45</v>
       </c>
-      <c r="I11" s="0">
+      <c r="I11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>45238</v>
       </c>
-      <c r="C12" t="s" s="0">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s" s="0">
+      <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s" s="0">
+      <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="0">
+      <c r="F12">
         <v>107</v>
       </c>
-      <c r="G12" s="0">
+      <c r="G12">
         <v>57</v>
       </c>
-      <c r="H12" s="0">
+      <c r="H12">
         <v>50</v>
       </c>
-      <c r="I12" s="0">
+      <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>45234</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>72</v>
       </c>
-      <c r="G13" s="0">
+      <c r="G13">
         <v>44</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <v>28</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s" s="0">
+      <c r="A14" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="1">
         <v>45234</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>97</v>
       </c>
-      <c r="G14" s="0">
+      <c r="G14">
         <v>51</v>
       </c>
-      <c r="H14" s="0">
+      <c r="H14">
         <v>30</v>
       </c>
-      <c r="I14" s="0">
+      <c r="I14">
         <v>0</v>
       </c>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s" s="0">
+      <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="1">
         <v>45234</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s" s="0">
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>54</v>
       </c>
-      <c r="G15" s="0">
+      <c r="G15">
         <v>26</v>
       </c>
-      <c r="H15" s="0">
+      <c r="H15">
         <v>28</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s" s="0">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>45234</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>82</v>
       </c>
-      <c r="G16" s="0">
+      <c r="G16">
         <v>32</v>
       </c>
-      <c r="H16" s="0">
+      <c r="H16">
         <v>50</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" t="s" s="0">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>45234</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>60</v>
       </c>
-      <c r="G17" s="0">
+      <c r="G17">
         <v>40</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H17">
         <v>20</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" t="s" s="0">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>45234</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s" s="0">
+      <c r="D18" t="s">
         <v>9</v>
       </c>
-      <c r="E18" t="s" s="0">
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>56</v>
       </c>
-      <c r="G18" s="0">
+      <c r="G18">
         <v>48</v>
       </c>
-      <c r="H18" s="0">
+      <c r="H18">
         <v>8</v>
       </c>
-      <c r="I18" s="0">
+      <c r="I18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" t="s" s="0">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>45234</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>60</v>
       </c>
-      <c r="G19" s="0">
+      <c r="G19">
         <v>30</v>
       </c>
-      <c r="H19" s="0">
+      <c r="H19">
         <v>30</v>
       </c>
-      <c r="I19" s="0">
+      <c r="I19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" t="s" s="0">
+      <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>45234</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s" s="0">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>39</v>
       </c>
-      <c r="G20" s="0">
+      <c r="G20">
         <v>34</v>
       </c>
-      <c r="H20" s="0">
+      <c r="H20">
         <v>5</v>
       </c>
-      <c r="I20" s="0">
+      <c r="I20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" t="s" s="0">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>45241</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s" s="0">
+      <c r="E21" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21">
         <v>32</v>
       </c>
-      <c r="G21" s="0">
+      <c r="G21">
         <v>4</v>
       </c>
-      <c r="H21" s="0">
+      <c r="H21">
         <v>28</v>
       </c>
-      <c r="I21" s="0">
-        <v>0</v>
-      </c>
-      <c r="K21" t="s" s="0">
-        <v>50</v>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" t="s" s="0">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>45241</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>4</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>83</v>
       </c>
-      <c r="G22" s="0">
+      <c r="G22">
         <v>55</v>
       </c>
-      <c r="H22" s="0">
+      <c r="H22">
         <v>28</v>
       </c>
-      <c r="I22" s="0">
-        <v>0</v>
-      </c>
-      <c r="K22" t="s" s="0">
-        <v>50</v>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" t="s" s="0">
+      <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>45241</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>3</v>
       </c>
-      <c r="D23" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E23" t="s" s="0">
+      <c r="D23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>56</v>
       </c>
-      <c r="G23" s="0">
+      <c r="G23">
         <v>26</v>
       </c>
-      <c r="H23" s="0">
+      <c r="H23">
         <v>30</v>
       </c>
-      <c r="I23" s="0">
-        <v>0</v>
-      </c>
-      <c r="K23" t="s" s="0">
-        <v>50</v>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" t="s" s="0">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>45241</v>
       </c>
-      <c r="C24" t="s" s="0">
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" t="s" s="0">
+      <c r="D24" t="s">
         <v>9</v>
       </c>
-      <c r="E24" t="s" s="0">
+      <c r="E24" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="0">
+      <c r="F24">
         <v>33</v>
       </c>
-      <c r="G24" s="0">
+      <c r="G24">
         <v>28</v>
       </c>
-      <c r="H24" s="0">
+      <c r="H24">
         <v>5</v>
       </c>
-      <c r="I24" s="0">
-        <v>0</v>
-      </c>
-      <c r="K24" t="s" s="0">
-        <v>50</v>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" t="s" s="0">
+      <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>45241</v>
       </c>
-      <c r="C25" t="s" s="0">
+      <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="D25" t="s" s="0">
+      <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" t="s" s="0">
+      <c r="E25" t="s">
         <v>1</v>
       </c>
-      <c r="F25" s="0">
+      <c r="F25">
         <v>56</v>
       </c>
-      <c r="G25" s="0">
+      <c r="G25">
         <v>36</v>
       </c>
-      <c r="H25" s="0">
+      <c r="H25">
         <v>20</v>
       </c>
-      <c r="I25" s="0">
-        <v>0</v>
-      </c>
-      <c r="K25" t="s" s="0">
-        <v>50</v>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" t="s" s="0">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="1">
         <v>45241</v>
       </c>
-      <c r="C26" t="s" s="0">
+      <c r="C26" t="s">
         <v>3</v>
       </c>
-      <c r="D26" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s" s="0">
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="0">
+      <c r="F26">
         <v>55</v>
       </c>
-      <c r="G26" s="0">
+      <c r="G26">
         <v>27</v>
       </c>
-      <c r="H26" s="0">
+      <c r="H26">
         <v>28</v>
       </c>
-      <c r="I26" s="0">
-        <v>0</v>
-      </c>
-      <c r="K26" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
+        <v>42</v>
+      </c>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="L27" t="s" s="0">
-        <v>58</v>
+      <c r="L27" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="5"/>
-      <c r="W31" s="5"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2516,8 +2544,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -2549,7 +2577,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="V2" t="s" s="0">
+      <c r="V2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2557,16 +2585,16 @@
       <c r="A3" s="1">
         <v>45237</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>106</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2574,25 +2602,25 @@
       <c r="A4" s="1">
         <v>45237</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>83</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" t="s" s="0">
+      <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="O4" t="s" s="0">
+      <c r="O4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2600,26 +2628,26 @@
       <c r="A5" s="1">
         <v>45237</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>89</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="M5" t="s" s="0">
+      <c r="M5" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="0">
+      <c r="N5">
         <f>(SUMIF($C$3:$C$100, M5, $B$3:$B$100)/COUNTIF($C$3:$C$100, M5))</f>
         <v>88.083333333333329</v>
       </c>
-      <c r="O5" s="0">
+      <c r="O5">
         <f>(SUMIF($C$3:$C$100, M5, $F$3:$F$100)/COUNTIF($C$13:$C$100, M5))</f>
         <v>42.428571428571431</v>
       </c>
@@ -2628,26 +2656,26 @@
       <c r="A6" s="1">
         <v>45238</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>71</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s" s="0">
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="M6" t="s" s="0">
+      <c r="M6" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="0">
+      <c r="N6">
         <f>(SUMIF($C$3:$C$100, M6, $B$3:$B$100)/COUNTIF($C$3:$C$100, M6))</f>
         <v>98.5</v>
       </c>
-      <c r="O6" s="0">
+      <c r="O6">
         <f>(SUMIF($C$3:$C$100, M6, $F$3:$F$100)/COUNTIF($C$13:$C$100, M6))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2656,26 +2684,26 @@
       <c r="A7" s="1">
         <v>45238</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>88</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="M7" t="s" s="0">
+      <c r="M7" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="0">
+      <c r="N7">
         <f>(SUMIF($C$3:$C$100, M7, $B$3:$B$100)/COUNTIF($C$3:$C$100, M7))</f>
         <v>86.25</v>
       </c>
-      <c r="O7" s="0">
+      <c r="O7">
         <f>(SUMIF($C$3:$C$100, M7, $F$3:$F$100)/COUNTIF($C$13:$C$100, M7))</f>
         <v>38</v>
       </c>
@@ -2684,16 +2712,16 @@
       <c r="A8" s="1">
         <v>45238</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8">
         <v>111</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>2</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2701,16 +2729,16 @@
       <c r="A9" s="1">
         <v>45238</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9">
         <v>34</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -2721,32 +2749,32 @@
       <c r="A10" s="1">
         <v>45238</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10">
         <v>120</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s" s="0">
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="M10" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="N10" s="0">
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="M10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <f>(SUMIF($D$3:$D$100, M10, $B$3:$B$100)/COUNTIF($D$3:$D$100, M10))</f>
         <v>96.666666666666671</v>
       </c>
-      <c r="O10" s="0">
+      <c r="O10">
         <f>(SUMIF($D$3:$D$100, M10, $F$3:$F$100)/COUNTIF($D$13:$D$100, M10))</f>
         <v>26</v>
       </c>
@@ -2755,34 +2783,34 @@
       <c r="A11" s="1">
         <v>45238</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11">
         <v>75</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="6" t="s">
+      <c r="I11" s="6"/>
+      <c r="J11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="M11" t="s" s="0">
+      <c r="K11" s="6"/>
+      <c r="M11" t="s">
         <v>9</v>
       </c>
-      <c r="N11" s="0">
+      <c r="N11">
         <f>(SUMIF($D$3:$D$100, M11, $B$3:$B$100)/COUNTIF($D$3:$D$100, M11))</f>
         <v>77</v>
       </c>
-      <c r="O11" s="0">
+      <c r="O11">
         <f>(SUMIF($D$3:$D$100, M11, $F$3:$F$100)/COUNTIF($D$13:$D$100, M11))</f>
         <v>45.166666666666664</v>
       </c>
@@ -2800,14 +2828,14 @@
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s" s="0">
+      <c r="M12" t="s">
         <v>2</v>
       </c>
-      <c r="N12" s="0">
+      <c r="N12">
         <f>(SUMIF($D$3:$D$100, M12, $B$3:$B$100)/COUNTIF($D$3:$D$100, M12))</f>
         <v>97.75</v>
       </c>
-      <c r="O12" s="0">
+      <c r="O12">
         <f>(SUMIF($D$3:$D$100, M12, $F$3:$F$100)/COUNTIF($D$13:$D$100, M12))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2816,26 +2844,26 @@
       <c r="A13" s="1">
         <v>45237</v>
       </c>
-      <c r="B13" s="0">
+      <c r="B13">
         <v>111</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>66</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <f t="shared" ref="H13:H23" si="0">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12)+SUMIF($M$15:$M$17, $E13, $N$15:$N$17))/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <f t="shared" ref="I13:I23" si="1">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12)+SUMIF($M$15:$M$17, $E13, $O$15:$O$17))/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -2843,7 +2871,7 @@
         <f t="shared" ref="J13:J23" si="2">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12))/2</f>
         <v>98.125</v>
       </c>
-      <c r="K13" s="0">
+      <c r="K13">
         <f t="shared" ref="K13:K23" si="3">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12))/2</f>
         <v>57.333333333333336</v>
       </c>
@@ -2852,26 +2880,26 @@
       <c r="A14" s="1">
         <v>45238</v>
       </c>
-      <c r="B14" s="0">
+      <c r="B14">
         <v>107</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>57</v>
       </c>
-      <c r="H14" s="0">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>84.49444444444444</v>
       </c>
-      <c r="I14" s="0">
+      <c r="I14">
         <f t="shared" si="1"/>
         <v>48.198412698412703</v>
       </c>
@@ -2879,7 +2907,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K14" s="0">
+      <c r="K14">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -2891,26 +2919,26 @@
       <c r="A15" s="1">
         <v>45234</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15">
         <v>108</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s" s="0">
+      <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="s" s="0">
+      <c r="E15" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>38</v>
       </c>
-      <c r="H15" s="0">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>63.166666666666664</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15">
         <f t="shared" si="1"/>
         <v>30.166666666666668</v>
       </c>
@@ -2918,18 +2946,18 @@
         <f t="shared" si="2"/>
         <v>43.125</v>
       </c>
-      <c r="K15" s="0">
+      <c r="K15">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="M15" t="s" s="0">
+      <c r="M15" t="s">
         <v>10</v>
       </c>
-      <c r="N15" s="0">
+      <c r="N15">
         <f>(SUMIF($E$3:$E$100, M15, $B$3:$B$100)/COUNTIF($E$3:$E$100, M15))</f>
         <v>83.166666666666671</v>
       </c>
-      <c r="O15" s="0">
+      <c r="O15">
         <f>(SUMIF($E$3:$E$100, M15, $F$3:$F$100)/COUNTIF($E$13:$E$100, M15))</f>
         <v>40</v>
       </c>
@@ -2938,26 +2966,26 @@
       <c r="A16" s="1">
         <v>45234</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16">
         <v>107</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>74</v>
       </c>
-      <c r="H16" s="0">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -2965,18 +2993,18 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K16" s="0">
+      <c r="K16">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
-      <c r="M16" t="s" s="0">
+      <c r="M16" t="s">
         <v>1</v>
       </c>
-      <c r="N16" s="0">
+      <c r="N16">
         <f>(SUMIF($E$3:$E$100, M16, $B$3:$B$100)/COUNTIF($E$3:$E$100, M16))</f>
         <v>88.4</v>
       </c>
-      <c r="O16" s="0">
+      <c r="O16">
         <f>(SUMIF($E$3:$E$100, M16, $F$3:$F$100)/COUNTIF($E$13:$E$100, M16))</f>
         <v>57</v>
       </c>
@@ -2985,26 +3013,26 @@
       <c r="A17" s="1">
         <v>45234</v>
       </c>
-      <c r="B17" s="0">
+      <c r="B17">
         <v>97</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>62</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I17">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3012,18 +3040,18 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K17" s="0">
+      <c r="K17">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
-      <c r="M17" t="s" s="0">
+      <c r="M17" t="s">
         <v>5</v>
       </c>
-      <c r="N17" s="0">
+      <c r="N17">
         <f>(SUMIF($E$3:$E$100, M17, $B$3:$B$100)/COUNTIF($E$3:$E$100, M17))</f>
         <v>103.25</v>
       </c>
-      <c r="O17" s="0">
+      <c r="O17">
         <f>(SUMIF($E$3:$E$100, M17, $F$3:$F$100)/COUNTIF($E$13:$E$100, M17))</f>
         <v>52.5</v>
       </c>
@@ -3032,26 +3060,26 @@
       <c r="A18" s="1">
         <v>45234</v>
       </c>
-      <c r="B18" s="0">
+      <c r="B18">
         <v>99</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s" s="0">
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>26</v>
       </c>
-      <c r="H18" s="0">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>89.305555555555557</v>
       </c>
-      <c r="I18" s="0">
+      <c r="I18">
         <f t="shared" si="1"/>
         <v>36.142857142857146</v>
       </c>
@@ -3059,7 +3087,7 @@
         <f t="shared" si="2"/>
         <v>92.375</v>
       </c>
-      <c r="K18" s="0">
+      <c r="K18">
         <f t="shared" si="3"/>
         <v>34.214285714285715</v>
       </c>
@@ -3068,26 +3096,26 @@
       <c r="A19" s="1">
         <v>45234</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19">
         <v>87</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>2</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>32</v>
       </c>
-      <c r="H19" s="0">
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I19" s="0">
+      <c r="I19">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -3095,7 +3123,7 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K19" s="0">
+      <c r="K19">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
@@ -3104,26 +3132,26 @@
       <c r="A20" s="1">
         <v>45234</v>
       </c>
-      <c r="B20" s="0">
+      <c r="B20">
         <v>76</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s" s="0">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>48</v>
       </c>
-      <c r="H20" s="0">
+      <c r="H20">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I20" s="0">
+      <c r="I20">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3131,7 +3159,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K20" s="0">
+      <c r="K20">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3140,26 +3168,26 @@
       <c r="A21" s="1">
         <v>45234</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21">
         <v>93</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s" s="0">
+      <c r="E21" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21">
         <v>40</v>
       </c>
-      <c r="H21" s="0">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I21" s="0">
+      <c r="I21">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3167,7 +3195,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K21" s="0">
+      <c r="K21">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3176,26 +3204,26 @@
       <c r="A22" s="1">
         <v>45234</v>
       </c>
-      <c r="B22" s="0">
+      <c r="B22">
         <v>85</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>30</v>
       </c>
-      <c r="H22" s="0">
+      <c r="H22">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I22" s="0">
+      <c r="I22">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3203,7 +3231,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K22" s="0">
+      <c r="K22">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3212,26 +3240,26 @@
       <c r="A23" s="1">
         <v>45234</v>
       </c>
-      <c r="B23" s="0">
+      <c r="B23">
         <v>49</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>11</v>
       </c>
-      <c r="D23" t="s" s="0">
+      <c r="D23" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s" s="0">
+      <c r="E23" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>34</v>
       </c>
-      <c r="H23" s="0">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I23" s="0">
+      <c r="I23">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3239,18 +3267,18 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K23" s="0">
+      <c r="K23">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T27" s="5" t="s">
+      <c r="T27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
       <c r="X27" s="2" t="s">
         <v>23</v>
       </c>
@@ -3259,141 +3287,141 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T28" s="0">
+      <c r="T28">
         <v>1</v>
       </c>
-      <c r="U28" t="s" s="0">
+      <c r="U28" t="s">
         <v>3</v>
       </c>
-      <c r="V28" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="W28" t="s" s="0">
+      <c r="V28" t="s">
+        <v>0</v>
+      </c>
+      <c r="W28" t="s">
         <v>1</v>
       </c>
-      <c r="X28" s="0">
+      <c r="X28">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y28" s="0">
+      <c r="Y28">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T29" s="0">
+      <c r="T29">
         <v>2</v>
       </c>
-      <c r="U29" t="s" s="0">
+      <c r="U29" t="s">
         <v>11</v>
       </c>
-      <c r="V29" t="s" s="0">
+      <c r="V29" t="s">
         <v>9</v>
       </c>
-      <c r="W29" t="s" s="0">
+      <c r="W29" t="s">
         <v>1</v>
       </c>
-      <c r="X29" s="0">
+      <c r="X29">
         <f>(N5+N11+N16)/3</f>
         <v>84.49444444444444</v>
       </c>
-      <c r="Y29" s="0">
+      <c r="Y29">
         <f>(O5+O11+O16)/3</f>
         <v>48.198412698412703</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T30" s="0">
+      <c r="T30">
         <v>3</v>
       </c>
-      <c r="U30" t="s" s="0">
+      <c r="U30" t="s">
         <v>4</v>
       </c>
-      <c r="V30" t="s" s="0">
+      <c r="V30" t="s">
         <v>9</v>
       </c>
-      <c r="W30" t="s" s="0">
+      <c r="W30" t="s">
         <v>1</v>
       </c>
-      <c r="X30" s="0">
+      <c r="X30">
         <f>(N6+N11+N16)/3</f>
         <v>87.966666666666654</v>
       </c>
-      <c r="Y30" s="0">
+      <c r="Y30">
         <f>(O6+O11+O16)/3</f>
         <v>53.166666666666664</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T32" s="5" t="s">
+      <c r="T32" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="W32" s="5"/>
+      <c r="U32" s="6"/>
+      <c r="V32" s="6"/>
+      <c r="W32" s="6"/>
     </row>
     <row r="33" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T33" s="0">
+      <c r="T33">
         <v>1</v>
       </c>
-      <c r="U33" t="s" s="0">
+      <c r="U33" t="s">
         <v>3</v>
       </c>
-      <c r="V33" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="W33" t="s" s="0">
+      <c r="V33" t="s">
+        <v>0</v>
+      </c>
+      <c r="W33" t="s">
         <v>1</v>
       </c>
-      <c r="X33" s="0">
+      <c r="X33">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y33" s="0">
+      <c r="Y33">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="34" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T34" s="0">
+      <c r="T34">
         <v>2</v>
       </c>
-      <c r="U34" t="s" s="0">
+      <c r="U34" t="s">
         <v>11</v>
       </c>
-      <c r="V34" t="s" s="0">
+      <c r="V34" t="s">
         <v>9</v>
       </c>
-      <c r="W34" t="s" s="0">
+      <c r="W34" t="s">
         <v>10</v>
       </c>
-      <c r="X34" s="0">
+      <c r="X34">
         <f>(N5+N11+N15)/3</f>
         <v>82.75</v>
       </c>
-      <c r="Y34" s="0">
+      <c r="Y34">
         <f>(O5+O11+O15)/3</f>
         <v>42.531746031746032</v>
       </c>
     </row>
     <row r="35" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T35" s="0">
+      <c r="T35">
         <v>3</v>
       </c>
-      <c r="U35" t="s" s="0">
+      <c r="U35" t="s">
         <v>4</v>
       </c>
-      <c r="V35" t="s" s="0">
+      <c r="V35" t="s">
         <v>2</v>
       </c>
-      <c r="W35" t="s" s="0">
+      <c r="W35" t="s">
         <v>5</v>
       </c>
-      <c r="X35" s="0">
+      <c r="X35">
         <f>(N6+N12+N17)/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="Y35" s="0">
+      <c r="Y35">
         <f>(O6+O12+O17)/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -3414,430 +3442,634 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>70.642857142857139</v>
+      </c>
+      <c r="B3">
+        <v>35.333333333333336</v>
+      </c>
+      <c r="C3">
+        <v>22.666666666666668</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>70.5515320334504</v>
+      </c>
+      <c r="F3" s="12">
+        <v>34.515555555777986</v>
+      </c>
+      <c r="G3" s="12">
+        <v>22.768888888861085</v>
+      </c>
+      <c r="H3" s="12">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s" s="0">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>82.166666666666671</v>
+      </c>
+      <c r="B4">
+        <v>46.6</v>
+      </c>
+      <c r="C4">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>81.721518987456733</v>
+      </c>
+      <c r="F4" s="12">
+        <v>46.924242424158905</v>
+      </c>
+      <c r="G4" s="12">
+        <v>33.363636363851789</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s" s="0">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="B5">
+        <v>26.5</v>
+      </c>
+      <c r="C5">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>68.90000000017001</v>
+      </c>
+      <c r="F5" s="12">
+        <v>26.500000000000004</v>
+      </c>
+      <c r="G5" s="12">
+        <v>29</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s" s="0">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>61</v>
+      </c>
+      <c r="B6">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="C6">
+        <v>22.4</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>60.53164556974118</v>
+      </c>
+      <c r="F6" s="12">
+        <v>37.778625954333798</v>
+      </c>
+      <c r="G6" s="12">
+        <v>22.591603053385391</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s" s="0">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>92.75</v>
+      </c>
+      <c r="B7">
+        <v>47.333333333333336</v>
+      </c>
+      <c r="C7">
+        <v>41</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>93.279411764564699</v>
+      </c>
+      <c r="F7" s="12">
+        <v>48.111111110890747</v>
+      </c>
+      <c r="G7" s="12">
+        <v>41.166666666619442</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>71.2</v>
+      </c>
+      <c r="B8">
+        <v>26.333333333333332</v>
+      </c>
+      <c r="C8">
+        <v>28.666666666666668</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>71.014598540191997</v>
+      </c>
+      <c r="F8" s="12">
+        <v>26.361445783125625</v>
+      </c>
+      <c r="G8" s="12">
+        <v>28.722891566251242</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>61</v>
+      </c>
+      <c r="B9">
+        <v>38.166666666666664</v>
+      </c>
+      <c r="C9">
+        <v>20.166666666666668</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>61.000000000000007</v>
+      </c>
+      <c r="F9" s="12">
+        <v>38.166666666666664</v>
+      </c>
+      <c r="G9" s="12">
+        <v>20.166666666666671</v>
+      </c>
+      <c r="H9" s="12">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>88.333333333333329</v>
+      </c>
+      <c r="B10">
+        <v>47.333333333333336</v>
+      </c>
+      <c r="C10">
+        <v>41</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>89.277777777510181</v>
+      </c>
+      <c r="F10" s="12">
+        <v>48.111111110890747</v>
+      </c>
+      <c r="G10" s="12">
+        <v>41.166666666619442</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="G1" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="H1" t="s" s="0">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="n" s="0">
-        <v>70.64285714285714</v>
-      </c>
-      <c r="B2" t="n" s="0">
-        <v>35.333333333333336</v>
-      </c>
-      <c r="C2" t="n" s="0">
-        <v>22.666666666666668</v>
-      </c>
-      <c r="D2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E2" t="n" s="0">
-        <v>70.5515320334504</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>34.515555555777986</v>
-      </c>
-      <c r="G2" t="n" s="0">
-        <v>22.768888888861085</v>
-      </c>
-      <c r="H2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M2" t="s" s="0">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>74.9375</v>
+      </c>
+      <c r="B11">
+        <v>33.285714285714285</v>
+      </c>
+      <c r="C11">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>73.914988814566513</v>
+      </c>
+      <c r="F11" s="12">
+        <v>32.942028985586283</v>
+      </c>
+      <c r="G11" s="12">
+        <v>26.666666666743321</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="n" s="0">
-        <v>82.16666666666667</v>
-      </c>
-      <c r="B3" t="n" s="0">
-        <v>46.6</v>
-      </c>
-      <c r="C3" t="n" s="0">
-        <v>34.2</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E3" t="n" s="0">
-        <v>81.72151898745673</v>
-      </c>
-      <c r="F3" t="n" s="0">
-        <v>46.924242424158905</v>
-      </c>
-      <c r="G3" t="n" s="0">
-        <v>33.36363636385179</v>
-      </c>
-      <c r="H3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M3" t="s" s="0">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="n" s="0">
-        <v>69.6</v>
-      </c>
-      <c r="B4" t="n" s="0">
-        <v>26.5</v>
-      </c>
-      <c r="C4" t="n" s="0">
-        <v>29.0</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E4" t="n" s="0">
-        <v>68.90000000017001</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <v>26.500000000000004</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>29.0</v>
-      </c>
-      <c r="H4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M4" t="s" s="0">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="n" s="0">
-        <v>61.0</v>
-      </c>
-      <c r="B5" t="n" s="0">
-        <v>38.3</v>
-      </c>
-      <c r="C5" t="n" s="0">
-        <v>22.4</v>
-      </c>
-      <c r="D5" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E5" t="n" s="0">
-        <v>60.53164556974118</v>
-      </c>
-      <c r="F5" t="n" s="0">
-        <v>37.7786259543338</v>
-      </c>
-      <c r="G5" t="n" s="0">
-        <v>22.59160305338539</v>
-      </c>
-      <c r="H5" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M5" t="s" s="0">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="n" s="0">
-        <v>92.75</v>
-      </c>
-      <c r="B6" t="n" s="0">
-        <v>47.333333333333336</v>
-      </c>
-      <c r="C6" t="n" s="0">
-        <v>41.0</v>
-      </c>
-      <c r="D6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E6" t="n" s="0">
-        <v>93.2794117645647</v>
-      </c>
-      <c r="F6" t="n" s="0">
-        <v>48.11111111089075</v>
-      </c>
-      <c r="G6" t="n" s="0">
-        <v>41.16666666661944</v>
-      </c>
-      <c r="H6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M6" t="s" s="0">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="n" s="0">
-        <v>71.2</v>
-      </c>
-      <c r="B7" t="n" s="0">
-        <v>26.333333333333332</v>
-      </c>
-      <c r="C7" t="n" s="0">
-        <v>28.666666666666668</v>
-      </c>
-      <c r="D7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E7" t="n" s="0">
-        <v>71.014598540192</v>
-      </c>
-      <c r="F7" t="n" s="0">
-        <v>26.361445783125625</v>
-      </c>
-      <c r="G7" t="n" s="0">
-        <v>28.722891566251242</v>
-      </c>
-      <c r="H7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M7" t="s" s="0">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="n" s="0">
-        <v>61.0</v>
-      </c>
-      <c r="B8" t="n" s="0">
-        <v>38.166666666666664</v>
-      </c>
-      <c r="C8" t="n" s="0">
-        <v>20.166666666666668</v>
-      </c>
-      <c r="D8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E8" t="n" s="0">
-        <v>61.00000000000001</v>
-      </c>
-      <c r="F8" t="n" s="0">
-        <v>38.166666666666664</v>
-      </c>
-      <c r="G8" t="n" s="0">
-        <v>20.16666666666667</v>
-      </c>
-      <c r="H8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M8" t="s" s="0">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="n" s="0">
-        <v>88.33333333333333</v>
-      </c>
-      <c r="B9" t="n" s="0">
-        <v>47.333333333333336</v>
-      </c>
-      <c r="C9" t="n" s="0">
-        <v>41.0</v>
-      </c>
-      <c r="D9" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E9" t="n" s="0">
-        <v>89.27777777751018</v>
-      </c>
-      <c r="F9" t="n" s="0">
-        <v>48.11111111089075</v>
-      </c>
-      <c r="G9" t="n" s="0">
-        <v>41.16666666661944</v>
-      </c>
-      <c r="H9" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M9" t="s" s="0">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="n" s="0">
-        <v>74.9375</v>
-      </c>
-      <c r="B10" t="n" s="0">
-        <v>33.285714285714285</v>
-      </c>
-      <c r="C10" t="n" s="0">
-        <v>27.0</v>
-      </c>
-      <c r="D10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E10" t="n" s="0">
-        <v>73.91498881456651</v>
-      </c>
-      <c r="F10" t="n" s="0">
-        <v>32.94202898558628</v>
-      </c>
-      <c r="G10" t="n" s="0">
-        <v>26.66666666674332</v>
-      </c>
-      <c r="H10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M10" t="s" s="0">
-        <v>49</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s" s="0">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="9"/>
+      <c r="T1" s="10"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="E2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="J2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="L2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>56</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>64.857142857142861</v>
+      </c>
+      <c r="B3">
+        <v>37.086666666666659</v>
+      </c>
+      <c r="C3">
+        <v>22.06</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>64.136274509803926</v>
+      </c>
+      <c r="F3">
+        <v>36.37936507936508</v>
+      </c>
+      <c r="G3">
+        <v>22.807936507936507</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>62.111111111111114</v>
+      </c>
+      <c r="J3">
+        <v>26.769593032228023</v>
+      </c>
+      <c r="K3" s="5">
+        <v>9</v>
+      </c>
+      <c r="L3" s="4">
+        <v>36.5</v>
+      </c>
+      <c r="M3">
+        <v>16.699016224231379</v>
+      </c>
+      <c r="N3">
+        <v>8</v>
+      </c>
+      <c r="O3" s="4">
+        <v>22</v>
+      </c>
+      <c r="P3">
+        <v>15.702593052468391</v>
+      </c>
+      <c r="Q3">
+        <v>8</v>
+      </c>
+      <c r="R3" s="4">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="5">
+        <v>9</v>
+      </c>
+      <c r="V3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="n" s="0">
-        <v>64.85714285714286</v>
-      </c>
-      <c r="B2" t="n" s="0">
-        <v>37.08666666666666</v>
-      </c>
-      <c r="C2" t="n" s="0">
-        <v>22.06</v>
-      </c>
-      <c r="D2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E2" t="n" s="0">
-        <v>64.13627450980393</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>36.37936507936508</v>
-      </c>
-      <c r="G2" t="n" s="0">
-        <v>22.807936507936507</v>
-      </c>
-      <c r="H2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="n" s="0">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
         <v>87.63333333333334</v>
       </c>
-      <c r="B3" t="n" s="0">
+      <c r="B4">
         <v>47.040000000000006</v>
       </c>
-      <c r="C3" t="n" s="0">
+      <c r="C4">
         <v>38.28</v>
       </c>
-      <c r="D3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E3" t="n" s="0">
-        <v>88.47222222222221</v>
-      </c>
-      <c r="F3" t="n" s="0">
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>88.472222222222214</v>
+      </c>
+      <c r="F4">
         <v>46.875</v>
       </c>
-      <c r="G3" t="n" s="0">
+      <c r="G4">
         <v>36.75</v>
       </c>
-      <c r="H3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="n" s="0">
-        <v>71.3075</v>
-      </c>
-      <c r="B4" t="n" s="0">
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>88.5</v>
+      </c>
+      <c r="J4">
+        <v>16.542873591570078</v>
+      </c>
+      <c r="K4" s="5">
+        <v>4</v>
+      </c>
+      <c r="L4" s="4">
+        <v>47.333333333333336</v>
+      </c>
+      <c r="M4">
+        <v>17.243356208503418</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4" s="4">
+        <v>41</v>
+      </c>
+      <c r="P4">
+        <v>11.532562594670797</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4" s="4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="5">
+        <v>4</v>
+      </c>
+      <c r="V4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>71.307500000000005</v>
+      </c>
+      <c r="B5">
         <v>27.790476190476188</v>
       </c>
-      <c r="C4" t="n" s="0">
-        <v>28.46666666666667</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E4" t="n" s="0">
-        <v>75.03571428571428</v>
-      </c>
-      <c r="F4" t="n" s="0">
+      <c r="C5">
+        <v>28.466666666666669</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>75.035714285714278</v>
+      </c>
+      <c r="F5">
         <v>28.160714285714285</v>
       </c>
-      <c r="G4" t="n" s="0">
-        <v>28.42857142857143</v>
-      </c>
-      <c r="H4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K4" t="s" s="0">
-        <v>53</v>
+      <c r="G5">
+        <v>28.428571428571431</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>77</v>
+      </c>
+      <c r="J5">
+        <v>37.242448899072144</v>
+      </c>
+      <c r="K5" s="5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="4">
+        <v>26.5</v>
+      </c>
+      <c r="M5">
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5" s="4">
+        <v>29</v>
+      </c>
+      <c r="P5">
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5" s="4">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5" s="5">
+        <v>3</v>
+      </c>
+      <c r="V5" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
There are numbers but I want to triple check the weighted formula for duo averages
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984A1CA8-DA65-4726-A692-7F9E029826F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD34F4AF-DA2F-4068-8AD3-AD3FB7907BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
   <sheets>
     <sheet name="Match Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="56">
   <si>
     <t>Cyrus</t>
   </si>
@@ -200,14 +200,19 @@
     <t>L+C</t>
   </si>
   <si>
-    <t>Date-Weighted Averages</t>
+    <t>Take with a grain of salt for right now</t>
+  </si>
+  <si>
+    <t>Weighted by comp/practice,   old/new robot,   and how old the matches are</t>
+  </si>
+  <si>
+    <t>All data here is weighted by    old/new robot,    practice/comp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1694,8 +1699,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -1728,31 +1733,31 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>45237</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>106</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>-1</v>
       </c>
-      <c r="H2" s="0">
+      <c r="H2">
         <v>-1</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2">
         <v>0</v>
       </c>
       <c r="M2" s="2"/>
@@ -1765,721 +1770,721 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>45237</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>83</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>-1</v>
       </c>
-      <c r="H3" s="0">
+      <c r="H3">
         <v>-1</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>45237</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4">
         <v>89</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4">
         <v>-1</v>
       </c>
-      <c r="H4" s="0">
+      <c r="H4">
         <v>-1</v>
       </c>
-      <c r="I4" s="0">
+      <c r="I4">
         <v>0</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>45238</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s" s="0">
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5">
         <v>71</v>
       </c>
-      <c r="G5" s="0">
+      <c r="G5">
         <v>-1</v>
       </c>
-      <c r="H5" s="0">
+      <c r="H5">
         <v>-1</v>
       </c>
-      <c r="I5" s="0">
+      <c r="I5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>45238</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>88</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6">
         <v>-1</v>
       </c>
-      <c r="H6" s="0">
+      <c r="H6">
         <v>-1</v>
       </c>
-      <c r="I6" s="0">
+      <c r="I6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>45238</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>111</v>
       </c>
-      <c r="G7" s="0">
+      <c r="G7">
         <v>-1</v>
       </c>
-      <c r="H7" s="0">
+      <c r="H7">
         <v>-1</v>
       </c>
-      <c r="I7" s="0">
+      <c r="I7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>45238</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <v>34</v>
       </c>
-      <c r="G8" s="0">
+      <c r="G8">
         <v>-1</v>
       </c>
-      <c r="H8" s="0">
+      <c r="H8">
         <v>-1</v>
       </c>
-      <c r="I8" s="0">
+      <c r="I8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>45238</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s" s="0">
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>120</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G9">
         <v>-1</v>
       </c>
-      <c r="H9" s="0">
+      <c r="H9">
         <v>-1</v>
       </c>
-      <c r="I9" s="0">
+      <c r="I9">
         <v>0</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>45238</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s" s="0">
+      <c r="E10" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="0">
+      <c r="F10">
         <v>75</v>
       </c>
-      <c r="G10" s="0">
+      <c r="G10">
         <v>-1</v>
       </c>
-      <c r="H10" s="0">
+      <c r="H10">
         <v>-1</v>
       </c>
-      <c r="I10" s="0">
+      <c r="I10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>45237</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>2</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="0">
+      <c r="F11">
         <v>111</v>
       </c>
-      <c r="G11" s="0">
+      <c r="G11">
         <v>66</v>
       </c>
-      <c r="H11" s="0">
+      <c r="H11">
         <v>45</v>
       </c>
-      <c r="I11" s="0">
+      <c r="I11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>45238</v>
       </c>
-      <c r="C12" t="s" s="0">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s" s="0">
+      <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s" s="0">
+      <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="0">
+      <c r="F12">
         <v>107</v>
       </c>
-      <c r="G12" s="0">
+      <c r="G12">
         <v>57</v>
       </c>
-      <c r="H12" s="0">
+      <c r="H12">
         <v>50</v>
       </c>
-      <c r="I12" s="0">
+      <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>45234</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>72</v>
       </c>
-      <c r="G13" s="0">
+      <c r="G13">
         <v>44</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <v>28</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s" s="0">
+      <c r="A14" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="1">
         <v>45234</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>97</v>
       </c>
-      <c r="G14" s="0">
+      <c r="G14">
         <v>51</v>
       </c>
-      <c r="H14" s="0">
+      <c r="H14">
         <v>30</v>
       </c>
-      <c r="I14" s="0">
+      <c r="I14">
         <v>0</v>
       </c>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s" s="0">
+      <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="1">
         <v>45234</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s" s="0">
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>54</v>
       </c>
-      <c r="G15" s="0">
+      <c r="G15">
         <v>26</v>
       </c>
-      <c r="H15" s="0">
+      <c r="H15">
         <v>28</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s" s="0">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>45234</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>82</v>
       </c>
-      <c r="G16" s="0">
+      <c r="G16">
         <v>32</v>
       </c>
-      <c r="H16" s="0">
+      <c r="H16">
         <v>50</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" t="s" s="0">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>45234</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>60</v>
       </c>
-      <c r="G17" s="0">
+      <c r="G17">
         <v>40</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H17">
         <v>20</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" t="s" s="0">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>45234</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s" s="0">
+      <c r="D18" t="s">
         <v>9</v>
       </c>
-      <c r="E18" t="s" s="0">
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>56</v>
       </c>
-      <c r="G18" s="0">
+      <c r="G18">
         <v>48</v>
       </c>
-      <c r="H18" s="0">
+      <c r="H18">
         <v>8</v>
       </c>
-      <c r="I18" s="0">
+      <c r="I18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" t="s" s="0">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>45234</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>60</v>
       </c>
-      <c r="G19" s="0">
+      <c r="G19">
         <v>30</v>
       </c>
-      <c r="H19" s="0">
+      <c r="H19">
         <v>30</v>
       </c>
-      <c r="I19" s="0">
+      <c r="I19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" t="s" s="0">
+      <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>45234</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s" s="0">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>39</v>
       </c>
-      <c r="G20" s="0">
+      <c r="G20">
         <v>34</v>
       </c>
-      <c r="H20" s="0">
+      <c r="H20">
         <v>5</v>
       </c>
-      <c r="I20" s="0">
+      <c r="I20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" t="s" s="0">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>45241</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s" s="0">
+      <c r="E21" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21">
         <v>32</v>
       </c>
-      <c r="G21" s="0">
+      <c r="G21">
         <v>4</v>
       </c>
-      <c r="H21" s="0">
+      <c r="H21">
         <v>28</v>
       </c>
-      <c r="I21" s="0">
-        <v>0</v>
-      </c>
-      <c r="K21" t="s" s="0">
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" t="s" s="0">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>45241</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>4</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>83</v>
       </c>
-      <c r="G22" s="0">
+      <c r="G22">
         <v>55</v>
       </c>
-      <c r="H22" s="0">
+      <c r="H22">
         <v>28</v>
       </c>
-      <c r="I22" s="0">
-        <v>0</v>
-      </c>
-      <c r="K22" t="s" s="0">
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" t="s" s="0">
+      <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>45241</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>3</v>
       </c>
-      <c r="D23" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E23" t="s" s="0">
+      <c r="D23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>56</v>
       </c>
-      <c r="G23" s="0">
+      <c r="G23">
         <v>26</v>
       </c>
-      <c r="H23" s="0">
+      <c r="H23">
         <v>30</v>
       </c>
-      <c r="I23" s="0">
-        <v>0</v>
-      </c>
-      <c r="K23" t="s" s="0">
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" t="s" s="0">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>45241</v>
       </c>
-      <c r="C24" t="s" s="0">
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" t="s" s="0">
+      <c r="D24" t="s">
         <v>9</v>
       </c>
-      <c r="E24" t="s" s="0">
+      <c r="E24" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="0">
+      <c r="F24">
         <v>33</v>
       </c>
-      <c r="G24" s="0">
+      <c r="G24">
         <v>28</v>
       </c>
-      <c r="H24" s="0">
+      <c r="H24">
         <v>5</v>
       </c>
-      <c r="I24" s="0">
-        <v>0</v>
-      </c>
-      <c r="K24" t="s" s="0">
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" t="s" s="0">
+      <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>45241</v>
       </c>
-      <c r="C25" t="s" s="0">
+      <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="D25" t="s" s="0">
+      <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" t="s" s="0">
+      <c r="E25" t="s">
         <v>1</v>
       </c>
-      <c r="F25" s="0">
+      <c r="F25">
         <v>56</v>
       </c>
-      <c r="G25" s="0">
+      <c r="G25">
         <v>36</v>
       </c>
-      <c r="H25" s="0">
+      <c r="H25">
         <v>20</v>
       </c>
-      <c r="I25" s="0">
-        <v>0</v>
-      </c>
-      <c r="K25" t="s" s="0">
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" t="s" s="0">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="1">
         <v>45241</v>
       </c>
-      <c r="C26" t="s" s="0">
+      <c r="C26" t="s">
         <v>3</v>
       </c>
-      <c r="D26" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s" s="0">
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="0">
+      <c r="F26">
         <v>55</v>
       </c>
-      <c r="G26" s="0">
+      <c r="G26">
         <v>27</v>
       </c>
-      <c r="H26" s="0">
+      <c r="H26">
         <v>28</v>
       </c>
-      <c r="I26" s="0">
-        <v>0</v>
-      </c>
-      <c r="K26" t="s" s="0">
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
         <v>42</v>
       </c>
       <c r="T26" s="6"/>
@@ -2490,7 +2495,7 @@
       <c r="Y26" s="2"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="L27" t="s" s="0">
+      <c r="L27" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2520,8 +2525,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -2553,7 +2558,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="V2" t="s" s="0">
+      <c r="V2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2561,16 +2566,16 @@
       <c r="A3" s="1">
         <v>45237</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>106</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2578,25 +2583,25 @@
       <c r="A4" s="1">
         <v>45237</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>83</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" t="s" s="0">
+      <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="O4" t="s" s="0">
+      <c r="O4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2604,26 +2609,26 @@
       <c r="A5" s="1">
         <v>45237</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>89</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="M5" t="s" s="0">
+      <c r="M5" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="0">
+      <c r="N5">
         <f>(SUMIF($C$3:$C$100, M5, $B$3:$B$100)/COUNTIF($C$3:$C$100, M5))</f>
         <v>88.083333333333329</v>
       </c>
-      <c r="O5" s="0">
+      <c r="O5">
         <f>(SUMIF($C$3:$C$100, M5, $F$3:$F$100)/COUNTIF($C$13:$C$100, M5))</f>
         <v>42.428571428571431</v>
       </c>
@@ -2632,26 +2637,26 @@
       <c r="A6" s="1">
         <v>45238</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>71</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s" s="0">
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="M6" t="s" s="0">
+      <c r="M6" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="0">
+      <c r="N6">
         <f>(SUMIF($C$3:$C$100, M6, $B$3:$B$100)/COUNTIF($C$3:$C$100, M6))</f>
         <v>98.5</v>
       </c>
-      <c r="O6" s="0">
+      <c r="O6">
         <f>(SUMIF($C$3:$C$100, M6, $F$3:$F$100)/COUNTIF($C$13:$C$100, M6))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2660,26 +2665,26 @@
       <c r="A7" s="1">
         <v>45238</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>88</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="M7" t="s" s="0">
+      <c r="M7" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="0">
+      <c r="N7">
         <f>(SUMIF($C$3:$C$100, M7, $B$3:$B$100)/COUNTIF($C$3:$C$100, M7))</f>
         <v>86.25</v>
       </c>
-      <c r="O7" s="0">
+      <c r="O7">
         <f>(SUMIF($C$3:$C$100, M7, $F$3:$F$100)/COUNTIF($C$13:$C$100, M7))</f>
         <v>38</v>
       </c>
@@ -2688,16 +2693,16 @@
       <c r="A8" s="1">
         <v>45238</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8">
         <v>111</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>2</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2705,16 +2710,16 @@
       <c r="A9" s="1">
         <v>45238</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9">
         <v>34</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -2725,16 +2730,16 @@
       <c r="A10" s="1">
         <v>45238</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10">
         <v>120</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s" s="0">
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="H10" s="6" t="s">
@@ -2743,14 +2748,14 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-      <c r="M10" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="N10" s="0">
+      <c r="M10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <f>(SUMIF($D$3:$D$100, M10, $B$3:$B$100)/COUNTIF($D$3:$D$100, M10))</f>
         <v>96.666666666666671</v>
       </c>
-      <c r="O10" s="0">
+      <c r="O10">
         <f>(SUMIF($D$3:$D$100, M10, $F$3:$F$100)/COUNTIF($D$13:$D$100, M10))</f>
         <v>26</v>
       </c>
@@ -2759,16 +2764,16 @@
       <c r="A11" s="1">
         <v>45238</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11">
         <v>75</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="H11" s="6" t="s">
@@ -2779,14 +2784,14 @@
         <v>22</v>
       </c>
       <c r="K11" s="6"/>
-      <c r="M11" t="s" s="0">
+      <c r="M11" t="s">
         <v>9</v>
       </c>
-      <c r="N11" s="0">
+      <c r="N11">
         <f>(SUMIF($D$3:$D$100, M11, $B$3:$B$100)/COUNTIF($D$3:$D$100, M11))</f>
         <v>77</v>
       </c>
-      <c r="O11" s="0">
+      <c r="O11">
         <f>(SUMIF($D$3:$D$100, M11, $F$3:$F$100)/COUNTIF($D$13:$D$100, M11))</f>
         <v>45.166666666666664</v>
       </c>
@@ -2804,14 +2809,14 @@
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s" s="0">
+      <c r="M12" t="s">
         <v>2</v>
       </c>
-      <c r="N12" s="0">
+      <c r="N12">
         <f>(SUMIF($D$3:$D$100, M12, $B$3:$B$100)/COUNTIF($D$3:$D$100, M12))</f>
         <v>97.75</v>
       </c>
-      <c r="O12" s="0">
+      <c r="O12">
         <f>(SUMIF($D$3:$D$100, M12, $F$3:$F$100)/COUNTIF($D$13:$D$100, M12))</f>
         <v>57.333333333333336</v>
       </c>
@@ -2820,26 +2825,26 @@
       <c r="A13" s="1">
         <v>45237</v>
       </c>
-      <c r="B13" s="0">
+      <c r="B13">
         <v>111</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>66</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <f t="shared" ref="H13:H23" si="0">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12)+SUMIF($M$15:$M$17, $E13, $N$15:$N$17))/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <f t="shared" ref="I13:I23" si="1">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12)+SUMIF($M$15:$M$17, $E13, $O$15:$O$17))/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -2847,7 +2852,7 @@
         <f t="shared" ref="J13:J23" si="2">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12))/2</f>
         <v>98.125</v>
       </c>
-      <c r="K13" s="0">
+      <c r="K13">
         <f t="shared" ref="K13:K23" si="3">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12))/2</f>
         <v>57.333333333333336</v>
       </c>
@@ -2856,26 +2861,26 @@
       <c r="A14" s="1">
         <v>45238</v>
       </c>
-      <c r="B14" s="0">
+      <c r="B14">
         <v>107</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>57</v>
       </c>
-      <c r="H14" s="0">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>84.49444444444444</v>
       </c>
-      <c r="I14" s="0">
+      <c r="I14">
         <f t="shared" si="1"/>
         <v>48.198412698412703</v>
       </c>
@@ -2883,7 +2888,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K14" s="0">
+      <c r="K14">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -2895,26 +2900,26 @@
       <c r="A15" s="1">
         <v>45234</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15">
         <v>108</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s" s="0">
+      <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="s" s="0">
+      <c r="E15" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>38</v>
       </c>
-      <c r="H15" s="0">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>63.166666666666664</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15">
         <f t="shared" si="1"/>
         <v>30.166666666666668</v>
       </c>
@@ -2922,18 +2927,18 @@
         <f t="shared" si="2"/>
         <v>43.125</v>
       </c>
-      <c r="K15" s="0">
+      <c r="K15">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="M15" t="s" s="0">
+      <c r="M15" t="s">
         <v>10</v>
       </c>
-      <c r="N15" s="0">
+      <c r="N15">
         <f>(SUMIF($E$3:$E$100, M15, $B$3:$B$100)/COUNTIF($E$3:$E$100, M15))</f>
         <v>83.166666666666671</v>
       </c>
-      <c r="O15" s="0">
+      <c r="O15">
         <f>(SUMIF($E$3:$E$100, M15, $F$3:$F$100)/COUNTIF($E$13:$E$100, M15))</f>
         <v>40</v>
       </c>
@@ -2942,26 +2947,26 @@
       <c r="A16" s="1">
         <v>45234</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16">
         <v>107</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>74</v>
       </c>
-      <c r="H16" s="0">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -2969,18 +2974,18 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K16" s="0">
+      <c r="K16">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
-      <c r="M16" t="s" s="0">
+      <c r="M16" t="s">
         <v>1</v>
       </c>
-      <c r="N16" s="0">
+      <c r="N16">
         <f>(SUMIF($E$3:$E$100, M16, $B$3:$B$100)/COUNTIF($E$3:$E$100, M16))</f>
         <v>88.4</v>
       </c>
-      <c r="O16" s="0">
+      <c r="O16">
         <f>(SUMIF($E$3:$E$100, M16, $F$3:$F$100)/COUNTIF($E$13:$E$100, M16))</f>
         <v>57</v>
       </c>
@@ -2989,26 +2994,26 @@
       <c r="A17" s="1">
         <v>45234</v>
       </c>
-      <c r="B17" s="0">
+      <c r="B17">
         <v>97</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>62</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I17">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3016,18 +3021,18 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K17" s="0">
+      <c r="K17">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
-      <c r="M17" t="s" s="0">
+      <c r="M17" t="s">
         <v>5</v>
       </c>
-      <c r="N17" s="0">
+      <c r="N17">
         <f>(SUMIF($E$3:$E$100, M17, $B$3:$B$100)/COUNTIF($E$3:$E$100, M17))</f>
         <v>103.25</v>
       </c>
-      <c r="O17" s="0">
+      <c r="O17">
         <f>(SUMIF($E$3:$E$100, M17, $F$3:$F$100)/COUNTIF($E$13:$E$100, M17))</f>
         <v>52.5</v>
       </c>
@@ -3036,26 +3041,26 @@
       <c r="A18" s="1">
         <v>45234</v>
       </c>
-      <c r="B18" s="0">
+      <c r="B18">
         <v>99</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s" s="0">
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>26</v>
       </c>
-      <c r="H18" s="0">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>89.305555555555557</v>
       </c>
-      <c r="I18" s="0">
+      <c r="I18">
         <f t="shared" si="1"/>
         <v>36.142857142857146</v>
       </c>
@@ -3063,7 +3068,7 @@
         <f t="shared" si="2"/>
         <v>92.375</v>
       </c>
-      <c r="K18" s="0">
+      <c r="K18">
         <f t="shared" si="3"/>
         <v>34.214285714285715</v>
       </c>
@@ -3072,26 +3077,26 @@
       <c r="A19" s="1">
         <v>45234</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19">
         <v>87</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>2</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>32</v>
       </c>
-      <c r="H19" s="0">
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I19" s="0">
+      <c r="I19">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -3099,7 +3104,7 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K19" s="0">
+      <c r="K19">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
@@ -3108,26 +3113,26 @@
       <c r="A20" s="1">
         <v>45234</v>
       </c>
-      <c r="B20" s="0">
+      <c r="B20">
         <v>76</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s" s="0">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>48</v>
       </c>
-      <c r="H20" s="0">
+      <c r="H20">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I20" s="0">
+      <c r="I20">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3135,7 +3140,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K20" s="0">
+      <c r="K20">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3144,26 +3149,26 @@
       <c r="A21" s="1">
         <v>45234</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21">
         <v>93</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s" s="0">
+      <c r="E21" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21">
         <v>40</v>
       </c>
-      <c r="H21" s="0">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I21" s="0">
+      <c r="I21">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3171,7 +3176,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K21" s="0">
+      <c r="K21">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3180,26 +3185,26 @@
       <c r="A22" s="1">
         <v>45234</v>
       </c>
-      <c r="B22" s="0">
+      <c r="B22">
         <v>85</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>30</v>
       </c>
-      <c r="H22" s="0">
+      <c r="H22">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I22" s="0">
+      <c r="I22">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3207,7 +3212,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K22" s="0">
+      <c r="K22">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3216,26 +3221,26 @@
       <c r="A23" s="1">
         <v>45234</v>
       </c>
-      <c r="B23" s="0">
+      <c r="B23">
         <v>49</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>11</v>
       </c>
-      <c r="D23" t="s" s="0">
+      <c r="D23" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s" s="0">
+      <c r="E23" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>34</v>
       </c>
-      <c r="H23" s="0">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I23" s="0">
+      <c r="I23">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -3243,7 +3248,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K23" s="0">
+      <c r="K23">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -3263,67 +3268,67 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T28" s="0">
+      <c r="T28">
         <v>1</v>
       </c>
-      <c r="U28" t="s" s="0">
+      <c r="U28" t="s">
         <v>3</v>
       </c>
-      <c r="V28" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="W28" t="s" s="0">
+      <c r="V28" t="s">
+        <v>0</v>
+      </c>
+      <c r="W28" t="s">
         <v>1</v>
       </c>
-      <c r="X28" s="0">
+      <c r="X28">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y28" s="0">
+      <c r="Y28">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T29" s="0">
+      <c r="T29">
         <v>2</v>
       </c>
-      <c r="U29" t="s" s="0">
+      <c r="U29" t="s">
         <v>11</v>
       </c>
-      <c r="V29" t="s" s="0">
+      <c r="V29" t="s">
         <v>9</v>
       </c>
-      <c r="W29" t="s" s="0">
+      <c r="W29" t="s">
         <v>1</v>
       </c>
-      <c r="X29" s="0">
+      <c r="X29">
         <f>(N5+N11+N16)/3</f>
         <v>84.49444444444444</v>
       </c>
-      <c r="Y29" s="0">
+      <c r="Y29">
         <f>(O5+O11+O16)/3</f>
         <v>48.198412698412703</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T30" s="0">
+      <c r="T30">
         <v>3</v>
       </c>
-      <c r="U30" t="s" s="0">
+      <c r="U30" t="s">
         <v>4</v>
       </c>
-      <c r="V30" t="s" s="0">
+      <c r="V30" t="s">
         <v>9</v>
       </c>
-      <c r="W30" t="s" s="0">
+      <c r="W30" t="s">
         <v>1</v>
       </c>
-      <c r="X30" s="0">
+      <c r="X30">
         <f>(N6+N11+N16)/3</f>
         <v>87.966666666666654</v>
       </c>
-      <c r="Y30" s="0">
+      <c r="Y30">
         <f>(O6+O11+O16)/3</f>
         <v>53.166666666666664</v>
       </c>
@@ -3337,67 +3342,67 @@
       <c r="W32" s="6"/>
     </row>
     <row r="33" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T33" s="0">
+      <c r="T33">
         <v>1</v>
       </c>
-      <c r="U33" t="s" s="0">
+      <c r="U33" t="s">
         <v>3</v>
       </c>
-      <c r="V33" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="W33" t="s" s="0">
+      <c r="V33" t="s">
+        <v>0</v>
+      </c>
+      <c r="W33" t="s">
         <v>1</v>
       </c>
-      <c r="X33" s="0">
+      <c r="X33">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y33" s="0">
+      <c r="Y33">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="34" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T34" s="0">
+      <c r="T34">
         <v>2</v>
       </c>
-      <c r="U34" t="s" s="0">
+      <c r="U34" t="s">
         <v>11</v>
       </c>
-      <c r="V34" t="s" s="0">
+      <c r="V34" t="s">
         <v>9</v>
       </c>
-      <c r="W34" t="s" s="0">
+      <c r="W34" t="s">
         <v>10</v>
       </c>
-      <c r="X34" s="0">
+      <c r="X34">
         <f>(N5+N11+N15)/3</f>
         <v>82.75</v>
       </c>
-      <c r="Y34" s="0">
+      <c r="Y34">
         <f>(O5+O11+O15)/3</f>
         <v>42.531746031746032</v>
       </c>
     </row>
     <row r="35" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T35" s="0">
+      <c r="T35">
         <v>3</v>
       </c>
-      <c r="U35" t="s" s="0">
+      <c r="U35" t="s">
         <v>4</v>
       </c>
-      <c r="V35" t="s" s="0">
+      <c r="V35" t="s">
         <v>2</v>
       </c>
-      <c r="W35" t="s" s="0">
+      <c r="W35" t="s">
         <v>5</v>
       </c>
-      <c r="X35" s="0">
+      <c r="X35">
         <f>(N6+N12+N17)/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="Y35" s="0">
+      <c r="Y35">
         <f>(O6+O12+O17)/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -3418,319 +3423,211 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
-      <c r="E1" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="E1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="n" s="0">
-        <v>64.08617594267274</v>
-      </c>
-      <c r="B3" t="n" s="0">
-        <v>33.08037825085841</v>
-      </c>
-      <c r="C3" t="n" s="0">
-        <v>21.030732860527774</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="F3" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="G3" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="H3" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="M3" t="s" s="0">
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>68.34761321914732</v>
+      </c>
+      <c r="B3">
+        <v>33.962659380931484</v>
+      </c>
+      <c r="C3">
+        <v>22.099271402535425</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="n" s="0">
-        <v>78.12121212133545</v>
-      </c>
-      <c r="B4" t="n" s="0">
-        <v>44.84033613435197</v>
-      </c>
-      <c r="C4" t="n" s="0">
-        <v>32.09243697502329</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="H4" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="M4" t="s" s="0">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>80.433604336161849</v>
+      </c>
+      <c r="B4">
+        <v>46.141955835871975</v>
+      </c>
+      <c r="C4">
+        <v>32.886435331452574</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="n" s="0">
-        <v>64.88000000016457</v>
-      </c>
-      <c r="B5" t="n" s="0">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>67.603225806624124</v>
+      </c>
+      <c r="B5">
         <v>26.500000000000004</v>
       </c>
-      <c r="C5" t="n" s="0">
-        <v>29.0</v>
-      </c>
-      <c r="D5" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="F5" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="G5" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="H5" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="M5" t="s" s="0">
+      <c r="C5">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="n" s="0">
-        <v>58.845735027374296</v>
-      </c>
-      <c r="B6" t="n" s="0">
-        <v>36.73440643878293</v>
-      </c>
-      <c r="C6" t="n" s="0">
-        <v>21.10261569412463</v>
-      </c>
-      <c r="D6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="4" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="F6" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="G6" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="H6" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="M6" t="s" s="0">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>59.911941294327768</v>
+      </c>
+      <c r="B6">
+        <v>37.374123149011183</v>
+      </c>
+      <c r="C6">
+        <v>22.014809041263188</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="n" s="0">
-        <v>90.28399999981394</v>
-      </c>
-      <c r="B7" t="n" s="0">
-        <v>44.16949152525964</v>
-      </c>
-      <c r="C7" t="n" s="0">
-        <v>40.32203389826992</v>
-      </c>
-      <c r="D7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="4" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="F7" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="G7" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="H7" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="M7" t="s" s="0">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>92.410672853670846</v>
+      </c>
+      <c r="B7">
+        <v>46.718562874046683</v>
+      </c>
+      <c r="C7">
+        <v>40.868263473010003</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="n" s="0">
-        <v>65.00454545457524</v>
-      </c>
-      <c r="B8" t="n" s="0">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>68.919175911293578</v>
+      </c>
+      <c r="B8">
         <v>26.361445783125625</v>
       </c>
-      <c r="C8" t="n" s="0">
+      <c r="C8">
         <v>28.722891566251242</v>
       </c>
-      <c r="D8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="4" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="F8" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="G8" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="H8" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="M8" t="s" s="0">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="n" s="0">
-        <v>61.00000000000001</v>
-      </c>
-      <c r="B9" t="n" s="0">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>61.000000000000007</v>
+      </c>
+      <c r="B9">
         <v>38.166666666666664</v>
       </c>
-      <c r="C9" t="n" s="0">
-        <v>20.16666666666667</v>
-      </c>
-      <c r="D9" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="4" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="F9" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="G9" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="H9" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="M9" t="s" s="0">
+      <c r="C9">
+        <v>20.166666666666671</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="n" s="0">
-        <v>84.49152542352957</v>
-      </c>
-      <c r="B10" t="n" s="0">
-        <v>44.16949152525964</v>
-      </c>
-      <c r="C10" t="n" s="0">
-        <v>40.32203389826992</v>
-      </c>
-      <c r="D10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E10" s="4" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="F10" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="G10" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="H10" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="M10" t="s" s="0">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>87.586826347056686</v>
+      </c>
+      <c r="B10">
+        <v>46.718562874046683</v>
+      </c>
+      <c r="C10">
+        <v>40.868263473010003</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="n" s="0">
-        <v>67.76714513581695</v>
-      </c>
-      <c r="B11" t="n" s="0">
-        <v>31.2635658915181</v>
-      </c>
-      <c r="C11" t="n" s="0">
-        <v>25.038759689966348</v>
-      </c>
-      <c r="D11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E11" s="4" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="F11" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="G11" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="H11" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-      <c r="M11" t="s" s="0">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>71.956300813263994</v>
+      </c>
+      <c r="B11">
+        <v>32.297619047685707</v>
+      </c>
+      <c r="C11">
+        <v>26.041666666731317</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" t="s">
         <v>41</v>
       </c>
     </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3738,10 +3635,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3776,10 +3673,10 @@
       <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>48</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -3788,10 +3685,10 @@
       <c r="E2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>47</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>48</v>
       </c>
       <c r="H2" s="5" t="s">
@@ -3800,93 +3697,208 @@
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="n">
-        <v>61.37276438801881</v>
-      </c>
-      <c r="B3" t="n" s="0">
-        <v>35.55924720918987</v>
-      </c>
-      <c r="C3" t="n" s="0">
-        <v>20.886672755194294</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>63.150450450906995</v>
-      </c>
-      <c r="F3" t="n" s="0">
-        <v>37.76972222268363</v>
-      </c>
-      <c r="G3" t="n" s="0">
-        <v>22.631388889134115</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="V3" t="s" s="0">
+      <c r="A3" s="4">
+        <v>63.503821805390032</v>
+      </c>
+      <c r="B3">
+        <v>36.168046345310401</v>
+      </c>
+      <c r="C3">
+        <v>21.67896551085278</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>74.380878530232863</v>
+      </c>
+      <c r="F3">
+        <v>36.304239587768087</v>
+      </c>
+      <c r="G3">
+        <v>20.306478089143628</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>60.767441860465119</v>
+      </c>
+      <c r="J3">
+        <v>4.3121189275161278</v>
+      </c>
+      <c r="K3">
+        <v>8.6</v>
+      </c>
+      <c r="L3">
+        <v>35.974358974358978</v>
+      </c>
+      <c r="M3">
+        <v>3.5701967278731908</v>
+      </c>
+      <c r="N3">
+        <v>7.8</v>
+      </c>
+      <c r="O3">
+        <v>21.282051282051281</v>
+      </c>
+      <c r="P3">
+        <v>3.5615679432207918</v>
+      </c>
+      <c r="Q3">
+        <v>7.8</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>8.6</v>
+      </c>
+      <c r="V3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="n">
-        <v>84.26038993316567</v>
-      </c>
-      <c r="B4" t="n" s="0">
-        <v>44.43782936889657</v>
-      </c>
-      <c r="C4" t="n" s="0">
-        <v>37.03019512897127</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>94.32191781163097</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <v>50.36842105392377</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>46.89473684413396</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="V4" t="s" s="0">
+      <c r="A4" s="4">
+        <v>86.65507614534441</v>
+      </c>
+      <c r="B4">
+        <v>46.487920058776801</v>
+      </c>
+      <c r="C4">
+        <v>37.675532216387033</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>87.366432474664705</v>
+      </c>
+      <c r="F4">
+        <v>43.954545452171118</v>
+      </c>
+      <c r="G4">
+        <v>62.92207795470113</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>87.222222222222214</v>
+      </c>
+      <c r="J4">
+        <v>3.6439857956134349</v>
+      </c>
+      <c r="K4">
+        <v>3.6</v>
+      </c>
+      <c r="L4">
+        <v>46.000000000000007</v>
+      </c>
+      <c r="M4">
+        <v>3.4512477614786103</v>
+      </c>
+      <c r="N4">
+        <v>2.8</v>
+      </c>
+      <c r="O4">
+        <v>40.714285714285715</v>
+      </c>
+      <c r="P4">
+        <v>3.7838420048226538</v>
+      </c>
+      <c r="Q4">
+        <v>2.8</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>3.6</v>
+      </c>
+      <c r="V4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="n">
-        <v>65.5072472090593</v>
-      </c>
-      <c r="B5" t="n" s="0">
-        <v>27.39729149155387</v>
-      </c>
-      <c r="C5" t="n" s="0">
-        <v>28.096908564493766</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>68.09899328955389</v>
-      </c>
-      <c r="F5" t="n" s="0">
-        <v>28.110663082307774</v>
-      </c>
-      <c r="G5" t="n" s="0">
-        <v>27.543906810174263</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="V5" t="s" s="0">
+      <c r="A5" s="4">
+        <v>69.000220849819883</v>
+      </c>
+      <c r="B5">
+        <v>27.604102122787396</v>
+      </c>
+      <c r="C5">
+        <v>28.297489959846757</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>71.769873547703241</v>
+      </c>
+      <c r="F5">
+        <v>28.440718157038901</v>
+      </c>
+      <c r="G5">
+        <v>27.911924119349408</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>73.928571428571431</v>
+      </c>
+      <c r="J5">
+        <v>5.5032457955023499</v>
+      </c>
+      <c r="K5">
+        <v>2.8</v>
+      </c>
+      <c r="L5">
+        <v>26.5</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>29</v>
+      </c>
+      <c r="P5">
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>2.8</v>
+      </c>
+      <c r="V5" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some things are working but the numbers are kinda weird
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD34F4AF-DA2F-4068-8AD3-AD3FB7907BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B707080B-96FE-4208-AC0E-D60263CA4A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="57">
   <si>
     <t>Cyrus</t>
   </si>
@@ -173,9 +173,6 @@
     <t>&lt;- NEW ROBOT</t>
   </si>
   <si>
-    <t>Basic Averages</t>
-  </si>
-  <si>
     <t>Weighted Averages</t>
   </si>
   <si>
@@ -191,6 +188,21 @@
     <t>penalties</t>
   </si>
   <si>
+    <t>Take with a grain of salt for right now</t>
+  </si>
+  <si>
+    <t>Weighted by comp/practice,   old/new robot,   and how old the matches are</t>
+  </si>
+  <si>
+    <t>All data here is weighted by    old/new robot,    practice/comp</t>
+  </si>
+  <si>
+    <t>Penalties</t>
+  </si>
+  <si>
+    <t>Duo Only</t>
+  </si>
+  <si>
     <t>B+M</t>
   </si>
   <si>
@@ -198,15 +210,6 @@
   </si>
   <si>
     <t>L+C</t>
-  </si>
-  <si>
-    <t>Take with a grain of salt for right now</t>
-  </si>
-  <si>
-    <t>Weighted by comp/practice,   old/new robot,   and how old the matches are</t>
-  </si>
-  <si>
-    <t>All data here is weighted by    old/new robot,    practice/comp</t>
   </si>
 </sst>
 </file>
@@ -238,7 +241,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -255,26 +258,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -284,12 +277,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2487,10 +2475,10 @@
       <c r="K26" t="s">
         <v>42</v>
       </c>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="6"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
     </row>
@@ -2500,10 +2488,10 @@
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T31" s="6"/>
-      <c r="U31" s="6"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="6"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2742,12 +2730,12 @@
       <c r="E10" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
       <c r="M10" t="s">
         <v>0</v>
       </c>
@@ -2776,14 +2764,14 @@
       <c r="E11" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7" t="s">
+      <c r="I11" s="5"/>
+      <c r="J11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="6"/>
+      <c r="K11" s="5"/>
       <c r="M11" t="s">
         <v>9</v>
       </c>
@@ -3254,12 +3242,12 @@
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T27" s="6" t="s">
+      <c r="T27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="6"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
       <c r="X27" s="2" t="s">
         <v>23</v>
       </c>
@@ -3334,12 +3322,12 @@
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T32" s="6" t="s">
+      <c r="T32" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="U32" s="6"/>
-      <c r="V32" s="6"/>
-      <c r="W32" s="6"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
     </row>
     <row r="33" spans="20:25" x14ac:dyDescent="0.3">
       <c r="T33">
@@ -3432,12 +3420,12 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="A1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="3"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -3445,28 +3433,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
       </c>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>68.34761321914732</v>
+        <v>70.529411764743259</v>
       </c>
       <c r="B3">
-        <v>33.962659380931484</v>
+        <v>34.311111111458672</v>
       </c>
       <c r="C3">
-        <v>22.099271402535425</v>
+        <v>22.794444444401002</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -3478,13 +3466,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>80.433604336161849</v>
+        <v>81.617187500175135</v>
       </c>
       <c r="B4">
-        <v>46.141955835871975</v>
+        <v>46.999999999872905</v>
       </c>
       <c r="C4">
-        <v>32.886435331452574</v>
+        <v>33.168224299393273</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3496,13 +3484,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>67.603225806624124</v>
+        <v>68.747826087208466</v>
       </c>
       <c r="B5">
-        <v>26.500000000000004</v>
+        <v>26.5</v>
       </c>
       <c r="C5">
-        <v>29</v>
+        <v>28.999999999999996</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3514,13 +3502,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>59.911941294327768</v>
+        <v>60.421875000184279</v>
       </c>
       <c r="B6">
-        <v>37.374123149011183</v>
+        <v>37.655660377565155</v>
       </c>
       <c r="C6">
-        <v>22.014809041263188</v>
+        <v>22.636792452754229</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -3532,13 +3520,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>92.410672853670846</v>
+        <v>93.408536585147431</v>
       </c>
       <c r="B7">
-        <v>46.718562874046683</v>
+        <v>48.3157894733326</v>
       </c>
       <c r="C7">
-        <v>40.868263473010003</v>
+        <v>41.210526315714127</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -3550,13 +3538,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>68.919175911293578</v>
+        <v>70.973214285783129</v>
       </c>
       <c r="B8">
-        <v>26.361445783125625</v>
+        <v>26.367647058813244</v>
       </c>
       <c r="C8">
-        <v>28.722891566251242</v>
+        <v>28.73529411762647</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -3568,13 +3556,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>61.000000000000007</v>
+        <v>61.000000000000014</v>
       </c>
       <c r="B9">
-        <v>38.166666666666664</v>
+        <v>38.166666666666671</v>
       </c>
       <c r="C9">
-        <v>20.166666666666671</v>
+        <v>20.166666666666668</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3586,13 +3574,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>87.586826347056686</v>
+        <v>89.52631578904672</v>
       </c>
       <c r="B10">
-        <v>46.718562874046683</v>
+        <v>48.3157894733326</v>
       </c>
       <c r="C10">
-        <v>40.868263473010003</v>
+        <v>41.210526315714127</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -3604,13 +3592,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>71.956300813263994</v>
+        <v>73.692098093012234</v>
       </c>
       <c r="B11">
-        <v>32.297619047685707</v>
+        <v>32.872093023370269</v>
       </c>
       <c r="C11">
-        <v>26.041666666731317</v>
+        <v>26.59883720941334</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -3622,7 +3610,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -3635,276 +3623,331 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:BL9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
+    <row r="1" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>46</v>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2"/>
+      <c r="BG1" s="2"/>
+      <c r="BH1" s="2"/>
+      <c r="BI1" s="2"/>
+      <c r="BJ1" s="2"/>
+      <c r="BK1" s="2"/>
+      <c r="BL1" s="2"/>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>46</v>
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>63.503821805390032</v>
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>62.111111111111114</v>
       </c>
       <c r="B3">
-        <v>36.168046345310401</v>
+        <v>36.5</v>
       </c>
       <c r="C3">
-        <v>21.67896551085278</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>74.380878530232863</v>
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>62.4</v>
       </c>
       <c r="F3">
-        <v>36.304239587768087</v>
+        <v>40.6</v>
       </c>
       <c r="G3">
-        <v>20.306478089143628</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4">
-        <v>60.767441860465119</v>
-      </c>
-      <c r="J3">
-        <v>4.3121189275161278</v>
-      </c>
-      <c r="K3">
-        <v>8.6</v>
+        <v>18.600000000000001</v>
+      </c>
+      <c r="H3">
+        <v>-1</v>
+      </c>
+      <c r="I3" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="J3" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="L3">
-        <v>35.974358974358978</v>
+        <v>-1</v>
       </c>
       <c r="M3">
-        <v>3.5701967278731908</v>
+        <v>61.75</v>
       </c>
       <c r="N3">
-        <v>7.8</v>
+        <v>29.666666666666668</v>
       </c>
       <c r="O3">
-        <v>21.282051282051281</v>
+        <v>27.666666666666668</v>
       </c>
       <c r="P3">
-        <v>3.5615679432207918</v>
-      </c>
-      <c r="Q3">
-        <v>7.8</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>8.6</v>
-      </c>
-      <c r="V3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>86.65507614534441</v>
+        <v>-1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>88.5</v>
       </c>
       <c r="B4">
-        <v>46.487920058776801</v>
+        <v>47.333333333333336</v>
       </c>
       <c r="C4">
-        <v>37.675532216387033</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>87.366432474664705</v>
-      </c>
-      <c r="F4">
-        <v>43.954545452171118</v>
-      </c>
-      <c r="G4">
-        <v>62.92207795470113</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4">
-        <v>87.222222222222214</v>
+        <v>41</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="F4" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G4" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H4">
+        <v>-1</v>
+      </c>
+      <c r="I4">
+        <v>88.333333333333329</v>
       </c>
       <c r="J4">
-        <v>3.6439857956134349</v>
+        <v>47.333333333333336</v>
       </c>
       <c r="K4">
-        <v>3.6</v>
+        <v>41</v>
       </c>
       <c r="L4">
-        <v>46.000000000000007</v>
+        <v>-1</v>
       </c>
       <c r="M4">
-        <v>3.4512477614786103</v>
-      </c>
-      <c r="N4">
-        <v>2.8</v>
-      </c>
-      <c r="O4">
-        <v>40.714285714285715</v>
+        <v>89</v>
+      </c>
+      <c r="N4" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="O4" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="P4">
-        <v>3.7838420048226538</v>
-      </c>
-      <c r="Q4">
-        <v>2.8</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>3.6</v>
-      </c>
-      <c r="V4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>69.000220849819883</v>
+        <v>-1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>77</v>
       </c>
       <c r="B5">
-        <v>27.604102122787396</v>
+        <v>26.5</v>
       </c>
       <c r="C5">
-        <v>28.297489959846757</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>71.769873547703241</v>
-      </c>
-      <c r="F5">
-        <v>28.440718157038901</v>
-      </c>
-      <c r="G5">
-        <v>27.911924119349408</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="4">
-        <v>73.928571428571431</v>
-      </c>
-      <c r="J5">
-        <v>5.5032457955023499</v>
-      </c>
-      <c r="K5">
-        <v>2.8</v>
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="F5" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G5" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H5">
+        <v>-1</v>
+      </c>
+      <c r="I5" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="J5" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K5" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="L5">
+        <v>-1</v>
+      </c>
+      <c r="M5">
+        <v>77</v>
+      </c>
+      <c r="N5">
         <v>26.5</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>2</v>
       </c>
       <c r="O5">
         <v>29</v>
       </c>
       <c r="P5">
-        <v>1.4142135623730951</v>
-      </c>
-      <c r="Q5">
-        <v>2</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>2.8</v>
-      </c>
-      <c r="V5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+        <v>-1</v>
+      </c>
+      <c r="S5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
       <c r="I9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="Y2:AB2"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Editing files with Excel while the program is running, but for some reason the averages change each time the spreadsheet is opened until program restarts?
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hallm\Desktop\FTCStats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60E51AF-1214-4C30-9DA9-3EB6554A4C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D1CE56-142E-4324-83EC-F57492915371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
   <sheets>
     <sheet name="Match Data" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="45">
   <si>
     <t>Cyrus</t>
   </si>
@@ -173,6 +173,9 @@
   <si>
     <t>Auto</t>
   </si>
+  <si>
+    <t>Added 30 points for an assumed good airplane; kept only 5 for parking, no hang</t>
+  </si>
 </sst>
 </file>
 
@@ -206,15 +209,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -404,11 +413,121 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -431,6 +550,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -439,6 +569,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -453,22 +595,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1066,8 +1196,123 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Teleop</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Per Member Data'!$E$3:$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Bredan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Erin</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Luca</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Per Member Data'!$B$3:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>38.764560098463477</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.772676371481538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50.08888888780875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CD42-48CE-84EF-6AD5468B8874}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Auton</c:v>
           </c:tx>
@@ -1163,13 +1408,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20.041867954962004</c:v>
+                  <c:v>20.939281288620283</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.199063231848733</c:v>
+                  <c:v>43.011198207946414</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.000000000000004</c:v>
+                  <c:v>28.755555555566755</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1177,121 +1422,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-CD42-48CE-84EF-6AD5468B8874}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Teleop</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Per Member Data'!$E$3:$E$5</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Bredan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Erin</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Luca</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Per Member Data'!$B$3:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>31.95008051580869</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>63.32396565126863</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26.500000000000007</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-CD42-48CE-84EF-6AD5468B8874}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1577,8 +1707,123 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Teleop</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Per Member Data'!$E$6:$E$8</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Mason</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Zoe</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Cyrus</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Per Member Data'!$B$6:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>40.453142226693522</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.235079171484685</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48.273972601126182</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FDBE-4159-8777-8C7A67663648}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Auton</c:v>
           </c:tx>
@@ -1674,13 +1919,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20.335570469740087</c:v>
+                  <c:v>21.082690187258269</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.490765171584485</c:v>
+                  <c:v>44.678440925575764</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.738461538439012</c:v>
+                  <c:v>28.698630136977371</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1688,121 +1933,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FDBE-4159-8777-8C7A67663648}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Teleop</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Per Member Data'!$E$6:$E$8</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Mason</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Zoe</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Cyrus</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Per Member Data'!$B$6:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>35.985234899598517</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>65.581354441018661</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26.369230769219499</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FDBE-4159-8777-8C7A67663648}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2088,8 +2218,123 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Teleop</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Per Member Data'!$E$9:$E$11</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Caleb</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Matt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Zach</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Per Member Data'!$B$9:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>48.061403507588665</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.664036076415229</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.261744966510754</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1E44-4500-8116-2BEDEEFEE37F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Auton</c:v>
           </c:tx>
@@ -2185,13 +2430,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20.166666666666661</c:v>
+                  <c:v>26.3903508764386</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.490765171584485</c:v>
+                  <c:v>41.949267192731156</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.110552763855971</c:v>
+                  <c:v>24.067114094025484</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2199,121 +2444,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1E44-4500-8116-2BEDEEFEE37F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Teleop</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Per Member Data'!$E$9:$E$11</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Caleb</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Matt</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Zach</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Per Member Data'!$B$9:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>38.166666666666643</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>65.581354441018661</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30.306532663354606</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1E44-4500-8116-2BEDEEFEE37F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2598,8 +2728,123 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Teleop</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Drive Team Data'!$Q$4:$Q$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>B+M</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>E+Z</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>L+C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Drive Team Data'!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>39.608851162578503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.003877771483111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.181430744467463</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-281A-4869-BADA-35E09581505F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Auton</c:v>
           </c:tx>
@@ -2695,13 +2940,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20.188719212351046</c:v>
+                  <c:v>21.010985737939276</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.844914201716605</c:v>
+                  <c:v>43.844819566761089</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.869230769219506</c:v>
+                  <c:v>28.727092846272065</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2709,121 +2954,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-281A-4869-BADA-35E09581505F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Teleop</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Drive Team Data'!$Q$4:$Q$6</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>B+M</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>E+Z</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>L+C</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Drive Team Data'!$B$4:$B$6</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>33.967657707703601</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64.452660046143649</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26.434615384609753</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-281A-4869-BADA-35E09581505F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3077,8 +3207,136 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Drive Team Data'!$M$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Teleop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Drive Team Data'!$A$22:$K$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Drive Team Data'!$A$22:$K$23</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Caleb</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Matt</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Zach</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Caleb</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Matt</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Zach</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Caleb</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Matt</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Zach</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>B+M</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>E+Z</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>L+C</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Drive Team Data'!$A$24:$K$24</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Drive Team Data'!$A$24:$C$24,'Drive Team Data'!$E$24:$G$24,'Drive Team Data'!$I$24:$K$24)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>36.420041928942865</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38.449866490276051</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.361127200283583</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45.759649122615542</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.789473683948721</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44.70073439395626</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.780392156858635</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.810216718191818</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.721477428199353</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-05A6-44A2-AA23-BE9D98EF0F83}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>'Drive Team Data'!$M$25</c:f>
@@ -3201,134 +3459,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-05A6-44A2-AA23-BE9D98EF0F83}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Drive Team Data'!$M$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Teleop</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Drive Team Data'!$A$22:$K$23</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Drive Team Data'!$A$22:$K$23</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="9"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Caleb</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Matt</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Zach</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Caleb</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Matt</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Zach</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Caleb</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Matt</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Zach</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>B+M</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>E+Z</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>L+C</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Drive Team Data'!$A$24:$K$24</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>('Drive Team Data'!$A$24:$C$24,'Drive Team Data'!$E$24:$G$24,'Drive Team Data'!$I$24:$K$24)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>36.420041928942865</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>38.449866490276051</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>35.361127200283583</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45.759649122615542</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>47.789473683948721</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44.70073439395626</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>28.780392156858635</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>30.810216718191818</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>27.721477428199353</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-05A6-44A2-AA23-BE9D98EF0F83}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3587,8 +3717,128 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Teleop</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Drive Team Data'!$A$22:$K$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Drive Team Data'!$A$22:$K$23</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Caleb</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Matt</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Zach</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Caleb</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Matt</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Zach</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Caleb</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Matt</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Zach</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>B+M</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>E+Z</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>L+C</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Drive Team Data'!$A$27:$K$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Drive Team Data'!$A$27:$C$27,'Drive Team Data'!$E$27:$G$27,'Drive Team Data'!$I$27:$K$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>40.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.333333333333336</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D4B-45BB-882E-36ED5E8AEC28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Auto</c:v>
           </c:tx>
@@ -3703,126 +3953,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2D4B-45BB-882E-36ED5E8AEC28}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Teleop</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Drive Team Data'!$A$22:$K$23</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Drive Team Data'!$A$22:$K$23</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="9"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Caleb</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Matt</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Zach</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Caleb</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Matt</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Zach</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Caleb</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Matt</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Zach</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>B+M</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>E+Z</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>L+C</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Drive Team Data'!$A$27:$K$27</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>('Drive Team Data'!$A$27:$C$27,'Drive Team Data'!$E$27:$G$27,'Drive Team Data'!$I$27:$K$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>40.6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>29.666666666666668</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>47.333333333333336</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>26.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2D4B-45BB-882E-36ED5E8AEC28}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4111,8 +4241,123 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Teleop</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Drive Team Data'!$Q$4:$Q$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>B+M</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>E+Z</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>L+C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Drive Team Data'!$B$10:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>38.073170731707314</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.641509433962263</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8C47-4A07-81E2-2EA9F703C12F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Auto</c:v>
           </c:tx>
@@ -4208,13 +4453,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>19.103448275862068</c:v>
+                  <c:v>19.951219512195124</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.666666666666664</c:v>
+                  <c:v>46.358490566037737</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>28.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4222,121 +4467,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8C47-4A07-81E2-2EA9F703C12F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Teleop</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Drive Team Data'!$Q$4:$Q$6</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>B+M</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>E+Z</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>L+C</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Drive Team Data'!$B$10:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>34.379310344827587</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41.111111111111114</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8C47-4A07-81E2-2EA9F703C12F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10651,19 +10781,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.7109375"/>
+    <col min="5" max="5" customWidth="true" width="10.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -10692,7 +10822,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
         <v>30</v>
       </c>
@@ -10729,7 +10859,7 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
         <v>30</v>
       </c>
@@ -10758,7 +10888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
         <v>30</v>
       </c>
@@ -10788,7 +10918,7 @@
       </c>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="0">
         <v>30</v>
       </c>
@@ -10817,7 +10947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s" s="0">
         <v>30</v>
       </c>
@@ -10846,7 +10976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s" s="0">
         <v>30</v>
       </c>
@@ -10875,7 +11005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s" s="0">
         <v>30</v>
       </c>
@@ -10904,7 +11034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s" s="0">
         <v>30</v>
       </c>
@@ -10934,7 +11064,7 @@
       </c>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s" s="0">
         <v>30</v>
       </c>
@@ -10963,7 +11093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s" s="0">
         <v>30</v>
       </c>
@@ -10992,7 +11122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s" s="0">
         <v>30</v>
       </c>
@@ -11023,7 +11153,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s" s="0">
         <v>31</v>
       </c>
@@ -11052,7 +11182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s" s="0">
         <v>31</v>
       </c>
@@ -11082,7 +11212,7 @@
       </c>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s" s="0">
         <v>31</v>
       </c>
@@ -11111,7 +11241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s" s="0">
         <v>31</v>
       </c>
@@ -11140,7 +11270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s" s="0">
         <v>31</v>
       </c>
@@ -11169,7 +11299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s" s="0">
         <v>31</v>
       </c>
@@ -11198,7 +11328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s" s="0">
         <v>31</v>
       </c>
@@ -11227,7 +11357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" t="s" s="0">
         <v>31</v>
       </c>
@@ -11256,7 +11386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" t="s" s="0">
         <v>31</v>
       </c>
@@ -11288,7 +11418,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" t="s" s="0">
         <v>31</v>
       </c>
@@ -11320,7 +11450,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" t="s" s="0">
         <v>31</v>
       </c>
@@ -11352,7 +11482,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" t="s" s="0">
         <v>31</v>
       </c>
@@ -11384,7 +11514,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" t="s" s="0">
         <v>31</v>
       </c>
@@ -11416,7 +11546,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" t="s" s="0">
         <v>31</v>
       </c>
@@ -11447,31 +11577,543 @@
       <c r="K26" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="T26" s="22"/>
-      <c r="U26" s="22"/>
-      <c r="V26" s="22"/>
-      <c r="W26" s="22"/>
+      <c r="T26" s="33"/>
+      <c r="U26" s="33"/>
+      <c r="V26" s="33"/>
+      <c r="W26" s="33"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="23"/>
-      <c r="V31" s="23"/>
-      <c r="W31" s="23"/>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A27" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45255</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F27" s="22">
+        <v>75</v>
+      </c>
+      <c r="G27" s="22">
+        <v>45</v>
+      </c>
+      <c r="H27" s="0">
+        <v>30</v>
+      </c>
+      <c r="I27" s="0">
+        <v>0</v>
+      </c>
+      <c r="L27" s="22"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A28" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45255</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F28" s="22">
+        <v>50</v>
+      </c>
+      <c r="G28" s="22">
+        <v>42</v>
+      </c>
+      <c r="H28" s="0">
+        <v>8</v>
+      </c>
+      <c r="I28" s="0">
+        <v>0</v>
+      </c>
+      <c r="L28" s="22"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A29" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45255</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F29" s="22">
+        <v>82</v>
+      </c>
+      <c r="G29" s="22">
+        <v>54</v>
+      </c>
+      <c r="H29" s="0">
+        <v>28</v>
+      </c>
+      <c r="I29" s="0">
+        <v>0</v>
+      </c>
+      <c r="L29" s="22"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A30" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F30" s="22">
+        <v>112</v>
+      </c>
+      <c r="G30" s="22">
+        <v>62</v>
+      </c>
+      <c r="H30" s="0">
+        <v>50</v>
+      </c>
+      <c r="I30" s="0">
+        <v>0</v>
+      </c>
+      <c r="L30" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A31" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F31" s="22">
+        <v>65</v>
+      </c>
+      <c r="G31" s="22">
+        <v>57</v>
+      </c>
+      <c r="H31" s="0">
+        <v>8</v>
+      </c>
+      <c r="I31" s="0">
+        <v>0</v>
+      </c>
+      <c r="L31" s="22"/>
+      <c r="T31" s="34"/>
+      <c r="U31" s="34"/>
+      <c r="V31" s="34"/>
+      <c r="W31" s="34"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A32" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F32" s="22">
+        <v>85</v>
+      </c>
+      <c r="G32" s="22">
+        <v>57</v>
+      </c>
+      <c r="H32" s="0">
+        <v>28</v>
+      </c>
+      <c r="I32" s="0">
+        <v>0</v>
+      </c>
+      <c r="L32" s="22"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F33" s="22">
+        <v>95</v>
+      </c>
+      <c r="G33" s="22">
+        <v>45</v>
+      </c>
+      <c r="H33" s="0">
+        <v>50</v>
+      </c>
+      <c r="I33" s="0">
+        <v>0</v>
+      </c>
+      <c r="L33" s="22"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B34" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F34" s="22">
+        <v>95</v>
+      </c>
+      <c r="G34" s="22">
+        <v>45</v>
+      </c>
+      <c r="H34" s="0">
+        <v>50</v>
+      </c>
+      <c r="I34" s="0">
+        <v>0</v>
+      </c>
+      <c r="L34" s="22"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B35" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F35" s="22">
+        <v>110</v>
+      </c>
+      <c r="G35" s="22">
+        <v>60</v>
+      </c>
+      <c r="H35" s="0">
+        <v>50</v>
+      </c>
+      <c r="I35" s="0">
+        <v>0</v>
+      </c>
+      <c r="L35" s="22"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B36" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F36" s="22">
+        <v>109</v>
+      </c>
+      <c r="G36" s="22">
+        <v>59</v>
+      </c>
+      <c r="H36" s="0">
+        <v>50</v>
+      </c>
+      <c r="I36" s="0">
+        <v>0</v>
+      </c>
+      <c r="L36" s="22"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B37" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F37" s="22">
+        <v>107</v>
+      </c>
+      <c r="G37" s="22">
+        <v>57</v>
+      </c>
+      <c r="H37" s="0">
+        <v>50</v>
+      </c>
+      <c r="I37" s="0">
+        <v>0</v>
+      </c>
+      <c r="L37" s="22"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B38" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F38" s="22">
+        <v>97</v>
+      </c>
+      <c r="G38" s="22">
+        <v>47</v>
+      </c>
+      <c r="H38" s="0">
+        <v>50</v>
+      </c>
+      <c r="I38" s="0">
+        <v>0</v>
+      </c>
+      <c r="L38" s="22"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B39" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F39" s="22">
+        <v>101</v>
+      </c>
+      <c r="G39" s="22">
+        <v>51</v>
+      </c>
+      <c r="H39" s="0">
+        <v>50</v>
+      </c>
+      <c r="I39" s="0">
+        <v>0</v>
+      </c>
+      <c r="L39" s="22"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B40" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F40" s="22">
+        <v>88</v>
+      </c>
+      <c r="G40" s="22">
+        <v>43</v>
+      </c>
+      <c r="H40" s="0">
+        <v>45</v>
+      </c>
+      <c r="I40" s="0">
+        <v>0</v>
+      </c>
+      <c r="L40" s="22"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B41" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E41" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F41" s="22">
+        <v>125</v>
+      </c>
+      <c r="G41" s="22">
+        <v>75</v>
+      </c>
+      <c r="H41" s="0">
+        <v>50</v>
+      </c>
+      <c r="I41" s="0">
+        <v>0</v>
+      </c>
+      <c r="L41" s="22"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B42" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F42" s="22">
+        <v>100</v>
+      </c>
+      <c r="G42" s="22">
+        <v>70</v>
+      </c>
+      <c r="H42" s="0">
+        <v>30</v>
+      </c>
+      <c r="I42" s="0">
+        <v>0</v>
+      </c>
+      <c r="L42" s="22"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B43" s="1">
+        <v>45256</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F43" s="22">
+        <v>103</v>
+      </c>
+      <c r="G43" s="22">
+        <v>53</v>
+      </c>
+      <c r="H43" s="0">
+        <v>50</v>
+      </c>
+      <c r="I43" s="0">
+        <v>0</v>
+      </c>
+      <c r="L43" s="22"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B48" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -11491,13 +12133,13 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.7109375"/>
+    <col min="5" max="5" customWidth="true" width="10.6640625"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -11530,7 +12172,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45237</v>
       </c>
@@ -11547,7 +12189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45237</v>
       </c>
@@ -11573,7 +12215,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45237</v>
       </c>
@@ -11601,7 +12243,7 @@
         <v>42.428571428571431</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45238</v>
       </c>
@@ -11629,7 +12271,7 @@
         <v>57.333333333333336</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45238</v>
       </c>
@@ -11657,7 +12299,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45238</v>
       </c>
@@ -11674,7 +12316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45238</v>
       </c>
@@ -11694,7 +12336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45238</v>
       </c>
@@ -11710,12 +12352,12 @@
       <c r="E10" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
       <c r="M10" t="s" s="0">
         <v>0</v>
       </c>
@@ -11728,7 +12370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45238</v>
       </c>
@@ -11744,14 +12386,14 @@
       <c r="E11" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="24" t="s">
+      <c r="I11" s="33"/>
+      <c r="J11" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="22"/>
+      <c r="K11" s="33"/>
       <c r="M11" t="s" s="0">
         <v>9</v>
       </c>
@@ -11764,7 +12406,7 @@
         <v>45.166666666666664</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="H12" s="2" t="s">
         <v>23</v>
       </c>
@@ -11789,7 +12431,7 @@
         <v>57.333333333333336</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45237</v>
       </c>
@@ -11825,7 +12467,7 @@
         <v>57.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45238</v>
       </c>
@@ -11864,7 +12506,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45234</v>
       </c>
@@ -11911,7 +12553,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45234</v>
       </c>
@@ -11958,7 +12600,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45234</v>
       </c>
@@ -12005,7 +12647,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45234</v>
       </c>
@@ -12041,7 +12683,7 @@
         <v>34.214285714285715</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45234</v>
       </c>
@@ -12077,7 +12719,7 @@
         <v>57.333333333333336</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45234</v>
       </c>
@@ -12113,7 +12755,7 @@
         <v>43.797619047619051</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45234</v>
       </c>
@@ -12149,7 +12791,7 @@
         <v>43.797619047619051</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45234</v>
       </c>
@@ -12185,7 +12827,7 @@
         <v>43.797619047619051</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45234</v>
       </c>
@@ -12221,13 +12863,13 @@
         <v>43.797619047619051</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="T27" s="22" t="s">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="T27" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="U27" s="22"/>
-      <c r="V27" s="22"/>
-      <c r="W27" s="22"/>
+      <c r="U27" s="33"/>
+      <c r="V27" s="33"/>
+      <c r="W27" s="33"/>
       <c r="X27" s="2" t="s">
         <v>23</v>
       </c>
@@ -12235,7 +12877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="T28" s="0">
         <v>1</v>
       </c>
@@ -12257,7 +12899,7 @@
         <v>40.333333333333336</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="T29" s="0">
         <v>2</v>
       </c>
@@ -12279,7 +12921,7 @@
         <v>48.198412698412703</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="T30" s="0">
         <v>3</v>
       </c>
@@ -12301,15 +12943,15 @@
         <v>53.166666666666664</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="T32" s="22" t="s">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="T32" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="U32" s="22"/>
-      <c r="V32" s="22"/>
-      <c r="W32" s="22"/>
-    </row>
-    <row r="33" spans="20:25" x14ac:dyDescent="0.25">
+      <c r="U32" s="33"/>
+      <c r="V32" s="33"/>
+      <c r="W32" s="33"/>
+    </row>
+    <row r="33" spans="20:25" x14ac:dyDescent="0.3">
       <c r="T33" s="0">
         <v>1</v>
       </c>
@@ -12331,7 +12973,7 @@
         <v>40.333333333333336</v>
       </c>
     </row>
-    <row r="34" spans="20:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="20:25" x14ac:dyDescent="0.3">
       <c r="T34" s="0">
         <v>2</v>
       </c>
@@ -12353,7 +12995,7 @@
         <v>42.531746031746032</v>
       </c>
     </row>
-    <row r="35" spans="20:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="20:25" x14ac:dyDescent="0.3">
       <c r="T35" s="0">
         <v>3</v>
       </c>
@@ -12393,193 +13035,193 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
       <c r="E1" s="3"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" s="24" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="n" s="0">
-        <v>59.5270508478269</v>
-      </c>
-      <c r="B3" t="n" s="0">
-        <v>32.03450489538631</v>
-      </c>
-      <c r="C3" t="n" s="0">
-        <v>20.1428342160633</v>
-      </c>
-      <c r="D3" t="n" s="0">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="n">
+        <v>63.04653802464488</v>
+      </c>
+      <c r="B3" s="26" t="n">
+        <v>38.764560098463484</v>
+      </c>
+      <c r="C3" s="26" t="n">
+        <v>20.939281288620293</v>
+      </c>
+      <c r="D3" s="23" t="n">
         <v>0.0</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="n" s="0">
-        <v>75.84946236580235</v>
-      </c>
-      <c r="B4" t="n" s="0">
-        <v>43.87428571409823</v>
-      </c>
-      <c r="C4" t="n" s="0">
-        <v>31.14857142897671</v>
-      </c>
-      <c r="D4" t="n" s="0">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="n">
+        <v>98.56542055987764</v>
+      </c>
+      <c r="B4" s="30" t="n">
+        <v>53.40400471101017</v>
+      </c>
+      <c r="C4" s="30" t="n">
+        <v>45.24028268506923</v>
+      </c>
+      <c r="D4" s="29" t="n">
         <v>0.0</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="n" s="0">
-        <v>61.64258262895983</v>
-      </c>
-      <c r="B5" t="n" s="0">
-        <v>26.500000000000007</v>
-      </c>
-      <c r="C5" t="n" s="0">
-        <v>29.000000000000004</v>
-      </c>
-      <c r="D5" t="n" s="0">
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="31" t="n">
+        <v>78.84931506750885</v>
+      </c>
+      <c r="B5" s="32" t="n">
+        <v>50.08888888780873</v>
+      </c>
+      <c r="C5" s="32" t="n">
+        <v>28.755555555566744</v>
+      </c>
+      <c r="D5" s="31" t="n">
         <v>0.0</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="n" s="0">
-        <v>57.72040842080632</v>
-      </c>
-      <c r="B6" t="n" s="0">
-        <v>36.04430464489396</v>
-      </c>
-      <c r="C6" t="n" s="0">
-        <v>20.41895328597979</v>
-      </c>
-      <c r="D6" t="n" s="0">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="n">
+        <v>62.061899679414424</v>
+      </c>
+      <c r="B6" s="26" t="n">
+        <v>40.45314222669349</v>
+      </c>
+      <c r="C6" s="26" t="n">
+        <v>21.08269018725826</v>
+      </c>
+      <c r="D6" s="23" t="n">
         <v>0.0</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="n" s="0">
-        <v>87.44226498854837</v>
-      </c>
-      <c r="B7" t="n" s="0">
-        <v>41.89873417701383</v>
-      </c>
-      <c r="C7" t="n" s="0">
-        <v>39.83544303793153</v>
-      </c>
-      <c r="D7" t="n" s="0">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="n">
+        <v>101.08671586657731</v>
+      </c>
+      <c r="B7" s="30" t="n">
+        <v>54.13642213607548</v>
+      </c>
+      <c r="C7" s="30" t="n">
+        <v>47.20849420829709</v>
+      </c>
+      <c r="D7" s="29" t="n">
         <v>0.0</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="n" s="0">
-        <v>61.20215545397455</v>
-      </c>
-      <c r="B8" t="n" s="0">
-        <v>26.3692307692195</v>
-      </c>
-      <c r="C8" t="n" s="0">
-        <v>28.73846153843901</v>
-      </c>
-      <c r="D8" t="n" s="0">
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="31" t="n">
+        <v>77.87785016147298</v>
+      </c>
+      <c r="B8" s="32" t="n">
+        <v>48.273972601126175</v>
+      </c>
+      <c r="C8" s="32" t="n">
+        <v>28.69863013697737</v>
+      </c>
+      <c r="D8" s="31" t="n">
         <v>0.0</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="n" s="0">
-        <v>60.999999999999986</v>
-      </c>
-      <c r="B9" t="n" s="0">
-        <v>38.16666666666664</v>
-      </c>
-      <c r="C9" t="n" s="0">
-        <v>20.16666666666666</v>
-      </c>
-      <c r="D9" t="n" s="0">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="n">
+        <v>75.22368420881257</v>
+      </c>
+      <c r="B9" s="26" t="n">
+        <v>48.06140350758862</v>
+      </c>
+      <c r="C9" s="26" t="n">
+        <v>26.390350876438607</v>
+      </c>
+      <c r="D9" s="23" t="n">
         <v>0.0</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="n" s="0">
-        <v>81.73417721494539</v>
-      </c>
-      <c r="B10" t="n" s="0">
-        <v>41.89873417701383</v>
-      </c>
-      <c r="C10" t="n" s="0">
-        <v>39.83544303793153</v>
-      </c>
-      <c r="D10" t="n" s="0">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="n">
+        <v>98.49940687975642</v>
+      </c>
+      <c r="B10" s="30" t="n">
+        <v>54.36061684427774</v>
+      </c>
+      <c r="C10" s="30" t="n">
+        <v>44.138790035478664</v>
+      </c>
+      <c r="D10" s="29" t="n">
         <v>0.0</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="n" s="0">
-        <v>62.65347766613021</v>
-      </c>
-      <c r="B11" t="n" s="0">
-        <v>30.400100150266862</v>
-      </c>
-      <c r="C11" t="n" s="0">
-        <v>24.201301952969676</v>
-      </c>
-      <c r="D11" t="n" s="0">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="n">
+        <v>61.59240069143186</v>
+      </c>
+      <c r="B11" s="28" t="n">
+        <v>30.261744966510754</v>
+      </c>
+      <c r="C11" s="28" t="n">
+        <v>24.067114094025488</v>
+      </c>
+      <c r="D11" s="27" t="n">
         <v>0.0</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s" s="0">
         <v>35</v>
       </c>
@@ -12589,6 +13231,18 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:A5">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:A8">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -12600,7 +13254,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:A8">
+  <conditionalFormatting sqref="A9:A11">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -12612,8 +13266,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A11">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="B3:B5">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -12624,7 +13278,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B5">
+  <conditionalFormatting sqref="B6:B8">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -12636,7 +13290,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B8">
+  <conditionalFormatting sqref="B9:B11">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -12648,8 +13302,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:B11">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="C3:C5">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -12660,7 +13314,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C5">
+  <conditionalFormatting sqref="C6:C8">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -12672,20 +13326,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C8">
+  <conditionalFormatting sqref="C9:C11">
     <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:C11">
-    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -12702,9 +13344,9 @@
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -12714,9 +13356,9 @@
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -12726,9 +13368,9 @@
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -12744,37 +13386,37 @@
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" bestFit="true" customWidth="true" width="9.5703125"/>
+    <col min="1" max="3" bestFit="true" customWidth="true" width="9.5546875"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="9.0"/>
-    <col min="5" max="7" bestFit="true" customWidth="true" width="9.5703125"/>
+    <col min="5" max="7" bestFit="true" customWidth="true" width="9.5546875"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="9.0"/>
-    <col min="9" max="11" bestFit="true" customWidth="true" width="9.5703125"/>
+    <col min="9" max="11" bestFit="true" customWidth="true" width="9.5546875"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="9.0"/>
-    <col min="13" max="15" bestFit="true" customWidth="true" width="9.5703125"/>
+    <col min="13" max="15" bestFit="true" customWidth="true" width="9.5546875"/>
     <col min="16" max="16" bestFit="true" customWidth="true" width="9.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="27"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="42"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
@@ -12824,41 +13466,41 @@
       <c r="BK1" s="2"/>
       <c r="BL1" s="2"/>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32" t="s">
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="30" t="s">
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="35"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
-    </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="40"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
         <v>23</v>
       </c>
@@ -12908,51 +13550,51 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="n">
-        <v>58.62372963431661</v>
+        <v>62.55421885202965</v>
       </c>
       <c r="B4" s="13" t="n">
-        <v>34.03940477014014</v>
+        <v>39.60885116257849</v>
       </c>
       <c r="C4" s="13" t="n">
-        <v>20.280893751021544</v>
+        <v>21.01098573793928</v>
       </c>
       <c r="D4" s="14" t="n">
         <v>0.0</v>
       </c>
       <c r="E4" s="15" t="n">
-        <v>59.098983707453286</v>
+        <v>65.08811192338624</v>
       </c>
       <c r="F4" s="13" t="n">
-        <v>34.864857149445434</v>
+        <v>41.29936163158052</v>
       </c>
       <c r="G4" s="13" t="n">
-        <v>20.258048334150565</v>
+        <v>22.086858765639143</v>
       </c>
       <c r="H4" s="14" t="n">
         <v>0.0</v>
       </c>
       <c r="I4" s="15" t="n">
-        <v>63.245819150442365</v>
+        <v>69.743256457575</v>
       </c>
       <c r="J4" s="13" t="n">
-        <v>35.61127065151488</v>
+        <v>42.55920429891834</v>
       </c>
       <c r="K4" s="13" t="n">
-        <v>24.19180360840354</v>
+        <v>25.636546597447158</v>
       </c>
       <c r="L4" s="14" t="n">
         <v>0.0</v>
       </c>
       <c r="M4" s="13" t="n">
-        <v>59.429679240679334</v>
+        <v>62.36185521991009</v>
       </c>
       <c r="N4" s="13" t="n">
-        <v>33.311543846165485</v>
+        <v>37.73942992336494</v>
       </c>
       <c r="O4" s="13" t="n">
-        <v>21.06497539141117</v>
+        <v>21.62221140915652</v>
       </c>
       <c r="P4" s="16" t="n">
         <v>0.0</v>
@@ -12961,51 +13603,51 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="n">
-        <v>81.64586367717536</v>
+        <v>99.82606821322747</v>
       </c>
       <c r="B5" s="13" t="n">
-        <v>42.88650994555603</v>
+        <v>53.77021342354283</v>
       </c>
       <c r="C5" s="13" t="n">
-        <v>35.49200723345412</v>
+        <v>46.224388446683164</v>
       </c>
       <c r="D5" s="14" t="n">
         <v>0.0</v>
       </c>
       <c r="E5" s="15" t="n">
-        <v>77.51669094174028</v>
+        <v>94.90559141234449</v>
       </c>
       <c r="F5" s="13" t="n">
-        <v>41.94254128977815</v>
+        <v>52.62845144035199</v>
       </c>
       <c r="G5" s="13" t="n">
-        <v>32.42693912009663</v>
+        <v>42.257580932634255</v>
       </c>
       <c r="H5" s="14" t="n">
         <v>0.0</v>
       </c>
       <c r="I5" s="15" t="n">
-        <v>81.66352638472935</v>
+        <v>99.56073594653326</v>
       </c>
       <c r="J5" s="13" t="n">
-        <v>42.68895479184759</v>
+        <v>53.88829410768981</v>
       </c>
       <c r="K5" s="13" t="n">
-        <v>36.3606943943496</v>
+        <v>45.80726876444227</v>
       </c>
       <c r="L5" s="14" t="n">
         <v>0.0</v>
       </c>
       <c r="M5" s="13" t="n">
-        <v>77.84738647496633</v>
+        <v>92.17933470886835</v>
       </c>
       <c r="N5" s="13" t="n">
-        <v>40.3892279864982</v>
+        <v>49.06851973213641</v>
       </c>
       <c r="O5" s="13" t="n">
-        <v>33.23386617735723</v>
+        <v>41.79293357615163</v>
       </c>
       <c r="P5" s="16" t="n">
         <v>0.0</v>
@@ -13014,51 +13656,51 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="n">
-        <v>61.42236904146719</v>
+        <v>78.36358261449092</v>
       </c>
       <c r="B6" s="17" t="n">
-        <v>26.434615384609753</v>
+        <v>49.18143074446745</v>
       </c>
       <c r="C6" s="17" t="n">
-        <v>28.869230769219506</v>
+        <v>28.727092846272058</v>
       </c>
       <c r="D6" s="18" t="n">
         <v>0.0</v>
       </c>
       <c r="E6" s="19" t="n">
-        <v>61.337895233173754</v>
+        <v>77.73560293335525</v>
       </c>
       <c r="F6" s="17" t="n">
-        <v>28.78102564102113</v>
+        <v>48.95742529709169</v>
       </c>
       <c r="G6" s="17" t="n">
-        <v>27.128717948708935</v>
+        <v>28.25974445230537</v>
       </c>
       <c r="H6" s="18" t="n">
         <v>0.0</v>
       </c>
       <c r="I6" s="19" t="n">
-        <v>65.48473067616283</v>
+        <v>82.39074746754402</v>
       </c>
       <c r="J6" s="17" t="n">
-        <v>29.527439143090568</v>
+        <v>50.2172679644295</v>
       </c>
       <c r="K6" s="17" t="n">
-        <v>31.06247322296191</v>
+        <v>31.80943228411338</v>
       </c>
       <c r="L6" s="18" t="n">
         <v>0.0</v>
       </c>
       <c r="M6" s="17" t="n">
-        <v>61.66859076639979</v>
+        <v>75.00934622987911</v>
       </c>
       <c r="N6" s="17" t="n">
-        <v>27.227712337741174</v>
+        <v>45.39749358887611</v>
       </c>
       <c r="O6" s="17" t="n">
-        <v>27.93564500596954</v>
+        <v>27.795097095822747</v>
       </c>
       <c r="P6" s="20" t="n">
         <v>0.0</v>
@@ -13067,53 +13709,53 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:64" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+    <row r="7" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="27"/>
-    </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="42"/>
+    </row>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="A8" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32" t="s">
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="32" t="s">
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="30" t="s">
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="34"/>
-    </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="46"/>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -13163,27 +13805,27 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="n">
-        <v>56.333333333333336</v>
+        <v>59.95238095238095</v>
       </c>
       <c r="B10" t="n" s="0">
-        <v>34.37931034482759</v>
+        <v>38.073170731707314</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>19.103448275862068</v>
+        <v>19.951219512195124</v>
       </c>
       <c r="D10" s="9" t="n">
         <v>0.0</v>
       </c>
       <c r="E10" s="11" t="n">
-        <v>62.4</v>
+        <v>64.875</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>40.6</v>
+        <v>43.0</v>
       </c>
       <c r="G10" t="n" s="0">
-        <v>18.6</v>
+        <v>19.875</v>
       </c>
       <c r="H10" s="9" t="n">
         <v>0.0</v>
@@ -13216,15 +13858,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="n">
-        <v>81.6</v>
+        <v>98.81481481481481</v>
       </c>
       <c r="B11" t="n" s="0">
-        <v>41.111111111111114</v>
+        <v>52.64150943396226</v>
       </c>
       <c r="C11" t="n" s="0">
-        <v>39.666666666666664</v>
+        <v>46.35849056603774</v>
       </c>
       <c r="D11" s="9" t="n">
         <v>0.0</v>
@@ -13242,13 +13884,13 @@
         <v>#NUM!</v>
       </c>
       <c r="I11" s="11" t="n">
-        <v>80.77777777777777</v>
+        <v>99.0</v>
       </c>
       <c r="J11" t="n" s="0">
-        <v>41.111111111111114</v>
+        <v>52.64150943396226</v>
       </c>
       <c r="K11" t="n" s="0">
-        <v>39.666666666666664</v>
+        <v>46.35849056603774</v>
       </c>
       <c r="L11" s="9" t="n">
         <v>0.0</v>
@@ -13269,42 +13911,42 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="n">
-        <v>62.666666666666664</v>
+        <v>76.76190476190476</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>26.5</v>
+        <v>45.8</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>29.0</v>
+        <v>28.8</v>
       </c>
       <c r="D12" s="10" t="n">
         <v>0.0</v>
       </c>
-      <c r="E12" s="12" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="F12" s="5" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="G12" s="5" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="H12" s="10" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="I12" s="12" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J12" s="5" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K12" s="5" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L12" s="10" t="e">
-        <v>#NUM!</v>
+      <c r="E12" s="12" t="n">
+        <v>98.5</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>59.5</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="H12" s="10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I12" s="12" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="K12" s="5" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="L12" s="10" t="n">
+        <v>0.0</v>
       </c>
       <c r="M12" s="5" t="n">
         <v>62.666666666666664</v>
@@ -13322,7 +13964,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s" s="0">
         <v>38</v>
       </c>
@@ -13333,7 +13975,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s" s="0">
         <v>10</v>
       </c>
@@ -13362,7 +14004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <f>F4</f>
         <v>36.420041928942865</v>
@@ -13403,7 +14045,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <f>G4</f>
         <v>22.205828092195425</v>
@@ -13444,7 +14086,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="0">
         <f>F10</f>
         <v>40.6</v>
@@ -13482,7 +14124,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="0">
         <f>G10</f>
         <v>18.600000000000001</v>
@@ -13522,18 +14164,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A7:P7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="M8:P8"/>
     <mergeCell ref="AC2:AF2"/>
     <mergeCell ref="Y2:AB2"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A7:P7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="M8:P8"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:A6">
     <cfRule type="colorScale" priority="11">
@@ -13617,7 +14259,127 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5 I5 M5">
+  <conditionalFormatting sqref="E4 I4 M4">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6 I6 M6">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10 I10 M10">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12 I12 M12">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5 N5 J5">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11 J11 N11">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4 O4 K4">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6 K6 O6">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10 K10 O10">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12 K12 O12">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5 E5 M5">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -13629,7 +14391,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11 I11 M11">
+  <conditionalFormatting sqref="I11 E11 M11">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -13641,7 +14403,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4 J4 N4">
+  <conditionalFormatting sqref="J4 F4 N4">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -13653,7 +14415,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6 J6 N6">
+  <conditionalFormatting sqref="J6 F6 N6">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -13665,7 +14427,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10 J10 N10">
+  <conditionalFormatting sqref="J10 F10 N10">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -13677,7 +14439,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12 J12 N12">
+  <conditionalFormatting sqref="J12 F12 N12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -13689,7 +14451,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5 K5 O5">
+  <conditionalFormatting sqref="K5 G5 O5">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -13701,128 +14463,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11 K11 O11">
+  <conditionalFormatting sqref="K11 G11 O11">
     <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4 E4 M4">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6 E6 M6">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10 E10 M10">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12 E12 M12">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J11 F11 N11">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K6 G6 O6">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10 G10 O10">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K12 G12 O12">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N5 F5 J5">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O4 G4 K4">
-    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13842,176 +14484,176 @@
   <dimension ref="H1:S42"/>
   <sheetViews>
     <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H1" s="21"/>
       <c r="S1" s="21"/>
     </row>
-    <row r="2" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H2" s="21"/>
       <c r="S2" s="21"/>
     </row>
-    <row r="3" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H3" s="21"/>
       <c r="S3" s="21"/>
     </row>
-    <row r="4" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H4" s="21"/>
       <c r="S4" s="21"/>
     </row>
-    <row r="5" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H5" s="21"/>
       <c r="S5" s="21"/>
     </row>
-    <row r="6" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H6" s="21"/>
       <c r="S6" s="21"/>
     </row>
-    <row r="7" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H7" s="21"/>
       <c r="S7" s="21"/>
     </row>
-    <row r="8" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H8" s="21"/>
       <c r="S8" s="21"/>
     </row>
-    <row r="9" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H9" s="21"/>
       <c r="S9" s="21"/>
     </row>
-    <row r="10" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H10" s="21"/>
       <c r="S10" s="21"/>
     </row>
-    <row r="11" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H11" s="21"/>
       <c r="S11" s="21"/>
     </row>
-    <row r="12" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H12" s="21"/>
       <c r="S12" s="21"/>
     </row>
-    <row r="13" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H13" s="21"/>
       <c r="S13" s="21"/>
     </row>
-    <row r="14" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H14" s="21"/>
       <c r="S14" s="21"/>
     </row>
-    <row r="15" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H15" s="21"/>
       <c r="S15" s="21"/>
     </row>
-    <row r="16" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H16" s="21"/>
       <c r="S16" s="21"/>
     </row>
-    <row r="17" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H17" s="21"/>
       <c r="S17" s="21"/>
     </row>
-    <row r="18" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H18" s="21"/>
       <c r="S18" s="21"/>
     </row>
-    <row r="19" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H19" s="21"/>
       <c r="S19" s="21"/>
     </row>
-    <row r="20" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H20" s="21"/>
       <c r="S20" s="21"/>
     </row>
-    <row r="21" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H21" s="21"/>
       <c r="S21" s="21"/>
     </row>
-    <row r="22" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H22" s="21"/>
       <c r="S22" s="21"/>
     </row>
-    <row r="23" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H23" s="21"/>
       <c r="S23" s="21"/>
     </row>
-    <row r="24" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H24" s="21"/>
       <c r="S24" s="21"/>
     </row>
-    <row r="25" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H25" s="21"/>
       <c r="S25" s="21"/>
     </row>
-    <row r="26" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H26" s="21"/>
       <c r="S26" s="21"/>
     </row>
-    <row r="27" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H27" s="21"/>
       <c r="S27" s="21"/>
     </row>
-    <row r="28" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H28" s="21"/>
       <c r="S28" s="21"/>
     </row>
-    <row r="29" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H29" s="21"/>
       <c r="S29" s="21"/>
     </row>
-    <row r="30" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H30" s="21"/>
       <c r="S30" s="21"/>
     </row>
-    <row r="31" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H31" s="21"/>
       <c r="S31" s="21"/>
     </row>
-    <row r="32" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H32" s="21"/>
       <c r="S32" s="21"/>
     </row>
-    <row r="33" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H33" s="21"/>
       <c r="S33" s="21"/>
     </row>
-    <row r="34" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H34" s="21"/>
       <c r="S34" s="21"/>
     </row>
-    <row r="35" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H35" s="21"/>
       <c r="S35" s="21"/>
     </row>
-    <row r="36" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H36" s="21"/>
       <c r="S36" s="21"/>
     </row>
-    <row r="37" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H37" s="21"/>
       <c r="S37" s="21"/>
     </row>
-    <row r="38" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H38" s="21"/>
       <c r="S38" s="21"/>
     </row>
-    <row r="39" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H39" s="21"/>
       <c r="S39" s="21"/>
     </row>
-    <row r="40" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H40" s="21"/>
       <c r="S40" s="21"/>
     </row>
-    <row r="41" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H41" s="21"/>
       <c r="S41" s="21"/>
     </row>
-    <row r="42" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:19" x14ac:dyDescent="0.3">
       <c r="S42" s="21"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oh also apparently the data saves without having to open the spreadsheet, so that's a win
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D1CE56-142E-4324-83EC-F57492915371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3085CBA-D30F-4756-9846-A3D9B6F45B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -571,18 +571,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,10 +583,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1293,13 +1293,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>38.764560098463477</c:v>
+                  <c:v>38.764560098463484</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.772676371481538</c:v>
+                  <c:v>40.446030330182737</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.08888888780875</c:v>
+                  <c:v>50.088888887808729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1408,13 +1408,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20.939281288620283</c:v>
+                  <c:v>20.939281288620293</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.011198207946414</c:v>
+                  <c:v>34.263157894769414</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.755555555566755</c:v>
+                  <c:v>28.755555555566744</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1804,13 +1804,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>40.453142226693522</c:v>
+                  <c:v>40.453142226693487</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.235079171484685</c:v>
+                  <c:v>40.099142040113222</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48.273972601126182</c:v>
+                  <c:v>48.273972601126175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1919,10 +1919,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>21.082690187258269</c:v>
+                  <c:v>21.082690187258262</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44.678440925575764</c:v>
+                  <c:v>34.967588179361691</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>28.698630136977371</c:v>
@@ -2315,10 +2315,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>48.061403507588665</c:v>
+                  <c:v>48.061403507588622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.664036076415229</c:v>
+                  <c:v>41.099551569560809</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>30.261744966510754</c:v>
@@ -2430,13 +2430,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>26.3903508764386</c:v>
+                  <c:v>26.390350876438607</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.949267192731156</c:v>
+                  <c:v>33.371300448591789</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.067114094025484</c:v>
+                  <c:v>24.067114094025488</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2825,13 +2825,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>39.608851162578503</c:v>
+                  <c:v>39.608851162578489</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.003877771483111</c:v>
+                  <c:v>40.272586185147979</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49.181430744467463</c:v>
+                  <c:v>49.181430744467448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2940,13 +2940,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>21.010985737939276</c:v>
+                  <c:v>21.010985737939279</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.844819566761089</c:v>
+                  <c:v>34.615373037065552</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.727092846272065</c:v>
+                  <c:v>28.727092846272058</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4341,7 +4341,7 @@
                   <c:v>38.073170731707314</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.641509433962263</c:v>
+                  <c:v>40.434782608695649</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>45.8</c:v>
@@ -4456,7 +4456,7 @@
                   <c:v>19.951219512195124</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.358490566037737</c:v>
+                  <c:v>35.608695652173914</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>28.8</c:v>
@@ -10784,13 +10784,13 @@
   <dimension ref="A1:Y48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O47" sqref="O47"/>
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -10823,31 +10823,31 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>45237</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>106</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>-1</v>
       </c>
-      <c r="H2" s="0">
+      <c r="H2">
         <v>-1</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2">
         <v>0</v>
       </c>
       <c r="M2" s="2"/>
@@ -10860,721 +10860,721 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>45237</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>83</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>-1</v>
       </c>
-      <c r="H3" s="0">
+      <c r="H3">
         <v>-1</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>45237</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4">
         <v>89</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4">
         <v>-1</v>
       </c>
-      <c r="H4" s="0">
+      <c r="H4">
         <v>-1</v>
       </c>
-      <c r="I4" s="0">
+      <c r="I4">
         <v>0</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>45238</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>0</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5">
         <v>71</v>
       </c>
-      <c r="G5" s="0">
+      <c r="G5">
         <v>-1</v>
       </c>
-      <c r="H5" s="0">
+      <c r="H5">
         <v>-1</v>
       </c>
-      <c r="I5" s="0">
+      <c r="I5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>45238</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>88</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6">
         <v>-1</v>
       </c>
-      <c r="H6" s="0">
+      <c r="H6">
         <v>-1</v>
       </c>
-      <c r="I6" s="0">
+      <c r="I6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>45238</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>111</v>
       </c>
-      <c r="G7" s="0">
+      <c r="G7">
         <v>-1</v>
       </c>
-      <c r="H7" s="0">
+      <c r="H7">
         <v>-1</v>
       </c>
-      <c r="I7" s="0">
+      <c r="I7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>45238</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <v>34</v>
       </c>
-      <c r="G8" s="0">
+      <c r="G8">
         <v>-1</v>
       </c>
-      <c r="H8" s="0">
+      <c r="H8">
         <v>-1</v>
       </c>
-      <c r="I8" s="0">
+      <c r="I8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>45238</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>0</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="E9" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>120</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G9">
         <v>-1</v>
       </c>
-      <c r="H9" s="0">
+      <c r="H9">
         <v>-1</v>
       </c>
-      <c r="I9" s="0">
+      <c r="I9">
         <v>0</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>45238</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s" s="0">
+      <c r="E10" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="0">
+      <c r="F10">
         <v>75</v>
       </c>
-      <c r="G10" s="0">
+      <c r="G10">
         <v>-1</v>
       </c>
-      <c r="H10" s="0">
+      <c r="H10">
         <v>-1</v>
       </c>
-      <c r="I10" s="0">
+      <c r="I10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>45237</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>2</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="0">
+      <c r="F11">
         <v>111</v>
       </c>
-      <c r="G11" s="0">
+      <c r="G11">
         <v>66</v>
       </c>
-      <c r="H11" s="0">
+      <c r="H11">
         <v>45</v>
       </c>
-      <c r="I11" s="0">
+      <c r="I11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>45238</v>
       </c>
-      <c r="C12" t="s" s="0">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s" s="0">
+      <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s" s="0">
+      <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="0">
+      <c r="F12">
         <v>107</v>
       </c>
-      <c r="G12" s="0">
+      <c r="G12">
         <v>57</v>
       </c>
-      <c r="H12" s="0">
+      <c r="H12">
         <v>50</v>
       </c>
-      <c r="I12" s="0">
+      <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>45234</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>72</v>
       </c>
-      <c r="G13" s="0">
+      <c r="G13">
         <v>44</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <v>28</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s" s="0">
+      <c r="A14" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="1">
         <v>45234</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>97</v>
       </c>
-      <c r="G14" s="0">
+      <c r="G14">
         <v>51</v>
       </c>
-      <c r="H14" s="0">
+      <c r="H14">
         <v>30</v>
       </c>
-      <c r="I14" s="0">
+      <c r="I14">
         <v>0</v>
       </c>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s" s="0">
+      <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="1">
         <v>45234</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s" s="0">
+      <c r="D15" t="s">
         <v>0</v>
       </c>
-      <c r="E15" t="s" s="0">
+      <c r="E15" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>54</v>
       </c>
-      <c r="G15" s="0">
+      <c r="G15">
         <v>26</v>
       </c>
-      <c r="H15" s="0">
+      <c r="H15">
         <v>28</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s" s="0">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>45234</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>82</v>
       </c>
-      <c r="G16" s="0">
+      <c r="G16">
         <v>32</v>
       </c>
-      <c r="H16" s="0">
+      <c r="H16">
         <v>50</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" t="s" s="0">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>45234</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>60</v>
       </c>
-      <c r="G17" s="0">
+      <c r="G17">
         <v>40</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H17">
         <v>20</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" t="s" s="0">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>45234</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s" s="0">
+      <c r="D18" t="s">
         <v>9</v>
       </c>
-      <c r="E18" t="s" s="0">
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>56</v>
       </c>
-      <c r="G18" s="0">
+      <c r="G18">
         <v>48</v>
       </c>
-      <c r="H18" s="0">
+      <c r="H18">
         <v>8</v>
       </c>
-      <c r="I18" s="0">
+      <c r="I18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" t="s" s="0">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>45234</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>60</v>
       </c>
-      <c r="G19" s="0">
+      <c r="G19">
         <v>30</v>
       </c>
-      <c r="H19" s="0">
+      <c r="H19">
         <v>30</v>
       </c>
-      <c r="I19" s="0">
+      <c r="I19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" t="s" s="0">
+      <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>45234</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s" s="0">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>39</v>
       </c>
-      <c r="G20" s="0">
+      <c r="G20">
         <v>34</v>
       </c>
-      <c r="H20" s="0">
+      <c r="H20">
         <v>5</v>
       </c>
-      <c r="I20" s="0">
+      <c r="I20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" t="s" s="0">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>45241</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s" s="0">
+      <c r="E21" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21">
         <v>32</v>
       </c>
-      <c r="G21" s="0">
+      <c r="G21">
         <v>4</v>
       </c>
-      <c r="H21" s="0">
+      <c r="H21">
         <v>28</v>
       </c>
-      <c r="I21" s="0">
+      <c r="I21">
         <v>0</v>
       </c>
-      <c r="K21" t="s" s="0">
+      <c r="K21" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" t="s" s="0">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>45241</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>4</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>83</v>
       </c>
-      <c r="G22" s="0">
+      <c r="G22">
         <v>55</v>
       </c>
-      <c r="H22" s="0">
+      <c r="H22">
         <v>28</v>
       </c>
-      <c r="I22" s="0">
+      <c r="I22">
         <v>0</v>
       </c>
-      <c r="K22" t="s" s="0">
+      <c r="K22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" t="s" s="0">
+      <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>45241</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>3</v>
       </c>
-      <c r="D23" t="s" s="0">
+      <c r="D23" t="s">
         <v>0</v>
       </c>
-      <c r="E23" t="s" s="0">
+      <c r="E23" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>56</v>
       </c>
-      <c r="G23" s="0">
+      <c r="G23">
         <v>26</v>
       </c>
-      <c r="H23" s="0">
+      <c r="H23">
         <v>30</v>
       </c>
-      <c r="I23" s="0">
+      <c r="I23">
         <v>0</v>
       </c>
-      <c r="K23" t="s" s="0">
+      <c r="K23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" t="s" s="0">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>45241</v>
       </c>
-      <c r="C24" t="s" s="0">
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" t="s" s="0">
+      <c r="D24" t="s">
         <v>9</v>
       </c>
-      <c r="E24" t="s" s="0">
+      <c r="E24" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="0">
+      <c r="F24">
         <v>33</v>
       </c>
-      <c r="G24" s="0">
+      <c r="G24">
         <v>28</v>
       </c>
-      <c r="H24" s="0">
+      <c r="H24">
         <v>5</v>
       </c>
-      <c r="I24" s="0">
+      <c r="I24">
         <v>0</v>
       </c>
-      <c r="K24" t="s" s="0">
+      <c r="K24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" t="s" s="0">
+      <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>45241</v>
       </c>
-      <c r="C25" t="s" s="0">
+      <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="D25" t="s" s="0">
+      <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" t="s" s="0">
+      <c r="E25" t="s">
         <v>1</v>
       </c>
-      <c r="F25" s="0">
+      <c r="F25">
         <v>56</v>
       </c>
-      <c r="G25" s="0">
+      <c r="G25">
         <v>36</v>
       </c>
-      <c r="H25" s="0">
+      <c r="H25">
         <v>20</v>
       </c>
-      <c r="I25" s="0">
+      <c r="I25">
         <v>0</v>
       </c>
-      <c r="K25" t="s" s="0">
+      <c r="K25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" t="s" s="0">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="1">
         <v>45241</v>
       </c>
-      <c r="C26" t="s" s="0">
+      <c r="C26" t="s">
         <v>3</v>
       </c>
-      <c r="D26" t="s" s="0">
+      <c r="D26" t="s">
         <v>0</v>
       </c>
-      <c r="E26" t="s" s="0">
+      <c r="E26" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="0">
+      <c r="F26">
         <v>55</v>
       </c>
-      <c r="G26" s="0">
+      <c r="G26">
         <v>27</v>
       </c>
-      <c r="H26" s="0">
+      <c r="H26">
         <v>28</v>
       </c>
-      <c r="I26" s="0">
+      <c r="I26">
         <v>0</v>
       </c>
-      <c r="K26" t="s" s="0">
+      <c r="K26" t="s">
         <v>33</v>
       </c>
       <c r="T26" s="33"/>
@@ -11585,19 +11585,19 @@
       <c r="Y26" s="2"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A27" t="s" s="0">
+      <c r="A27" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="1">
         <v>45255</v>
       </c>
-      <c r="C27" t="s" s="0">
+      <c r="C27" t="s">
         <v>11</v>
       </c>
-      <c r="D27" t="s" s="0">
+      <c r="D27" t="s">
         <v>9</v>
       </c>
-      <c r="E27" t="s" s="0">
+      <c r="E27" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="22">
@@ -11606,28 +11606,28 @@
       <c r="G27" s="22">
         <v>45</v>
       </c>
-      <c r="H27" s="0">
+      <c r="H27">
         <v>30</v>
       </c>
-      <c r="I27" s="0">
+      <c r="I27">
         <v>0</v>
       </c>
       <c r="L27" s="22"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A28" t="s" s="0">
+      <c r="A28" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="1">
         <v>45255</v>
       </c>
-      <c r="C28" t="s" s="0">
+      <c r="C28" t="s">
         <v>11</v>
       </c>
-      <c r="D28" t="s" s="0">
+      <c r="D28" t="s">
         <v>9</v>
       </c>
-      <c r="E28" t="s" s="0">
+      <c r="E28" t="s">
         <v>10</v>
       </c>
       <c r="F28" s="22">
@@ -11636,28 +11636,28 @@
       <c r="G28" s="22">
         <v>42</v>
       </c>
-      <c r="H28" s="0">
+      <c r="H28">
         <v>8</v>
       </c>
-      <c r="I28" s="0">
+      <c r="I28">
         <v>0</v>
       </c>
       <c r="L28" s="22"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A29" t="s" s="0">
+      <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="1">
         <v>45255</v>
       </c>
-      <c r="C29" t="s" s="0">
+      <c r="C29" t="s">
         <v>11</v>
       </c>
-      <c r="D29" t="s" s="0">
+      <c r="D29" t="s">
         <v>9</v>
       </c>
-      <c r="E29" t="s" s="0">
+      <c r="E29" t="s">
         <v>10</v>
       </c>
       <c r="F29" s="22">
@@ -11666,28 +11666,28 @@
       <c r="G29" s="22">
         <v>54</v>
       </c>
-      <c r="H29" s="0">
+      <c r="H29">
         <v>28</v>
       </c>
-      <c r="I29" s="0">
+      <c r="I29">
         <v>0</v>
       </c>
       <c r="L29" s="22"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A30" t="s" s="0">
+      <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="1">
         <v>45256</v>
       </c>
-      <c r="C30" t="s" s="0">
+      <c r="C30" t="s">
         <v>3</v>
       </c>
-      <c r="D30" t="s" s="0">
+      <c r="D30" t="s">
         <v>0</v>
       </c>
-      <c r="E30" t="s" s="0">
+      <c r="E30" t="s">
         <v>10</v>
       </c>
       <c r="F30" s="22">
@@ -11696,10 +11696,10 @@
       <c r="G30" s="22">
         <v>62</v>
       </c>
-      <c r="H30" s="0">
+      <c r="H30">
         <v>50</v>
       </c>
-      <c r="I30" s="0">
+      <c r="I30">
         <v>0</v>
       </c>
       <c r="L30" s="22" t="s">
@@ -11707,19 +11707,19 @@
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A31" t="s" s="0">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>45256</v>
       </c>
-      <c r="C31" t="s" s="0">
+      <c r="C31" t="s">
         <v>3</v>
       </c>
-      <c r="D31" t="s" s="0">
+      <c r="D31" t="s">
         <v>0</v>
       </c>
-      <c r="E31" t="s" s="0">
+      <c r="E31" t="s">
         <v>5</v>
       </c>
       <c r="F31" s="22">
@@ -11728,10 +11728,10 @@
       <c r="G31" s="22">
         <v>57</v>
       </c>
-      <c r="H31" s="0">
+      <c r="H31">
         <v>8</v>
       </c>
-      <c r="I31" s="0">
+      <c r="I31">
         <v>0</v>
       </c>
       <c r="L31" s="22"/>
@@ -11741,19 +11741,19 @@
       <c r="W31" s="34"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" t="s" s="0">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="1">
         <v>45256</v>
       </c>
-      <c r="C32" t="s" s="0">
+      <c r="C32" t="s">
         <v>3</v>
       </c>
-      <c r="D32" t="s" s="0">
+      <c r="D32" t="s">
         <v>0</v>
       </c>
-      <c r="E32" t="s" s="0">
+      <c r="E32" t="s">
         <v>10</v>
       </c>
       <c r="F32" s="22">
@@ -11762,28 +11762,28 @@
       <c r="G32" s="22">
         <v>57</v>
       </c>
-      <c r="H32" s="0">
+      <c r="H32">
         <v>28</v>
       </c>
-      <c r="I32" s="0">
+      <c r="I32">
         <v>0</v>
       </c>
       <c r="L32" s="22"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" t="s" s="0">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
       <c r="B33" s="1">
         <v>45256</v>
       </c>
-      <c r="C33" t="s" s="0">
+      <c r="C33" t="s">
         <v>4</v>
       </c>
-      <c r="D33" t="s" s="0">
+      <c r="D33" t="s">
         <v>2</v>
       </c>
-      <c r="E33" t="s" s="0">
+      <c r="E33" t="s">
         <v>5</v>
       </c>
       <c r="F33" s="22">
@@ -11792,28 +11792,28 @@
       <c r="G33" s="22">
         <v>45</v>
       </c>
-      <c r="H33" s="0">
+      <c r="H33">
         <v>50</v>
       </c>
-      <c r="I33" s="0">
+      <c r="I33">
         <v>0</v>
       </c>
       <c r="L33" s="22"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" t="s" s="0">
+      <c r="A34" t="s">
         <v>30</v>
       </c>
       <c r="B34" s="1">
         <v>45256</v>
       </c>
-      <c r="C34" t="s" s="0">
+      <c r="C34" t="s">
         <v>4</v>
       </c>
-      <c r="D34" t="s" s="0">
+      <c r="D34" t="s">
         <v>2</v>
       </c>
-      <c r="E34" t="s" s="0">
+      <c r="E34" t="s">
         <v>5</v>
       </c>
       <c r="F34" s="22">
@@ -11822,28 +11822,28 @@
       <c r="G34" s="22">
         <v>45</v>
       </c>
-      <c r="H34" s="0">
+      <c r="H34">
         <v>50</v>
       </c>
-      <c r="I34" s="0">
+      <c r="I34">
         <v>0</v>
       </c>
       <c r="L34" s="22"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" t="s" s="0">
+      <c r="A35" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="1">
         <v>45256</v>
       </c>
-      <c r="C35" t="s" s="0">
+      <c r="C35" t="s">
         <v>4</v>
       </c>
-      <c r="D35" t="s" s="0">
+      <c r="D35" t="s">
         <v>2</v>
       </c>
-      <c r="E35" t="s" s="0">
+      <c r="E35" t="s">
         <v>5</v>
       </c>
       <c r="F35" s="22">
@@ -11852,28 +11852,28 @@
       <c r="G35" s="22">
         <v>60</v>
       </c>
-      <c r="H35" s="0">
+      <c r="H35">
         <v>50</v>
       </c>
-      <c r="I35" s="0">
+      <c r="I35">
         <v>0</v>
       </c>
       <c r="L35" s="22"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" t="s" s="0">
+      <c r="A36" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="1">
         <v>45256</v>
       </c>
-      <c r="C36" t="s" s="0">
+      <c r="C36" t="s">
         <v>4</v>
       </c>
-      <c r="D36" t="s" s="0">
+      <c r="D36" t="s">
         <v>2</v>
       </c>
-      <c r="E36" t="s" s="0">
+      <c r="E36" t="s">
         <v>5</v>
       </c>
       <c r="F36" s="22">
@@ -11882,28 +11882,28 @@
       <c r="G36" s="22">
         <v>59</v>
       </c>
-      <c r="H36" s="0">
+      <c r="H36">
         <v>50</v>
       </c>
-      <c r="I36" s="0">
+      <c r="I36">
         <v>0</v>
       </c>
       <c r="L36" s="22"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" t="s" s="0">
+      <c r="A37" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="1">
         <v>45256</v>
       </c>
-      <c r="C37" t="s" s="0">
+      <c r="C37" t="s">
         <v>4</v>
       </c>
-      <c r="D37" t="s" s="0">
+      <c r="D37" t="s">
         <v>2</v>
       </c>
-      <c r="E37" t="s" s="0">
+      <c r="E37" t="s">
         <v>5</v>
       </c>
       <c r="F37" s="22">
@@ -11912,28 +11912,28 @@
       <c r="G37" s="22">
         <v>57</v>
       </c>
-      <c r="H37" s="0">
+      <c r="H37">
         <v>50</v>
       </c>
-      <c r="I37" s="0">
+      <c r="I37">
         <v>0</v>
       </c>
       <c r="L37" s="22"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" t="s" s="0">
+      <c r="A38" t="s">
         <v>30</v>
       </c>
       <c r="B38" s="1">
         <v>45256</v>
       </c>
-      <c r="C38" t="s" s="0">
+      <c r="C38" t="s">
         <v>4</v>
       </c>
-      <c r="D38" t="s" s="0">
+      <c r="D38" t="s">
         <v>2</v>
       </c>
-      <c r="E38" t="s" s="0">
+      <c r="E38" t="s">
         <v>5</v>
       </c>
       <c r="F38" s="22">
@@ -11942,28 +11942,28 @@
       <c r="G38" s="22">
         <v>47</v>
       </c>
-      <c r="H38" s="0">
+      <c r="H38">
         <v>50</v>
       </c>
-      <c r="I38" s="0">
+      <c r="I38">
         <v>0</v>
       </c>
       <c r="L38" s="22"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" t="s" s="0">
+      <c r="A39" t="s">
         <v>30</v>
       </c>
       <c r="B39" s="1">
         <v>45256</v>
       </c>
-      <c r="C39" t="s" s="0">
+      <c r="C39" t="s">
         <v>4</v>
       </c>
-      <c r="D39" t="s" s="0">
+      <c r="D39" t="s">
         <v>2</v>
       </c>
-      <c r="E39" t="s" s="0">
+      <c r="E39" t="s">
         <v>5</v>
       </c>
       <c r="F39" s="22">
@@ -11972,28 +11972,28 @@
       <c r="G39" s="22">
         <v>51</v>
       </c>
-      <c r="H39" s="0">
+      <c r="H39">
         <v>50</v>
       </c>
-      <c r="I39" s="0">
+      <c r="I39">
         <v>0</v>
       </c>
       <c r="L39" s="22"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" t="s" s="0">
+      <c r="A40" t="s">
         <v>30</v>
       </c>
       <c r="B40" s="1">
         <v>45256</v>
       </c>
-      <c r="C40" t="s" s="0">
+      <c r="C40" t="s">
         <v>4</v>
       </c>
-      <c r="D40" t="s" s="0">
+      <c r="D40" t="s">
         <v>2</v>
       </c>
-      <c r="E40" t="s" s="0">
+      <c r="E40" t="s">
         <v>5</v>
       </c>
       <c r="F40" s="22">
@@ -12002,28 +12002,28 @@
       <c r="G40" s="22">
         <v>43</v>
       </c>
-      <c r="H40" s="0">
+      <c r="H40">
         <v>45</v>
       </c>
-      <c r="I40" s="0">
+      <c r="I40">
         <v>0</v>
       </c>
       <c r="L40" s="22"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" t="s" s="0">
+      <c r="A41" t="s">
         <v>30</v>
       </c>
       <c r="B41" s="1">
         <v>45256</v>
       </c>
-      <c r="C41" t="s" s="0">
+      <c r="C41" t="s">
         <v>4</v>
       </c>
-      <c r="D41" t="s" s="0">
+      <c r="D41" t="s">
         <v>2</v>
       </c>
-      <c r="E41" t="s" s="0">
+      <c r="E41" t="s">
         <v>5</v>
       </c>
       <c r="F41" s="22">
@@ -12032,28 +12032,28 @@
       <c r="G41" s="22">
         <v>75</v>
       </c>
-      <c r="H41" s="0">
+      <c r="H41">
         <v>50</v>
       </c>
-      <c r="I41" s="0">
+      <c r="I41">
         <v>0</v>
       </c>
       <c r="L41" s="22"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" t="s" s="0">
+      <c r="A42" t="s">
         <v>30</v>
       </c>
       <c r="B42" s="1">
         <v>45256</v>
       </c>
-      <c r="C42" t="s" s="0">
+      <c r="C42" t="s">
         <v>4</v>
       </c>
-      <c r="D42" t="s" s="0">
+      <c r="D42" t="s">
         <v>2</v>
       </c>
-      <c r="E42" t="s" s="0">
+      <c r="E42" t="s">
         <v>5</v>
       </c>
       <c r="F42" s="22">
@@ -12062,28 +12062,28 @@
       <c r="G42" s="22">
         <v>70</v>
       </c>
-      <c r="H42" s="0">
+      <c r="H42">
         <v>30</v>
       </c>
-      <c r="I42" s="0">
+      <c r="I42">
         <v>0</v>
       </c>
       <c r="L42" s="22"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" t="s" s="0">
+      <c r="A43" t="s">
         <v>30</v>
       </c>
       <c r="B43" s="1">
         <v>45256</v>
       </c>
-      <c r="C43" t="s" s="0">
+      <c r="C43" t="s">
         <v>4</v>
       </c>
-      <c r="D43" t="s" s="0">
+      <c r="D43" t="s">
         <v>2</v>
       </c>
-      <c r="E43" t="s" s="0">
+      <c r="E43" t="s">
         <v>5</v>
       </c>
       <c r="F43" s="22">
@@ -12092,10 +12092,10 @@
       <c r="G43" s="22">
         <v>53</v>
       </c>
-      <c r="H43" s="0">
+      <c r="H43">
         <v>50</v>
       </c>
-      <c r="I43" s="0">
+      <c r="I43">
         <v>0</v>
       </c>
       <c r="L43" s="22"/>
@@ -12135,8 +12135,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="5" max="5" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -12168,7 +12168,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="V2" t="s" s="0">
+      <c r="V2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -12176,16 +12176,16 @@
       <c r="A3" s="1">
         <v>45237</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>106</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -12193,25 +12193,25 @@
       <c r="A4" s="1">
         <v>45237</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>83</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" t="s" s="0">
+      <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="O4" t="s" s="0">
+      <c r="O4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -12219,26 +12219,26 @@
       <c r="A5" s="1">
         <v>45237</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>89</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="M5" t="s" s="0">
+      <c r="M5" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="0">
+      <c r="N5">
         <f>(SUMIF($C$3:$C$100, M5, $B$3:$B$100)/COUNTIF($C$3:$C$100, M5))</f>
         <v>88.083333333333329</v>
       </c>
-      <c r="O5" s="0">
+      <c r="O5">
         <f>(SUMIF($C$3:$C$100, M5, $F$3:$F$100)/COUNTIF($C$13:$C$100, M5))</f>
         <v>42.428571428571431</v>
       </c>
@@ -12247,26 +12247,26 @@
       <c r="A6" s="1">
         <v>45238</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>71</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>0</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="M6" t="s" s="0">
+      <c r="M6" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="0">
+      <c r="N6">
         <f>(SUMIF($C$3:$C$100, M6, $B$3:$B$100)/COUNTIF($C$3:$C$100, M6))</f>
         <v>98.5</v>
       </c>
-      <c r="O6" s="0">
+      <c r="O6">
         <f>(SUMIF($C$3:$C$100, M6, $F$3:$F$100)/COUNTIF($C$13:$C$100, M6))</f>
         <v>57.333333333333336</v>
       </c>
@@ -12275,26 +12275,26 @@
       <c r="A7" s="1">
         <v>45238</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>88</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="M7" t="s" s="0">
+      <c r="M7" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="0">
+      <c r="N7">
         <f>(SUMIF($C$3:$C$100, M7, $B$3:$B$100)/COUNTIF($C$3:$C$100, M7))</f>
         <v>86.25</v>
       </c>
-      <c r="O7" s="0">
+      <c r="O7">
         <f>(SUMIF($C$3:$C$100, M7, $F$3:$F$100)/COUNTIF($C$13:$C$100, M7))</f>
         <v>38</v>
       </c>
@@ -12303,16 +12303,16 @@
       <c r="A8" s="1">
         <v>45238</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8">
         <v>111</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>2</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -12320,16 +12320,16 @@
       <c r="A9" s="1">
         <v>45238</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9">
         <v>34</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -12340,16 +12340,16 @@
       <c r="A10" s="1">
         <v>45238</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10">
         <v>120</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>0</v>
       </c>
-      <c r="E10" t="s" s="0">
+      <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="H10" s="33" t="s">
@@ -12358,14 +12358,14 @@
       <c r="I10" s="33"/>
       <c r="J10" s="33"/>
       <c r="K10" s="33"/>
-      <c r="M10" t="s" s="0">
+      <c r="M10" t="s">
         <v>0</v>
       </c>
-      <c r="N10" s="0">
+      <c r="N10">
         <f>(SUMIF($D$3:$D$100, M10, $B$3:$B$100)/COUNTIF($D$3:$D$100, M10))</f>
         <v>96.666666666666671</v>
       </c>
-      <c r="O10" s="0">
+      <c r="O10">
         <f>(SUMIF($D$3:$D$100, M10, $F$3:$F$100)/COUNTIF($D$13:$D$100, M10))</f>
         <v>26</v>
       </c>
@@ -12374,16 +12374,16 @@
       <c r="A11" s="1">
         <v>45238</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11">
         <v>75</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="H11" s="33" t="s">
@@ -12394,14 +12394,14 @@
         <v>22</v>
       </c>
       <c r="K11" s="33"/>
-      <c r="M11" t="s" s="0">
+      <c r="M11" t="s">
         <v>9</v>
       </c>
-      <c r="N11" s="0">
+      <c r="N11">
         <f>(SUMIF($D$3:$D$100, M11, $B$3:$B$100)/COUNTIF($D$3:$D$100, M11))</f>
         <v>77</v>
       </c>
-      <c r="O11" s="0">
+      <c r="O11">
         <f>(SUMIF($D$3:$D$100, M11, $F$3:$F$100)/COUNTIF($D$13:$D$100, M11))</f>
         <v>45.166666666666664</v>
       </c>
@@ -12419,14 +12419,14 @@
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s" s="0">
+      <c r="M12" t="s">
         <v>2</v>
       </c>
-      <c r="N12" s="0">
+      <c r="N12">
         <f>(SUMIF($D$3:$D$100, M12, $B$3:$B$100)/COUNTIF($D$3:$D$100, M12))</f>
         <v>97.75</v>
       </c>
-      <c r="O12" s="0">
+      <c r="O12">
         <f>(SUMIF($D$3:$D$100, M12, $F$3:$F$100)/COUNTIF($D$13:$D$100, M12))</f>
         <v>57.333333333333336</v>
       </c>
@@ -12435,26 +12435,26 @@
       <c r="A13" s="1">
         <v>45237</v>
       </c>
-      <c r="B13" s="0">
+      <c r="B13">
         <v>111</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s" s="0">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>66</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <f t="shared" ref="H13:H23" si="0">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12)+SUMIF($M$15:$M$17, $E13, $N$15:$N$17))/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <f t="shared" ref="I13:I23" si="1">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12)+SUMIF($M$15:$M$17, $E13, $O$15:$O$17))/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -12462,7 +12462,7 @@
         <f t="shared" ref="J13:J23" si="2">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12))/2</f>
         <v>98.125</v>
       </c>
-      <c r="K13" s="0">
+      <c r="K13">
         <f t="shared" ref="K13:K23" si="3">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12))/2</f>
         <v>57.333333333333336</v>
       </c>
@@ -12471,26 +12471,26 @@
       <c r="A14" s="1">
         <v>45238</v>
       </c>
-      <c r="B14" s="0">
+      <c r="B14">
         <v>107</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>57</v>
       </c>
-      <c r="H14" s="0">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>84.49444444444444</v>
       </c>
-      <c r="I14" s="0">
+      <c r="I14">
         <f t="shared" si="1"/>
         <v>48.198412698412703</v>
       </c>
@@ -12498,7 +12498,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K14" s="0">
+      <c r="K14">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -12510,26 +12510,26 @@
       <c r="A15" s="1">
         <v>45234</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15">
         <v>108</v>
       </c>
-      <c r="C15" t="s" s="0">
+      <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" t="s" s="0">
+      <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="s" s="0">
+      <c r="E15" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>38</v>
       </c>
-      <c r="H15" s="0">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>63.166666666666664</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15">
         <f t="shared" si="1"/>
         <v>30.166666666666668</v>
       </c>
@@ -12537,18 +12537,18 @@
         <f t="shared" si="2"/>
         <v>43.125</v>
       </c>
-      <c r="K15" s="0">
+      <c r="K15">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="M15" t="s" s="0">
+      <c r="M15" t="s">
         <v>10</v>
       </c>
-      <c r="N15" s="0">
+      <c r="N15">
         <f>(SUMIF($E$3:$E$100, M15, $B$3:$B$100)/COUNTIF($E$3:$E$100, M15))</f>
         <v>83.166666666666671</v>
       </c>
-      <c r="O15" s="0">
+      <c r="O15">
         <f>(SUMIF($E$3:$E$100, M15, $F$3:$F$100)/COUNTIF($E$13:$E$100, M15))</f>
         <v>40</v>
       </c>
@@ -12557,26 +12557,26 @@
       <c r="A16" s="1">
         <v>45234</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16">
         <v>107</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s" s="0">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>74</v>
       </c>
-      <c r="H16" s="0">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -12584,18 +12584,18 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K16" s="0">
+      <c r="K16">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
-      <c r="M16" t="s" s="0">
+      <c r="M16" t="s">
         <v>1</v>
       </c>
-      <c r="N16" s="0">
+      <c r="N16">
         <f>(SUMIF($E$3:$E$100, M16, $B$3:$B$100)/COUNTIF($E$3:$E$100, M16))</f>
         <v>88.4</v>
       </c>
-      <c r="O16" s="0">
+      <c r="O16">
         <f>(SUMIF($E$3:$E$100, M16, $F$3:$F$100)/COUNTIF($E$13:$E$100, M16))</f>
         <v>57</v>
       </c>
@@ -12604,26 +12604,26 @@
       <c r="A17" s="1">
         <v>45234</v>
       </c>
-      <c r="B17" s="0">
+      <c r="B17">
         <v>97</v>
       </c>
-      <c r="C17" t="s" s="0">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s" s="0">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>62</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I17">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -12631,18 +12631,18 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K17" s="0">
+      <c r="K17">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
-      <c r="M17" t="s" s="0">
+      <c r="M17" t="s">
         <v>5</v>
       </c>
-      <c r="N17" s="0">
+      <c r="N17">
         <f>(SUMIF($E$3:$E$100, M17, $B$3:$B$100)/COUNTIF($E$3:$E$100, M17))</f>
         <v>103.25</v>
       </c>
-      <c r="O17" s="0">
+      <c r="O17">
         <f>(SUMIF($E$3:$E$100, M17, $F$3:$F$100)/COUNTIF($E$13:$E$100, M17))</f>
         <v>52.5</v>
       </c>
@@ -12651,26 +12651,26 @@
       <c r="A18" s="1">
         <v>45234</v>
       </c>
-      <c r="B18" s="0">
+      <c r="B18">
         <v>99</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" t="s" s="0">
+      <c r="D18" t="s">
         <v>0</v>
       </c>
-      <c r="E18" t="s" s="0">
+      <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>26</v>
       </c>
-      <c r="H18" s="0">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>89.305555555555557</v>
       </c>
-      <c r="I18" s="0">
+      <c r="I18">
         <f t="shared" si="1"/>
         <v>36.142857142857146</v>
       </c>
@@ -12678,7 +12678,7 @@
         <f t="shared" si="2"/>
         <v>92.375</v>
       </c>
-      <c r="K18" s="0">
+      <c r="K18">
         <f t="shared" si="3"/>
         <v>34.214285714285715</v>
       </c>
@@ -12687,26 +12687,26 @@
       <c r="A19" s="1">
         <v>45234</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19">
         <v>87</v>
       </c>
-      <c r="C19" t="s" s="0">
+      <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="D19" t="s" s="0">
+      <c r="D19" t="s">
         <v>2</v>
       </c>
-      <c r="E19" t="s" s="0">
+      <c r="E19" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>32</v>
       </c>
-      <c r="H19" s="0">
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I19" s="0">
+      <c r="I19">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -12714,7 +12714,7 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K19" s="0">
+      <c r="K19">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
@@ -12723,26 +12723,26 @@
       <c r="A20" s="1">
         <v>45234</v>
       </c>
-      <c r="B20" s="0">
+      <c r="B20">
         <v>76</v>
       </c>
-      <c r="C20" t="s" s="0">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s" s="0">
+      <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>48</v>
       </c>
-      <c r="H20" s="0">
+      <c r="H20">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I20" s="0">
+      <c r="I20">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -12750,7 +12750,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K20" s="0">
+      <c r="K20">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -12759,26 +12759,26 @@
       <c r="A21" s="1">
         <v>45234</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21">
         <v>93</v>
       </c>
-      <c r="C21" t="s" s="0">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s" s="0">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" t="s" s="0">
+      <c r="E21" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21">
         <v>40</v>
       </c>
-      <c r="H21" s="0">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I21" s="0">
+      <c r="I21">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -12786,7 +12786,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K21" s="0">
+      <c r="K21">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -12795,26 +12795,26 @@
       <c r="A22" s="1">
         <v>45234</v>
       </c>
-      <c r="B22" s="0">
+      <c r="B22">
         <v>85</v>
       </c>
-      <c r="C22" t="s" s="0">
+      <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>30</v>
       </c>
-      <c r="H22" s="0">
+      <c r="H22">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I22" s="0">
+      <c r="I22">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -12822,7 +12822,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K22" s="0">
+      <c r="K22">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -12831,26 +12831,26 @@
       <c r="A23" s="1">
         <v>45234</v>
       </c>
-      <c r="B23" s="0">
+      <c r="B23">
         <v>49</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>11</v>
       </c>
-      <c r="D23" t="s" s="0">
+      <c r="D23" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s" s="0">
+      <c r="E23" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>34</v>
       </c>
-      <c r="H23" s="0">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I23" s="0">
+      <c r="I23">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -12858,7 +12858,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K23" s="0">
+      <c r="K23">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -12878,67 +12878,67 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T28" s="0">
+      <c r="T28">
         <v>1</v>
       </c>
-      <c r="U28" t="s" s="0">
+      <c r="U28" t="s">
         <v>3</v>
       </c>
-      <c r="V28" t="s" s="0">
+      <c r="V28" t="s">
         <v>0</v>
       </c>
-      <c r="W28" t="s" s="0">
+      <c r="W28" t="s">
         <v>1</v>
       </c>
-      <c r="X28" s="0">
+      <c r="X28">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y28" s="0">
+      <c r="Y28">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T29" s="0">
+      <c r="T29">
         <v>2</v>
       </c>
-      <c r="U29" t="s" s="0">
+      <c r="U29" t="s">
         <v>11</v>
       </c>
-      <c r="V29" t="s" s="0">
+      <c r="V29" t="s">
         <v>9</v>
       </c>
-      <c r="W29" t="s" s="0">
+      <c r="W29" t="s">
         <v>1</v>
       </c>
-      <c r="X29" s="0">
+      <c r="X29">
         <f>(N5+N11+N16)/3</f>
         <v>84.49444444444444</v>
       </c>
-      <c r="Y29" s="0">
+      <c r="Y29">
         <f>(O5+O11+O16)/3</f>
         <v>48.198412698412703</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T30" s="0">
+      <c r="T30">
         <v>3</v>
       </c>
-      <c r="U30" t="s" s="0">
+      <c r="U30" t="s">
         <v>4</v>
       </c>
-      <c r="V30" t="s" s="0">
+      <c r="V30" t="s">
         <v>9</v>
       </c>
-      <c r="W30" t="s" s="0">
+      <c r="W30" t="s">
         <v>1</v>
       </c>
-      <c r="X30" s="0">
+      <c r="X30">
         <f>(N6+N11+N16)/3</f>
         <v>87.966666666666654</v>
       </c>
-      <c r="Y30" s="0">
+      <c r="Y30">
         <f>(O6+O11+O16)/3</f>
         <v>53.166666666666664</v>
       </c>
@@ -12952,67 +12952,67 @@
       <c r="W32" s="33"/>
     </row>
     <row r="33" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T33" s="0">
+      <c r="T33">
         <v>1</v>
       </c>
-      <c r="U33" t="s" s="0">
+      <c r="U33" t="s">
         <v>3</v>
       </c>
-      <c r="V33" t="s" s="0">
+      <c r="V33" t="s">
         <v>0</v>
       </c>
-      <c r="W33" t="s" s="0">
+      <c r="W33" t="s">
         <v>1</v>
       </c>
-      <c r="X33" s="0">
+      <c r="X33">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y33" s="0">
+      <c r="Y33">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="34" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T34" s="0">
+      <c r="T34">
         <v>2</v>
       </c>
-      <c r="U34" t="s" s="0">
+      <c r="U34" t="s">
         <v>11</v>
       </c>
-      <c r="V34" t="s" s="0">
+      <c r="V34" t="s">
         <v>9</v>
       </c>
-      <c r="W34" t="s" s="0">
+      <c r="W34" t="s">
         <v>10</v>
       </c>
-      <c r="X34" s="0">
+      <c r="X34">
         <f>(N5+N11+N15)/3</f>
         <v>82.75</v>
       </c>
-      <c r="Y34" s="0">
+      <c r="Y34">
         <f>(O5+O11+O15)/3</f>
         <v>42.531746031746032</v>
       </c>
     </row>
     <row r="35" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T35" s="0">
+      <c r="T35">
         <v>3</v>
       </c>
-      <c r="U35" t="s" s="0">
+      <c r="U35" t="s">
         <v>4</v>
       </c>
-      <c r="V35" t="s" s="0">
+      <c r="V35" t="s">
         <v>2</v>
       </c>
-      <c r="W35" t="s" s="0">
+      <c r="W35" t="s">
         <v>5</v>
       </c>
-      <c r="X35" s="0">
+      <c r="X35">
         <f>(N6+N12+N17)/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="Y35" s="0">
+      <c r="Y35">
         <f>(O6+O12+O17)/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -13069,160 +13069,160 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="n">
-        <v>63.04653802464488</v>
-      </c>
-      <c r="B3" s="26" t="n">
+      <c r="A3" s="23">
+        <v>63.046538024644882</v>
+      </c>
+      <c r="B3" s="26">
         <v>38.764560098463484</v>
       </c>
-      <c r="C3" s="26" t="n">
+      <c r="C3" s="26">
         <v>20.939281288620293</v>
       </c>
-      <c r="D3" s="23" t="n">
-        <v>0.0</v>
+      <c r="D3" s="23">
+        <v>0</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="n">
-        <v>98.56542055987764</v>
-      </c>
-      <c r="B4" s="30" t="n">
-        <v>53.40400471101017</v>
-      </c>
-      <c r="C4" s="30" t="n">
-        <v>45.24028268506923</v>
-      </c>
-      <c r="D4" s="29" t="n">
-        <v>0.0</v>
+      <c r="A4" s="29">
+        <v>74.797872340599682</v>
+      </c>
+      <c r="B4" s="30">
+        <v>40.446030330182737</v>
+      </c>
+      <c r="C4" s="30">
+        <v>34.263157894769414</v>
+      </c>
+      <c r="D4" s="29">
+        <v>0</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="31" t="n">
-        <v>78.84931506750885</v>
-      </c>
-      <c r="B5" s="32" t="n">
-        <v>50.08888888780873</v>
-      </c>
-      <c r="C5" s="32" t="n">
+      <c r="A5" s="31">
+        <v>78.849315067508854</v>
+      </c>
+      <c r="B5" s="32">
+        <v>50.088888887808729</v>
+      </c>
+      <c r="C5" s="32">
         <v>28.755555555566744</v>
       </c>
-      <c r="D5" s="31" t="n">
-        <v>0.0</v>
+      <c r="D5" s="31">
+        <v>0</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="n">
+      <c r="A6" s="23">
         <v>62.061899679414424</v>
       </c>
-      <c r="B6" s="26" t="n">
-        <v>40.45314222669349</v>
-      </c>
-      <c r="C6" s="26" t="n">
-        <v>21.08269018725826</v>
-      </c>
-      <c r="D6" s="23" t="n">
-        <v>0.0</v>
+      <c r="B6" s="26">
+        <v>40.453142226693487</v>
+      </c>
+      <c r="C6" s="26">
+        <v>21.082690187258262</v>
+      </c>
+      <c r="D6" s="23">
+        <v>0</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="n">
-        <v>101.08671586657731</v>
-      </c>
-      <c r="B7" s="30" t="n">
-        <v>54.13642213607548</v>
-      </c>
-      <c r="C7" s="30" t="n">
-        <v>47.20849420829709</v>
-      </c>
-      <c r="D7" s="29" t="n">
-        <v>0.0</v>
+      <c r="A7" s="29">
+        <v>75.74516129069508</v>
+      </c>
+      <c r="B7" s="30">
+        <v>40.099142040113222</v>
+      </c>
+      <c r="C7" s="30">
+        <v>34.967588179361691</v>
+      </c>
+      <c r="D7" s="29">
+        <v>0</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="31" t="n">
-        <v>77.87785016147298</v>
-      </c>
-      <c r="B8" s="32" t="n">
+      <c r="A8" s="31">
+        <v>77.877850161472978</v>
+      </c>
+      <c r="B8" s="32">
         <v>48.273972601126175</v>
       </c>
-      <c r="C8" s="32" t="n">
-        <v>28.69863013697737</v>
-      </c>
-      <c r="D8" s="31" t="n">
-        <v>0.0</v>
+      <c r="C8" s="32">
+        <v>28.698630136977371</v>
+      </c>
+      <c r="D8" s="31">
+        <v>0</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="n">
-        <v>75.22368420881257</v>
-      </c>
-      <c r="B9" s="26" t="n">
-        <v>48.06140350758862</v>
-      </c>
-      <c r="C9" s="26" t="n">
+      <c r="A9" s="23">
+        <v>75.223684208812571</v>
+      </c>
+      <c r="B9" s="26">
+        <v>48.061403507588622</v>
+      </c>
+      <c r="C9" s="26">
         <v>26.390350876438607</v>
       </c>
-      <c r="D9" s="23" t="n">
-        <v>0.0</v>
+      <c r="D9" s="23">
+        <v>0</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="n">
-        <v>98.49940687975642</v>
-      </c>
-      <c r="B10" s="30" t="n">
-        <v>54.36061684427774</v>
-      </c>
-      <c r="C10" s="30" t="n">
-        <v>44.138790035478664</v>
-      </c>
-      <c r="D10" s="29" t="n">
-        <v>0.0</v>
+      <c r="A10" s="29">
+        <v>74.470852018152613</v>
+      </c>
+      <c r="B10" s="30">
+        <v>41.099551569560809</v>
+      </c>
+      <c r="C10" s="30">
+        <v>33.371300448591789</v>
+      </c>
+      <c r="D10" s="29">
+        <v>0</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="27" t="n">
-        <v>61.59240069143186</v>
-      </c>
-      <c r="B11" s="28" t="n">
+      <c r="A11" s="27">
+        <v>61.592400691431862</v>
+      </c>
+      <c r="B11" s="28">
         <v>30.261744966510754</v>
       </c>
-      <c r="C11" s="28" t="n">
+      <c r="C11" s="28">
         <v>24.067114094025488</v>
       </c>
-      <c r="D11" s="27" t="n">
-        <v>0.0</v>
+      <c r="D11" s="27">
+        <v>0</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>35</v>
       </c>
     </row>
@@ -13388,35 +13388,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" bestFit="true" customWidth="true" width="9.5546875"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0"/>
-    <col min="5" max="7" bestFit="true" customWidth="true" width="9.5546875"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.0"/>
-    <col min="9" max="11" bestFit="true" customWidth="true" width="9.5546875"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="9.0"/>
-    <col min="13" max="15" bestFit="true" customWidth="true" width="9.5546875"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="9.0"/>
+    <col min="1" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="42"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="38"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
@@ -13467,30 +13467,30 @@
       <c r="BL1" s="2"/>
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="39" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="39" t="s">
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="37" t="s">
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="40"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="46"/>
       <c r="Y2" s="33"/>
       <c r="Z2" s="33"/>
       <c r="AA2" s="33"/>
@@ -13501,13 +13501,13 @@
       <c r="AF2" s="33"/>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -13516,10 +13516,10 @@
       <c r="E3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>28</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -13528,22 +13528,22 @@
       <c r="I3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" t="s" s="0">
+      <c r="K3" t="s">
         <v>28</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M3" t="s" s="0">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="N3" t="s" s="0">
+      <c r="N3" t="s">
         <v>17</v>
       </c>
-      <c r="O3" t="s" s="0">
+      <c r="O3" t="s">
         <v>28</v>
       </c>
       <c r="P3" s="6" t="s">
@@ -13551,218 +13551,218 @@
       </c>
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="n">
-        <v>62.55421885202965</v>
-      </c>
-      <c r="B4" s="13" t="n">
-        <v>39.60885116257849</v>
-      </c>
-      <c r="C4" s="13" t="n">
-        <v>21.01098573793928</v>
-      </c>
-      <c r="D4" s="14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="15" t="n">
-        <v>65.08811192338624</v>
-      </c>
-      <c r="F4" s="13" t="n">
-        <v>41.29936163158052</v>
-      </c>
-      <c r="G4" s="13" t="n">
+      <c r="A4" s="13">
+        <v>62.554218852029649</v>
+      </c>
+      <c r="B4" s="13">
+        <v>39.608851162578489</v>
+      </c>
+      <c r="C4" s="13">
+        <v>21.010985737939279</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="15">
+        <v>65.088111923386236</v>
+      </c>
+      <c r="F4" s="13">
+        <v>41.299361631580517</v>
+      </c>
+      <c r="G4" s="13">
         <v>22.086858765639143</v>
       </c>
-      <c r="H4" s="14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I4" s="15" t="n">
-        <v>69.743256457575</v>
-      </c>
-      <c r="J4" s="13" t="n">
-        <v>42.55920429891834</v>
-      </c>
-      <c r="K4" s="13" t="n">
-        <v>25.636546597447158</v>
-      </c>
-      <c r="L4" s="14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M4" s="13" t="n">
+      <c r="H4" s="14">
+        <v>0</v>
+      </c>
+      <c r="I4" s="15">
+        <v>64.937545485254233</v>
+      </c>
+      <c r="J4" s="13">
+        <v>39.906991243974957</v>
+      </c>
+      <c r="K4" s="13">
+        <v>23.483048680069782</v>
+      </c>
+      <c r="L4" s="14">
+        <v>0</v>
+      </c>
+      <c r="M4" s="13">
         <v>62.36185521991009</v>
       </c>
-      <c r="N4" s="13" t="n">
-        <v>37.73942992336494</v>
-      </c>
-      <c r="O4" s="13" t="n">
+      <c r="N4" s="13">
+        <v>37.739429923364938</v>
+      </c>
+      <c r="O4" s="13">
         <v>21.62221140915652</v>
       </c>
-      <c r="P4" s="16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q4" t="s" s="0">
+      <c r="P4" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="n">
-        <v>99.82606821322747</v>
-      </c>
-      <c r="B5" s="13" t="n">
-        <v>53.77021342354283</v>
-      </c>
-      <c r="C5" s="13" t="n">
-        <v>46.224388446683164</v>
-      </c>
-      <c r="D5" s="14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="15" t="n">
-        <v>94.90559141234449</v>
-      </c>
-      <c r="F5" s="13" t="n">
-        <v>52.62845144035199</v>
-      </c>
-      <c r="G5" s="13" t="n">
-        <v>42.257580932634255</v>
-      </c>
-      <c r="H5" s="14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I5" s="15" t="n">
-        <v>99.56073594653326</v>
-      </c>
-      <c r="J5" s="13" t="n">
-        <v>53.88829410768981</v>
-      </c>
-      <c r="K5" s="13" t="n">
-        <v>45.80726876444227</v>
-      </c>
-      <c r="L5" s="14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M5" s="13" t="n">
-        <v>92.17933470886835</v>
-      </c>
-      <c r="N5" s="13" t="n">
-        <v>49.06851973213641</v>
-      </c>
-      <c r="O5" s="13" t="n">
-        <v>41.79293357615163</v>
-      </c>
-      <c r="P5" s="16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q5" t="s" s="0">
+      <c r="A5" s="13">
+        <v>75.271516815647374</v>
+      </c>
+      <c r="B5" s="13">
+        <v>40.272586185147979</v>
+      </c>
+      <c r="C5" s="13">
+        <v>34.615373037065552</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15">
+        <v>75.26195029428041</v>
+      </c>
+      <c r="F5" s="13">
+        <v>41.830349649636105</v>
+      </c>
+      <c r="G5" s="13">
+        <v>32.970368604940163</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0</v>
+      </c>
+      <c r="I5" s="15">
+        <v>75.111383856148422</v>
+      </c>
+      <c r="J5" s="13">
+        <v>40.437979262030545</v>
+      </c>
+      <c r="K5" s="13">
+        <v>34.366558519370798</v>
+      </c>
+      <c r="L5" s="14">
+        <v>0</v>
+      </c>
+      <c r="M5" s="13">
+        <v>72.535693590804271</v>
+      </c>
+      <c r="N5" s="13">
+        <v>38.270417941420533</v>
+      </c>
+      <c r="O5" s="13">
+        <v>32.50572124845754</v>
+      </c>
+      <c r="P5" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="n">
-        <v>78.36358261449092</v>
-      </c>
-      <c r="B6" s="17" t="n">
-        <v>49.18143074446745</v>
-      </c>
-      <c r="C6" s="17" t="n">
+      <c r="A6" s="17">
+        <v>78.363582614490923</v>
+      </c>
+      <c r="B6" s="17">
+        <v>49.181430744467448</v>
+      </c>
+      <c r="C6" s="17">
         <v>28.727092846272058</v>
       </c>
-      <c r="D6" s="18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="19" t="n">
-        <v>77.73560293335525</v>
-      </c>
-      <c r="F6" s="17" t="n">
-        <v>48.95742529709169</v>
-      </c>
-      <c r="G6" s="17" t="n">
+      <c r="D6" s="18">
+        <v>0</v>
+      </c>
+      <c r="E6" s="19">
+        <v>77.735602933355253</v>
+      </c>
+      <c r="F6" s="17">
+        <v>48.957425297091689</v>
+      </c>
+      <c r="G6" s="17">
         <v>28.25974445230537</v>
       </c>
-      <c r="H6" s="18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I6" s="19" t="n">
-        <v>82.39074746754402</v>
-      </c>
-      <c r="J6" s="17" t="n">
-        <v>50.2172679644295</v>
-      </c>
-      <c r="K6" s="17" t="n">
-        <v>31.80943228411338</v>
-      </c>
-      <c r="L6" s="18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M6" s="17" t="n">
-        <v>75.00934622987911</v>
-      </c>
-      <c r="N6" s="17" t="n">
+      <c r="H6" s="18">
+        <v>0</v>
+      </c>
+      <c r="I6" s="19">
+        <v>77.585036495223264</v>
+      </c>
+      <c r="J6" s="17">
+        <v>47.565054909486122</v>
+      </c>
+      <c r="K6" s="17">
+        <v>29.655934366736005</v>
+      </c>
+      <c r="L6" s="18">
+        <v>0</v>
+      </c>
+      <c r="M6" s="17">
+        <v>75.009346229879114</v>
+      </c>
+      <c r="N6" s="17">
         <v>45.39749358887611</v>
       </c>
-      <c r="O6" s="17" t="n">
+      <c r="O6" s="17">
         <v>27.795097095822747</v>
       </c>
-      <c r="P6" s="20" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q6" t="s" s="0">
+      <c r="P6" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="42"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="38"/>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="39" t="s">
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="39" t="s">
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="37" t="s">
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="46"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="45"/>
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -13771,10 +13771,10 @@
       <c r="E9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F9" t="s" s="0">
+      <c r="F9" t="s">
         <v>17</v>
       </c>
-      <c r="G9" t="s" s="0">
+      <c r="G9" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -13783,22 +13783,22 @@
       <c r="I9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J9" t="s" s="0">
+      <c r="J9" t="s">
         <v>17</v>
       </c>
-      <c r="K9" t="s" s="0">
+      <c r="K9" t="s">
         <v>28</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M9" t="s" s="0">
+      <c r="M9" t="s">
         <v>23</v>
       </c>
-      <c r="N9" t="s" s="0">
+      <c r="N9" t="s">
         <v>17</v>
       </c>
-      <c r="O9" t="s" s="0">
+      <c r="O9" t="s">
         <v>28</v>
       </c>
       <c r="P9" s="6" t="s">
@@ -13806,201 +13806,201 @@
       </c>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="n">
-        <v>59.95238095238095</v>
-      </c>
-      <c r="B10" t="n" s="0">
+      <c r="A10" s="4">
+        <v>59.952380952380949</v>
+      </c>
+      <c r="B10">
         <v>38.073170731707314</v>
       </c>
-      <c r="C10" t="n" s="0">
+      <c r="C10">
         <v>19.951219512195124</v>
       </c>
-      <c r="D10" s="9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E10" s="11" t="n">
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="11">
         <v>64.875</v>
       </c>
-      <c r="F10" t="n" s="0">
-        <v>43.0</v>
-      </c>
-      <c r="G10" t="n" s="0">
+      <c r="F10">
+        <v>43</v>
+      </c>
+      <c r="G10">
         <v>19.875</v>
       </c>
-      <c r="H10" s="9" t="n">
-        <v>0.0</v>
+      <c r="H10" s="9">
+        <v>0</v>
       </c>
       <c r="I10" s="11" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="J10" t="e" s="0">
+      <c r="J10" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="K10" t="e" s="0">
+      <c r="K10" t="e">
         <v>#NUM!</v>
       </c>
       <c r="L10" s="9" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="M10" t="n" s="0">
+      <c r="M10">
         <v>44.2</v>
       </c>
-      <c r="N10" t="n" s="0">
+      <c r="N10">
         <v>20.555555555555557</v>
       </c>
-      <c r="O10" t="n" s="0">
-        <v>20.22222222222222</v>
-      </c>
-      <c r="P10" s="6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q10" t="s" s="0">
+      <c r="O10">
+        <v>20.222222222222221</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="n">
-        <v>98.81481481481481</v>
-      </c>
-      <c r="B11" t="n" s="0">
-        <v>52.64150943396226</v>
-      </c>
-      <c r="C11" t="n" s="0">
-        <v>46.35849056603774</v>
-      </c>
-      <c r="D11" s="9" t="n">
-        <v>0.0</v>
+      <c r="A11" s="4">
+        <v>76.228571428571428</v>
+      </c>
+      <c r="B11">
+        <v>40.434782608695649</v>
+      </c>
+      <c r="C11">
+        <v>35.608695652173914</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
       </c>
       <c r="E11" s="11" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="F11" t="e" s="0">
+      <c r="F11" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G11" t="e" s="0">
+      <c r="G11" t="e">
         <v>#NUM!</v>
       </c>
       <c r="H11" s="9" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="I11" s="11" t="n">
-        <v>99.0</v>
-      </c>
-      <c r="J11" t="n" s="0">
-        <v>52.64150943396226</v>
-      </c>
-      <c r="K11" t="n" s="0">
-        <v>46.35849056603774</v>
-      </c>
-      <c r="L11" s="9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M11" t="n" s="0">
-        <v>89.0</v>
-      </c>
-      <c r="N11" t="e" s="0">
+      <c r="I11" s="11">
+        <v>76.043478260869563</v>
+      </c>
+      <c r="J11">
+        <v>40.434782608695649</v>
+      </c>
+      <c r="K11">
+        <v>35.608695652173914</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>89</v>
+      </c>
+      <c r="N11" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="O11" t="e" s="0">
+      <c r="O11" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="P11" s="6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q11" t="s" s="0">
+      <c r="P11" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="n">
-        <v>76.76190476190476</v>
-      </c>
-      <c r="B12" s="5" t="n">
+      <c r="A12" s="8">
+        <v>76.761904761904759</v>
+      </c>
+      <c r="B12" s="5">
         <v>45.8</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="5">
         <v>28.8</v>
       </c>
-      <c r="D12" s="10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E12" s="12" t="n">
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="12">
         <v>98.5</v>
       </c>
-      <c r="F12" s="5" t="n">
+      <c r="F12" s="5">
         <v>59.5</v>
       </c>
-      <c r="G12" s="5" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="H12" s="10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I12" s="12" t="n">
-        <v>65.0</v>
-      </c>
-      <c r="J12" s="5" t="n">
-        <v>57.0</v>
-      </c>
-      <c r="K12" s="5" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="L12" s="10" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M12" s="5" t="n">
+      <c r="G12" s="5">
+        <v>39</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12">
+        <v>65</v>
+      </c>
+      <c r="J12" s="5">
+        <v>57</v>
+      </c>
+      <c r="K12" s="5">
+        <v>8</v>
+      </c>
+      <c r="L12" s="10">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
         <v>62.666666666666664</v>
       </c>
-      <c r="N12" s="5" t="n">
+      <c r="N12" s="5">
         <v>26.5</v>
       </c>
-      <c r="O12" s="5" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="P12" s="7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q12" t="s" s="0">
+      <c r="O12" s="5">
+        <v>29</v>
+      </c>
+      <c r="P12" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" t="s" s="0">
+      <c r="A22" t="s">
         <v>38</v>
       </c>
-      <c r="E22" t="s" s="0">
+      <c r="E22" t="s">
         <v>39</v>
       </c>
-      <c r="I22" t="s" s="0">
+      <c r="I22" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" t="s" s="0">
+      <c r="A23" t="s">
         <v>10</v>
       </c>
-      <c r="B23" t="s" s="0">
+      <c r="B23" t="s">
         <v>5</v>
       </c>
-      <c r="C23" t="s" s="0">
+      <c r="C23" t="s">
         <v>1</v>
       </c>
-      <c r="E23" t="s" s="0">
+      <c r="E23" t="s">
         <v>10</v>
       </c>
-      <c r="F23" t="s" s="0">
+      <c r="F23" t="s">
         <v>5</v>
       </c>
-      <c r="G23" t="s" s="0">
+      <c r="G23" t="s">
         <v>1</v>
       </c>
-      <c r="I23" t="s" s="0">
+      <c r="I23" t="s">
         <v>10</v>
       </c>
-      <c r="J23" t="s" s="0">
+      <c r="J23" t="s">
         <v>5</v>
       </c>
-      <c r="K23" t="s" s="0">
+      <c r="K23" t="s">
         <v>1</v>
       </c>
     </row>
@@ -14041,7 +14041,7 @@
         <f>N6</f>
         <v>27.721477428199353</v>
       </c>
-      <c r="M24" t="s" s="0">
+      <c r="M24" t="s">
         <v>17</v>
       </c>
     </row>
@@ -14082,100 +14082,100 @@
         <f>O6</f>
         <v>28.413885088933256</v>
       </c>
-      <c r="M25" t="s" s="0">
+      <c r="M25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="0">
+      <c r="A27">
         <f>F10</f>
         <v>40.6</v>
       </c>
-      <c r="B27" t="e" s="0">
+      <c r="B27" t="e">
         <f>J10</f>
         <v>#NUM!</v>
       </c>
-      <c r="C27" s="0">
+      <c r="C27">
         <f>N10</f>
         <v>29.666666666666668</v>
       </c>
-      <c r="E27" t="e" s="0">
+      <c r="E27" t="e">
         <f>F11</f>
         <v>#NUM!</v>
       </c>
-      <c r="F27" s="0">
+      <c r="F27">
         <f>J11</f>
         <v>47.333333333333336</v>
       </c>
-      <c r="G27" t="e" s="0">
+      <c r="G27" t="e">
         <f>N11</f>
         <v>#NUM!</v>
       </c>
-      <c r="I27" t="e" s="0">
+      <c r="I27" t="e">
         <f>F12</f>
         <v>#NUM!</v>
       </c>
-      <c r="J27" t="e" s="0">
+      <c r="J27" t="e">
         <f>J12</f>
         <v>#NUM!</v>
       </c>
-      <c r="K27" s="0">
+      <c r="K27">
         <f>N12</f>
         <v>26.5</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="0">
+      <c r="A28">
         <f>G10</f>
         <v>18.600000000000001</v>
       </c>
-      <c r="B28" t="e" s="0">
+      <c r="B28" t="e">
         <f>K10</f>
         <v>#NUM!</v>
       </c>
-      <c r="C28" s="0">
+      <c r="C28">
         <f>O10</f>
         <v>27.666666666666668</v>
       </c>
-      <c r="E28" t="e" s="0">
+      <c r="E28" t="e">
         <f>G11</f>
         <v>#NUM!</v>
       </c>
-      <c r="F28" s="0">
+      <c r="F28">
         <f>K11</f>
         <v>41</v>
       </c>
-      <c r="G28" t="e" s="0">
+      <c r="G28" t="e">
         <f>O11</f>
         <v>#NUM!</v>
       </c>
-      <c r="I28" t="e" s="0">
+      <c r="I28" t="e">
         <f>G12</f>
         <v>#NUM!</v>
       </c>
-      <c r="J28" t="e" s="0">
+      <c r="J28" t="e">
         <f>K12</f>
         <v>#NUM!</v>
       </c>
-      <c r="K28" s="0">
+      <c r="K28">
         <f>O12</f>
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="Y2:AB2"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="M2:P2"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A7:P7"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="I8:L8"/>
     <mergeCell ref="M8:P8"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="Y2:AB2"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="M2:P2"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:A6">
     <cfRule type="colorScale" priority="11">
@@ -14259,7 +14259,103 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 I4 M4">
+  <conditionalFormatting sqref="E5 I5 M5">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11 I11 M11">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4 J4 N4">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6 J6 N6">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10 J10 N10">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12 J12 N12">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5 K5 O5">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11 K11 O11">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 E4 M4">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -14271,7 +14367,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6 I6 M6">
+  <conditionalFormatting sqref="I6 E6 M6">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -14283,7 +14379,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10 I10 M10">
+  <conditionalFormatting sqref="I10 E10 M10">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -14295,7 +14391,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12 I12 M12">
+  <conditionalFormatting sqref="I12 E12 M12">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -14307,7 +14403,55 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5 N5 J5">
+  <conditionalFormatting sqref="J11 F11 N11">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6 G6 O6">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10 G10 O10">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12 G12 O12">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5 F5 J5">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -14319,152 +14463,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11 J11 N11">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4 O4 K4">
+  <conditionalFormatting sqref="O4 G4 K4">
     <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6 K6 O6">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G10 K10 O10">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12 K12 O12">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5 E5 M5">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11 E11 M11">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4 F4 N4">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J6 F6 N6">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10 F10 N10">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J12 F12 N12">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K5 G5 O5">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11 G11 O11">
-    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Fixed the issue with averages changing, it was pulling in the matches each time without erasing the old matches, stacking them up over time.
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3085CBA-D30F-4756-9846-A3D9B6F45B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7543573F-D8AE-40C6-B1AA-D65ED048A9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
   <sheets>
     <sheet name="Match Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="45">
   <si>
     <t>Cyrus</t>
   </si>
@@ -174,7 +174,7 @@
     <t>Auto</t>
   </si>
   <si>
-    <t>Added 30 points for an assumed good airplane; kept only 5 for parking, no hang</t>
+    <t>Added 20 points for an assumed average airplane; kept only 5 for parking, no hang</t>
   </si>
 </sst>
 </file>
@@ -571,6 +571,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,22 +595,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1293,13 +1293,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>38.764560098463484</c:v>
+                  <c:v>36.550387596685354</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.446030330182737</c:v>
+                  <c:v>28.46172763642895</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.088888887808729</c:v>
+                  <c:v>41.264406779346508</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1408,13 +1408,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20.939281288620293</c:v>
+                  <c:v>24.964341084739846</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.263157894769414</c:v>
+                  <c:v>28.399938518511142</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.755555555566744</c:v>
+                  <c:v>29.450847457615403</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1804,13 +1804,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>40.453142226693487</c:v>
+                  <c:v>38.010101010074557</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.099142040113222</c:v>
+                  <c:v>25.978370027409998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48.273972601126175</c:v>
+                  <c:v>41.664285713072118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1919,13 +1919,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>21.082690187258262</c:v>
+                  <c:v>28.113442112952178</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.967588179361691</c:v>
+                  <c:v>27.387022016561566</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.698630136977371</c:v>
+                  <c:v>28.699999999990283</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2315,13 +2315,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>48.061403507588622</c:v>
+                  <c:v>40.709821428407864</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.099551569560809</c:v>
+                  <c:v>28.034216706101521</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.261744966510754</c:v>
+                  <c:v>33.58526315763708</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2430,13 +2430,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>26.390350876438607</c:v>
+                  <c:v>28.529017856603677</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.371300448591789</c:v>
+                  <c:v>26.785977860076873</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.067114094025488</c:v>
+                  <c:v>29.861052631104354</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2825,13 +2825,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>39.608851162578489</c:v>
+                  <c:v>37.280244303379959</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.272586185147979</c:v>
+                  <c:v>27.220048831919474</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49.181430744467448</c:v>
+                  <c:v>41.464346246209317</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2940,13 +2940,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>21.010985737939279</c:v>
+                  <c:v>26.538891598846014</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.615373037065552</c:v>
+                  <c:v>27.893480267536354</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.727092846272058</c:v>
+                  <c:v>29.075423728802843</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4338,13 +4338,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>38.073170731707314</c:v>
+                  <c:v>36.578947368421055</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.434782608695649</c:v>
+                  <c:v>44.339622641509436</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.8</c:v>
+                  <c:v>39.799999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4453,10 +4453,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>19.951219512195124</c:v>
+                  <c:v>22.982456140350877</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.608695652173914</c:v>
+                  <c:v>46.358490566037737</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>28.8</c:v>
@@ -10781,16 +10781,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
-  <dimension ref="A1:Y48"/>
+  <dimension ref="A1:Y58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView topLeftCell="A42" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="10.0"/>
+    <col min="5" max="5" customWidth="true" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -10823,31 +10823,31 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>45237</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>106</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>-1</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0">
         <v>-1</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>0</v>
       </c>
       <c r="M2" s="2"/>
@@ -10860,721 +10860,721 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>45237</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>83</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>-1</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0">
         <v>-1</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>45237</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>89</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>-1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0">
         <v>-1</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>0</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>45238</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>71</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>-1</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0">
         <v>-1</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>45238</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>88</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>-1</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0">
         <v>-1</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>45238</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>111</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>-1</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0">
         <v>-1</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>45238</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>34</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>-1</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="0">
         <v>-1</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>45238</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>120</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>-1</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="0">
         <v>-1</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="0">
         <v>0</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>45238</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="0">
         <v>75</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="0">
         <v>-1</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="0">
         <v>-1</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>45237</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="0">
         <v>111</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="0">
         <v>66</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="0">
         <v>45</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>45238</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="0">
         <v>107</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="0">
         <v>57</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="0">
         <v>50</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="0">
         <v>0</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>45234</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>72</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="0">
         <v>44</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0">
         <v>28</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B14" s="1">
         <v>45234</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0">
         <v>97</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="0">
         <v>51</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="0">
         <v>30</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="0">
         <v>0</v>
       </c>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B15" s="1">
         <v>45234</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>54</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="0">
         <v>26</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="0">
         <v>28</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>45234</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>82</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="0">
         <v>32</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="0">
         <v>50</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>45234</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>60</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="0">
         <v>40</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="0">
         <v>20</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>45234</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>56</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="0">
         <v>48</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0">
         <v>8</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>45234</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>60</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="0">
         <v>30</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0">
         <v>30</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>45234</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>39</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="0">
         <v>34</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0">
         <v>5</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>45241</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="0">
         <v>32</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="0">
         <v>4</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="0">
         <v>28</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="0">
         <v>0</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" t="s" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>45241</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="0">
         <v>83</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="0">
         <v>55</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="0">
         <v>28</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="0">
         <v>0</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" t="s" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>45241</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>56</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="0">
         <v>26</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="0">
         <v>30</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="0">
         <v>0</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" t="s" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>45241</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="0">
         <v>33</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="0">
         <v>28</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="0">
         <v>5</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="0">
         <v>0</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" t="s" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>45241</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="0">
         <v>56</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="0">
         <v>36</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="0">
         <v>20</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="0">
         <v>0</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" t="s" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>31</v>
       </c>
       <c r="B26" s="1">
         <v>45241</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="0">
         <v>55</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="0">
         <v>27</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="0">
         <v>28</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="0">
         <v>0</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" t="s" s="0">
         <v>33</v>
       </c>
       <c r="T26" s="33"/>
@@ -11585,121 +11585,121 @@
       <c r="Y26" s="2"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B27" s="1">
         <v>45255</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" t="s" s="0">
         <v>10</v>
       </c>
       <c r="F27" s="22">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="G27" s="22">
-        <v>45</v>
-      </c>
-      <c r="H27">
+        <v>35</v>
+      </c>
+      <c r="H27" s="0">
         <v>30</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="0">
         <v>0</v>
       </c>
       <c r="L27" s="22"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B28" s="1">
         <v>45255</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" t="s" s="0">
         <v>10</v>
       </c>
       <c r="F28" s="22">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G28" s="22">
-        <v>42</v>
-      </c>
-      <c r="H28">
+        <v>32</v>
+      </c>
+      <c r="H28" s="0">
         <v>8</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="0">
         <v>0</v>
       </c>
       <c r="L28" s="22"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B29" s="1">
         <v>45255</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" t="s" s="0">
         <v>10</v>
       </c>
       <c r="F29" s="22">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="G29" s="22">
-        <v>54</v>
-      </c>
-      <c r="H29">
+        <v>44</v>
+      </c>
+      <c r="H29" s="0">
         <v>28</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="0">
         <v>0</v>
       </c>
       <c r="L29" s="22"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B30" s="1">
         <v>45256</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" t="s" s="0">
         <v>10</v>
       </c>
       <c r="F30" s="22">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G30" s="22">
-        <v>62</v>
-      </c>
-      <c r="H30">
+        <v>52</v>
+      </c>
+      <c r="H30" s="0">
         <v>50</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="0">
         <v>0</v>
       </c>
       <c r="L30" s="22" t="s">
@@ -11707,31 +11707,31 @@
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>45256</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" t="s" s="0">
         <v>5</v>
       </c>
       <c r="F31" s="22">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G31" s="22">
-        <v>57</v>
-      </c>
-      <c r="H31">
+        <v>47</v>
+      </c>
+      <c r="H31" s="0">
         <v>8</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="0">
         <v>0</v>
       </c>
       <c r="L31" s="22"/>
@@ -11741,379 +11741,747 @@
       <c r="W31" s="34"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B32" s="1">
         <v>45256</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" t="s" s="0">
         <v>10</v>
       </c>
       <c r="F32" s="22">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="G32" s="22">
-        <v>57</v>
-      </c>
-      <c r="H32">
+        <v>47</v>
+      </c>
+      <c r="H32" s="0">
         <v>28</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="0">
         <v>0</v>
       </c>
       <c r="L32" s="22"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B33" s="1">
         <v>45256</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" t="s" s="0">
         <v>5</v>
       </c>
       <c r="F33" s="22">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="G33" s="22">
-        <v>45</v>
-      </c>
-      <c r="H33">
+        <v>35</v>
+      </c>
+      <c r="H33" s="0">
         <v>50</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="0">
         <v>0</v>
       </c>
       <c r="L33" s="22"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B34" s="1">
         <v>45256</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" t="s" s="0">
         <v>5</v>
       </c>
       <c r="F34" s="22">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="G34" s="22">
-        <v>45</v>
-      </c>
-      <c r="H34">
+        <v>35</v>
+      </c>
+      <c r="H34" s="0">
         <v>50</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="0">
         <v>0</v>
       </c>
       <c r="L34" s="22"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B35" s="1">
         <v>45256</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" t="s" s="0">
         <v>5</v>
       </c>
       <c r="F35" s="22">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G35" s="22">
-        <v>60</v>
-      </c>
-      <c r="H35">
         <v>50</v>
       </c>
-      <c r="I35">
+      <c r="H35" s="0">
+        <v>50</v>
+      </c>
+      <c r="I35" s="0">
         <v>0</v>
       </c>
       <c r="L35" s="22"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B36" s="1">
         <v>45256</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" t="s" s="0">
         <v>5</v>
       </c>
       <c r="F36" s="22">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G36" s="22">
-        <v>59</v>
-      </c>
-      <c r="H36">
+        <v>49</v>
+      </c>
+      <c r="H36" s="0">
         <v>50</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="0">
         <v>0</v>
       </c>
       <c r="L36" s="22"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B37" s="1">
         <v>45256</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" t="s" s="0">
         <v>5</v>
       </c>
       <c r="F37" s="22">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="G37" s="22">
-        <v>57</v>
-      </c>
-      <c r="H37">
+        <v>47</v>
+      </c>
+      <c r="H37" s="0">
         <v>50</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="0">
         <v>0</v>
       </c>
       <c r="L37" s="22"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B38" s="1">
         <v>45256</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" t="s" s="0">
         <v>5</v>
       </c>
       <c r="F38" s="22">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G38" s="22">
-        <v>47</v>
-      </c>
-      <c r="H38">
+        <v>37</v>
+      </c>
+      <c r="H38" s="0">
         <v>50</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="0">
         <v>0</v>
       </c>
       <c r="L38" s="22"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B39" s="1">
         <v>45256</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" t="s" s="0">
         <v>5</v>
       </c>
       <c r="F39" s="22">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="G39" s="22">
-        <v>51</v>
-      </c>
-      <c r="H39">
+        <v>41</v>
+      </c>
+      <c r="H39" s="0">
         <v>50</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="0">
         <v>0</v>
       </c>
       <c r="L39" s="22"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B40" s="1">
         <v>45256</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" t="s" s="0">
         <v>5</v>
       </c>
       <c r="F40" s="22">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="G40" s="22">
-        <v>43</v>
-      </c>
-      <c r="H40">
+        <v>33</v>
+      </c>
+      <c r="H40" s="0">
         <v>45</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="0">
         <v>0</v>
       </c>
       <c r="L40" s="22"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B41" s="1">
         <v>45256</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" t="s" s="0">
         <v>5</v>
       </c>
       <c r="F41" s="22">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="G41" s="22">
-        <v>75</v>
-      </c>
-      <c r="H41">
+        <v>65</v>
+      </c>
+      <c r="H41" s="0">
         <v>50</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="0">
         <v>0</v>
       </c>
       <c r="L41" s="22"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B42" s="1">
         <v>45256</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" t="s" s="0">
         <v>5</v>
       </c>
       <c r="F42" s="22">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G42" s="22">
-        <v>70</v>
-      </c>
-      <c r="H42">
+        <v>60</v>
+      </c>
+      <c r="H42" s="0">
         <v>30</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="0">
         <v>0</v>
       </c>
       <c r="L42" s="22"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" t="s" s="0">
         <v>30</v>
       </c>
       <c r="B43" s="1">
         <v>45256</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" t="s" s="0">
         <v>5</v>
       </c>
       <c r="F43" s="22">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="G43" s="22">
+        <v>43</v>
+      </c>
+      <c r="H43" s="0">
+        <v>50</v>
+      </c>
+      <c r="I43" s="0">
+        <v>0</v>
+      </c>
+      <c r="L43" s="22"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B44" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F44" s="0">
+        <v>42</v>
+      </c>
+      <c r="G44" s="0">
+        <v>12</v>
+      </c>
+      <c r="H44" s="0">
+        <v>30</v>
+      </c>
+      <c r="I44" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B45" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F45" s="0">
+        <v>85</v>
+      </c>
+      <c r="G45" s="0">
+        <v>52</v>
+      </c>
+      <c r="H45" s="0">
+        <v>33</v>
+      </c>
+      <c r="I45" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B46" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E46" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="F46" s="0">
+        <v>70</v>
+      </c>
+      <c r="G46" s="0">
+        <v>42</v>
+      </c>
+      <c r="H46" s="0">
+        <v>28</v>
+      </c>
+      <c r="I46" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B47" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="F47" s="0">
+        <v>44</v>
+      </c>
+      <c r="G47" s="0">
+        <v>14</v>
+      </c>
+      <c r="H47" s="0">
+        <v>30</v>
+      </c>
+      <c r="I47" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B48" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E48" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="F48" s="0">
+        <v>72</v>
+      </c>
+      <c r="G48" s="0">
+        <v>42</v>
+      </c>
+      <c r="H48" s="0">
+        <v>30</v>
+      </c>
+      <c r="I48" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B49" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="F49" s="0">
+        <v>97</v>
+      </c>
+      <c r="G49" s="0">
+        <v>47</v>
+      </c>
+      <c r="H49" s="0">
+        <v>50</v>
+      </c>
+      <c r="I49" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B50" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E50" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F50" s="0">
+        <v>104</v>
+      </c>
+      <c r="G50" s="0">
+        <v>54</v>
+      </c>
+      <c r="H50" s="0">
+        <v>50</v>
+      </c>
+      <c r="I50" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B51" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E51" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="F51" s="0">
+        <v>34</v>
+      </c>
+      <c r="G51" s="0">
+        <v>24</v>
+      </c>
+      <c r="H51" s="0">
+        <v>10</v>
+      </c>
+      <c r="I51" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B52" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E52" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F52" s="0">
+        <v>104</v>
+      </c>
+      <c r="G52" s="0">
+        <v>74</v>
+      </c>
+      <c r="H52" s="0">
+        <v>30</v>
+      </c>
+      <c r="I52" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B53" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E53" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F53" s="0">
         <v>53</v>
       </c>
-      <c r="H43">
+      <c r="G53" s="0">
+        <v>23</v>
+      </c>
+      <c r="H53" s="0">
+        <v>30</v>
+      </c>
+      <c r="I53" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B54" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D54" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E54" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F54" s="0">
+        <v>80</v>
+      </c>
+      <c r="G54" s="0">
         <v>50</v>
       </c>
-      <c r="I43">
+      <c r="H54" s="0">
+        <v>30</v>
+      </c>
+      <c r="I54" s="0">
         <v>0</v>
       </c>
-      <c r="L43" s="22"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B48" s="1"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B55" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E55" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F55" s="0">
+        <v>66</v>
+      </c>
+      <c r="G55" s="0">
+        <v>36</v>
+      </c>
+      <c r="H55" s="0">
+        <v>30</v>
+      </c>
+      <c r="I55" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B56" s="1">
+        <v>45257</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D56" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E56" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F56" s="0">
+        <v>66</v>
+      </c>
+      <c r="G56" s="0">
+        <v>36</v>
+      </c>
+      <c r="H56" s="0">
+        <v>30</v>
+      </c>
+      <c r="I56" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B58" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -12135,8 +12503,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="10.0"/>
+    <col min="5" max="5" customWidth="true" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -12168,7 +12536,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="V2" t="s">
+      <c r="V2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
@@ -12176,16 +12544,16 @@
       <c r="A3" s="1">
         <v>45237</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>106</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -12193,25 +12561,25 @@
       <c r="A4" s="1">
         <v>45237</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>83</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" t="s" s="0">
         <v>24</v>
       </c>
     </row>
@@ -12219,26 +12587,26 @@
       <c r="A5" s="1">
         <v>45237</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>89</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="0">
         <f>(SUMIF($C$3:$C$100, M5, $B$3:$B$100)/COUNTIF($C$3:$C$100, M5))</f>
         <v>88.083333333333329</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="0">
         <f>(SUMIF($C$3:$C$100, M5, $F$3:$F$100)/COUNTIF($C$13:$C$100, M5))</f>
         <v>42.428571428571431</v>
       </c>
@@ -12247,26 +12615,26 @@
       <c r="A6" s="1">
         <v>45238</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>71</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="0">
         <f>(SUMIF($C$3:$C$100, M6, $B$3:$B$100)/COUNTIF($C$3:$C$100, M6))</f>
         <v>98.5</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="0">
         <f>(SUMIF($C$3:$C$100, M6, $F$3:$F$100)/COUNTIF($C$13:$C$100, M6))</f>
         <v>57.333333333333336</v>
       </c>
@@ -12275,26 +12643,26 @@
       <c r="A7" s="1">
         <v>45238</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>88</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="0">
         <f>(SUMIF($C$3:$C$100, M7, $B$3:$B$100)/COUNTIF($C$3:$C$100, M7))</f>
         <v>86.25</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="0">
         <f>(SUMIF($C$3:$C$100, M7, $F$3:$F$100)/COUNTIF($C$13:$C$100, M7))</f>
         <v>38</v>
       </c>
@@ -12303,16 +12671,16 @@
       <c r="A8" s="1">
         <v>45238</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>111</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -12320,16 +12688,16 @@
       <c r="A9" s="1">
         <v>45238</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="s" s="0">
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -12340,16 +12708,16 @@
       <c r="A10" s="1">
         <v>45238</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <v>120</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="s" s="0">
         <v>1</v>
       </c>
       <c r="H10" s="33" t="s">
@@ -12358,14 +12726,14 @@
       <c r="I10" s="33"/>
       <c r="J10" s="33"/>
       <c r="K10" s="33"/>
-      <c r="M10" t="s">
+      <c r="M10" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="0">
         <f>(SUMIF($D$3:$D$100, M10, $B$3:$B$100)/COUNTIF($D$3:$D$100, M10))</f>
         <v>96.666666666666671</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="0">
         <f>(SUMIF($D$3:$D$100, M10, $F$3:$F$100)/COUNTIF($D$13:$D$100, M10))</f>
         <v>26</v>
       </c>
@@ -12374,16 +12742,16 @@
       <c r="A11" s="1">
         <v>45238</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0">
         <v>75</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="s" s="0">
         <v>1</v>
       </c>
       <c r="H11" s="33" t="s">
@@ -12394,14 +12762,14 @@
         <v>22</v>
       </c>
       <c r="K11" s="33"/>
-      <c r="M11" t="s">
+      <c r="M11" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="0">
         <f>(SUMIF($D$3:$D$100, M11, $B$3:$B$100)/COUNTIF($D$3:$D$100, M11))</f>
         <v>77</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="0">
         <f>(SUMIF($D$3:$D$100, M11, $F$3:$F$100)/COUNTIF($D$13:$D$100, M11))</f>
         <v>45.166666666666664</v>
       </c>
@@ -12419,14 +12787,14 @@
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="0">
         <f>(SUMIF($D$3:$D$100, M12, $B$3:$B$100)/COUNTIF($D$3:$D$100, M12))</f>
         <v>97.75</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="0">
         <f>(SUMIF($D$3:$D$100, M12, $F$3:$F$100)/COUNTIF($D$13:$D$100, M12))</f>
         <v>57.333333333333336</v>
       </c>
@@ -12435,26 +12803,26 @@
       <c r="A13" s="1">
         <v>45237</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="0">
         <v>111</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>66</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="0">
         <f t="shared" ref="H13:H23" si="0">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12)+SUMIF($M$15:$M$17, $E13, $N$15:$N$17))/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="0">
         <f t="shared" ref="I13:I23" si="1">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12)+SUMIF($M$15:$M$17, $E13, $O$15:$O$17))/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -12462,7 +12830,7 @@
         <f t="shared" ref="J13:J23" si="2">(SUMIF($M$5:$M$7, $C13, $N$5:$N$7)+SUMIF($M$10:$M$12, $D13, $N$10:$N$12))/2</f>
         <v>98.125</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="0">
         <f t="shared" ref="K13:K23" si="3">(SUMIF($M$5:$M$7, $C13, $O$5:$O$7)+SUMIF($M$10:$M$12, $D13, $O$10:$O$12))/2</f>
         <v>57.333333333333336</v>
       </c>
@@ -12471,26 +12839,26 @@
       <c r="A14" s="1">
         <v>45238</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="0">
         <v>107</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0">
         <v>57</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="0">
         <f t="shared" si="0"/>
         <v>84.49444444444444</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="0">
         <f t="shared" si="1"/>
         <v>48.198412698412703</v>
       </c>
@@ -12498,7 +12866,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -12510,26 +12878,26 @@
       <c r="A15" s="1">
         <v>45234</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="0">
         <v>108</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>38</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="0">
         <f t="shared" si="0"/>
         <v>63.166666666666664</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="0">
         <f t="shared" si="1"/>
         <v>30.166666666666668</v>
       </c>
@@ -12537,18 +12905,18 @@
         <f t="shared" si="2"/>
         <v>43.125</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="0">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="0">
         <f>(SUMIF($E$3:$E$100, M15, $B$3:$B$100)/COUNTIF($E$3:$E$100, M15))</f>
         <v>83.166666666666671</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="0">
         <f>(SUMIF($E$3:$E$100, M15, $F$3:$F$100)/COUNTIF($E$13:$E$100, M15))</f>
         <v>40</v>
       </c>
@@ -12557,26 +12925,26 @@
       <c r="A16" s="1">
         <v>45234</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="0">
         <v>107</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>74</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="0">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="0">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -12584,18 +12952,18 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="0">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="0">
         <f>(SUMIF($E$3:$E$100, M16, $B$3:$B$100)/COUNTIF($E$3:$E$100, M16))</f>
         <v>88.4</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="0">
         <f>(SUMIF($E$3:$E$100, M16, $F$3:$F$100)/COUNTIF($E$13:$E$100, M16))</f>
         <v>57</v>
       </c>
@@ -12604,26 +12972,26 @@
       <c r="A17" s="1">
         <v>45234</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="0">
         <v>97</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>62</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -12631,18 +12999,18 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="0">
         <f>(SUMIF($E$3:$E$100, M17, $B$3:$B$100)/COUNTIF($E$3:$E$100, M17))</f>
         <v>103.25</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="0">
         <f>(SUMIF($E$3:$E$100, M17, $F$3:$F$100)/COUNTIF($E$13:$E$100, M17))</f>
         <v>52.5</v>
       </c>
@@ -12651,26 +13019,26 @@
       <c r="A18" s="1">
         <v>45234</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="0">
         <v>99</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>26</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0">
         <f t="shared" si="0"/>
         <v>89.305555555555557</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="0">
         <f t="shared" si="1"/>
         <v>36.142857142857146</v>
       </c>
@@ -12678,7 +13046,7 @@
         <f t="shared" si="2"/>
         <v>92.375</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="0">
         <f t="shared" si="3"/>
         <v>34.214285714285715</v>
       </c>
@@ -12687,26 +13055,26 @@
       <c r="A19" s="1">
         <v>45234</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="0">
         <v>87</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>32</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0">
         <f t="shared" si="0"/>
         <v>99.833333333333329</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="0">
         <f t="shared" si="1"/>
         <v>55.722222222222229</v>
       </c>
@@ -12714,7 +13082,7 @@
         <f t="shared" si="2"/>
         <v>98.125</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="0">
         <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
@@ -12723,26 +13091,26 @@
       <c r="A20" s="1">
         <v>45234</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="0">
         <v>76</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>48</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -12750,7 +13118,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -12759,26 +13127,26 @@
       <c r="A21" s="1">
         <v>45234</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="0">
         <v>93</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="0">
         <v>40</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -12786,7 +13154,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -12795,26 +13163,26 @@
       <c r="A22" s="1">
         <v>45234</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="0">
         <v>85</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="0">
         <v>30</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -12822,7 +13190,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -12831,26 +13199,26 @@
       <c r="A23" s="1">
         <v>45234</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="0">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>34</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="0">
         <f t="shared" si="0"/>
         <v>82.75</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="0">
         <f t="shared" si="1"/>
         <v>42.531746031746032</v>
       </c>
@@ -12858,7 +13226,7 @@
         <f t="shared" si="2"/>
         <v>82.541666666666657</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="0">
         <f t="shared" si="3"/>
         <v>43.797619047619051</v>
       </c>
@@ -12878,67 +13246,67 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T28">
+      <c r="T28" s="0">
         <v>1</v>
       </c>
-      <c r="U28" t="s">
+      <c r="U28" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="V28" t="s">
+      <c r="V28" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="W28" t="s">
+      <c r="W28" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X28">
+      <c r="X28" s="0">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y28">
+      <c r="Y28" s="0">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T29">
+      <c r="T29" s="0">
         <v>2</v>
       </c>
-      <c r="U29" t="s">
+      <c r="U29" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="V29" t="s">
+      <c r="V29" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W29" t="s">
+      <c r="W29" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X29">
+      <c r="X29" s="0">
         <f>(N5+N11+N16)/3</f>
         <v>84.49444444444444</v>
       </c>
-      <c r="Y29">
+      <c r="Y29" s="0">
         <f>(O5+O11+O16)/3</f>
         <v>48.198412698412703</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="T30">
+      <c r="T30" s="0">
         <v>3</v>
       </c>
-      <c r="U30" t="s">
+      <c r="U30" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="V30" t="s">
+      <c r="V30" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W30" t="s">
+      <c r="W30" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X30">
+      <c r="X30" s="0">
         <f>(N6+N11+N16)/3</f>
         <v>87.966666666666654</v>
       </c>
-      <c r="Y30">
+      <c r="Y30" s="0">
         <f>(O6+O11+O16)/3</f>
         <v>53.166666666666664</v>
       </c>
@@ -12952,67 +13320,67 @@
       <c r="W32" s="33"/>
     </row>
     <row r="33" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T33">
+      <c r="T33" s="0">
         <v>1</v>
       </c>
-      <c r="U33" t="s">
+      <c r="U33" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="V33" t="s">
+      <c r="V33" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="W33" t="s">
+      <c r="W33" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="X33">
+      <c r="X33" s="0">
         <f>(N7+N10+N16)/3</f>
         <v>90.438888888888911</v>
       </c>
-      <c r="Y33">
+      <c r="Y33" s="0">
         <f>(O7+O10+O16)/3</f>
         <v>40.333333333333336</v>
       </c>
     </row>
     <row r="34" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T34">
+      <c r="T34" s="0">
         <v>2</v>
       </c>
-      <c r="U34" t="s">
+      <c r="U34" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="V34" t="s">
+      <c r="V34" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="W34" t="s">
+      <c r="W34" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="X34">
+      <c r="X34" s="0">
         <f>(N5+N11+N15)/3</f>
         <v>82.75</v>
       </c>
-      <c r="Y34">
+      <c r="Y34" s="0">
         <f>(O5+O11+O15)/3</f>
         <v>42.531746031746032</v>
       </c>
     </row>
     <row r="35" spans="20:25" x14ac:dyDescent="0.3">
-      <c r="T35">
+      <c r="T35" s="0">
         <v>3</v>
       </c>
-      <c r="U35" t="s">
+      <c r="U35" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="V35" t="s">
+      <c r="V35" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="W35" t="s">
+      <c r="W35" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="X35">
+      <c r="X35" s="0">
         <f>(N6+N12+N17)/3</f>
         <v>99.833333333333329</v>
       </c>
-      <c r="Y35">
+      <c r="Y35" s="0">
         <f>(O6+O12+O17)/3</f>
         <v>55.722222222222229</v>
       </c>
@@ -13035,8 +13403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13069,160 +13437,160 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="23">
-        <v>63.046538024644882</v>
-      </c>
-      <c r="B3" s="26">
-        <v>38.764560098463484</v>
-      </c>
-      <c r="C3" s="26">
-        <v>20.939281288620293</v>
-      </c>
-      <c r="D3" s="23">
-        <v>0</v>
+      <c r="A3" s="23" t="n">
+        <v>63.43046357585669</v>
+      </c>
+      <c r="B3" s="26" t="n">
+        <v>36.550387596685354</v>
+      </c>
+      <c r="C3" s="26" t="n">
+        <v>24.964341084739846</v>
+      </c>
+      <c r="D3" s="23" t="n">
+        <v>2.913907284406357</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="29">
-        <v>74.797872340599682</v>
-      </c>
-      <c r="B4" s="30">
-        <v>40.446030330182737</v>
-      </c>
-      <c r="C4" s="30">
-        <v>34.263157894769414</v>
-      </c>
-      <c r="D4" s="29">
-        <v>0</v>
+      <c r="A4" s="29" t="n">
+        <v>85.45821854887244</v>
+      </c>
+      <c r="B4" s="30" t="n">
+        <v>42.76489607390647</v>
+      </c>
+      <c r="C4" s="30" t="n">
+        <v>42.672055426985544</v>
+      </c>
+      <c r="D4" s="29" t="n">
+        <v>0.6060606060378997</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="31">
-        <v>78.849315067508854</v>
-      </c>
-      <c r="B5" s="32">
-        <v>50.088888887808729</v>
-      </c>
-      <c r="C5" s="32">
-        <v>28.755555555566744</v>
-      </c>
-      <c r="D5" s="31">
-        <v>0</v>
+      <c r="A5" s="31" t="n">
+        <v>70.99017198992931</v>
+      </c>
+      <c r="B5" s="32" t="n">
+        <v>41.26440677934651</v>
+      </c>
+      <c r="C5" s="32" t="n">
+        <v>29.450847457615403</v>
+      </c>
+      <c r="D5" s="31" t="n">
+        <v>0.0</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="23">
-        <v>62.061899679414424</v>
-      </c>
-      <c r="B6" s="26">
-        <v>40.453142226693487</v>
-      </c>
-      <c r="C6" s="26">
-        <v>21.082690187258262</v>
-      </c>
-      <c r="D6" s="23">
-        <v>0</v>
+      <c r="A6" s="23" t="n">
+        <v>66.24442736312962</v>
+      </c>
+      <c r="B6" s="26" t="n">
+        <v>38.01010101007456</v>
+      </c>
+      <c r="C6" s="26" t="n">
+        <v>28.11344211295218</v>
+      </c>
+      <c r="D6" s="23" t="n">
+        <v>2.0292083011786106</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="29">
-        <v>75.74516129069508</v>
-      </c>
-      <c r="B7" s="30">
-        <v>40.099142040113222</v>
-      </c>
-      <c r="C7" s="30">
-        <v>34.967588179361691</v>
-      </c>
-      <c r="D7" s="29">
-        <v>0</v>
+      <c r="A7" s="29" t="n">
+        <v>92.19579081605175</v>
+      </c>
+      <c r="B7" s="30" t="n">
+        <v>44.808794137129176</v>
+      </c>
+      <c r="C7" s="30" t="n">
+        <v>47.238507661347654</v>
+      </c>
+      <c r="D7" s="29" t="n">
+        <v>0.0</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="31">
-        <v>77.877850161472978</v>
-      </c>
-      <c r="B8" s="32">
-        <v>48.273972601126175</v>
-      </c>
-      <c r="C8" s="32">
-        <v>28.698630136977371</v>
-      </c>
-      <c r="D8" s="31">
-        <v>0</v>
+      <c r="A8" s="31" t="n">
+        <v>71.56122448885235</v>
+      </c>
+      <c r="B8" s="32" t="n">
+        <v>41.66428571307212</v>
+      </c>
+      <c r="C8" s="32" t="n">
+        <v>28.699999999990283</v>
+      </c>
+      <c r="D8" s="31" t="n">
+        <v>0.0</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="23">
-        <v>75.223684208812571</v>
-      </c>
-      <c r="B9" s="26">
-        <v>48.061403507588622</v>
-      </c>
-      <c r="C9" s="26">
-        <v>26.390350876438607</v>
-      </c>
-      <c r="D9" s="23">
-        <v>0</v>
+      <c r="A9" s="23" t="n">
+        <v>69.5959821422997</v>
+      </c>
+      <c r="B9" s="26" t="n">
+        <v>40.709821428407864</v>
+      </c>
+      <c r="C9" s="26" t="n">
+        <v>28.529017856603677</v>
+      </c>
+      <c r="D9" s="23" t="n">
+        <v>2.2098214284230315</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="29">
-        <v>74.470852018152613</v>
-      </c>
-      <c r="B10" s="30">
-        <v>41.099551569560809</v>
-      </c>
-      <c r="C10" s="30">
-        <v>33.371300448591789</v>
-      </c>
-      <c r="D10" s="29">
-        <v>0</v>
+      <c r="A10" s="29" t="n">
+        <v>86.3280507130376</v>
+      </c>
+      <c r="B10" s="30" t="n">
+        <v>44.146856840922915</v>
+      </c>
+      <c r="C10" s="30" t="n">
+        <v>42.18119387211468</v>
+      </c>
+      <c r="D10" s="29" t="n">
+        <v>0.0</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="27">
-        <v>61.592400691431862</v>
-      </c>
-      <c r="B11" s="28">
-        <v>30.261744966510754</v>
-      </c>
-      <c r="C11" s="28">
-        <v>24.067114094025488</v>
-      </c>
-      <c r="D11" s="27">
-        <v>0</v>
+      <c r="A11" s="27" t="n">
+        <v>66.052190120987</v>
+      </c>
+      <c r="B11" s="28" t="n">
+        <v>33.58526315763708</v>
+      </c>
+      <c r="C11" s="28" t="n">
+        <v>29.861052631104354</v>
+      </c>
+      <c r="D11" s="27" t="n">
+        <v>1.2301957128180179</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>35</v>
       </c>
     </row>
@@ -13388,35 +13756,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" bestFit="true" customWidth="true" width="9.5546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0"/>
+    <col min="5" max="7" bestFit="true" customWidth="true" width="9.5546875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.0"/>
+    <col min="9" max="11" bestFit="true" customWidth="true" width="9.5546875"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.0"/>
+    <col min="13" max="15" bestFit="true" customWidth="true" width="9.5546875"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="9.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="38"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="42"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
@@ -13467,30 +13835,30 @@
       <c r="BL1" s="2"/>
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="43" t="s">
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="41" t="s">
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="46"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="40"/>
       <c r="Y2" s="33"/>
       <c r="Z2" s="33"/>
       <c r="AA2" s="33"/>
@@ -13501,13 +13869,13 @@
       <c r="AF2" s="33"/>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>28</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -13516,10 +13884,10 @@
       <c r="E3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>28</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -13528,22 +13896,22 @@
       <c r="I3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" t="s" s="0">
         <v>28</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" t="s" s="0">
         <v>28</v>
       </c>
       <c r="P3" s="6" t="s">
@@ -13551,218 +13919,218 @@
       </c>
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
-        <v>62.554218852029649</v>
-      </c>
-      <c r="B4" s="13">
-        <v>39.608851162578489</v>
-      </c>
-      <c r="C4" s="13">
-        <v>21.010985737939279</v>
-      </c>
-      <c r="D4" s="14">
-        <v>0</v>
-      </c>
-      <c r="E4" s="15">
-        <v>65.088111923386236</v>
-      </c>
-      <c r="F4" s="13">
-        <v>41.299361631580517</v>
-      </c>
-      <c r="G4" s="13">
-        <v>22.086858765639143</v>
-      </c>
-      <c r="H4" s="14">
-        <v>0</v>
-      </c>
-      <c r="I4" s="15">
-        <v>64.937545485254233</v>
-      </c>
-      <c r="J4" s="13">
-        <v>39.906991243974957</v>
-      </c>
-      <c r="K4" s="13">
-        <v>23.483048680069782</v>
-      </c>
-      <c r="L4" s="14">
-        <v>0</v>
-      </c>
-      <c r="M4" s="13">
-        <v>62.36185521991009</v>
-      </c>
-      <c r="N4" s="13">
-        <v>37.739429923364938</v>
-      </c>
-      <c r="O4" s="13">
-        <v>21.62221140915652</v>
-      </c>
-      <c r="P4" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="A4" s="13" t="n">
+        <v>64.83744546949316</v>
+      </c>
+      <c r="B4" s="13" t="n">
+        <v>37.28024430337996</v>
+      </c>
+      <c r="C4" s="13" t="n">
+        <v>26.538891598846014</v>
+      </c>
+      <c r="D4" s="14" t="n">
+        <v>2.471557792792484</v>
+      </c>
+      <c r="E4" s="15" t="n">
+        <v>65.78915280405447</v>
+      </c>
+      <c r="F4" s="13" t="n">
+        <v>37.966159728385534</v>
+      </c>
+      <c r="G4" s="13" t="n">
+        <v>26.936916850397544</v>
+      </c>
+      <c r="H4" s="14" t="n">
+        <v>2.4192105199185936</v>
+      </c>
+      <c r="I4" s="15" t="n">
+        <v>69.13556651820205</v>
+      </c>
+      <c r="J4" s="13" t="n">
+        <v>38.65356681088855</v>
+      </c>
+      <c r="K4" s="13" t="n">
+        <v>29.667352053499748</v>
+      </c>
+      <c r="L4" s="14" t="n">
+        <v>1.9772462342339872</v>
+      </c>
+      <c r="M4" s="13" t="n">
+        <v>65.08039439979193</v>
+      </c>
+      <c r="N4" s="13" t="n">
+        <v>36.54124807423138</v>
+      </c>
+      <c r="O4" s="13" t="n">
+        <v>27.20332380529768</v>
+      </c>
+      <c r="P4" s="16" t="n">
+        <v>2.2232853767975906</v>
+      </c>
+      <c r="Q4" t="s" s="0">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
-        <v>75.271516815647374</v>
-      </c>
-      <c r="B5" s="13">
-        <v>40.272586185147979</v>
-      </c>
-      <c r="C5" s="13">
-        <v>34.615373037065552</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0</v>
-      </c>
-      <c r="E5" s="15">
-        <v>75.26195029428041</v>
-      </c>
-      <c r="F5" s="13">
-        <v>41.830349649636105</v>
-      </c>
-      <c r="G5" s="13">
-        <v>32.970368604940163</v>
-      </c>
-      <c r="H5" s="14">
-        <v>0</v>
-      </c>
-      <c r="I5" s="15">
-        <v>75.111383856148422</v>
-      </c>
-      <c r="J5" s="13">
-        <v>40.437979262030545</v>
-      </c>
-      <c r="K5" s="13">
-        <v>34.366558519370798</v>
-      </c>
-      <c r="L5" s="14">
-        <v>0</v>
-      </c>
-      <c r="M5" s="13">
-        <v>72.535693590804271</v>
-      </c>
-      <c r="N5" s="13">
-        <v>38.270417941420533</v>
-      </c>
-      <c r="O5" s="13">
-        <v>32.50572124845754</v>
-      </c>
-      <c r="P5" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="A5" s="13" t="n">
+        <v>88.8270046824621</v>
+      </c>
+      <c r="B5" s="13" t="n">
+        <v>43.78684510551783</v>
+      </c>
+      <c r="C5" s="13" t="n">
+        <v>44.955281544166596</v>
+      </c>
+      <c r="D5" s="14" t="n">
+        <v>0.30303030301894984</v>
+      </c>
+      <c r="E5" s="15" t="n">
+        <v>84.98080017442962</v>
+      </c>
+      <c r="F5" s="13" t="n">
+        <v>43.17144037009583</v>
+      </c>
+      <c r="G5" s="13" t="n">
+        <v>41.67002880665401</v>
+      </c>
+      <c r="H5" s="14" t="n">
+        <v>0.6843885280997661</v>
+      </c>
+      <c r="I5" s="15" t="n">
+        <v>88.3272138885772</v>
+      </c>
+      <c r="J5" s="13" t="n">
+        <v>43.858847452598845</v>
+      </c>
+      <c r="K5" s="13" t="n">
+        <v>44.40046400975621</v>
+      </c>
+      <c r="L5" s="14" t="n">
+        <v>0.24242424241515986</v>
+      </c>
+      <c r="M5" s="13" t="n">
+        <v>84.27204177016708</v>
+      </c>
+      <c r="N5" s="13" t="n">
+        <v>41.74652871594168</v>
+      </c>
+      <c r="O5" s="13" t="n">
+        <v>41.936435761554144</v>
+      </c>
+      <c r="P5" s="16" t="n">
+        <v>0.4884633849787635</v>
+      </c>
+      <c r="Q5" t="s" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="17">
-        <v>78.363582614490923</v>
-      </c>
-      <c r="B6" s="17">
-        <v>49.181430744467448</v>
-      </c>
-      <c r="C6" s="17">
-        <v>28.727092846272058</v>
-      </c>
-      <c r="D6" s="18">
-        <v>0</v>
-      </c>
-      <c r="E6" s="19">
-        <v>77.735602933355253</v>
-      </c>
-      <c r="F6" s="17">
-        <v>48.957425297091689</v>
-      </c>
-      <c r="G6" s="17">
-        <v>28.25974445230537</v>
-      </c>
-      <c r="H6" s="18">
-        <v>0</v>
-      </c>
-      <c r="I6" s="19">
-        <v>77.585036495223264</v>
-      </c>
-      <c r="J6" s="17">
-        <v>47.565054909486122</v>
-      </c>
-      <c r="K6" s="17">
-        <v>29.655934366736005</v>
-      </c>
-      <c r="L6" s="18">
-        <v>0</v>
-      </c>
-      <c r="M6" s="17">
-        <v>75.009346229879114</v>
-      </c>
-      <c r="N6" s="17">
-        <v>45.39749358887611</v>
-      </c>
-      <c r="O6" s="17">
-        <v>27.795097095822747</v>
-      </c>
-      <c r="P6" s="20">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="A6" s="17" t="n">
+        <v>71.27569823939083</v>
+      </c>
+      <c r="B6" s="17" t="n">
+        <v>41.46434624620932</v>
+      </c>
+      <c r="C6" s="17" t="n">
+        <v>29.075423728802843</v>
+      </c>
+      <c r="D6" s="18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="19" t="n">
+        <v>70.93975501997261</v>
+      </c>
+      <c r="F6" s="17" t="n">
+        <v>41.31344128264902</v>
+      </c>
+      <c r="G6" s="17" t="n">
+        <v>28.96614255436301</v>
+      </c>
+      <c r="H6" s="18" t="n">
+        <v>0.44196428568460633</v>
+      </c>
+      <c r="I6" s="19" t="n">
+        <v>74.2861687341202</v>
+      </c>
+      <c r="J6" s="17" t="n">
+        <v>42.00084836515204</v>
+      </c>
+      <c r="K6" s="17" t="n">
+        <v>31.696577757465214</v>
+      </c>
+      <c r="L6" s="18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M6" s="17" t="n">
+        <v>70.23099661571007</v>
+      </c>
+      <c r="N6" s="17" t="n">
+        <v>39.88852962849487</v>
+      </c>
+      <c r="O6" s="17" t="n">
+        <v>29.232549509263144</v>
+      </c>
+      <c r="P6" s="20" t="n">
+        <v>0.24603914256360357</v>
+      </c>
+      <c r="Q6" t="s" s="0">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="38"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="42"/>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="43" t="s">
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="43" t="s">
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="41" t="s">
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="N8" s="44"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="46"/>
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>28</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -13771,10 +14139,10 @@
       <c r="E9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" t="s" s="0">
         <v>28</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -13783,22 +14151,22 @@
       <c r="I9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" t="s" s="0">
         <v>28</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" t="s" s="0">
         <v>28</v>
       </c>
       <c r="P9" s="6" t="s">
@@ -13806,201 +14174,201 @@
       </c>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>59.952380952380949</v>
-      </c>
-      <c r="B10">
-        <v>38.073170731707314</v>
-      </c>
-      <c r="C10">
-        <v>19.951219512195124</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-      <c r="E10" s="11">
-        <v>64.875</v>
-      </c>
-      <c r="F10">
-        <v>43</v>
-      </c>
-      <c r="G10">
-        <v>19.875</v>
-      </c>
-      <c r="H10" s="9">
-        <v>0</v>
+      <c r="A10" s="4" t="n">
+        <v>60.93103448275862</v>
+      </c>
+      <c r="B10" t="n" s="0">
+        <v>36.578947368421055</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>22.982456140350877</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <v>2.0689655172413794</v>
+      </c>
+      <c r="E10" s="11" t="n">
+        <v>64.41666666666667</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>39.583333333333336</v>
+      </c>
+      <c r="G10" t="n" s="0">
+        <v>23.5</v>
+      </c>
+      <c r="H10" s="9" t="n">
+        <v>2.5</v>
       </c>
       <c r="I10" s="11" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="J10" t="e">
+      <c r="J10" t="e" s="0">
         <v>#NUM!</v>
       </c>
-      <c r="K10" t="e">
+      <c r="K10" t="e" s="0">
         <v>#NUM!</v>
       </c>
       <c r="L10" s="9" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="M10">
+      <c r="M10" t="n" s="0">
         <v>44.2</v>
       </c>
-      <c r="N10">
+      <c r="N10" t="n" s="0">
         <v>20.555555555555557</v>
       </c>
-      <c r="O10">
-        <v>20.222222222222221</v>
-      </c>
-      <c r="P10" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="s">
+      <c r="O10" t="n" s="0">
+        <v>20.22222222222222</v>
+      </c>
+      <c r="P10" s="6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q10" t="s" s="0">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>76.228571428571428</v>
-      </c>
-      <c r="B11">
-        <v>40.434782608695649</v>
-      </c>
-      <c r="C11">
-        <v>35.608695652173914</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0</v>
+      <c r="A11" s="4" t="n">
+        <v>90.66666666666667</v>
+      </c>
+      <c r="B11" t="n" s="0">
+        <v>44.339622641509436</v>
+      </c>
+      <c r="C11" t="n" s="0">
+        <v>46.35849056603774</v>
+      </c>
+      <c r="D11" s="9" t="n">
+        <v>0.0</v>
       </c>
       <c r="E11" s="11" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="F11" t="e">
+      <c r="F11" t="e" s="0">
         <v>#NUM!</v>
       </c>
-      <c r="G11" t="e">
+      <c r="G11" t="e" s="0">
         <v>#NUM!</v>
       </c>
       <c r="H11" s="9" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="I11" s="11">
-        <v>76.043478260869563</v>
-      </c>
-      <c r="J11">
-        <v>40.434782608695649</v>
-      </c>
-      <c r="K11">
-        <v>35.608695652173914</v>
-      </c>
-      <c r="L11" s="9">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>89</v>
-      </c>
-      <c r="N11" t="e">
+      <c r="I11" s="11" t="n">
+        <v>90.69811320754717</v>
+      </c>
+      <c r="J11" t="n" s="0">
+        <v>44.339622641509436</v>
+      </c>
+      <c r="K11" t="n" s="0">
+        <v>46.35849056603774</v>
+      </c>
+      <c r="L11" s="9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M11" t="n" s="0">
+        <v>89.0</v>
+      </c>
+      <c r="N11" t="e" s="0">
         <v>#NUM!</v>
       </c>
-      <c r="O11" t="e">
+      <c r="O11" t="e" s="0">
         <v>#NUM!</v>
       </c>
-      <c r="P11" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="P11" s="6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q11" t="s" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:64" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8">
-        <v>76.761904761904759</v>
-      </c>
-      <c r="B12" s="5">
-        <v>45.8</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="A12" s="8" t="n">
+        <v>71.04761904761905</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>39.8</v>
+      </c>
+      <c r="C12" s="5" t="n">
         <v>28.8</v>
       </c>
-      <c r="D12" s="10">
-        <v>0</v>
-      </c>
-      <c r="E12" s="12">
-        <v>98.5</v>
-      </c>
-      <c r="F12" s="5">
-        <v>59.5</v>
-      </c>
-      <c r="G12" s="5">
+      <c r="D12" s="10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E12" s="12" t="n">
+        <v>88.5</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="H12" s="10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I12" s="12" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="K12" s="5" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="L12" s="10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M12" s="5" t="n">
+        <v>62.666666666666664</v>
+      </c>
+      <c r="N12" s="5" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="O12" s="5" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="P12" s="7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q12" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="H12" s="10">
-        <v>0</v>
-      </c>
-      <c r="I12" s="12">
-        <v>65</v>
-      </c>
-      <c r="J12" s="5">
-        <v>57</v>
-      </c>
-      <c r="K12" s="5">
-        <v>8</v>
-      </c>
-      <c r="L12" s="10">
-        <v>0</v>
-      </c>
-      <c r="M12" s="5">
-        <v>62.666666666666664</v>
-      </c>
-      <c r="N12" s="5">
-        <v>26.5</v>
-      </c>
-      <c r="O12" s="5">
-        <v>29</v>
-      </c>
-      <c r="P12" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="s">
+      <c r="I22" t="s" s="0">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" t="s">
-        <v>39</v>
-      </c>
-      <c r="I22" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -14041,7 +14409,7 @@
         <f>N6</f>
         <v>27.721477428199353</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" t="s" s="0">
         <v>17</v>
       </c>
     </row>
@@ -14082,100 +14450,100 @@
         <f>O6</f>
         <v>28.413885088933256</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" t="s" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="0">
         <f>F10</f>
         <v>40.6</v>
       </c>
-      <c r="B27" t="e">
+      <c r="B27" t="e" s="0">
         <f>J10</f>
         <v>#NUM!</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="0">
         <f>N10</f>
         <v>29.666666666666668</v>
       </c>
-      <c r="E27" t="e">
+      <c r="E27" t="e" s="0">
         <f>F11</f>
         <v>#NUM!</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="0">
         <f>J11</f>
         <v>47.333333333333336</v>
       </c>
-      <c r="G27" t="e">
+      <c r="G27" t="e" s="0">
         <f>N11</f>
         <v>#NUM!</v>
       </c>
-      <c r="I27" t="e">
+      <c r="I27" t="e" s="0">
         <f>F12</f>
         <v>#NUM!</v>
       </c>
-      <c r="J27" t="e">
+      <c r="J27" t="e" s="0">
         <f>J12</f>
         <v>#NUM!</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="0">
         <f>N12</f>
         <v>26.5</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="0">
         <f>G10</f>
         <v>18.600000000000001</v>
       </c>
-      <c r="B28" t="e">
+      <c r="B28" t="e" s="0">
         <f>K10</f>
         <v>#NUM!</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="0">
         <f>O10</f>
         <v>27.666666666666668</v>
       </c>
-      <c r="E28" t="e">
+      <c r="E28" t="e" s="0">
         <f>G11</f>
         <v>#NUM!</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="0">
         <f>K11</f>
         <v>41</v>
       </c>
-      <c r="G28" t="e">
+      <c r="G28" t="e" s="0">
         <f>O11</f>
         <v>#NUM!</v>
       </c>
-      <c r="I28" t="e">
+      <c r="I28" t="e" s="0">
         <f>G12</f>
         <v>#NUM!</v>
       </c>
-      <c r="J28" t="e">
+      <c r="J28" t="e" s="0">
         <f>K12</f>
         <v>#NUM!</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="0">
         <f>O12</f>
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A7:P7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="M8:P8"/>
     <mergeCell ref="AC2:AF2"/>
     <mergeCell ref="Y2:AB2"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A7:P7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="M8:P8"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:A6">
     <cfRule type="colorScale" priority="11">
@@ -14259,6 +14627,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E4 I4 M4">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E5 I5 M5">
     <cfRule type="colorScale" priority="19">
       <colorScale>
@@ -14271,8 +14651,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11 I11 M11">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="E6 I6 M6">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14295,6 +14675,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F5 N5 J5">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F6 J6 N6">
     <cfRule type="colorScale" priority="15">
       <colorScale>
@@ -14307,20 +14699,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10 J10 N10">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12 J12 N12">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="G4 O4 K4">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14343,32 +14723,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11 K11 O11">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4 E4 M4">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6 E6 M6">
-    <cfRule type="colorScale" priority="16">
+  <conditionalFormatting sqref="G6 K6 O6">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14391,8 +14747,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I11 E11 M11">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I12 E12 M12">
     <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10 F10 N10">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14415,8 +14795,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6 G6 O6">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="J12 F12 N12">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14439,8 +14819,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K12 G12 O12">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="K11 G11 O11">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14451,20 +14831,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5 F5 J5">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O4 G4 K4">
-    <cfRule type="colorScale" priority="20">
+  <conditionalFormatting sqref="K12 G12 O12">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Shifted things around so date weight is calculated by the matches, not the team members
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -13442,34 +13442,34 @@
         <v>100.26811812702532</v>
       </c>
       <c r="K5" s="22" t="n">
-        <v>59.679245283018865</v>
+        <v>59.09564474825818</v>
       </c>
       <c r="L5" s="12" t="n">
-        <v>25.733333333333334</v>
+        <v>27.370449678300258</v>
       </c>
       <c r="M5" s="12" t="n">
-        <v>15.150537634408602</v>
+        <v>16.565002471134697</v>
       </c>
       <c r="N5" s="12" t="n">
-        <v>3.0136986301369864</v>
+        <v>3.0637701471444605</v>
       </c>
       <c r="O5" s="12" t="n">
-        <v>4.797752808988764</v>
+        <v>4.917836713430747</v>
       </c>
       <c r="P5" s="12" t="n">
-        <v>0.3424657534246575</v>
+        <v>0.428170988057082</v>
       </c>
       <c r="Q5" s="12" t="n">
-        <v>0.011235955056179775</v>
+        <v>0.0036401456082147607</v>
       </c>
       <c r="R5" s="12" t="n">
-        <v>16.774193548387096</v>
+        <v>12.387543253966445</v>
       </c>
       <c r="S5" s="12" t="n">
-        <v>-1.509433962264151</v>
+        <v>-1.3321947054345664</v>
       </c>
       <c r="T5" s="17" t="n">
-        <v>99.92315537986426</v>
+        <v>101.37244838466259</v>
       </c>
       <c r="U5" t="s" s="0">
         <v>33</v>
@@ -13507,7 +13507,7 @@
         <v>107.62936213978517</v>
       </c>
       <c r="K6" s="23" t="n">
-        <v>101.66666666666667</v>
+        <v>101.450000000221</v>
       </c>
       <c r="L6" s="13" t="e">
         <v>#NUM!</v>
@@ -13572,7 +13572,7 @@
         <v>91.14582463786836</v>
       </c>
       <c r="K7" s="30" t="n">
-        <v>71.8</v>
+        <v>71.63157894766981</v>
       </c>
       <c r="L7" s="14" t="n">
         <v>28.0</v>
@@ -13599,7 +13599,7 @@
         <v>-0.0</v>
       </c>
       <c r="T7" s="31" t="n">
-        <v>70.89387089618795</v>
+        <v>70.88354235810294</v>
       </c>
       <c r="U7" t="s" s="0">
         <v>35</v>
@@ -13637,19 +13637,19 @@
         <v>106.49347988644098</v>
       </c>
       <c r="K8" s="23" t="n">
-        <v>72.0</v>
+        <v>71.35483870988972</v>
       </c>
       <c r="L8" s="13" t="n">
-        <v>31.0</v>
+        <v>32.80645161230885</v>
       </c>
       <c r="M8" s="13" t="n">
-        <v>8.333333333333334</v>
+        <v>10.304347825212854</v>
       </c>
       <c r="N8" s="13" t="n">
         <v>2.0</v>
       </c>
       <c r="O8" s="13" t="n">
-        <v>3.5</v>
+        <v>3.4999999999999996</v>
       </c>
       <c r="P8" s="13" t="n">
         <v>0.0</v>
@@ -13661,10 +13661,10 @@
         <v>45.0</v>
       </c>
       <c r="S8" s="13" t="n">
-        <v>-1.6666666666666667</v>
+        <v>-2.096774193406868</v>
       </c>
       <c r="T8" s="18" t="n">
-        <v>89.33802698418249</v>
+        <v>97.1023898048047</v>
       </c>
       <c r="U8" t="s" s="0">
         <v>36</v>
@@ -13702,34 +13702,34 @@
         <v>113.85472389920083</v>
       </c>
       <c r="K9" s="23" t="n">
-        <v>74.73469387755102</v>
+        <v>70.6513470692239</v>
       </c>
       <c r="L9" s="13" t="n">
-        <v>45.618556701030926</v>
+        <v>45.055599682434995</v>
       </c>
       <c r="M9" s="13" t="n">
-        <v>16.2680412371134</v>
+        <v>15.833200953251318</v>
       </c>
       <c r="N9" s="13" t="n">
-        <v>2.452054794520548</v>
+        <v>2.4244004171083042</v>
       </c>
       <c r="O9" s="13" t="n">
-        <v>4.739726027397261</v>
+        <v>4.642335766448563</v>
       </c>
       <c r="P9" s="13" t="n">
-        <v>0.1780821917808219</v>
+        <v>0.11366006258184523</v>
       </c>
       <c r="Q9" s="13" t="n">
-        <v>0.3424657534246575</v>
+        <v>0.3660062565111129</v>
       </c>
       <c r="R9" s="13" t="n">
-        <v>13.092783505154639</v>
+        <v>10.285941223928274</v>
       </c>
       <c r="S9" s="13" t="n">
-        <v>-1.6326530612244898</v>
+        <v>-1.9651347067267961</v>
       </c>
       <c r="T9" s="18" t="n">
-        <v>116.53225979387153</v>
+        <v>114.50229143613548</v>
       </c>
       <c r="U9" t="s" s="0">
         <v>37</v>
@@ -13832,7 +13832,7 @@
         <v>90.59349865792196</v>
       </c>
       <c r="K11" s="22" t="n">
-        <v>68.82352941176471</v>
+        <v>70.3877068553645</v>
       </c>
       <c r="L11" s="12" t="n">
         <v>30.0</v>
@@ -13962,34 +13962,34 @@
         <v>81.471205168765</v>
       </c>
       <c r="K13" s="24" t="n">
-        <v>65.85365853658537</v>
+        <v>63.96424581064444</v>
       </c>
       <c r="L13" s="25" t="n">
-        <v>28.4</v>
+        <v>27.432432432728802</v>
       </c>
       <c r="M13" s="25" t="n">
-        <v>11.6</v>
+        <v>13.049549549105542</v>
       </c>
       <c r="N13" s="25" t="n">
-        <v>2.2</v>
+        <v>2.054054054098758</v>
       </c>
       <c r="O13" s="25" t="n">
-        <v>3.8</v>
+        <v>4.103603603510607</v>
       </c>
       <c r="P13" s="25" t="n">
-        <v>0.2</v>
+        <v>0.22522522521749858</v>
       </c>
       <c r="Q13" s="25" t="n">
-        <v>0.1</v>
+        <v>0.11261261260874929</v>
       </c>
       <c r="R13" s="25" t="n">
-        <v>24.5</v>
+        <v>23.040540540987582</v>
       </c>
       <c r="S13" s="25" t="n">
         <v>-0.0</v>
       </c>
       <c r="T13" s="20" t="n">
-        <v>78.18259186629821</v>
+        <v>81.45043734013018</v>
       </c>
       <c r="U13" t="s" s="0">
         <v>41</v>
@@ -14116,34 +14116,34 @@
         <v>99.76084834563407</v>
       </c>
       <c r="K16" s="22" t="n">
-        <v>66.25</v>
+        <v>66.27368421051614</v>
       </c>
       <c r="L16" s="9" t="n">
-        <v>24.583333333333332</v>
+        <v>26.68421052541352</v>
       </c>
       <c r="M16" s="9" t="n">
-        <v>11.777777777777779</v>
+        <v>11.946428571336416</v>
       </c>
       <c r="N16" s="9" t="n">
-        <v>2.625</v>
+        <v>1.9310344831925486</v>
       </c>
       <c r="O16" s="9" t="n">
-        <v>4.5</v>
+        <v>3.6551724143213637</v>
       </c>
       <c r="P16" s="9" t="n">
-        <v>0.25</v>
+        <v>0.3103448275484741</v>
       </c>
       <c r="Q16" s="9" t="n">
         <v>0.0</v>
       </c>
       <c r="R16" s="9" t="n">
-        <v>27.22222222222222</v>
+        <v>20.625000003604914</v>
       </c>
       <c r="S16" s="9" t="n">
-        <v>-3.3333333333333335</v>
+        <v>-4.105263157563213</v>
       </c>
       <c r="T16" s="17" t="n">
-        <v>117.88812005926775</v>
+        <v>122.00496218651159</v>
       </c>
       <c r="U16" t="s" s="0">
         <v>33</v>
@@ -14639,34 +14639,34 @@
         <v>84.72331797902581</v>
       </c>
       <c r="K24" s="24" t="n">
-        <v>64.83333333333333</v>
+        <v>63.201149425670074</v>
       </c>
       <c r="L24" s="19" t="n">
-        <v>29.666666666666668</v>
+        <v>29.02298850589806</v>
       </c>
       <c r="M24" s="19" t="n">
-        <v>13.5</v>
+        <v>12.741379310522712</v>
       </c>
       <c r="N24" s="19" t="n">
         <v>2.0</v>
       </c>
       <c r="O24" s="19" t="n">
-        <v>4.333333333333333</v>
+        <v>4.2873563218498605</v>
       </c>
       <c r="P24" s="19" t="n">
-        <v>0.16666666666666666</v>
+        <v>0.14367816092493066</v>
       </c>
       <c r="Q24" s="19" t="n">
-        <v>0.16666666666666666</v>
+        <v>0.14367816092493066</v>
       </c>
       <c r="R24" s="19" t="n">
-        <v>21.666666666666668</v>
+        <v>21.436781609249305</v>
       </c>
       <c r="S24" s="19" t="n">
         <v>-0.0</v>
       </c>
       <c r="T24" s="20" t="n">
-        <v>81.80910879043918</v>
+        <v>76.89834309861402</v>
       </c>
       <c r="U24" t="s" s="0">
         <v>41</v>
@@ -15056,34 +15056,34 @@
         <v>113.73215034413748</v>
       </c>
       <c r="K31" s="23" t="n">
-        <v>74.58762886597938</v>
+        <v>70.60762510032772</v>
       </c>
       <c r="L31" s="13" t="n">
-        <v>45.618556701030926</v>
+        <v>45.055599682434995</v>
       </c>
       <c r="M31" s="13" t="n">
-        <v>16.2680412371134</v>
+        <v>15.833200953251318</v>
       </c>
       <c r="N31" s="13" t="n">
-        <v>2.452054794520548</v>
+        <v>2.4244004171083042</v>
       </c>
       <c r="O31" s="13" t="n">
-        <v>4.739726027397261</v>
+        <v>4.642335766448563</v>
       </c>
       <c r="P31" s="13" t="n">
-        <v>0.1780821917808219</v>
+        <v>0.11366006258184523</v>
       </c>
       <c r="Q31" s="13" t="n">
-        <v>0.3424657534246575</v>
+        <v>0.3660062565111129</v>
       </c>
       <c r="R31" s="13" t="n">
-        <v>13.092783505154639</v>
+        <v>10.285941223928274</v>
       </c>
       <c r="S31" s="13" t="n">
-        <v>-1.6494845360824741</v>
+        <v>-1.9698173152457137</v>
       </c>
       <c r="T31" s="18" t="n">
-        <v>116.7238086229994</v>
+        <v>114.55540918708306</v>
       </c>
       <c r="U31" t="s" s="0">
         <v>37</v>
@@ -15189,7 +15189,7 @@
         <v>69.0</v>
       </c>
       <c r="L33" s="12" t="n">
-        <v>30.0</v>
+        <v>29.999999999999996</v>
       </c>
       <c r="M33" s="12" t="e">
         <v>#NUM!</v>
@@ -15316,34 +15316,34 @@
         <v>87.82533535978882</v>
       </c>
       <c r="K35" s="24" t="n">
-        <v>47.5</v>
+        <v>53.39285713999491</v>
       </c>
       <c r="L35" s="25" t="n">
-        <v>14.0</v>
+        <v>9.285714288004081</v>
       </c>
       <c r="M35" s="25" t="n">
-        <v>11.0</v>
+        <v>19.642857138659185</v>
       </c>
       <c r="N35" s="25" t="n">
         <v>1.0</v>
       </c>
       <c r="O35" s="25" t="n">
-        <v>1.5</v>
+        <v>2.6785714279989796</v>
       </c>
       <c r="P35" s="25" t="n">
-        <v>0.5</v>
+        <v>0.8928571426663265</v>
       </c>
       <c r="Q35" s="25" t="n">
         <v>0.0</v>
       </c>
       <c r="R35" s="25" t="n">
-        <v>22.5</v>
+        <v>24.46428571333163</v>
       </c>
       <c r="S35" s="25" t="n">
         <v>-0.0</v>
       </c>
       <c r="T35" s="20" t="n">
-        <v>77.80350249854101</v>
+        <v>119.65465824202485</v>
       </c>
       <c r="U35" t="s" s="0">
         <v>41</v>
@@ -15470,34 +15470,34 @@
         <v>98.5292372532197</v>
       </c>
       <c r="K38" s="22" t="n">
-        <v>54.241379310344826</v>
+        <v>55.647281921267705</v>
       </c>
       <c r="L38" s="9" t="n">
-        <v>26.70175438596491</v>
+        <v>27.701587301341245</v>
       </c>
       <c r="M38" s="9" t="n">
-        <v>17.280701754385966</v>
+        <v>17.878730158582986</v>
       </c>
       <c r="N38" s="9" t="n">
-        <v>3.317073170731707</v>
+        <v>3.429101019433519</v>
       </c>
       <c r="O38" s="9" t="n">
-        <v>4.964912280701754</v>
+        <v>5.196825396768324</v>
       </c>
       <c r="P38" s="9" t="n">
-        <v>0.4146341463414634</v>
+        <v>0.4661723818217156</v>
       </c>
       <c r="Q38" s="9" t="n">
-        <v>0.017543859649122806</v>
+        <v>0.004444444447668148</v>
       </c>
       <c r="R38" s="9" t="n">
-        <v>10.175438596491228</v>
+        <v>10.04444444447668</v>
       </c>
       <c r="S38" s="9" t="n">
         <v>-0.0</v>
       </c>
       <c r="T38" s="17" t="n">
-        <v>85.26753478337457</v>
+        <v>89.23197499716709</v>
       </c>
       <c r="U38" t="s" s="0">
         <v>33</v>
@@ -15538,7 +15538,7 @@
         <v>104.4182324634276</v>
       </c>
       <c r="K39" s="23" t="n">
-        <v>101.66666666666667</v>
+        <v>101.450000000221</v>
       </c>
       <c r="L39" s="10" t="e">
         <v>#NUM!</v>
@@ -15668,19 +15668,19 @@
         <v>103.50952666075223</v>
       </c>
       <c r="K41" s="22" t="n">
-        <v>72.0</v>
+        <v>71.35483870988972</v>
       </c>
       <c r="L41" s="9" t="n">
-        <v>31.0</v>
+        <v>32.80645161230885</v>
       </c>
       <c r="M41" s="9" t="n">
-        <v>8.333333333333334</v>
+        <v>10.304347825212854</v>
       </c>
       <c r="N41" s="9" t="n">
         <v>2.0</v>
       </c>
       <c r="O41" s="9" t="n">
-        <v>3.5</v>
+        <v>3.4999999999999996</v>
       </c>
       <c r="P41" s="9" t="n">
         <v>0.0</v>
@@ -15692,10 +15692,10 @@
         <v>45.0</v>
       </c>
       <c r="S41" s="9" t="n">
-        <v>-1.6666666666666667</v>
+        <v>-2.096774193406868</v>
       </c>
       <c r="T41" s="17" t="n">
-        <v>89.33802698418249</v>
+        <v>97.1023898048047</v>
       </c>
       <c r="U41" t="s" s="0">
         <v>36</v>
@@ -15993,7 +15993,7 @@
         <v>83.49170688661147</v>
       </c>
       <c r="K46" s="24" t="n">
-        <v>84.88888888888889</v>
+        <v>83.67816092039192</v>
       </c>
       <c r="L46" s="19" t="n">
         <v>39.0</v>
@@ -16020,7 +16020,7 @@
         <v>-0.0</v>
       </c>
       <c r="T46" s="20" t="n">
-        <v>67.53621187030274</v>
+        <v>67.46196313619156</v>
       </c>
       <c r="U46" t="s" s="0">
         <v>41</v>

</xml_diff>

<commit_message>
I guess the grade works for drive teams too
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9C77EC-2CFE-4D20-B58C-4A268EADCC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19326DF9-F5E3-4770-88C5-D3A9B714030E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
@@ -874,15 +874,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -893,6 +884,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2408,19 +2408,19 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>100.40620738948833</c:v>
+                  <c:v>-3.5567052061310243</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65.886643347004579</c:v>
+                  <c:v>6.9088004812459207</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84.460186422171603</c:v>
+                  <c:v>-11.46303565018658</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>121.59511864449674</c:v>
+                  <c:v>5.2001634839811572</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2432,7 +2432,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>77.002628519678595</c:v>
+                  <c:v>2.2930925827348165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3550,31 +3550,31 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>97.334399313645378</c:v>
+                  <c:v>-3.1963437456007147</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>109.5557532426223</c:v>
+                  <c:v>1.4450645858110902</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87.226245976655221</c:v>
+                  <c:v>-8.9635456729177054E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>106.97062624454742</c:v>
+                  <c:v>-0.44990728864085194</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>119.19198017352433</c:v>
+                  <c:v>4.1915010427709571</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>96.862472907557262</c:v>
+                  <c:v>2.656801000230689</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>86.714924979659912</c:v>
+                  <c:v>-0.54862380879740957</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>98.936278908636837</c:v>
+                  <c:v>4.092784522614398</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>76.60677164266977</c:v>
+                  <c:v>2.558084480074128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13282,35 +13282,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AJ53"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="87" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:AA52"/>
+    <sheetView zoomScale="87" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:36" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="58"/>
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
       <c r="W1" s="8"/>
@@ -13329,56 +13329,56 @@
       <c r="AJ1" s="8"/>
     </row>
     <row r="2" spans="1:36" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="62" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="63"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="60"/>
     </row>
     <row r="3" spans="1:36" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="59" t="s">
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="58"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="61"/>
+      <c r="S3" s="61"/>
+      <c r="T3" s="62"/>
     </row>
     <row r="4" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
@@ -13471,7 +13471,7 @@
         <v>-1.3957311152344514</v>
       </c>
       <c r="J5" s="26">
-        <v>97.334399313645378</v>
+        <v>-3.1963437456007147</v>
       </c>
       <c r="K5" s="22">
         <v>59.77048496578729</v>
@@ -13501,7 +13501,7 @@
         <v>-1.5227694991239451</v>
       </c>
       <c r="T5" s="17">
-        <v>100.40620738948833</v>
+        <v>-3.5567052061310243</v>
       </c>
       <c r="U5" t="s">
         <v>33</v>
@@ -13536,7 +13536,7 @@
         <v>-1.493681321980505</v>
       </c>
       <c r="J6" s="27">
-        <v>109.5557532426223</v>
+        <v>1.4450645858110902</v>
       </c>
       <c r="K6" s="23">
         <v>101.66395494367676</v>
@@ -13601,7 +13601,7 @@
         <v>-0.70927747656311746</v>
       </c>
       <c r="J7" s="28">
-        <v>87.226245976655221</v>
+        <v>-8.9635456729177054E-2</v>
       </c>
       <c r="K7" s="30">
         <v>71.765920070225988</v>
@@ -13631,7 +13631,7 @@
         <v>0</v>
       </c>
       <c r="T7" s="31">
-        <v>65.886643347004579</v>
+        <v>6.9088004812459207</v>
       </c>
       <c r="U7" t="s">
         <v>35</v>
@@ -13666,7 +13666,7 @@
         <v>-1.5141107521616552</v>
       </c>
       <c r="J8" s="27">
-        <v>106.97062624454742</v>
+        <v>-0.44990728864085194</v>
       </c>
       <c r="K8" s="23">
         <v>71.894736841988916</v>
@@ -13696,7 +13696,7 @@
         <v>-1.7368421053407199</v>
       </c>
       <c r="T8" s="18">
-        <v>84.460186422171603</v>
+        <v>-11.46303565018658</v>
       </c>
       <c r="U8" t="s">
         <v>36</v>
@@ -13731,7 +13731,7 @@
         <v>-1.6120609589077088</v>
       </c>
       <c r="J9" s="27">
-        <v>119.19198017352433</v>
+        <v>4.1915010427709571</v>
       </c>
       <c r="K9" s="23">
         <v>74.688707874091122</v>
@@ -13761,7 +13761,7 @@
         <v>-1.6355214821944859</v>
       </c>
       <c r="T9" s="18">
-        <v>121.59511864449674</v>
+        <v>5.2001634839811572</v>
       </c>
       <c r="U9" t="s">
         <v>37</v>
@@ -13796,7 +13796,7 @@
         <v>-0.82765711349032134</v>
       </c>
       <c r="J10" s="27">
-        <v>96.862472907557262</v>
+        <v>2.656801000230689</v>
       </c>
       <c r="K10" s="23" t="e">
         <v>#NUM!</v>
@@ -13861,7 +13861,7 @@
         <v>-0.68645363867133391</v>
       </c>
       <c r="J11" s="26">
-        <v>86.714924979659912</v>
+        <v>-0.54862380879740957</v>
       </c>
       <c r="K11" s="22">
         <v>68.804142077699083</v>
@@ -13926,7 +13926,7 @@
         <v>-0.7844038454173875</v>
       </c>
       <c r="J12" s="27">
-        <v>98.936278908636837</v>
+        <v>4.092784522614398</v>
       </c>
       <c r="K12" s="23">
         <v>83</v>
@@ -13991,7 +13991,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="29">
-        <v>76.60677164266977</v>
+        <v>2.558084480074128</v>
       </c>
       <c r="K13" s="24">
         <v>66.099174361504566</v>
@@ -14021,37 +14021,37 @@
         <v>0</v>
       </c>
       <c r="T13" s="20">
-        <v>77.002628519678595</v>
+        <v>2.2930925827348165</v>
       </c>
       <c r="U13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:36" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="59" t="s">
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="57"/>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="58"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="61"/>
+      <c r="P14" s="61"/>
+      <c r="Q14" s="61"/>
+      <c r="R14" s="61"/>
+      <c r="S14" s="61"/>
+      <c r="T14" s="62"/>
     </row>
     <row r="15" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
@@ -14145,7 +14145,7 @@
         <v>-1.5014066629853289</v>
       </c>
       <c r="J16" s="17">
-        <v>98.147728662373652</v>
+        <v>-4.3750300198451972</v>
       </c>
       <c r="K16" s="22">
         <v>66.253077975379753</v>
@@ -14175,7 +14175,7 @@
         <v>-3.4336525308950323</v>
       </c>
       <c r="T16" s="17">
-        <v>118.27041392673847</v>
+        <v>-20.664353527672162</v>
       </c>
       <c r="U16" t="s">
         <v>33</v>
@@ -14213,7 +14213,7 @@
         <v>-1.5797668283821718</v>
       </c>
       <c r="J17" s="18">
-        <v>107.92481180555518</v>
+        <v>-0.66190335471574802</v>
       </c>
       <c r="K17" s="23" t="e">
         <v>#NUM!</v>
@@ -14278,7 +14278,7 @@
         <v>-0.95224375204826173</v>
       </c>
       <c r="J18" s="18">
-        <v>90.06120599278151</v>
+        <v>-1.8896633887479708</v>
       </c>
       <c r="K18" s="23">
         <v>72</v>
@@ -14308,7 +14308,7 @@
         <v>0</v>
       </c>
       <c r="T18" s="18">
-        <v>65.900568369056742</v>
+        <v>6.9305881518404489</v>
       </c>
       <c r="U18" t="s">
         <v>35</v>
@@ -14343,7 +14343,7 @@
         <v>-1.596110372527092</v>
       </c>
       <c r="J19" s="17">
-        <v>105.85671020709528</v>
+        <v>-2.1778808542773049</v>
       </c>
       <c r="K19" s="22" t="e">
         <v>#NUM!</v>
@@ -14408,7 +14408,7 @@
         <v>-1.6744705379239349</v>
       </c>
       <c r="J20" s="18">
-        <v>115.63379335027679</v>
+        <v>1.5352458108521443</v>
       </c>
       <c r="K20" s="23" t="e">
         <v>#NUM!</v>
@@ -14473,7 +14473,7 @@
         <v>-1.0469474615900247</v>
       </c>
       <c r="J21" s="18">
-        <v>97.770187537503134</v>
+        <v>0.30748577681992728</v>
       </c>
       <c r="K21" s="23" t="e">
         <v>#NUM!</v>
@@ -14538,7 +14538,7 @@
         <v>-0.93398468173483484</v>
       </c>
       <c r="J22" s="17">
-        <v>89.65214919518526</v>
+        <v>-2.256854070402551</v>
       </c>
       <c r="K22" s="22">
         <v>73</v>
@@ -14603,7 +14603,7 @@
         <v>-1.0123448471316778</v>
       </c>
       <c r="J23" s="18">
-        <v>99.429232338366802</v>
+        <v>1.4562725947268966</v>
       </c>
       <c r="K23" s="23" t="e">
         <v>#NUM!</v>
@@ -14668,7 +14668,7 @@
         <v>-0.3848217707977678</v>
       </c>
       <c r="J24" s="20">
-        <v>81.565626525593146</v>
+        <v>0.22851256069468029</v>
       </c>
       <c r="K24" s="24">
         <v>65.016795865832179</v>
@@ -14698,37 +14698,37 @@
         <v>0</v>
       </c>
       <c r="T24" s="20">
-        <v>81.056207478780209</v>
+        <v>5.0789414150025314</v>
       </c>
       <c r="U24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="59" t="s">
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="L25" s="57"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="57"/>
-      <c r="O25" s="57"/>
-      <c r="P25" s="57"/>
-      <c r="Q25" s="57"/>
-      <c r="R25" s="57"/>
-      <c r="S25" s="57"/>
-      <c r="T25" s="58"/>
+      <c r="L25" s="61"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="61"/>
+      <c r="O25" s="61"/>
+      <c r="P25" s="61"/>
+      <c r="Q25" s="61"/>
+      <c r="R25" s="61"/>
+      <c r="S25" s="61"/>
+      <c r="T25" s="62"/>
     </row>
     <row r="26" spans="1:22" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
@@ -14822,7 +14822,7 @@
         <v>-1.4009306054828301</v>
       </c>
       <c r="J27" s="17">
-        <v>101.22503992862249</v>
+        <v>-1.6172372164257025</v>
       </c>
       <c r="K27" s="22" t="e">
         <v>#NUM!</v>
@@ -14890,7 +14890,7 @@
         <v>-1.479290770879673</v>
       </c>
       <c r="J28" s="18">
-        <v>111.00212307180404</v>
+        <v>2.0958894487037396</v>
       </c>
       <c r="K28" s="23" t="e">
         <v>#NUM!</v>
@@ -14955,7 +14955,7 @@
         <v>-0.85176769454576284</v>
       </c>
       <c r="J29" s="18">
-        <v>93.138517259030394</v>
+        <v>0.86812941467152915</v>
       </c>
       <c r="K29" s="23" t="e">
         <v>#NUM!</v>
@@ -15020,7 +15020,7 @@
         <v>-1.4956343150245932</v>
       </c>
       <c r="J30" s="17">
-        <v>108.93402147334413</v>
+        <v>0.57991194914218891</v>
       </c>
       <c r="K30" s="22" t="e">
         <v>#NUM!</v>
@@ -15085,7 +15085,7 @@
         <v>-1.5739944804214361</v>
       </c>
       <c r="J31" s="18">
-        <v>118.71110461652566</v>
+        <v>4.2930386142716319</v>
       </c>
       <c r="K31" s="23">
         <v>74.535071434279288</v>
@@ -15115,7 +15115,7 @@
         <v>-1.6530793445838095</v>
       </c>
       <c r="T31" s="18">
-        <v>121.81631418651652</v>
+        <v>5.0649884562557341</v>
       </c>
       <c r="U31" t="s">
         <v>37</v>
@@ -15150,7 +15150,7 @@
         <v>-0.94647140408752595</v>
       </c>
       <c r="J32" s="18">
-        <v>100.84749880375199</v>
+        <v>3.0652785802394238</v>
       </c>
       <c r="K32" s="23" t="e">
         <v>#NUM!</v>
@@ -15215,7 +15215,7 @@
         <v>-0.83350862423233596</v>
       </c>
       <c r="J33" s="17">
-        <v>92.729460461434144</v>
+        <v>0.50093873301694769</v>
       </c>
       <c r="K33" s="22">
         <v>68.999999999999986</v>
@@ -15280,7 +15280,7 @@
         <v>-0.91186878962917883</v>
       </c>
       <c r="J34" s="18">
-        <v>102.50654360461566</v>
+        <v>4.2140653981463911</v>
       </c>
       <c r="K34" s="23" t="e">
         <v>#NUM!</v>
@@ -15345,7 +15345,7 @@
         <v>-0.28434571329526892</v>
       </c>
       <c r="J35" s="20">
-        <v>84.642937791842002</v>
+        <v>2.9863053641141732</v>
       </c>
       <c r="K35" s="24">
         <v>48.187500000802082</v>
@@ -15375,37 +15375,37 @@
         <v>0</v>
       </c>
       <c r="T35" s="20">
-        <v>79.117333951344733</v>
+        <v>-4.3566944184023662</v>
       </c>
       <c r="U35" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="57"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="58"/>
-      <c r="K36" s="59" t="s">
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="61"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="L36" s="57"/>
-      <c r="M36" s="57"/>
-      <c r="N36" s="57"/>
-      <c r="O36" s="57"/>
-      <c r="P36" s="57"/>
-      <c r="Q36" s="57"/>
-      <c r="R36" s="57"/>
-      <c r="S36" s="57"/>
-      <c r="T36" s="58"/>
+      <c r="L36" s="61"/>
+      <c r="M36" s="61"/>
+      <c r="N36" s="61"/>
+      <c r="O36" s="61"/>
+      <c r="P36" s="61"/>
+      <c r="Q36" s="61"/>
+      <c r="R36" s="61"/>
+      <c r="S36" s="61"/>
+      <c r="T36" s="62"/>
     </row>
     <row r="37" spans="1:22" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
@@ -15499,7 +15499,7 @@
         <v>-1.2019406421866381</v>
       </c>
       <c r="J38" s="17">
-        <v>94.705100202520612</v>
+        <v>-1.8479996324941204</v>
       </c>
       <c r="K38" s="22">
         <v>54.604551339231307</v>
@@ -15529,7 +15529,7 @@
         <v>0</v>
       </c>
       <c r="T38" s="17">
-        <v>85.562915002990536</v>
+        <v>9.7555614361352863</v>
       </c>
       <c r="U38" t="s">
         <v>33</v>
@@ -15567,7 +15567,7 @@
         <v>-1.280300807583481</v>
       </c>
       <c r="J39" s="18">
-        <v>104.48218334570213</v>
+        <v>1.865127032635322</v>
       </c>
       <c r="K39" s="23">
         <v>101.66395494367676</v>
@@ -15632,7 +15632,7 @@
         <v>-0.65277773124957095</v>
       </c>
       <c r="J40" s="18">
-        <v>86.61857753292847</v>
+        <v>0.63736699860310919</v>
       </c>
       <c r="K40" s="23">
         <v>71</v>
@@ -15697,7 +15697,7 @@
         <v>-1.2966443517284012</v>
       </c>
       <c r="J41" s="17">
-        <v>102.41408174724224</v>
+        <v>0.34914953307376878</v>
       </c>
       <c r="K41" s="22">
         <v>71.894736841988916</v>
@@ -15727,7 +15727,7 @@
         <v>-1.7368421053407199</v>
       </c>
       <c r="T41" s="17">
-        <v>84.460186422171603</v>
+        <v>-11.46303565018658</v>
       </c>
       <c r="U41" t="s">
         <v>36</v>
@@ -15762,7 +15762,7 @@
         <v>-1.3750045171252441</v>
       </c>
       <c r="J42" s="18">
-        <v>112.19116489042374</v>
+        <v>4.0622761982032118</v>
       </c>
       <c r="K42" s="23">
         <v>89</v>
@@ -15827,7 +15827,7 @@
         <v>-0.74748144079133405</v>
       </c>
       <c r="J43" s="18">
-        <v>94.327559077650108</v>
+        <v>2.8345161641710037</v>
       </c>
       <c r="K43" s="23" t="e">
         <v>#NUM!</v>
@@ -15892,7 +15892,7 @@
         <v>-0.63451866093614417</v>
       </c>
       <c r="J44" s="17">
-        <v>86.209520735332219</v>
+        <v>0.27017631694852273</v>
       </c>
       <c r="K44" s="22">
         <v>34</v>
@@ -15957,7 +15957,7 @@
         <v>-0.71287882633298705</v>
       </c>
       <c r="J45" s="18">
-        <v>95.986603878513748</v>
+        <v>3.9833029820779693</v>
       </c>
       <c r="K45" s="23">
         <v>83</v>
@@ -16022,7 +16022,7 @@
         <v>-8.5355749999076996E-2</v>
       </c>
       <c r="J46" s="20">
-        <v>78.122998065740106</v>
+        <v>2.7555429480457549</v>
       </c>
       <c r="K46" s="24">
         <v>85.459599529535083</v>
@@ -16052,7 +16052,7 @@
         <v>0</v>
       </c>
       <c r="T46" s="20">
-        <v>61.126050657994782</v>
+        <v>-0.3807357396422919</v>
       </c>
       <c r="U46" t="s">
         <v>41</v>
@@ -16404,17 +16404,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="K2:T2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="K3:T3"/>
     <mergeCell ref="A14:J14"/>
     <mergeCell ref="K14:T14"/>
     <mergeCell ref="K25:T25"/>
     <mergeCell ref="A25:J25"/>
     <mergeCell ref="A36:J36"/>
     <mergeCell ref="K36:T36"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="K2:T2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="K3:T3"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:A13">
     <cfRule type="colorScale" priority="40">

</xml_diff>

<commit_message>
Relative weights are calculated and shown but I lost the scores from 12/6 :(
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19326DF9-F5E3-4770-88C5-D3A9B714030E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8C3A18-7E8F-4A09-A992-F0DF9DCE365C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
   <sheets>
     <sheet name="Match Data" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="45">
   <si>
     <t>Cyrus</t>
   </si>
@@ -173,14 +173,18 @@
   <si>
     <t>Overall Team Averages</t>
   </si>
+  <si>
+    <t>Weight</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -804,7 +808,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -855,6 +859,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1091,13 +1096,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-3.5386524343082773</c:v>
+                  <c:v>-4.3840737299157748</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.744164228515336</c:v>
+                  <c:v>6.6197191097381562</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6747641434348015</c:v>
+                  <c:v>3.1451187619641061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2408,19 +2413,19 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-3.5567052061310243</c:v>
+                  <c:v>-4.4808222023825603</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.9088004812459207</c:v>
+                  <c:v>6.2592774224969174</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-11.46303565018658</c:v>
+                  <c:v>-12.902339425822223</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2001634839811572</c:v>
+                  <c:v>6.0454382197238257</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2432,7 +2437,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.2930925827348165</c:v>
+                  <c:v>2.8571809414190055</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2796,13 +2801,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-2.8540350568931556</c:v>
+                  <c:v>-3.7237839783619879</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6388378570265791</c:v>
+                  <c:v>3.1784283501878239</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4414048167134634</c:v>
+                  <c:v>2.9940088379451248</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3162,13 +3167,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-9.0897751168231178</c:v>
+                  <c:v>-9.7405982272386495</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.6991889002743497</c:v>
+                  <c:v>5.5126317734811883</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5453768199322515</c:v>
+                  <c:v>3.1466853974271798</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3550,31 +3555,31 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-3.1963437456007147</c:v>
+                  <c:v>-4.0539288541388769</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4450645858110902</c:v>
+                  <c:v>1.4479675656880822</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-8.9635456729177054E-2</c:v>
+                  <c:v>-0.28933260819893736</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.44990728864085194</c:v>
+                  <c:v>-0.60282268986397369</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1915010427709571</c:v>
+                  <c:v>4.899073729962991</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.656801000230689</c:v>
+                  <c:v>3.1617735560759668</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.54862380879740957</c:v>
+                  <c:v>-0.69503244598532499</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.092784522614398</c:v>
+                  <c:v>4.8068639738416392</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.558084480074128</c:v>
+                  <c:v>3.0695637999546177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9857,8 +9862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
   <dimension ref="A1:Y74"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N67" sqref="N67"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9910,6 +9915,9 @@
       <c r="N1" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="O1" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -9954,6 +9962,9 @@
       <c r="N2">
         <v>0</v>
       </c>
+      <c r="O2" s="50">
+        <v>5.9151785710937502E-2</v>
+      </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
@@ -10001,7 +10012,9 @@
       <c r="N3">
         <v>0</v>
       </c>
-      <c r="O3" s="2"/>
+      <c r="O3" s="50">
+        <v>5.9151785710937502E-2</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
@@ -10048,6 +10061,9 @@
       <c r="N4">
         <v>0</v>
       </c>
+      <c r="O4" s="50">
+        <v>5.9151785710937502E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -10092,6 +10108,9 @@
       <c r="N5">
         <v>0</v>
       </c>
+      <c r="O5" s="50">
+        <v>5.9263392853906249E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -10136,6 +10155,9 @@
       <c r="N6">
         <v>0</v>
       </c>
+      <c r="O6" s="50">
+        <v>5.9263392853906249E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -10180,6 +10202,9 @@
       <c r="N7">
         <v>0</v>
       </c>
+      <c r="O7" s="50">
+        <v>5.9263392853906249E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -10224,6 +10249,9 @@
       <c r="N8">
         <v>0</v>
       </c>
+      <c r="O8" s="50">
+        <v>5.9263392853906249E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -10268,6 +10296,9 @@
       <c r="N9">
         <v>0</v>
       </c>
+      <c r="O9" s="50">
+        <v>5.9263392853906249E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -10312,6 +10343,9 @@
       <c r="N10">
         <v>0</v>
       </c>
+      <c r="O10" s="50">
+        <v>5.9263392853906249E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -10356,6 +10390,9 @@
       <c r="N11">
         <v>0</v>
       </c>
+      <c r="O11" s="50">
+        <v>5.9151785710937502E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -10400,6 +10437,9 @@
       <c r="N12">
         <v>0</v>
       </c>
+      <c r="O12" s="50">
+        <v>5.9263392853906249E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -10444,6 +10484,9 @@
       <c r="N13">
         <v>0</v>
       </c>
+      <c r="O13" s="50">
+        <v>0.1910714285125</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -10488,6 +10531,9 @@
       <c r="N14">
         <v>0</v>
       </c>
+      <c r="O14" s="50">
+        <v>0.1910714285125</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -10532,6 +10578,9 @@
       <c r="N15">
         <v>0</v>
       </c>
+      <c r="O15" s="50">
+        <v>0.1910714285125</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -10576,6 +10625,9 @@
       <c r="N16">
         <v>0</v>
       </c>
+      <c r="O16" s="50">
+        <v>0.1910714285125</v>
+      </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -10620,6 +10672,9 @@
       <c r="N17">
         <v>0</v>
       </c>
+      <c r="O17" s="50">
+        <v>0.1910714285125</v>
+      </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -10664,6 +10719,9 @@
       <c r="N18">
         <v>10</v>
       </c>
+      <c r="O18" s="50">
+        <v>0.1910714285125</v>
+      </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -10708,6 +10766,9 @@
       <c r="N19">
         <v>0</v>
       </c>
+      <c r="O19" s="50">
+        <v>0.1910714285125</v>
+      </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -10752,6 +10813,9 @@
       <c r="N20">
         <v>0</v>
       </c>
+      <c r="O20" s="50">
+        <v>0.1910714285125</v>
+      </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -10796,6 +10860,9 @@
       <c r="N21">
         <v>0</v>
       </c>
+      <c r="O21" s="50">
+        <v>0.1910714285125</v>
+      </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -10840,6 +10907,9 @@
       <c r="N22">
         <v>0</v>
       </c>
+      <c r="O22" s="50">
+        <v>0.20357142852499999</v>
+      </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -10884,6 +10954,9 @@
       <c r="N23">
         <v>0</v>
       </c>
+      <c r="O23" s="50">
+        <v>0.20357142852499999</v>
+      </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -10928,6 +11001,9 @@
       <c r="N24">
         <v>0</v>
       </c>
+      <c r="O24" s="50">
+        <v>0.20357142852499999</v>
+      </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -10972,6 +11048,9 @@
       <c r="N25">
         <v>0</v>
       </c>
+      <c r="O25" s="50">
+        <v>0.20357142852499999</v>
+      </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -11016,10 +11095,13 @@
       <c r="N26">
         <v>0</v>
       </c>
-      <c r="T26" s="50"/>
-      <c r="U26" s="50"/>
-      <c r="V26" s="50"/>
-      <c r="W26" s="50"/>
+      <c r="O26" s="50">
+        <v>0.20357142852499999</v>
+      </c>
+      <c r="T26" s="51"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="51"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
     </row>
@@ -11066,6 +11148,9 @@
       <c r="N27">
         <v>0</v>
       </c>
+      <c r="O27" s="50">
+        <v>0.20357142852499999</v>
+      </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -11110,6 +11195,9 @@
       <c r="N28">
         <v>0</v>
       </c>
+      <c r="O28" s="50">
+        <v>0.22857142855000001</v>
+      </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -11154,6 +11242,9 @@
       <c r="N29">
         <v>0</v>
       </c>
+      <c r="O29" s="50">
+        <v>0.22857142855000001</v>
+      </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -11198,6 +11289,9 @@
       <c r="N30">
         <v>0</v>
       </c>
+      <c r="O30" s="50">
+        <v>0.22857142855000001</v>
+      </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -11242,10 +11336,13 @@
       <c r="N31">
         <v>0</v>
       </c>
-      <c r="T31" s="51"/>
-      <c r="U31" s="51"/>
-      <c r="V31" s="51"/>
-      <c r="W31" s="51"/>
+      <c r="O31" s="50">
+        <v>0.2303571428375</v>
+      </c>
+      <c r="T31" s="52"/>
+      <c r="U31" s="52"/>
+      <c r="V31" s="52"/>
+      <c r="W31" s="52"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -11290,8 +11387,11 @@
       <c r="N32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O32" s="50">
+        <v>0.2303571428375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -11334,8 +11434,11 @@
       <c r="N33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O33" s="50">
+        <v>0.2303571428375</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
@@ -11378,8 +11481,11 @@
       <c r="N34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O34" s="50">
+        <v>0.2303571428375</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -11422,8 +11528,11 @@
       <c r="N35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O35" s="50">
+        <v>0.2303571428375</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>17</v>
       </c>
@@ -11466,8 +11575,11 @@
       <c r="N36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O36" s="50">
+        <v>0.2303571428375</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -11510,8 +11622,11 @@
       <c r="N37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O37" s="50">
+        <v>0.2303571428375</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>17</v>
       </c>
@@ -11554,8 +11669,11 @@
       <c r="N38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O38" s="50">
+        <v>0.2303571428375</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -11598,8 +11716,11 @@
       <c r="N39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O39" s="50">
+        <v>0.2303571428375</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -11642,8 +11763,11 @@
       <c r="N40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O40" s="50">
+        <v>0.2303571428375</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -11686,8 +11810,11 @@
       <c r="N41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O41" s="50">
+        <v>0.2303571428375</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -11730,8 +11857,11 @@
       <c r="N42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O42" s="50">
+        <v>0.2303571428375</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -11774,8 +11904,11 @@
       <c r="N43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O43" s="50">
+        <v>0.2303571428375</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -11818,8 +11951,11 @@
       <c r="N44">
         <v>30</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O44" s="50">
+        <v>0.2303571428375</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -11862,8 +11998,11 @@
       <c r="N45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O45" s="50">
+        <v>0.23214285712499999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -11906,8 +12045,11 @@
       <c r="N46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O46" s="50">
+        <v>0.23214285712499999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -11950,8 +12092,11 @@
       <c r="N47">
         <v>10</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O47" s="50">
+        <v>0.23214285712499999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -11994,8 +12139,11 @@
       <c r="N48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O48" s="50">
+        <v>0.23214285712499999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -12038,8 +12186,11 @@
       <c r="N49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O49" s="50">
+        <v>0.23214285712499999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -12082,8 +12233,11 @@
       <c r="N50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O50" s="50">
+        <v>0.23214285712499999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -12126,8 +12280,11 @@
       <c r="N51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O51" s="50">
+        <v>0.23214285712499999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -12170,8 +12327,11 @@
       <c r="N52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O52" s="50">
+        <v>0.23214285712499999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -12214,8 +12374,11 @@
       <c r="N53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O53" s="50">
+        <v>0.23214285712499999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -12258,8 +12421,11 @@
       <c r="N54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O54" s="50">
+        <v>0.23214285712499999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -12302,8 +12468,11 @@
       <c r="N55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O55" s="50">
+        <v>0.23214285712499999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -12346,8 +12515,11 @@
       <c r="N56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O56" s="50">
+        <v>0.85714285700000004</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -12390,8 +12562,11 @@
       <c r="N57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O57" s="50">
+        <v>0.85714285700000004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -12434,8 +12609,11 @@
       <c r="N58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O58" s="50">
+        <v>0.85714285700000004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>18</v>
       </c>
@@ -12478,8 +12656,11 @@
       <c r="N59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O59" s="50">
+        <v>0.85714285700000004</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -12522,8 +12703,11 @@
       <c r="N60">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O60" s="50">
+        <v>0.85714285700000004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -12566,8 +12750,11 @@
       <c r="N61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O61" s="50">
+        <v>0.85714285700000004</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -12610,11 +12797,14 @@
       <c r="N62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O62" s="50">
+        <v>0.85714285700000004</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B63" s="1"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B64" s="1"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
@@ -12665,17 +12855,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="47" t="s">
@@ -12708,60 +12898,60 @@
     </row>
     <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="48">
-        <v>67.912489671026307</v>
+        <v>68.160924174512843</v>
       </c>
       <c r="B3" s="48">
-        <v>33.756068778545512</v>
+        <v>33.750195912303219</v>
       </c>
       <c r="C3" s="48">
-        <v>14.858773192993356</v>
+        <v>14.877761152643359</v>
       </c>
       <c r="D3" s="48">
-        <v>2.5917252784166198</v>
+        <v>2.5898496040682621</v>
       </c>
       <c r="E3" s="48">
-        <v>4.5758386480009836</v>
+        <v>4.5725838942746373</v>
       </c>
       <c r="F3" s="48">
-        <v>0.23692081543175117</v>
+        <v>0.23881596429526403</v>
       </c>
       <c r="G3" s="48">
-        <v>0.14643957307611954</v>
+        <v>0.14674003833130575</v>
       </c>
       <c r="H3" s="48">
-        <v>17.345913510848902</v>
+        <v>17.576346880121402</v>
       </c>
       <c r="I3" s="48">
-        <v>-1.2318358627211052</v>
+        <v>-1.2277836087081295</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="49">
-        <v>42.974751019562667</v>
+        <v>44.199615985889501</v>
       </c>
       <c r="B4" s="49">
-        <v>22.154957269759365</v>
+        <v>22.423936882376182</v>
       </c>
       <c r="C4" s="49">
-        <v>10.618036368184788</v>
+        <v>10.741451308433424</v>
       </c>
       <c r="D4" s="49">
-        <v>2.1426871744494203</v>
+        <v>2.1493651950667534</v>
       </c>
       <c r="E4" s="49">
-        <v>3.4002983709785184</v>
+        <v>3.4371941076668193</v>
       </c>
       <c r="F4" s="49">
-        <v>0.43507938412963576</v>
+        <v>0.42004389838336215</v>
       </c>
       <c r="G4" s="49">
-        <v>0.29275188239167427</v>
+        <v>0.2830651056777681</v>
       </c>
       <c r="H4" s="49">
-        <v>13.744893968583026</v>
+        <v>14.027023260806274</v>
       </c>
       <c r="I4" s="49">
-        <v>2.3241042614663106</v>
+        <v>2.193051357750972</v>
       </c>
       <c r="J4" s="49"/>
     </row>
@@ -12777,25 +12967,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
+    <sheetView zoomScale="167" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="56"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="57"/>
     </row>
     <row r="2" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42" t="s">
@@ -12831,34 +13021,34 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
-        <v>61.435227212652997</v>
+        <v>61.558661367125907</v>
       </c>
       <c r="B3" s="6">
-        <v>26.043145467943607</v>
+        <v>25.998921812340129</v>
       </c>
       <c r="C3" s="6">
-        <v>15.304445517963448</v>
+        <v>15.236985492183043</v>
       </c>
       <c r="D3" s="6">
-        <v>3.007848284353746</v>
+        <v>2.9974134334398119</v>
       </c>
       <c r="E3" s="6">
-        <v>4.84768808346859</v>
+        <v>4.8351323478687673</v>
       </c>
       <c r="F3" s="6">
-        <v>0.33613692980725429</v>
+        <v>0.3329439577348503</v>
       </c>
       <c r="G3" s="6">
-        <v>1.1707852829209114E-2</v>
+        <v>1.2169130287011991E-2</v>
       </c>
       <c r="H3" s="6">
-        <v>16.764452656807816</v>
+        <v>16.925972121460397</v>
       </c>
       <c r="I3" s="33">
-        <v>-1.4185549531262349</v>
+        <v>-1.447804663653359</v>
       </c>
       <c r="J3" s="36">
-        <v>-2.8540350568931556</v>
+        <v>-3.7237839783619879</v>
       </c>
       <c r="K3" t="s">
         <v>8</v>
@@ -12866,34 +13056,34 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
-        <v>74.142912222020357</v>
+        <v>74.520321958725916</v>
       </c>
       <c r="B4" s="4">
-        <v>42.767580530223789</v>
+        <v>42.757659138998996</v>
       </c>
       <c r="C4" s="4">
-        <v>15.518237631050075</v>
+        <v>15.590195270266204</v>
       </c>
       <c r="D4" s="4">
-        <v>2.4117762705248738</v>
+        <v>2.4142629441182315</v>
       </c>
       <c r="E4" s="4">
-        <v>4.628133294025659</v>
+        <v>4.6372564142348178</v>
       </c>
       <c r="F4" s="4">
-        <v>0.15895016219232228</v>
+        <v>0.16376163299265328</v>
       </c>
       <c r="G4" s="4">
-        <v>0.31740882729769149</v>
+        <v>0.31718854440813593</v>
       </c>
       <c r="H4" s="4">
-        <v>15.236915220829209</v>
+        <v>15.576225576285669</v>
       </c>
       <c r="I4" s="34">
-        <v>-1.6553142269806427</v>
+        <v>-1.6230958557654807</v>
       </c>
       <c r="J4" s="37">
-        <v>2.6388378570265791</v>
+        <v>3.1784283501878239</v>
       </c>
       <c r="K4" t="s">
         <v>4</v>
@@ -12901,34 +13091,34 @@
     </row>
     <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
-        <v>67.209325595587885</v>
+        <v>67.407219325194006</v>
       </c>
       <c r="B5" s="7">
-        <v>28.824126268283695</v>
+        <v>28.876887340324448</v>
       </c>
       <c r="C5" s="7">
-        <v>11.962279294147022</v>
+        <v>12.047420965579359</v>
       </c>
       <c r="D5" s="7">
-        <v>2.1797752808761524</v>
+        <v>2.1830282861699168</v>
       </c>
       <c r="E5" s="7">
-        <v>3.8483146067958587</v>
+        <v>3.8460898503032661</v>
       </c>
       <c r="F5" s="7">
-        <v>0.21027287320576407</v>
+        <v>0.21464226291222893</v>
       </c>
       <c r="G5" s="7">
-        <v>0.10513643660288204</v>
+        <v>0.10732113145611447</v>
       </c>
       <c r="H5" s="7">
-        <v>24.369983948489548</v>
+        <v>24.45507487515566</v>
       </c>
       <c r="I5" s="32">
         <v>0</v>
       </c>
       <c r="J5" s="38">
-        <v>2.4414048167134634</v>
+        <v>2.9940088379451248</v>
       </c>
       <c r="K5" t="s">
         <v>3</v>
@@ -12936,34 +13126,34 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
-        <v>62.863886746105742</v>
+        <v>62.967824860193531</v>
       </c>
       <c r="B6" s="6">
-        <v>27.332253059156269</v>
+        <v>27.322044955257606</v>
       </c>
       <c r="C6" s="6">
-        <v>14.591226475559932</v>
+        <v>14.513346072781751</v>
       </c>
       <c r="D6" s="6">
-        <v>2.913004758147983</v>
+        <v>2.9012694307207929</v>
       </c>
       <c r="E6" s="6">
-        <v>4.7000400059062635</v>
+        <v>4.6844923306414517</v>
       </c>
       <c r="F6" s="6">
-        <v>0.31930485230614158</v>
+        <v>0.31593254335675225</v>
       </c>
       <c r="G6" s="6">
-        <v>1.1222706505161127E-2</v>
+        <v>1.1652147200477157E-2</v>
       </c>
       <c r="H6" s="6">
-        <v>18.412551169941192</v>
+        <v>18.606066967086367</v>
       </c>
       <c r="I6" s="33">
-        <v>-1.3729072773426678</v>
+        <v>-1.3948614778884973</v>
       </c>
       <c r="J6" s="39">
-        <v>-3.5386524343082773</v>
+        <v>-4.3840737299157748</v>
       </c>
       <c r="K6" t="s">
         <v>6</v>
@@ -12971,34 +13161,34 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
-        <v>75.598893101985681</v>
+        <v>76.09432048736798</v>
       </c>
       <c r="B7" s="4">
-        <v>45.582775042337076</v>
+        <v>45.636520132698813</v>
       </c>
       <c r="C7" s="4">
-        <v>16.333360238993215</v>
+        <v>16.432380232794362</v>
       </c>
       <c r="D7" s="4">
-        <v>2.453109789076342</v>
+        <v>2.4571347517789408</v>
       </c>
       <c r="E7" s="4">
-        <v>4.741373715523725</v>
+        <v>4.7549503546275851</v>
       </c>
       <c r="F7" s="4">
-        <v>0.17490535424202625</v>
+        <v>0.18070921986120261</v>
       </c>
       <c r="G7" s="4">
-        <v>0.34926987561595862</v>
+        <v>0.35001418440591714</v>
       </c>
       <c r="H7" s="4">
-        <v>13.007506659039624</v>
+        <v>13.32283662956074</v>
       </c>
       <c r="I7" s="34">
-        <v>-1.568807690834775</v>
+        <v>-1.5272640495890966</v>
       </c>
       <c r="J7" s="37">
-        <v>5.744164228515336</v>
+        <v>6.6197191097381562</v>
       </c>
       <c r="K7" t="s">
         <v>2</v>
@@ -13006,34 +13196,34 @@
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
-        <v>66.66644684798591</v>
+        <v>66.923429974139211</v>
       </c>
       <c r="B8" s="7">
-        <v>28.299630996237216</v>
+        <v>28.359052711988493</v>
       </c>
       <c r="C8" s="7">
-        <v>12.126199262342691</v>
+        <v>12.20702826630926</v>
       </c>
       <c r="D8" s="7">
-        <v>2.2457564575339224</v>
+        <v>2.2498090144879344</v>
       </c>
       <c r="E8" s="7">
-        <v>4.0214022140464643</v>
+        <v>4.0221543162980273</v>
       </c>
       <c r="F8" s="7">
-        <v>0.19335793359245107</v>
+        <v>0.19709702064440748</v>
       </c>
       <c r="G8" s="7">
-        <v>9.6678966796225535E-2</v>
+        <v>9.8548510322203742E-2</v>
       </c>
       <c r="H8" s="7">
-        <v>24.822878228580983</v>
+        <v>24.908326967042644</v>
       </c>
       <c r="I8" s="32">
         <v>0</v>
       </c>
       <c r="J8" s="38">
-        <v>2.6747641434348015</v>
+        <v>3.1451187619641061</v>
       </c>
       <c r="K8" t="s">
         <v>0</v>
@@ -13041,34 +13231,34 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
-        <v>66.809122269121815</v>
+        <v>66.940228077280494</v>
       </c>
       <c r="B9" s="6">
-        <v>26.95668838662808</v>
+        <v>26.979158474549241</v>
       </c>
       <c r="C9" s="6">
-        <v>12.629553617316676</v>
+        <v>12.689381933589125</v>
       </c>
       <c r="D9" s="6">
-        <v>2.3481848184219958</v>
+        <v>2.3520408162694357</v>
       </c>
       <c r="E9" s="6">
-        <v>4.4807480747467388</v>
+        <v>4.486394557767249</v>
       </c>
       <c r="F9" s="6">
-        <v>0.20352035203926994</v>
+        <v>0.2063492063567649</v>
       </c>
       <c r="G9" s="6">
-        <v>7.2057205726798759E-2</v>
+        <v>7.3129251708373824E-2</v>
       </c>
       <c r="H9" s="6">
-        <v>24.802462800850442</v>
+        <v>24.854727944519066</v>
       </c>
       <c r="I9" s="33">
-        <v>-1.9241088539888389</v>
+        <v>-1.9425874951282762</v>
       </c>
       <c r="J9" s="39">
-        <v>-9.0897751168231178</v>
+        <v>-9.7405982272386495</v>
       </c>
       <c r="K9" t="s">
         <v>7</v>
@@ -13076,34 +13266,34 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
-        <v>72.373412009827661</v>
+        <v>72.746265971384958</v>
       </c>
       <c r="B10" s="4">
-        <v>42.298993405094762</v>
+        <v>42.278243656653714</v>
       </c>
       <c r="C10" s="4">
-        <v>16.022323769742158</v>
+        <v>16.1086948067347</v>
       </c>
       <c r="D10" s="4">
-        <v>2.316413522791585</v>
+        <v>2.3161482088951084</v>
       </c>
       <c r="E10" s="4">
-        <v>4.4493875551529687</v>
+        <v>4.453543791357883</v>
       </c>
       <c r="F10" s="4">
-        <v>0.20979911807928678</v>
+        <v>0.21611233537341401</v>
       </c>
       <c r="G10" s="4">
-        <v>0.31641352279158536</v>
+        <v>0.31614820889510792</v>
       </c>
       <c r="H10" s="4">
-        <v>13.706644692373033</v>
+        <v>14.0140050576157</v>
       </c>
       <c r="I10" s="34">
-        <v>-1.4217285664763446</v>
+        <v>-1.3820406693873586</v>
       </c>
       <c r="J10" s="37">
-        <v>4.6991889002743497</v>
+        <v>5.5126317734811883</v>
       </c>
       <c r="K10" t="s">
         <v>5</v>
@@ -13111,34 +13301,34 @@
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
-        <v>63.649160385755181</v>
+        <v>63.852261032555759</v>
       </c>
       <c r="B11" s="5">
-        <v>29.092922829219592</v>
+        <v>29.118384498834605</v>
       </c>
       <c r="C11" s="5">
-        <v>15.051359595700772</v>
+        <v>14.959721273625995</v>
       </c>
       <c r="D11" s="5">
-        <v>3.2448579474757016</v>
+        <v>3.238010061498688</v>
       </c>
       <c r="E11" s="5">
-        <v>4.7945647676005461</v>
+        <v>4.7776618861651698</v>
       </c>
       <c r="F11" s="5">
-        <v>0.31101842941602353</v>
+        <v>0.30598099497845777</v>
       </c>
       <c r="G11" s="5">
-        <v>1.4705476618600078E-2</v>
+        <v>1.5384615386612288E-2</v>
       </c>
       <c r="H11" s="5">
-        <v>16.291902330881857</v>
+        <v>16.495436766366318</v>
       </c>
       <c r="I11" s="35">
-        <v>-0.42677874999538501</v>
+        <v>-0.43687383171064736</v>
       </c>
       <c r="J11" s="40">
-        <v>3.5453768199322515</v>
+        <v>3.1466853974271798</v>
       </c>
       <c r="K11" t="s">
         <v>1</v>
@@ -13289,28 +13479,28 @@
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:36" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="59"/>
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
       <c r="W1" s="8"/>
@@ -13329,56 +13519,56 @@
       <c r="AJ1" s="8"/>
     </row>
     <row r="2" spans="1:36" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="59" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="61"/>
     </row>
     <row r="3" spans="1:36" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="63" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="61"/>
-      <c r="S3" s="61"/>
-      <c r="T3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="62"/>
+      <c r="R3" s="62"/>
+      <c r="S3" s="62"/>
+      <c r="T3" s="63"/>
     </row>
     <row r="4" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
@@ -13444,64 +13634,64 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
-        <v>62.149556979379369</v>
+        <v>62.263243113659719</v>
       </c>
       <c r="B5" s="12">
-        <v>26.687699263549938</v>
+        <v>26.660483383798869</v>
       </c>
       <c r="C5" s="12">
-        <v>14.94783599676169</v>
+        <v>14.875165782482398</v>
       </c>
       <c r="D5" s="12">
-        <v>2.9604265212508647</v>
+        <v>2.9493414320803026</v>
       </c>
       <c r="E5" s="12">
-        <v>4.7738640446874268</v>
+        <v>4.7598123392551095</v>
       </c>
       <c r="F5" s="12">
-        <v>0.32772089105669794</v>
+        <v>0.32443825054580128</v>
       </c>
       <c r="G5" s="12">
-        <v>1.1465279667185121E-2</v>
+        <v>1.1910638743744574E-2</v>
       </c>
       <c r="H5" s="12">
-        <v>17.588501913374504</v>
+        <v>17.766019544273384</v>
       </c>
       <c r="I5" s="12">
-        <v>-1.3957311152344514</v>
+        <v>-1.4213330707709282</v>
       </c>
       <c r="J5" s="26">
-        <v>-3.1963437456007147</v>
+        <v>-4.0539288541388769</v>
       </c>
       <c r="K5" s="22">
-        <v>59.77048496578729</v>
+        <v>59.849836479178187</v>
       </c>
       <c r="L5" s="12">
-        <v>25.977783310945046</v>
+        <v>25.930714556147212</v>
       </c>
       <c r="M5" s="12">
-        <v>15.354033611844674</v>
+        <v>15.285129697569952</v>
       </c>
       <c r="N5" s="12">
-        <v>3.0082328809400809</v>
+        <v>2.9972841164421626</v>
       </c>
       <c r="O5" s="12">
-        <v>4.8017861629519896</v>
+        <v>4.7875629129473589</v>
       </c>
       <c r="P5" s="12">
-        <v>0.35260895221598398</v>
+        <v>0.34958969717288874</v>
       </c>
       <c r="Q5" s="12">
-        <v>1.2174230831793784E-2</v>
+        <v>1.2666078288082373E-2</v>
       </c>
       <c r="R5" s="12">
-        <v>16.261307408359063</v>
+        <v>16.417123240534789</v>
       </c>
       <c r="S5" s="12">
-        <v>-1.5227694991239451</v>
+        <v>-1.5571929548610064</v>
       </c>
       <c r="T5" s="17">
-        <v>-3.5567052061310243</v>
+        <v>-4.4808222023825603</v>
       </c>
       <c r="U5" t="s">
         <v>33</v>
@@ -13509,37 +13699,37 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
-        <v>68.517060157319335</v>
+        <v>68.826490927246937</v>
       </c>
       <c r="B6" s="13">
-        <v>35.812960255140339</v>
+        <v>35.817720972519467</v>
       </c>
       <c r="C6" s="13">
-        <v>15.818902878478331</v>
+        <v>15.834682862488702</v>
       </c>
       <c r="D6" s="13">
-        <v>2.7304790367150442</v>
+        <v>2.7272740926093766</v>
       </c>
       <c r="E6" s="13">
-        <v>4.7945308994961575</v>
+        <v>4.7950413512481767</v>
       </c>
       <c r="F6" s="13">
-        <v>0.25552114202464027</v>
+        <v>0.25682658879802645</v>
       </c>
       <c r="G6" s="13">
-        <v>0.18048886422258387</v>
+        <v>0.18109165734646457</v>
       </c>
       <c r="H6" s="13">
-        <v>14.88597965792372</v>
+        <v>15.124404375510569</v>
       </c>
       <c r="I6" s="13">
-        <v>-1.493681321980505</v>
+        <v>-1.4875343566212278</v>
       </c>
       <c r="J6" s="27">
-        <v>1.4450645858110902</v>
+        <v>1.4479675656880822</v>
       </c>
       <c r="K6" s="23">
-        <v>101.66395494367676</v>
+        <v>101.66394472361523</v>
       </c>
       <c r="L6" s="13" t="e">
         <v>#NUM!</v>
@@ -13574,37 +13764,37 @@
     </row>
     <row r="7" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
-        <v>64.050837030319457</v>
+        <v>64.241045670632559</v>
       </c>
       <c r="B7" s="14">
-        <v>27.171388232090411</v>
+        <v>27.178987262164313</v>
       </c>
       <c r="C7" s="14">
-        <v>13.715322390153069</v>
+        <v>13.722006879246152</v>
       </c>
       <c r="D7" s="14">
-        <v>2.6268023709438344</v>
+        <v>2.6236112239638731</v>
       </c>
       <c r="E7" s="14">
-        <v>4.4345451487575271</v>
+        <v>4.4286433320833973</v>
       </c>
       <c r="F7" s="14">
-        <v>0.26474743169985271</v>
+        <v>0.26502048918962889</v>
       </c>
       <c r="G7" s="14">
-        <v>5.4193409812717322E-2</v>
+        <v>5.535882030460787E-2</v>
       </c>
       <c r="H7" s="14">
-        <v>20.793665442694397</v>
+        <v>20.917149544251522</v>
       </c>
       <c r="I7" s="14">
-        <v>-0.70927747656311746</v>
+        <v>-0.72390233182667951</v>
       </c>
       <c r="J7" s="28">
-        <v>-8.9635456729177054E-2</v>
+        <v>-0.28933260819893736</v>
       </c>
       <c r="K7" s="30">
-        <v>71.765920070225988</v>
+        <v>71.763263486356266</v>
       </c>
       <c r="L7" s="14">
         <v>28</v>
@@ -13613,10 +13803,10 @@
         <v>14</v>
       </c>
       <c r="N7" s="14">
-        <v>2.9999999999999996</v>
+        <v>3</v>
       </c>
       <c r="O7" s="14">
-        <v>5.9999999999999991</v>
+        <v>6</v>
       </c>
       <c r="P7" s="14">
         <v>0</v>
@@ -13631,7 +13821,7 @@
         <v>0</v>
       </c>
       <c r="T7" s="31">
-        <v>6.9088004812459207</v>
+        <v>6.2592774224969174</v>
       </c>
       <c r="U7" t="s">
         <v>35</v>
@@ -13639,49 +13829,49 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
-        <v>68.503399484063053</v>
+        <v>68.74407340945973</v>
       </c>
       <c r="B8" s="13">
-        <v>35.049916794690027</v>
+        <v>35.039852047128299</v>
       </c>
       <c r="C8" s="13">
-        <v>15.054732053305003</v>
+        <v>15.051770671523977</v>
       </c>
       <c r="D8" s="13">
-        <v>2.6623905143364284</v>
+        <v>2.6577661874195124</v>
       </c>
       <c r="E8" s="13">
-        <v>4.6640866499659612</v>
+        <v>4.6608743724381352</v>
       </c>
       <c r="F8" s="13">
-        <v>0.23912750724923193</v>
+        <v>0.23984708817470277</v>
       </c>
       <c r="G8" s="13">
-        <v>0.1643157669014263</v>
+        <v>0.16442034580430653</v>
       </c>
       <c r="H8" s="13">
-        <v>16.8247331953852</v>
+        <v>17.091146271686018</v>
       </c>
       <c r="I8" s="13">
-        <v>-1.5141107521616552</v>
+        <v>-1.5089786668269891</v>
       </c>
       <c r="J8" s="27">
-        <v>-0.44990728864085194</v>
+        <v>-0.60282268986397369</v>
       </c>
       <c r="K8" s="23">
-        <v>71.894736841988916</v>
+        <v>71.893048128222148</v>
       </c>
       <c r="L8" s="13">
-        <v>31.294736842431018</v>
+        <v>31.299465240978016</v>
       </c>
       <c r="M8" s="13">
-        <v>8.5824175827049878</v>
+        <v>8.5865921790680702</v>
       </c>
       <c r="N8" s="13">
         <v>2</v>
       </c>
       <c r="O8" s="13">
-        <v>3.5</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="P8" s="13">
         <v>0</v>
@@ -13693,10 +13883,10 @@
         <v>45</v>
       </c>
       <c r="S8" s="13">
-        <v>-1.7368421053407199</v>
+        <v>-1.7379679145185738</v>
       </c>
       <c r="T8" s="18">
-        <v>-11.46303565018658</v>
+        <v>-12.902339425822223</v>
       </c>
       <c r="U8" t="s">
         <v>36</v>
@@ -13704,64 +13894,64 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
-        <v>74.870902662003019</v>
+        <v>75.307321223046955</v>
       </c>
       <c r="B9" s="13">
-        <v>44.175177786280429</v>
+        <v>44.197089635848904</v>
       </c>
       <c r="C9" s="13">
-        <v>15.925798935021646</v>
+        <v>16.011287751530283</v>
       </c>
       <c r="D9" s="13">
-        <v>2.4324430298006079</v>
+        <v>2.4356988479485864</v>
       </c>
       <c r="E9" s="13">
-        <v>4.684753504774692</v>
+        <v>4.6961033844312015</v>
       </c>
       <c r="F9" s="13">
-        <v>0.16692775821717426</v>
+        <v>0.17223542642692796</v>
       </c>
       <c r="G9" s="13">
-        <v>0.33333935145682503</v>
+        <v>0.33360136440702653</v>
       </c>
       <c r="H9" s="13">
-        <v>14.122210939934416</v>
+        <v>14.449531102923205</v>
       </c>
       <c r="I9" s="13">
-        <v>-1.6120609589077088</v>
+        <v>-1.5751799526772885</v>
       </c>
       <c r="J9" s="27">
-        <v>4.1915010427709571</v>
+        <v>4.899073729962991</v>
       </c>
       <c r="K9" s="23">
-        <v>74.688707874091122</v>
+        <v>75.173158376049784</v>
       </c>
       <c r="L9" s="13">
-        <v>45.582775042337076</v>
+        <v>45.636520132698813</v>
       </c>
       <c r="M9" s="13">
-        <v>16.333360238993215</v>
+        <v>16.432380232794362</v>
       </c>
       <c r="N9" s="13">
-        <v>2.453109789076342</v>
+        <v>2.4571347517789408</v>
       </c>
       <c r="O9" s="13">
-        <v>4.741373715523725</v>
+        <v>4.7549503546275851</v>
       </c>
       <c r="P9" s="13">
-        <v>0.17490535424202625</v>
+        <v>0.18070921986120261</v>
       </c>
       <c r="Q9" s="13">
-        <v>0.34926987561595862</v>
+        <v>0.35001418440591714</v>
       </c>
       <c r="R9" s="13">
-        <v>13.007506659039624</v>
+        <v>13.32283662956074</v>
       </c>
       <c r="S9" s="13">
-        <v>-1.6355214821944859</v>
+        <v>-1.5945519474692509</v>
       </c>
       <c r="T9" s="18">
-        <v>5.2001634839811572</v>
+        <v>6.0454382197238257</v>
       </c>
       <c r="U9" t="s">
         <v>37</v>
@@ -13769,34 +13959,34 @@
     </row>
     <row r="10" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
-        <v>70.40467953500314</v>
+        <v>70.721875966432563</v>
       </c>
       <c r="B10" s="13">
-        <v>35.533605763230504</v>
+        <v>35.558355925493743</v>
       </c>
       <c r="C10" s="13">
-        <v>13.822218446696382</v>
+        <v>13.898611768287733</v>
       </c>
       <c r="D10" s="13">
-        <v>2.3287663640293981</v>
+        <v>2.3320359793030829</v>
       </c>
       <c r="E10" s="13">
-        <v>4.3247677540360616</v>
+        <v>4.3297053652664221</v>
       </c>
       <c r="F10" s="13">
-        <v>0.17615404789238667</v>
+        <v>0.18042932681853038</v>
       </c>
       <c r="G10" s="13">
-        <v>0.20704389704695852</v>
+        <v>0.20786852736516984</v>
       </c>
       <c r="H10" s="13">
-        <v>20.029896724705097</v>
+        <v>20.242276271664156</v>
       </c>
       <c r="I10" s="13">
-        <v>-0.82765711349032134</v>
+        <v>-0.81154792788274033</v>
       </c>
       <c r="J10" s="27">
-        <v>2.656801000230689</v>
+        <v>3.1617735560759668</v>
       </c>
       <c r="K10" s="23" t="e">
         <v>#NUM!</v>
@@ -13834,37 +14024,37 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
-        <v>65.03660617084681</v>
+        <v>65.187522092693769</v>
       </c>
       <c r="B11" s="12">
-        <v>28.078189663719982</v>
+        <v>28.099466147791027</v>
       </c>
       <c r="C11" s="12">
-        <v>13.276752884853476</v>
+        <v>13.280383519180555</v>
       </c>
       <c r="D11" s="12">
-        <v>2.5463900195120677</v>
+        <v>2.5421488584453549</v>
       </c>
       <c r="E11" s="12">
-        <v>4.2741773063510609</v>
+        <v>4.2652910904723589</v>
       </c>
       <c r="F11" s="12">
-        <v>0.26478886275595281</v>
+        <v>0.26528740313449062</v>
       </c>
       <c r="G11" s="12">
-        <v>5.8179571554021578E-2</v>
+        <v>5.9486639328295815E-2</v>
       </c>
       <c r="H11" s="12">
-        <v>21.391267559215372</v>
+        <v>21.530570921121011</v>
       </c>
       <c r="I11" s="12">
-        <v>-0.68645363867133391</v>
+        <v>-0.69743073894424867</v>
       </c>
       <c r="J11" s="26">
-        <v>-0.54862380879740957</v>
+        <v>-0.69503244598532499</v>
       </c>
       <c r="K11" s="22">
-        <v>68.804142077699083</v>
+        <v>68.780250819069934</v>
       </c>
       <c r="L11" s="12">
         <v>30</v>
@@ -13899,34 +14089,34 @@
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
-        <v>71.40410934878679</v>
+        <v>71.750769906280993</v>
       </c>
       <c r="B12" s="13">
-        <v>37.203450655310384</v>
+        <v>37.256703736511632</v>
       </c>
       <c r="C12" s="13">
-        <v>14.14781976657012</v>
+        <v>14.239900599186861</v>
       </c>
       <c r="D12" s="13">
-        <v>2.3164425349762472</v>
+        <v>2.3200815189744288</v>
       </c>
       <c r="E12" s="13">
-        <v>4.2948441611597916</v>
+        <v>4.3005201024654252</v>
       </c>
       <c r="F12" s="13">
-        <v>0.19258911372389514</v>
+        <v>0.19767574138671579</v>
       </c>
       <c r="G12" s="13">
-        <v>0.22720315610942032</v>
+        <v>0.22866765793101579</v>
       </c>
       <c r="H12" s="13">
-        <v>18.688745303764584</v>
+        <v>18.8889557523582</v>
       </c>
       <c r="I12" s="13">
-        <v>-0.7844038454173875</v>
+        <v>-0.76363202479454828</v>
       </c>
       <c r="J12" s="27">
-        <v>4.092784522614398</v>
+        <v>4.8068639738416392</v>
       </c>
       <c r="K12" s="23">
         <v>83</v>
@@ -13964,94 +14154,94 @@
     </row>
     <row r="13" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19">
-        <v>66.937886221786897</v>
+        <v>67.165324649666616</v>
       </c>
       <c r="B13" s="25">
-        <v>28.561878632260456</v>
+        <v>28.61797002615647</v>
       </c>
       <c r="C13" s="25">
-        <v>12.044239278244856</v>
+        <v>12.127224615944311</v>
       </c>
       <c r="D13" s="25">
-        <v>2.2127658692050374</v>
+        <v>2.2164186503289258</v>
       </c>
       <c r="E13" s="25">
-        <v>3.9348584104211612</v>
+        <v>3.9341220833006467</v>
       </c>
       <c r="F13" s="25">
-        <v>0.20181540339910758</v>
+        <v>0.20586964177831821</v>
       </c>
       <c r="G13" s="25">
-        <v>0.10090770169955379</v>
+        <v>0.1029348208891591</v>
       </c>
       <c r="H13" s="25">
-        <v>24.596431088535265</v>
+        <v>24.68170092109915</v>
       </c>
       <c r="I13" s="25">
         <v>0</v>
       </c>
       <c r="J13" s="29">
-        <v>2.558084480074128</v>
+        <v>3.0695637999546177</v>
       </c>
       <c r="K13" s="24">
-        <v>66.099174361504566</v>
+        <v>66.374133482363504</v>
       </c>
       <c r="L13" s="25">
-        <v>28.325842696545887</v>
+        <v>28.39101497503113</v>
       </c>
       <c r="M13" s="25">
-        <v>11.962279294147022</v>
+        <v>12.047420965579359</v>
       </c>
       <c r="N13" s="25">
-        <v>2.1797752808761524</v>
+        <v>2.1830282861699168</v>
       </c>
       <c r="O13" s="25">
-        <v>3.8483146067958587</v>
+        <v>3.8460898503032661</v>
       </c>
       <c r="P13" s="25">
-        <v>0.21027287320576407</v>
+        <v>0.21464226291222893</v>
       </c>
       <c r="Q13" s="25">
-        <v>0.10513643660288204</v>
+        <v>0.10732113145611447</v>
       </c>
       <c r="R13" s="25">
-        <v>24.369983948489548</v>
+        <v>24.45507487515566</v>
       </c>
       <c r="S13" s="25">
         <v>0</v>
       </c>
       <c r="T13" s="20">
-        <v>2.2930925827348165</v>
+        <v>2.8571809414190055</v>
       </c>
       <c r="U13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:36" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="62"/>
-      <c r="K14" s="63" t="s">
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="61"/>
-      <c r="M14" s="61"/>
-      <c r="N14" s="61"/>
-      <c r="O14" s="61"/>
-      <c r="P14" s="61"/>
-      <c r="Q14" s="61"/>
-      <c r="R14" s="61"/>
-      <c r="S14" s="61"/>
-      <c r="T14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="62"/>
+      <c r="O14" s="62"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="62"/>
+      <c r="T14" s="63"/>
     </row>
     <row r="15" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
@@ -14118,64 +14308,64 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
-        <v>63.081470037327861</v>
+        <v>63.19864010638387</v>
       </c>
       <c r="B16" s="9">
-        <v>26.741497088165566</v>
+        <v>26.724218401948946</v>
       </c>
       <c r="C16" s="9">
-        <v>14.484179520872686</v>
+        <v>14.438009012703741</v>
       </c>
       <c r="D16" s="9">
-        <v>2.8379781806850906</v>
+        <v>2.8298813089181296</v>
       </c>
       <c r="E16" s="9">
-        <v>4.7152408506992893</v>
+        <v>4.7051287829575372</v>
       </c>
       <c r="F16" s="9">
-        <v>0.30288078325321233</v>
+        <v>0.30082044170799399</v>
       </c>
       <c r="G16" s="9">
-        <v>2.358366487910785E-2</v>
+        <v>2.4154361336670423E-2</v>
       </c>
       <c r="H16" s="9">
-        <v>19.031294090869693</v>
+        <v>19.18376122432252</v>
       </c>
       <c r="I16" s="9">
-        <v>-1.5014066629853289</v>
+        <v>-1.5255839556423978</v>
       </c>
       <c r="J16" s="17">
-        <v>-4.3750300198451972</v>
+        <v>-5.1912627287588347</v>
       </c>
       <c r="K16" s="22">
-        <v>66.253077975379753</v>
+        <v>66.253129346317991</v>
       </c>
       <c r="L16" s="9">
-        <v>24.856361149424551</v>
+        <v>24.860917941909836</v>
       </c>
       <c r="M16" s="9">
-        <v>11.795497185762034</v>
+        <v>11.795801526739227</v>
       </c>
       <c r="N16" s="9">
-        <v>2.5604278074092823</v>
+        <v>2.5593035907795647</v>
       </c>
       <c r="O16" s="9">
-        <v>4.4213903742373875</v>
+        <v>4.4200217626881662</v>
       </c>
       <c r="P16" s="9">
-        <v>0.25561497326875804</v>
+        <v>0.25571273123655958</v>
       </c>
       <c r="Q16" s="9">
         <v>0</v>
       </c>
       <c r="R16" s="9">
-        <v>26.529080674602856</v>
+        <v>26.517175571671412</v>
       </c>
       <c r="S16" s="9">
-        <v>-3.4336525308950323</v>
+        <v>-3.4353268429564316</v>
       </c>
       <c r="T16" s="17">
-        <v>-20.664353527672162</v>
+        <v>-22.243572804720383</v>
       </c>
       <c r="U16" t="s">
         <v>33</v>
@@ -14186,34 +14376,34 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
-        <v>68.175472579679834</v>
+        <v>68.449238357253648</v>
       </c>
       <c r="B17" s="10">
-        <v>34.041705881437892</v>
+        <v>34.050008472925427</v>
       </c>
       <c r="C17" s="10">
-        <v>15.181033026246002</v>
+        <v>15.205622676708789</v>
       </c>
       <c r="D17" s="10">
-        <v>2.6540201930564344</v>
+        <v>2.6522274373413888</v>
       </c>
       <c r="E17" s="10">
-        <v>4.7317743345462739</v>
+        <v>4.7333119925519913</v>
       </c>
       <c r="F17" s="10">
-        <v>0.24512098402756619</v>
+        <v>0.24673111230977413</v>
       </c>
       <c r="G17" s="10">
-        <v>0.15880253252342685</v>
+        <v>0.15949917621884641</v>
       </c>
       <c r="H17" s="10">
-        <v>16.869276286509063</v>
+        <v>17.070469089312269</v>
       </c>
       <c r="I17" s="10">
-        <v>-1.5797668283821718</v>
+        <v>-1.5785449843226373</v>
       </c>
       <c r="J17" s="18">
-        <v>-0.66190335471574802</v>
+        <v>-0.78974559289725732</v>
       </c>
       <c r="K17" s="23" t="e">
         <v>#NUM!</v>
@@ -14251,34 +14441,34 @@
     </row>
     <row r="18" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
-        <v>64.602494078079928</v>
+        <v>64.780882151962146</v>
       </c>
       <c r="B18" s="10">
-        <v>27.128448262997942</v>
+        <v>27.139021504641299</v>
       </c>
       <c r="C18" s="10">
-        <v>13.49816863558579</v>
+        <v>13.515481890114746</v>
       </c>
       <c r="D18" s="10">
-        <v>2.5710788604394663</v>
+        <v>2.5692971424249853</v>
       </c>
       <c r="E18" s="10">
-        <v>4.4437857339553695</v>
+        <v>4.4401935772201675</v>
       </c>
       <c r="F18" s="10">
-        <v>0.25250201576773612</v>
+        <v>0.25328623262305611</v>
       </c>
       <c r="G18" s="10">
-        <v>5.7766168995533607E-2</v>
+        <v>5.8912906585361059E-2</v>
       </c>
       <c r="H18" s="10">
-        <v>21.595424914325605</v>
+        <v>21.704665224305032</v>
       </c>
       <c r="I18" s="10">
-        <v>-0.95224375204826173</v>
+        <v>-0.96763936448699894</v>
       </c>
       <c r="J18" s="18">
-        <v>-1.8896633887479708</v>
+        <v>-2.1795857320068821</v>
       </c>
       <c r="K18" s="23">
         <v>72</v>
@@ -14290,10 +14480,10 @@
         <v>14</v>
       </c>
       <c r="N18" s="10">
-        <v>2.9999999999999996</v>
+        <v>3</v>
       </c>
       <c r="O18" s="10">
-        <v>5.9999999999999991</v>
+        <v>6</v>
       </c>
       <c r="P18" s="10">
         <v>0</v>
@@ -14308,7 +14498,7 @@
         <v>0</v>
       </c>
       <c r="T18" s="18">
-        <v>6.9305881518404489</v>
+        <v>6.2807017275152521</v>
       </c>
       <c r="U18" t="s">
         <v>35</v>
@@ -14316,34 +14506,34 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
-        <v>68.164544041074805</v>
+        <v>68.38330434302388</v>
       </c>
       <c r="B19" s="9">
-        <v>33.431271113077642</v>
+        <v>33.427713332612491</v>
       </c>
       <c r="C19" s="9">
-        <v>14.569696366107337</v>
+        <v>14.579292923937007</v>
       </c>
       <c r="D19" s="9">
-        <v>2.5995493751535421</v>
+        <v>2.5966211131894972</v>
       </c>
       <c r="E19" s="9">
-        <v>4.6274189349221171</v>
+        <v>4.6259784095039578</v>
       </c>
       <c r="F19" s="9">
-        <v>0.23200607620723951</v>
+        <v>0.2331475118111152</v>
       </c>
       <c r="G19" s="9">
-        <v>0.14586405466650079</v>
+        <v>0.14616212698511999</v>
       </c>
       <c r="H19" s="9">
-        <v>18.420279116478248</v>
+        <v>18.643862606252629</v>
       </c>
       <c r="I19" s="9">
-        <v>-1.596110372527092</v>
+        <v>-1.5957004324872464</v>
       </c>
       <c r="J19" s="17">
-        <v>-2.1778808542773049</v>
+        <v>-2.4303777973389047</v>
       </c>
       <c r="K19" s="22" t="e">
         <v>#NUM!</v>
@@ -14381,34 +14571,34 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
-        <v>73.258546583426778</v>
+        <v>73.633902593893666</v>
       </c>
       <c r="B20" s="10">
-        <v>40.731479906349961</v>
+        <v>40.753503403588972</v>
       </c>
       <c r="C20" s="10">
-        <v>15.266549871480652</v>
+        <v>15.346906587942049</v>
       </c>
       <c r="D20" s="10">
-        <v>2.4155913875248856</v>
+        <v>2.4189672416127563</v>
       </c>
       <c r="E20" s="10">
-        <v>4.6439524187691017</v>
+        <v>4.654161619098411</v>
       </c>
       <c r="F20" s="10">
-        <v>0.1742462769815934</v>
+        <v>0.17905818241289534</v>
       </c>
       <c r="G20" s="10">
-        <v>0.28108292231081977</v>
+        <v>0.28150694186729602</v>
       </c>
       <c r="H20" s="10">
-        <v>16.258261312117622</v>
+        <v>16.530570471242378</v>
       </c>
       <c r="I20" s="10">
-        <v>-1.6744705379239349</v>
+        <v>-1.6486614611674859</v>
       </c>
       <c r="J20" s="18">
-        <v>1.5352458108521443</v>
+        <v>1.971139338522665</v>
       </c>
       <c r="K20" s="23" t="e">
         <v>#NUM!</v>
@@ -14446,34 +14636,34 @@
     </row>
     <row r="21" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
-        <v>69.685568081826872</v>
+        <v>69.965546388602149</v>
       </c>
       <c r="B21" s="10">
-        <v>33.818222287910018</v>
+        <v>33.842516435304844</v>
       </c>
       <c r="C21" s="10">
-        <v>13.58368548082044</v>
+        <v>13.656765801348012</v>
       </c>
       <c r="D21" s="10">
-        <v>2.3326500549079179</v>
+        <v>2.3360369466963533</v>
       </c>
       <c r="E21" s="10">
-        <v>4.3559638181781972</v>
+        <v>4.3610432037665872</v>
       </c>
       <c r="F21" s="10">
-        <v>0.18162730872176333</v>
+        <v>0.18561330272617729</v>
       </c>
       <c r="G21" s="10">
-        <v>0.18004655878292658</v>
+        <v>0.18092067223381064</v>
       </c>
       <c r="H21" s="10">
-        <v>20.984409939934164</v>
+        <v>21.164766606235141</v>
       </c>
       <c r="I21" s="10">
-        <v>-1.0469474615900247</v>
+        <v>-1.0377558413318475</v>
       </c>
       <c r="J21" s="18">
-        <v>0.30748577681992728</v>
+        <v>0.58129919941304675</v>
       </c>
       <c r="K21" s="23" t="e">
         <v>#NUM!</v>
@@ -14511,34 +14701,34 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
-        <v>65.391109390501811</v>
+        <v>65.538063289611117</v>
       </c>
       <c r="B22" s="9">
-        <v>27.853889408301605</v>
+        <v>27.87540461314267</v>
       </c>
       <c r="C22" s="9">
-        <v>13.147313031346116</v>
+        <v>13.16218320206227</v>
       </c>
       <c r="D22" s="9">
-        <v>2.5067489792940534</v>
+        <v>2.5041272500101712</v>
       </c>
       <c r="E22" s="9">
-        <v>4.3154914600301968</v>
+        <v>4.3095117839313364</v>
       </c>
       <c r="F22" s="9">
-        <v>0.25253516061261622</v>
+        <v>0.25349976377894545</v>
       </c>
       <c r="G22" s="9">
-        <v>6.095509838857701E-2</v>
+        <v>6.2215161804311414E-2</v>
       </c>
       <c r="H22" s="9">
-        <v>22.073506607542384</v>
+        <v>22.195402325800622</v>
       </c>
       <c r="I22" s="9">
-        <v>-0.93398468173483484</v>
+        <v>-0.94646209018105409</v>
       </c>
       <c r="J22" s="17">
-        <v>-2.256854070402551</v>
+        <v>-2.5041456022359907</v>
       </c>
       <c r="K22" s="22">
         <v>73</v>
@@ -14576,34 +14766,34 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
-        <v>70.485111932853798</v>
+        <v>70.788661540480888</v>
       </c>
       <c r="B23" s="10">
-        <v>35.154098201573923</v>
+        <v>35.201194684119159</v>
       </c>
       <c r="C23" s="10">
-        <v>13.844166536719431</v>
+        <v>13.929796866067312</v>
       </c>
       <c r="D23" s="10">
-        <v>2.3227909916653973</v>
+        <v>2.3264733784334304</v>
       </c>
       <c r="E23" s="10">
-        <v>4.3320249438771814</v>
+        <v>4.3376949935257896</v>
       </c>
       <c r="F23" s="10">
-        <v>0.1947753613869701</v>
+        <v>0.19941043438072562</v>
       </c>
       <c r="G23" s="10">
-        <v>0.196173966032896</v>
+        <v>0.19755997668648739</v>
       </c>
       <c r="H23" s="10">
-        <v>19.911488803181754</v>
+        <v>20.082110190790374</v>
       </c>
       <c r="I23" s="10">
-        <v>-1.0123448471316778</v>
+        <v>-0.99942311886129398</v>
       </c>
       <c r="J23" s="18">
-        <v>1.4562725947268966</v>
+        <v>1.8973715336255768</v>
       </c>
       <c r="K23" s="23" t="e">
         <v>#NUM!</v>
@@ -14641,94 +14831,94 @@
     </row>
     <row r="24" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="19">
-        <v>66.912133431253878</v>
+        <v>67.120305335189386</v>
       </c>
       <c r="B24" s="19">
-        <v>28.240840583133981</v>
+        <v>28.290207715835027</v>
       </c>
       <c r="C24" s="19">
-        <v>12.161302146059219</v>
+        <v>12.239656079473274</v>
       </c>
       <c r="D24" s="19">
-        <v>2.2398496590484291</v>
+        <v>2.2435430835170278</v>
       </c>
       <c r="E24" s="19">
-        <v>4.0440363432862769</v>
+        <v>4.0445765781939667</v>
       </c>
       <c r="F24" s="19">
-        <v>0.20215639312714004</v>
+        <v>0.20596555469400757</v>
       </c>
       <c r="G24" s="19">
-        <v>9.5137602505002777E-2</v>
+        <v>9.697370705300204E-2</v>
       </c>
       <c r="H24" s="19">
-        <v>24.637637430998304</v>
+        <v>24.716306325783133</v>
       </c>
       <c r="I24" s="19">
-        <v>-0.3848217707977678</v>
+        <v>-0.38851749902565524</v>
       </c>
       <c r="J24" s="20">
-        <v>0.22851256069468029</v>
+        <v>0.50753139451596407</v>
       </c>
       <c r="K24" s="24">
-        <v>65.016795865832179</v>
+        <v>65.410569106348078</v>
       </c>
       <c r="L24" s="19">
-        <v>29.739018087933815</v>
+        <v>29.894308943348534</v>
       </c>
       <c r="M24" s="19">
-        <v>13.585271317922</v>
+        <v>13.768292683232202</v>
       </c>
       <c r="N24" s="19">
         <v>2</v>
       </c>
       <c r="O24" s="19">
-        <v>4.3385012919952723</v>
+        <v>4.3495934959534672</v>
       </c>
       <c r="P24" s="19">
-        <v>0.16925064599763637</v>
+        <v>0.17479674797673342</v>
       </c>
       <c r="Q24" s="19">
-        <v>0.16925064599763637</v>
+        <v>0.17479674797673342</v>
       </c>
       <c r="R24" s="19">
-        <v>21.692506459976364</v>
+        <v>21.747967479767333</v>
       </c>
       <c r="S24" s="19">
         <v>0</v>
       </c>
       <c r="T24" s="20">
-        <v>5.0789414150025314</v>
+        <v>6.1024623343456987</v>
       </c>
       <c r="U24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="61" t="s">
+      <c r="A25" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="62"/>
-      <c r="K25" s="63" t="s">
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="L25" s="61"/>
-      <c r="M25" s="61"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="61"/>
-      <c r="P25" s="61"/>
-      <c r="Q25" s="61"/>
-      <c r="R25" s="61"/>
-      <c r="S25" s="61"/>
-      <c r="T25" s="62"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="62"/>
+      <c r="N25" s="62"/>
+      <c r="O25" s="62"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="62"/>
+      <c r="R25" s="62"/>
+      <c r="S25" s="62"/>
+      <c r="T25" s="63"/>
     </row>
     <row r="26" spans="1:22" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
@@ -14795,34 +14985,34 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
-        <v>64.194327985469016</v>
+        <v>64.35984768520477</v>
       </c>
       <c r="B27" s="12">
-        <v>29.809958091858903</v>
+        <v>29.784035438369834</v>
       </c>
       <c r="C27" s="12">
-        <v>15.162733551357784</v>
+        <v>15.121871587332858</v>
       </c>
       <c r="D27" s="12">
-        <v>2.8316239215590087</v>
+        <v>2.8227027874432635</v>
       </c>
       <c r="E27" s="12">
-        <v>4.7089687467805348</v>
+        <v>4.6985586296756647</v>
       </c>
       <c r="F27" s="12">
-        <v>0.30413653646121575</v>
+        <v>0.30277306751132382</v>
       </c>
       <c r="G27" s="12">
-        <v>7.2454928292065165E-2</v>
+        <v>7.2758152774017246E-2</v>
       </c>
       <c r="H27" s="12">
-        <v>16.81213046917421</v>
+        <v>17.015616646941847</v>
       </c>
       <c r="I27" s="9">
-        <v>-1.4009306054828301</v>
+        <v>-1.4134745904942143</v>
       </c>
       <c r="J27" s="17">
-        <v>-1.6172372164257025</v>
+        <v>-2.1406167286148636</v>
       </c>
       <c r="K27" s="22" t="e">
         <v>#NUM!</v>
@@ -14863,34 +15053,34 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
-        <v>69.288330527820989</v>
+        <v>69.610445936074541</v>
       </c>
       <c r="B28" s="13">
-        <v>37.110166885131221</v>
+        <v>37.109825509346322</v>
       </c>
       <c r="C28" s="13">
-        <v>15.859587056731096</v>
+        <v>15.889485251337902</v>
       </c>
       <c r="D28" s="13">
-        <v>2.6476659339303525</v>
+        <v>2.6450489158665227</v>
       </c>
       <c r="E28" s="13">
-        <v>4.7255022306275194</v>
+        <v>4.7267418392701179</v>
       </c>
       <c r="F28" s="13">
-        <v>0.24637673723556958</v>
+        <v>0.24868373811310396</v>
       </c>
       <c r="G28" s="13">
-        <v>0.20767379593638419</v>
+        <v>0.20810296765619324</v>
       </c>
       <c r="H28" s="13">
-        <v>14.650112664813582</v>
+        <v>14.902324511931596</v>
       </c>
       <c r="I28" s="10">
-        <v>-1.479290770879673</v>
+        <v>-1.4664356191744541</v>
       </c>
       <c r="J28" s="18">
-        <v>2.0958894487037396</v>
+        <v>2.2609004072467056</v>
       </c>
       <c r="K28" s="23" t="e">
         <v>#NUM!</v>
@@ -14928,34 +15118,34 @@
     </row>
     <row r="29" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
-        <v>65.715352026221098</v>
+        <v>65.942089730783039</v>
       </c>
       <c r="B29" s="13">
-        <v>30.196909266691286</v>
+        <v>30.198838541062194</v>
       </c>
       <c r="C29" s="13">
-        <v>14.176722666070887</v>
+        <v>14.199344464743863</v>
       </c>
       <c r="D29" s="13">
-        <v>2.5647246013133844</v>
+        <v>2.5621186209501206</v>
       </c>
       <c r="E29" s="13">
-        <v>4.4375136300366149</v>
+        <v>4.433623423938295</v>
       </c>
       <c r="F29" s="13">
-        <v>0.25375776897573954</v>
+        <v>0.25523885842638594</v>
       </c>
       <c r="G29" s="13">
-        <v>0.10663743240849093</v>
+        <v>0.10751669802270789</v>
       </c>
       <c r="H29" s="13">
-        <v>19.376261292630126</v>
+        <v>19.536520646924359</v>
       </c>
       <c r="I29" s="10">
-        <v>-0.85176769454576284</v>
+        <v>-0.85552999933881535</v>
       </c>
       <c r="J29" s="18">
-        <v>0.86812941467152915</v>
+        <v>0.87106026813709503</v>
       </c>
       <c r="K29" s="23" t="e">
         <v>#NUM!</v>
@@ -14993,34 +15183,34 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
-        <v>69.277401989215974</v>
+        <v>69.544511921844773</v>
       </c>
       <c r="B30" s="12">
-        <v>36.499732116770971</v>
+        <v>36.487530369033379</v>
       </c>
       <c r="C30" s="12">
-        <v>15.248250396592434</v>
+        <v>15.263155498566121</v>
       </c>
       <c r="D30" s="12">
-        <v>2.5931951160274598</v>
+        <v>2.5894425917146315</v>
       </c>
       <c r="E30" s="12">
-        <v>4.6211468310033625</v>
+        <v>4.6194082562220853</v>
       </c>
       <c r="F30" s="12">
-        <v>0.23326182941524293</v>
+        <v>0.23510013761444498</v>
       </c>
       <c r="G30" s="12">
-        <v>0.19473531807945813</v>
+        <v>0.19476591842246682</v>
       </c>
       <c r="H30" s="12">
-        <v>16.201115494782766</v>
+        <v>16.475718028871956</v>
       </c>
       <c r="I30" s="9">
-        <v>-1.4956343150245932</v>
+        <v>-1.4835910673390631</v>
       </c>
       <c r="J30" s="17">
-        <v>0.57991194914218891</v>
+        <v>0.62026820280505834</v>
       </c>
       <c r="K30" s="22" t="e">
         <v>#NUM!</v>
@@ -15058,64 +15248,64 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
-        <v>74.371404531567947</v>
+        <v>74.795110172714558</v>
       </c>
       <c r="B31" s="13">
-        <v>43.799940910043297</v>
+        <v>43.813320440009861</v>
       </c>
       <c r="C31" s="13">
-        <v>15.945103901965748</v>
+        <v>16.030769162571168</v>
       </c>
       <c r="D31" s="13">
-        <v>2.4092371283988032</v>
+        <v>2.4117887201378907</v>
       </c>
       <c r="E31" s="13">
-        <v>4.6376803148503472</v>
+        <v>4.6475914658165376</v>
       </c>
       <c r="F31" s="13">
-        <v>0.17550203018959676</v>
+        <v>0.18101080821622517</v>
       </c>
       <c r="G31" s="13">
-        <v>0.3299541857237771</v>
+        <v>0.3301107333046428</v>
       </c>
       <c r="H31" s="13">
-        <v>14.039097690422139</v>
+        <v>14.362425893861703</v>
       </c>
       <c r="I31" s="10">
-        <v>-1.5739944804214361</v>
+        <v>-1.5365520960193026</v>
       </c>
       <c r="J31" s="18">
-        <v>4.2930386142716319</v>
+        <v>5.0217853386666338</v>
       </c>
       <c r="K31" s="23">
-        <v>74.535071434279288</v>
+        <v>75.019313935916529</v>
       </c>
       <c r="L31" s="13">
-        <v>45.582775042337076</v>
+        <v>45.636520132698813</v>
       </c>
       <c r="M31" s="13">
-        <v>16.333360238993215</v>
+        <v>16.432380232794362</v>
       </c>
       <c r="N31" s="13">
-        <v>2.453109789076342</v>
+        <v>2.4571347517789408</v>
       </c>
       <c r="O31" s="13">
-        <v>4.741373715523725</v>
+        <v>4.7549503546275851</v>
       </c>
       <c r="P31" s="13">
-        <v>0.17490535424202625</v>
+        <v>0.18070921986120261</v>
       </c>
       <c r="Q31" s="13">
-        <v>0.34926987561595862</v>
+        <v>0.35001418440591714</v>
       </c>
       <c r="R31" s="13">
-        <v>13.007506659039624</v>
+        <v>13.32283662956074</v>
       </c>
       <c r="S31" s="13">
-        <v>-1.6530793445838095</v>
+        <v>-1.6122937397233021</v>
       </c>
       <c r="T31" s="18">
-        <v>5.0649884562557341</v>
+        <v>5.9020754756030751</v>
       </c>
       <c r="U31" t="s">
         <v>37</v>
@@ -15123,34 +15313,34 @@
     </row>
     <row r="32" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
-        <v>70.798426029968056</v>
+        <v>71.126753967423042</v>
       </c>
       <c r="B32" s="13">
-        <v>36.886683291603354</v>
+        <v>36.90233347172574</v>
       </c>
       <c r="C32" s="13">
-        <v>14.262239511305538</v>
+        <v>14.340628375977127</v>
       </c>
       <c r="D32" s="13">
-        <v>2.3262957957818355</v>
+        <v>2.3288584252214881</v>
       </c>
       <c r="E32" s="13">
-        <v>4.3496917142594427</v>
+        <v>4.3544730504847147</v>
       </c>
       <c r="F32" s="13">
-        <v>0.18288306192976669</v>
+        <v>0.1875659285295071</v>
       </c>
       <c r="G32" s="13">
-        <v>0.22891782219588391</v>
+        <v>0.22952446367115745</v>
       </c>
       <c r="H32" s="13">
-        <v>18.765246318238685</v>
+        <v>18.996622028854468</v>
       </c>
       <c r="I32" s="10">
-        <v>-0.94647140408752595</v>
+        <v>-0.92564647618366391</v>
       </c>
       <c r="J32" s="18">
-        <v>3.0652785802394238</v>
+        <v>3.6319451995570171</v>
       </c>
       <c r="K32" s="23" t="e">
         <v>#NUM!</v>
@@ -15188,40 +15378,40 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
-        <v>66.50396733864298</v>
+        <v>66.699270868432009</v>
       </c>
       <c r="B33" s="12">
-        <v>30.922350411994938</v>
+        <v>30.935221649563562</v>
       </c>
       <c r="C33" s="12">
-        <v>13.825867061831213</v>
+        <v>13.846045776691383</v>
       </c>
       <c r="D33" s="12">
-        <v>2.500394720167971</v>
+        <v>2.4969487285353056</v>
       </c>
       <c r="E33" s="12">
-        <v>4.3092193561114431</v>
+        <v>4.3029416306494639</v>
       </c>
       <c r="F33" s="12">
-        <v>0.25379091382061963</v>
+        <v>0.25545238958227529</v>
       </c>
       <c r="G33" s="12">
-        <v>0.10982636180153434</v>
+        <v>0.11081895324165822</v>
       </c>
       <c r="H33" s="12">
-        <v>19.854342985846905</v>
+        <v>20.027257748419949</v>
       </c>
       <c r="I33" s="9">
-        <v>-0.83350862423233596</v>
+        <v>-0.83435272503287072</v>
       </c>
       <c r="J33" s="17">
-        <v>0.50093873301694769</v>
+        <v>0.54650039790797544</v>
       </c>
       <c r="K33" s="22">
-        <v>68.999999999999986</v>
+        <v>69</v>
       </c>
       <c r="L33" s="12">
-        <v>29.999999999999996</v>
+        <v>30</v>
       </c>
       <c r="M33" s="12" t="e">
         <v>#NUM!</v>
@@ -15253,34 +15443,34 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="10">
-        <v>71.597969880994967</v>
+        <v>71.949869119301781</v>
       </c>
       <c r="B34" s="13">
-        <v>38.22255920526726</v>
+        <v>38.261011720540047</v>
       </c>
       <c r="C34" s="13">
-        <v>14.522720567204527</v>
+        <v>14.613659440696429</v>
       </c>
       <c r="D34" s="13">
-        <v>2.3164367325393149</v>
+        <v>2.3192948569585647</v>
       </c>
       <c r="E34" s="13">
-        <v>4.3257528399584277</v>
+        <v>4.3311248402439171</v>
       </c>
       <c r="F34" s="13">
-        <v>0.19603111459497347</v>
+        <v>0.20136306018405542</v>
       </c>
       <c r="G34" s="13">
-        <v>0.24504522944585333</v>
+        <v>0.24616376812383423</v>
       </c>
       <c r="H34" s="13">
-        <v>17.692325181486275</v>
+        <v>17.913965613409701</v>
       </c>
       <c r="I34" s="10">
-        <v>-0.91186878962917883</v>
+        <v>-0.88731375371311039</v>
       </c>
       <c r="J34" s="18">
-        <v>4.2140653981463911</v>
+        <v>4.9480175337695513</v>
       </c>
       <c r="K34" s="23" t="e">
         <v>#NUM!</v>
@@ -15318,94 +15508,94 @@
     </row>
     <row r="35" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="19">
-        <v>68.024991379395061</v>
+        <v>68.281512914010278</v>
       </c>
       <c r="B35" s="25">
-        <v>31.309301586827313</v>
+        <v>31.350024752255923</v>
       </c>
       <c r="C35" s="25">
-        <v>12.839856176544316</v>
+        <v>12.92351865410239</v>
       </c>
       <c r="D35" s="25">
-        <v>2.2334953999223468</v>
+        <v>2.2363645620421622</v>
       </c>
       <c r="E35" s="25">
-        <v>4.0377642393675233</v>
+        <v>4.0380064249120942</v>
       </c>
       <c r="F35" s="25">
-        <v>0.20341214633514343</v>
+        <v>0.20791818049733735</v>
       </c>
       <c r="G35" s="25">
-        <v>0.14400886591796008</v>
+        <v>0.14557749849034887</v>
       </c>
       <c r="H35" s="25">
-        <v>22.418473809302817</v>
+        <v>22.54816174840246</v>
       </c>
       <c r="I35" s="19">
-        <v>-0.28434571329526892</v>
+        <v>-0.27640813387747171</v>
       </c>
       <c r="J35" s="20">
-        <v>2.9863053641141732</v>
+        <v>3.5581773946599329</v>
       </c>
       <c r="K35" s="24">
-        <v>48.187500000802082</v>
+        <v>48.199152543202388</v>
       </c>
       <c r="L35" s="25">
-        <v>13.449999999358333</v>
+        <v>13.440677965438093</v>
       </c>
       <c r="M35" s="25">
-        <v>12.008333334509722</v>
+        <v>12.025423730030163</v>
       </c>
       <c r="N35" s="25">
         <v>1</v>
       </c>
       <c r="O35" s="25">
-        <v>1.6375000001604167</v>
+        <v>1.639830508640477</v>
       </c>
       <c r="P35" s="25">
-        <v>0.54583333338680551</v>
+        <v>0.54661016954682562</v>
       </c>
       <c r="Q35" s="25">
         <v>0</v>
       </c>
       <c r="R35" s="25">
-        <v>22.729166666934027</v>
+        <v>22.733050847734127</v>
       </c>
       <c r="S35" s="25">
         <v>0</v>
       </c>
       <c r="T35" s="20">
-        <v>-4.3566944184023662</v>
+        <v>-3.83635592699728</v>
       </c>
       <c r="U35" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="61" t="s">
+      <c r="A36" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="61"/>
-      <c r="C36" s="61"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="61"/>
-      <c r="F36" s="61"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="61"/>
-      <c r="I36" s="61"/>
-      <c r="J36" s="62"/>
-      <c r="K36" s="63" t="s">
+      <c r="B36" s="62"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="63"/>
+      <c r="K36" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="L36" s="61"/>
-      <c r="M36" s="61"/>
-      <c r="N36" s="61"/>
-      <c r="O36" s="61"/>
-      <c r="P36" s="61"/>
-      <c r="Q36" s="61"/>
-      <c r="R36" s="61"/>
-      <c r="S36" s="61"/>
-      <c r="T36" s="62"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="62"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="62"/>
+      <c r="R36" s="62"/>
+      <c r="S36" s="62"/>
+      <c r="T36" s="63"/>
     </row>
     <row r="37" spans="1:22" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
@@ -15472,64 +15662,64 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="9">
-        <v>62.44947766065453</v>
+        <v>62.581046697438936</v>
       </c>
       <c r="B38" s="9">
-        <v>27.168743976683867</v>
+        <v>27.152063606806017</v>
       </c>
       <c r="C38" s="9">
-        <v>14.968540716549507</v>
+        <v>14.892076880711119</v>
       </c>
       <c r="D38" s="9">
-        <v>3.0173128064958319</v>
+        <v>3.0070751579639796</v>
       </c>
       <c r="E38" s="9">
-        <v>4.7780041892700513</v>
+        <v>4.7633822486371216</v>
       </c>
       <c r="F38" s="9">
-        <v>0.32438039872856306</v>
+        <v>0.32074679943233259</v>
       </c>
       <c r="G38" s="9">
-        <v>1.2113319057468113E-2</v>
+        <v>1.2605434072318117E-2</v>
       </c>
       <c r="H38" s="9">
-        <v>17.329181996875974</v>
+        <v>17.511902988691968</v>
       </c>
       <c r="I38" s="9">
-        <v>-1.2019406421866381</v>
+        <v>-1.2244412229588719</v>
       </c>
       <c r="J38" s="17">
-        <v>-1.8479996324941204</v>
+        <v>-2.6138060038256619</v>
       </c>
       <c r="K38" s="22">
-        <v>54.604551339231307</v>
+        <v>54.540756757107175</v>
       </c>
       <c r="L38" s="9">
-        <v>26.887963637831572</v>
+        <v>26.835004959927012</v>
       </c>
       <c r="M38" s="9">
-        <v>17.459942403307355</v>
+        <v>17.434696351993665</v>
       </c>
       <c r="N38" s="9">
-        <v>3.3329778467383373</v>
+        <v>3.3268846921656827</v>
       </c>
       <c r="O38" s="9">
-        <v>4.9992366677455884</v>
+        <v>4.9861126419294139</v>
       </c>
       <c r="P38" s="9">
-        <v>0.42294827670710611</v>
+        <v>0.42023645018315309</v>
       </c>
       <c r="Q38" s="9">
-        <v>1.8493459631182513E-2</v>
+        <v>1.9508431612576108E-2</v>
       </c>
       <c r="R38" s="9">
-        <v>10.184934596311823</v>
+        <v>10.195084316125762</v>
       </c>
       <c r="S38" s="9">
         <v>0</v>
       </c>
       <c r="T38" s="17">
-        <v>9.7555614361352863</v>
+        <v>9.8781057792120972</v>
       </c>
       <c r="U38" t="s">
         <v>33</v>
@@ -15540,37 +15730,37 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="10">
-        <v>67.54348020300651</v>
+        <v>67.831644948308707</v>
       </c>
       <c r="B39" s="10">
-        <v>34.468952769956189</v>
+        <v>34.477853677782498</v>
       </c>
       <c r="C39" s="10">
-        <v>15.665394221922819</v>
+        <v>15.65969054471616</v>
       </c>
       <c r="D39" s="10">
-        <v>2.8333548188671758</v>
+        <v>2.8294212863872388</v>
       </c>
       <c r="E39" s="10">
-        <v>4.7945376731170359</v>
+        <v>4.7915654582315756</v>
       </c>
       <c r="F39" s="10">
-        <v>0.26662059950291689</v>
+        <v>0.26665747003411272</v>
       </c>
       <c r="G39" s="10">
-        <v>0.1473321867017871</v>
+        <v>0.1479502489544941</v>
       </c>
       <c r="H39" s="10">
-        <v>15.167164192515347</v>
+        <v>15.398610853681721</v>
       </c>
       <c r="I39" s="10">
-        <v>-1.280300807583481</v>
+        <v>-1.2774022516391117</v>
       </c>
       <c r="J39" s="18">
-        <v>1.865127032635322</v>
+        <v>1.7877111320359038</v>
       </c>
       <c r="K39" s="23">
-        <v>101.66395494367676</v>
+        <v>101.66394472361523</v>
       </c>
       <c r="L39" s="10" t="e">
         <v>#NUM!</v>
@@ -15605,34 +15795,34 @@
     </row>
     <row r="40" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="10">
-        <v>63.970501701406604</v>
+        <v>64.163288743017205</v>
       </c>
       <c r="B40" s="10">
-        <v>27.55569515151625</v>
+        <v>27.566866709498374</v>
       </c>
       <c r="C40" s="10">
-        <v>13.98252983126261</v>
+        <v>13.969549758122122</v>
       </c>
       <c r="D40" s="10">
-        <v>2.7504134862502077</v>
+        <v>2.7464909914708362</v>
       </c>
       <c r="E40" s="10">
-        <v>4.5065490725261315</v>
+        <v>4.4984470428997518</v>
       </c>
       <c r="F40" s="10">
-        <v>0.27400163124308685</v>
+        <v>0.27321259034739465</v>
       </c>
       <c r="G40" s="10">
-        <v>4.6295823173893871E-2</v>
+        <v>4.7363979321008755E-2</v>
       </c>
       <c r="H40" s="10">
-        <v>19.893312820331889</v>
+        <v>20.03280698867448</v>
       </c>
       <c r="I40" s="10">
-        <v>-0.65277773124957095</v>
+        <v>-0.66649663180347307</v>
       </c>
       <c r="J40" s="18">
-        <v>0.63736699860310919</v>
+        <v>0.39787099292628808</v>
       </c>
       <c r="K40" s="23">
         <v>71</v>
@@ -15670,49 +15860,49 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="9">
-        <v>67.532551664401481</v>
+        <v>67.765710934078939</v>
       </c>
       <c r="B41" s="9">
-        <v>33.858518001595939</v>
+        <v>33.855558537469562</v>
       </c>
       <c r="C41" s="9">
-        <v>15.054057561784157</v>
+        <v>15.03336079194438</v>
       </c>
       <c r="D41" s="9">
-        <v>2.778884000964283</v>
+        <v>2.7738149622353476</v>
       </c>
       <c r="E41" s="9">
-        <v>4.6901822734928782</v>
+        <v>4.6842318751835421</v>
       </c>
       <c r="F41" s="9">
-        <v>0.25350569168259024</v>
+        <v>0.2530738695354538</v>
       </c>
       <c r="G41" s="9">
-        <v>0.13439370884486107</v>
+        <v>0.13461319972076768</v>
       </c>
       <c r="H41" s="9">
-        <v>16.718167022484529</v>
+        <v>16.972004370622081</v>
       </c>
       <c r="I41" s="9">
-        <v>-1.2966443517284012</v>
+        <v>-1.2945576998037207</v>
       </c>
       <c r="J41" s="17">
-        <v>0.34914953307376878</v>
+        <v>0.14707892759426106</v>
       </c>
       <c r="K41" s="22">
-        <v>71.894736841988916</v>
+        <v>71.893048128222148</v>
       </c>
       <c r="L41" s="9">
-        <v>31.294736842431018</v>
+        <v>31.299465240978016</v>
       </c>
       <c r="M41" s="9">
-        <v>8.5824175827049878</v>
+        <v>8.5865921790680702</v>
       </c>
       <c r="N41" s="9">
         <v>2</v>
       </c>
       <c r="O41" s="9">
-        <v>3.5</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="P41" s="9">
         <v>0</v>
@@ -15724,10 +15914,10 @@
         <v>45</v>
       </c>
       <c r="S41" s="9">
-        <v>-1.7368421053407199</v>
+        <v>-1.7379679145185738</v>
       </c>
       <c r="T41" s="17">
-        <v>-11.46303565018658</v>
+        <v>-12.902339425822223</v>
       </c>
       <c r="U41" t="s">
         <v>36</v>
@@ -15735,34 +15925,34 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="10">
-        <v>72.626554206753454</v>
+        <v>73.01630918494871</v>
       </c>
       <c r="B42" s="10">
-        <v>41.158726794868258</v>
+        <v>41.181348608446044</v>
       </c>
       <c r="C42" s="10">
-        <v>15.750911067157471</v>
+        <v>15.800974455949426</v>
       </c>
       <c r="D42" s="10">
-        <v>2.5949260133356264</v>
+        <v>2.5961610906586068</v>
       </c>
       <c r="E42" s="10">
-        <v>4.7067157573398628</v>
+        <v>4.7124150847779953</v>
       </c>
       <c r="F42" s="10">
-        <v>0.19574589245694413</v>
+        <v>0.19898454013723393</v>
       </c>
       <c r="G42" s="10">
-        <v>0.26961257648918002</v>
+        <v>0.26995801460294366</v>
       </c>
       <c r="H42" s="10">
-        <v>14.556149218123903</v>
+        <v>14.858712235611828</v>
       </c>
       <c r="I42" s="10">
-        <v>-1.3750045171252441</v>
+        <v>-1.3475187284839603</v>
       </c>
       <c r="J42" s="18">
-        <v>4.0622761982032118</v>
+        <v>4.5485960634558307</v>
       </c>
       <c r="K42" s="23">
         <v>89</v>
@@ -15800,34 +15990,34 @@
     </row>
     <row r="43" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="10">
-        <v>69.053575705153548</v>
+        <v>69.347952979657208</v>
       </c>
       <c r="B43" s="10">
-        <v>34.245469176428323</v>
+        <v>34.270361640161916</v>
       </c>
       <c r="C43" s="10">
-        <v>14.068046676497261</v>
+        <v>14.110833669355383</v>
       </c>
       <c r="D43" s="10">
-        <v>2.5119846807186588</v>
+        <v>2.5132307957422038</v>
       </c>
       <c r="E43" s="10">
-        <v>4.4187271567489592</v>
+        <v>4.4192966694461715</v>
       </c>
       <c r="F43" s="10">
-        <v>0.20312692419711403</v>
+        <v>0.20553966045051589</v>
       </c>
       <c r="G43" s="10">
-        <v>0.16857621296128683</v>
+        <v>0.16937174496945834</v>
       </c>
       <c r="H43" s="10">
-        <v>19.282297845940448</v>
+        <v>19.492908370604589</v>
       </c>
       <c r="I43" s="10">
-        <v>-0.74748144079133405</v>
+        <v>-0.73661310864832175</v>
       </c>
       <c r="J43" s="18">
-        <v>2.8345161641710037</v>
+        <v>3.1587559243462069</v>
       </c>
       <c r="K43" s="23" t="e">
         <v>#NUM!</v>
@@ -15865,37 +16055,37 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44" s="9">
-        <v>64.759117013828487</v>
+        <v>64.920469880666161</v>
       </c>
       <c r="B44" s="9">
-        <v>28.281136296819902</v>
+        <v>28.303249817999745</v>
       </c>
       <c r="C44" s="9">
-        <v>13.631674227022936</v>
+        <v>13.616251070069643</v>
       </c>
       <c r="D44" s="9">
-        <v>2.6860836051047943</v>
+        <v>2.6813210990560217</v>
       </c>
       <c r="E44" s="9">
-        <v>4.3782547986009579</v>
+        <v>4.3677652496109207</v>
       </c>
       <c r="F44" s="9">
-        <v>0.27403477608796695</v>
+        <v>0.27342612150328405</v>
       </c>
       <c r="G44" s="9">
-        <v>4.9484752566937282E-2</v>
+        <v>5.066623453995911E-2</v>
       </c>
       <c r="H44" s="9">
-        <v>20.371394513548669</v>
+        <v>20.52354409017007</v>
       </c>
       <c r="I44" s="9">
-        <v>-0.63451866093614417</v>
+        <v>-0.64531935749752845</v>
       </c>
       <c r="J44" s="17">
-        <v>0.27017631694852273</v>
+        <v>7.3311122697171882E-2</v>
       </c>
       <c r="K44" s="22">
-        <v>34</v>
+        <v>34.000000000000007</v>
       </c>
       <c r="L44" s="9" t="e">
         <v>#NUM!</v>
@@ -15930,34 +16120,34 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="10">
-        <v>69.853119556180474</v>
+        <v>70.171068131535947</v>
       </c>
       <c r="B45" s="10">
-        <v>35.581345090092228</v>
+        <v>35.62903988897623</v>
       </c>
       <c r="C45" s="10">
-        <v>14.32852773239625</v>
+        <v>14.383864734074688</v>
       </c>
       <c r="D45" s="10">
-        <v>2.5021256174761382</v>
+        <v>2.5036672274792808</v>
       </c>
       <c r="E45" s="10">
-        <v>4.3947882824479425</v>
+        <v>4.3959484592053739</v>
       </c>
       <c r="F45" s="10">
-        <v>0.21627497686232083</v>
+        <v>0.21933679210506418</v>
       </c>
       <c r="G45" s="10">
-        <v>0.18470362021125628</v>
+        <v>0.18601104942213509</v>
       </c>
       <c r="H45" s="10">
-        <v>18.209376709188039</v>
+        <v>18.410251955159822</v>
       </c>
       <c r="I45" s="10">
-        <v>-0.71287882633298705</v>
+        <v>-0.69828038617776811</v>
       </c>
       <c r="J45" s="18">
-        <v>3.9833029820779693</v>
+        <v>4.4748282585587482</v>
       </c>
       <c r="K45" s="23">
         <v>83</v>
@@ -15995,37 +16185,37 @@
     </row>
     <row r="46" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="19">
-        <v>66.280141054580554</v>
+        <v>66.502711926244444</v>
       </c>
       <c r="B46" s="19">
-        <v>28.668087471652285</v>
+        <v>28.718052920692099</v>
       </c>
       <c r="C46" s="19">
-        <v>12.645663341736039</v>
+        <v>12.693723947480647</v>
       </c>
       <c r="D46" s="19">
-        <v>2.41918428485917</v>
+        <v>2.4207369325628783</v>
       </c>
       <c r="E46" s="19">
-        <v>4.106799681857038</v>
+        <v>4.102830043873551</v>
       </c>
       <c r="F46" s="19">
-        <v>0.2236560086024908</v>
+        <v>0.22589191241834614</v>
       </c>
       <c r="G46" s="19">
-        <v>8.3667256683363042E-2</v>
+        <v>8.5424779788649735E-2</v>
       </c>
       <c r="H46" s="19">
-        <v>22.935525337004584</v>
+        <v>23.044448090152581</v>
       </c>
       <c r="I46" s="19">
-        <v>-8.5355749999076996E-2</v>
+        <v>-8.737476634212947E-2</v>
       </c>
       <c r="J46" s="20">
-        <v>2.7555429480457549</v>
+        <v>3.084988119449128</v>
       </c>
       <c r="K46" s="24">
-        <v>85.459599529535083</v>
+        <v>85.519023690637923</v>
       </c>
       <c r="L46" s="19">
         <v>39</v>
@@ -16037,7 +16227,7 @@
         <v>4</v>
       </c>
       <c r="O46" s="19">
-        <v>4.4999999999999991</v>
+        <v>4.5</v>
       </c>
       <c r="P46" s="19">
         <v>0</v>
@@ -16052,7 +16242,7 @@
         <v>0</v>
       </c>
       <c r="T46" s="20">
-        <v>-0.3807357396422919</v>
+        <v>-0.97107830740497458</v>
       </c>
       <c r="U46" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Put the december 6 stuff in but without the scores because I lost them :(
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8C3A18-7E8F-4A09-A992-F0DF9DCE365C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4436935D-14B8-4062-85D1-AD6D3152B19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="46">
   <si>
     <t>Cyrus</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>**</t>
   </si>
 </sst>
 </file>
@@ -879,6 +882,15 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -889,15 +901,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9862,8 +9865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
   <dimension ref="A1:Y74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P60" sqref="P60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12143,7 +12146,7 @@
         <v>0.23214285712499999</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -12190,7 +12193,7 @@
         <v>0.23214285712499999</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -12237,7 +12240,7 @@
         <v>0.23214285712499999</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -12284,7 +12287,7 @@
         <v>0.23214285712499999</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -12331,7 +12334,7 @@
         <v>0.23214285712499999</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -12378,7 +12381,7 @@
         <v>0.23214285712499999</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -12425,7 +12428,7 @@
         <v>0.23214285712499999</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -12472,7 +12475,7 @@
         <v>0.23214285712499999</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -12519,7 +12522,7 @@
         <v>0.85714285700000004</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -12566,7 +12569,7 @@
         <v>0.85714285700000004</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -12613,7 +12616,7 @@
         <v>0.85714285700000004</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>18</v>
       </c>
@@ -12660,7 +12663,7 @@
         <v>0.85714285700000004</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -12707,7 +12710,7 @@
         <v>0.85714285700000004</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -12754,7 +12757,7 @@
         <v>0.85714285700000004</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -12801,34 +12804,480 @@
         <v>0.85714285700000004</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B64" s="1"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B65" s="1"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B70" s="1"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B72" s="1"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" s="1">
+        <v>45266</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>-1</v>
+      </c>
+      <c r="G63">
+        <v>-1</v>
+      </c>
+      <c r="H63">
+        <v>-1</v>
+      </c>
+      <c r="I63">
+        <v>-1</v>
+      </c>
+      <c r="J63">
+        <v>-1</v>
+      </c>
+      <c r="K63">
+        <v>-1</v>
+      </c>
+      <c r="L63">
+        <v>-1</v>
+      </c>
+      <c r="M63">
+        <v>-1</v>
+      </c>
+      <c r="N63">
+        <v>-1</v>
+      </c>
+      <c r="P63" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64" s="1">
+        <v>45266</v>
+      </c>
+      <c r="C64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" t="s">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64">
+        <v>-1</v>
+      </c>
+      <c r="G64">
+        <v>-1</v>
+      </c>
+      <c r="H64">
+        <v>-1</v>
+      </c>
+      <c r="I64">
+        <v>-1</v>
+      </c>
+      <c r="J64">
+        <v>-1</v>
+      </c>
+      <c r="K64">
+        <v>-1</v>
+      </c>
+      <c r="L64">
+        <v>-1</v>
+      </c>
+      <c r="M64">
+        <v>-1</v>
+      </c>
+      <c r="N64">
+        <v>-1</v>
+      </c>
+      <c r="P64" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65" s="1">
+        <v>45266</v>
+      </c>
+      <c r="C65" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" t="s">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>-1</v>
+      </c>
+      <c r="G65">
+        <v>-1</v>
+      </c>
+      <c r="H65">
+        <v>-1</v>
+      </c>
+      <c r="I65">
+        <v>-1</v>
+      </c>
+      <c r="J65">
+        <v>-1</v>
+      </c>
+      <c r="K65">
+        <v>-1</v>
+      </c>
+      <c r="L65">
+        <v>-1</v>
+      </c>
+      <c r="M65">
+        <v>-1</v>
+      </c>
+      <c r="N65">
+        <v>-1</v>
+      </c>
+      <c r="P65" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66" s="1">
+        <v>45266</v>
+      </c>
+      <c r="C66" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>5</v>
+      </c>
+      <c r="F66">
+        <v>-1</v>
+      </c>
+      <c r="G66">
+        <v>-1</v>
+      </c>
+      <c r="H66">
+        <v>-1</v>
+      </c>
+      <c r="I66">
+        <v>-1</v>
+      </c>
+      <c r="J66">
+        <v>-1</v>
+      </c>
+      <c r="K66">
+        <v>-1</v>
+      </c>
+      <c r="L66">
+        <v>-1</v>
+      </c>
+      <c r="M66">
+        <v>-1</v>
+      </c>
+      <c r="N66">
+        <v>-1</v>
+      </c>
+      <c r="P66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" s="1">
+        <v>45266</v>
+      </c>
+      <c r="C67" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>-1</v>
+      </c>
+      <c r="G67">
+        <v>-1</v>
+      </c>
+      <c r="H67">
+        <v>-1</v>
+      </c>
+      <c r="I67">
+        <v>-1</v>
+      </c>
+      <c r="J67">
+        <v>-1</v>
+      </c>
+      <c r="K67">
+        <v>-1</v>
+      </c>
+      <c r="L67">
+        <v>-1</v>
+      </c>
+      <c r="M67">
+        <v>-1</v>
+      </c>
+      <c r="N67">
+        <v>-1</v>
+      </c>
+      <c r="P67" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68" s="1">
+        <v>45266</v>
+      </c>
+      <c r="C68" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" t="s">
+        <v>5</v>
+      </c>
+      <c r="F68">
+        <v>-1</v>
+      </c>
+      <c r="G68">
+        <v>-1</v>
+      </c>
+      <c r="H68">
+        <v>-1</v>
+      </c>
+      <c r="I68">
+        <v>-1</v>
+      </c>
+      <c r="J68">
+        <v>-1</v>
+      </c>
+      <c r="K68">
+        <v>-1</v>
+      </c>
+      <c r="L68">
+        <v>-1</v>
+      </c>
+      <c r="M68">
+        <v>-1</v>
+      </c>
+      <c r="N68">
+        <v>-1</v>
+      </c>
+      <c r="P68" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69" s="1">
+        <v>45266</v>
+      </c>
+      <c r="C69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E69" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>-1</v>
+      </c>
+      <c r="G69">
+        <v>-1</v>
+      </c>
+      <c r="H69">
+        <v>-1</v>
+      </c>
+      <c r="I69">
+        <v>-1</v>
+      </c>
+      <c r="J69">
+        <v>-1</v>
+      </c>
+      <c r="K69">
+        <v>-1</v>
+      </c>
+      <c r="L69">
+        <v>-1</v>
+      </c>
+      <c r="M69">
+        <v>-1</v>
+      </c>
+      <c r="N69">
+        <v>-1</v>
+      </c>
+      <c r="P69" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="1">
+        <v>45266</v>
+      </c>
+      <c r="C70" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70" t="s">
+        <v>5</v>
+      </c>
+      <c r="F70">
+        <v>-1</v>
+      </c>
+      <c r="G70">
+        <v>-1</v>
+      </c>
+      <c r="H70">
+        <v>-1</v>
+      </c>
+      <c r="I70">
+        <v>-1</v>
+      </c>
+      <c r="J70">
+        <v>-1</v>
+      </c>
+      <c r="K70">
+        <v>-1</v>
+      </c>
+      <c r="L70">
+        <v>-1</v>
+      </c>
+      <c r="M70">
+        <v>-1</v>
+      </c>
+      <c r="N70">
+        <v>-1</v>
+      </c>
+      <c r="P70" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71" s="1">
+        <v>45266</v>
+      </c>
+      <c r="C71" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" t="s">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>-1</v>
+      </c>
+      <c r="G71">
+        <v>-1</v>
+      </c>
+      <c r="H71">
+        <v>-1</v>
+      </c>
+      <c r="I71">
+        <v>-1</v>
+      </c>
+      <c r="J71">
+        <v>-1</v>
+      </c>
+      <c r="K71">
+        <v>-1</v>
+      </c>
+      <c r="L71">
+        <v>-1</v>
+      </c>
+      <c r="M71">
+        <v>-1</v>
+      </c>
+      <c r="N71">
+        <v>-1</v>
+      </c>
+      <c r="P71" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72" s="1">
+        <v>45266</v>
+      </c>
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" t="s">
+        <v>5</v>
+      </c>
+      <c r="F72">
+        <v>-1</v>
+      </c>
+      <c r="G72">
+        <v>-1</v>
+      </c>
+      <c r="H72">
+        <v>-1</v>
+      </c>
+      <c r="I72">
+        <v>-1</v>
+      </c>
+      <c r="J72">
+        <v>-1</v>
+      </c>
+      <c r="K72">
+        <v>-1</v>
+      </c>
+      <c r="L72">
+        <v>-1</v>
+      </c>
+      <c r="M72">
+        <v>-1</v>
+      </c>
+      <c r="N72">
+        <v>-1</v>
+      </c>
+      <c r="P72" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B73" s="1"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B74" s="1"/>
     </row>
   </sheetData>
@@ -13479,28 +13928,28 @@
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:36" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="62"/>
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
       <c r="W1" s="8"/>
@@ -13519,56 +13968,56 @@
       <c r="AJ1" s="8"/>
     </row>
     <row r="2" spans="1:36" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="60" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="61"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="64"/>
     </row>
     <row r="3" spans="1:36" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="64" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="62"/>
-      <c r="S3" s="62"/>
-      <c r="T3" s="63"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="59"/>
     </row>
     <row r="4" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
@@ -14218,30 +14667,30 @@
       </c>
     </row>
     <row r="14" spans="1:36" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="62"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="62"/>
-      <c r="I14" s="62"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="64" t="s">
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="62"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="62"/>
-      <c r="O14" s="62"/>
-      <c r="P14" s="62"/>
-      <c r="Q14" s="62"/>
-      <c r="R14" s="62"/>
-      <c r="S14" s="62"/>
-      <c r="T14" s="63"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="58"/>
+      <c r="S14" s="58"/>
+      <c r="T14" s="59"/>
     </row>
     <row r="15" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
@@ -14895,30 +15344,30 @@
       </c>
     </row>
     <row r="25" spans="1:22" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="62" t="s">
+      <c r="A25" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="62"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="63"/>
-      <c r="K25" s="64" t="s">
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L25" s="62"/>
-      <c r="M25" s="62"/>
-      <c r="N25" s="62"/>
-      <c r="O25" s="62"/>
-      <c r="P25" s="62"/>
-      <c r="Q25" s="62"/>
-      <c r="R25" s="62"/>
-      <c r="S25" s="62"/>
-      <c r="T25" s="63"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="58"/>
+      <c r="Q25" s="58"/>
+      <c r="R25" s="58"/>
+      <c r="S25" s="58"/>
+      <c r="T25" s="59"/>
     </row>
     <row r="26" spans="1:22" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
@@ -15572,30 +16021,30 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="62" t="s">
+      <c r="A36" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="62"/>
-      <c r="C36" s="62"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62"/>
-      <c r="G36" s="62"/>
-      <c r="H36" s="62"/>
-      <c r="I36" s="62"/>
-      <c r="J36" s="63"/>
-      <c r="K36" s="64" t="s">
+      <c r="B36" s="58"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="59"/>
+      <c r="K36" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="L36" s="62"/>
-      <c r="M36" s="62"/>
-      <c r="N36" s="62"/>
-      <c r="O36" s="62"/>
-      <c r="P36" s="62"/>
-      <c r="Q36" s="62"/>
-      <c r="R36" s="62"/>
-      <c r="S36" s="62"/>
-      <c r="T36" s="63"/>
+      <c r="L36" s="58"/>
+      <c r="M36" s="58"/>
+      <c r="N36" s="58"/>
+      <c r="O36" s="58"/>
+      <c r="P36" s="58"/>
+      <c r="Q36" s="58"/>
+      <c r="R36" s="58"/>
+      <c r="S36" s="58"/>
+      <c r="T36" s="59"/>
     </row>
     <row r="37" spans="1:22" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
@@ -16594,17 +17043,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="K2:T2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="K3:T3"/>
     <mergeCell ref="A14:J14"/>
     <mergeCell ref="K14:T14"/>
     <mergeCell ref="K25:T25"/>
     <mergeCell ref="A25:J25"/>
     <mergeCell ref="A36:J36"/>
     <mergeCell ref="K36:T36"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="K2:T2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="K3:T3"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:A13">
     <cfRule type="colorScale" priority="40">

</xml_diff>

<commit_message>
Fixed the spreadsheet up a bit more - i have to commit each time so I don't lose it :/
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB28590F-4EE6-4B78-8578-A5D2143E1AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160584DD-3DAC-46C7-A73B-7FCBB10BBAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
@@ -882,15 +882,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -901,6 +892,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1099,13 +1099,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-6.1280155961706955</c:v>
+                  <c:v>-0.97524710273244863</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8925406540189602</c:v>
+                  <c:v>-0.27444547492562932</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.4882038632626138</c:v>
+                  <c:v>7.069907056814932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1471,7 +1471,7 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Matt</c:v>
+                    <c:v>Caleb</c:v>
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>Matt</c:v>
@@ -1490,85 +1490,85 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>66.234839164722985</c:v>
+                  <c:v>-2.8894910932888722</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65.742305935746685</c:v>
+                  <c:v>-2.609170442166139</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.098061417107019</c:v>
+                  <c:v>0.32857057053008187</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64.767198704393138</c:v>
+                  <c:v>-14.720317075108222</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>64.274665475416825</c:v>
+                  <c:v>-14.439996423985498</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>69.630420956777158</c:v>
+                  <c:v>-11.502255411289271</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70.986913965221305</c:v>
+                  <c:v>1.1418642152158067</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70.494380736244992</c:v>
+                  <c:v>1.4221848663385317</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75.850136217605339</c:v>
+                  <c:v>4.3599258790347601</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>69.879595568809521</c:v>
+                  <c:v>4.0344067790843505</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>69.387062339833221</c:v>
+                  <c:v>4.3147274302070793</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>74.742817821193569</c:v>
+                  <c:v>7.252468442903294</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>68.411955108479674</c:v>
+                  <c:v>-7.7964192027350085</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>67.919421879503375</c:v>
+                  <c:v>-7.5160985516122771</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>73.275177360863708</c:v>
+                  <c:v>-4.5783575389160589</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>74.631670369307855</c:v>
+                  <c:v>8.0657620875890217</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>74.139137140331528</c:v>
+                  <c:v>8.3460827387117504</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>79.494892621691889</c:v>
+                  <c:v>11.283823751407976</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>71.634369636016089</c:v>
+                  <c:v>5.757375087877727</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>71.141836407039804</c:v>
+                  <c:v>6.0376957390004531</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>76.497591888400137</c:v>
+                  <c:v>8.9754367516966713</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>70.166729175686257</c:v>
+                  <c:v>-6.0734508939416347</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>69.674195946709958</c:v>
+                  <c:v>-5.7931302428189069</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>75.029951428070277</c:v>
+                  <c:v>-2.8553892301226864</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>76.386444436514424</c:v>
+                  <c:v>9.7887303963823946</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>75.893911207538125</c:v>
+                  <c:v>10.069051047505127</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>81.249666688898458</c:v>
+                  <c:v>13.00679206020135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1939,7 +1939,7 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Matt</c:v>
+                    <c:v>Caleb</c:v>
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>Matt</c:v>
@@ -1958,13 +1958,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>38.446599589058643</c:v>
+                  <c:v>-52.901939192699373</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.906136035185824</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1982,13 +1982,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81.809108790439183</c:v>
+                  <c:v>-10.798028350673622</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>139.80116925437443</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -1997,7 +1997,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>77.412540761452632</c:v>
+                  <c:v>-19.83072445294458</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -2009,10 +2009,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>77.803502498541008</c:v>
+                  <c:v>9.4569880872890462</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>85.267534783374572</c:v>
+                  <c:v>1.3891790374763895</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -2021,7 +2021,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>49.617266749077956</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -2036,7 +2036,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>67.536211870302736</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2416,10 +2416,10 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-7.8131568023122044</c:v>
+                  <c:v>-11.355187540147956</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>128.60882549606845</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2428,7 +2428,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-7.2575351682520548</c:v>
+                  <c:v>-19.83072445294458</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2440,7 +2440,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.7061300761323235</c:v>
+                  <c:v>-7.7843061815675902</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2804,13 +2804,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6.2894618195883139</c:v>
+                  <c:v>8.5510419779700104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-8.4516910685519395</c:v>
+                  <c:v>-21.026022976578382</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.2470371951106376</c:v>
+                  <c:v>18.629430249231707</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3170,13 +3170,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-17.850949128688761</c:v>
+                  <c:v>-29.599045216919471</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.9735060261693862</c:v>
+                  <c:v>5.0204441449465964</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6284132448837005</c:v>
+                  <c:v>13.635285688913468</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3558,31 +3558,31 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>8.0723111708814188E-2</c:v>
+                  <c:v>3.7878974376187848</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.591001236803641</c:v>
+                  <c:v>4.1382982515221949</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.3888328414254643</c:v>
+                  <c:v>7.8104745173924686</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-7.2898533323613135</c:v>
+                  <c:v>-11.000635039655407</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.7795752072664861</c:v>
+                  <c:v>-10.650234225752001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.98174360264466143</c:v>
+                  <c:v>-6.9780579598817241</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0595107994699706</c:v>
+                  <c:v>8.8270915732496285</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.5697889245648007</c:v>
+                  <c:v>9.1774923871530394</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.3676205291866266</c:v>
+                  <c:v>12.849668653023318</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9865,8 +9865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
   <dimension ref="A1:Y74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="120" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="120" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13353,7 +13353,7 @@
         <v>68.37800252904573</v>
       </c>
       <c r="B3" s="48">
-        <v>35.174355300894987</v>
+        <v>36.516872964343207</v>
       </c>
       <c r="C3" s="48">
         <v>17.138855473654178</v>
@@ -13365,13 +13365,13 @@
         <v>4.927106599015592</v>
       </c>
       <c r="F3" s="48">
-        <v>0.32559219694737607</v>
+        <v>0.62749685085934492</v>
       </c>
       <c r="G3" s="48">
-        <v>0.21019640619048729</v>
+        <v>0.37386118935437246</v>
       </c>
       <c r="H3" s="48">
-        <v>13.608108108420012</v>
+        <v>14.487752161722719</v>
       </c>
       <c r="I3" s="48">
         <v>-1.1911589008131793</v>
@@ -13382,7 +13382,7 @@
         <v>45.591212173593902</v>
       </c>
       <c r="B4" s="49">
-        <v>24.111045378115655</v>
+        <v>23.920400356252845</v>
       </c>
       <c r="C4" s="49">
         <v>12.668783897972499</v>
@@ -13394,13 +13394,13 @@
         <v>3.807262672579343</v>
       </c>
       <c r="F4" s="49">
-        <v>0.52728928508672612</v>
+        <v>0.71477432901960947</v>
       </c>
       <c r="G4" s="49">
-        <v>0.36431306976744315</v>
+        <v>0.43169622181271528</v>
       </c>
       <c r="H4" s="49">
-        <v>11.348571630369468</v>
+        <v>11.304383650954478</v>
       </c>
       <c r="I4" s="49">
         <v>2.2480096919371211</v>
@@ -13420,7 +13420,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView zoomScale="167" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13476,7 +13476,7 @@
         <v>63.807413376938257</v>
       </c>
       <c r="B3" s="6">
-        <v>27.83098591548033</v>
+        <v>31.180434782962227</v>
       </c>
       <c r="C3" s="6">
         <v>19.150095602532136</v>
@@ -13488,19 +13488,19 @@
         <v>5.4529019981436297</v>
       </c>
       <c r="F3" s="6">
-        <v>0.59743762644888421</v>
+        <v>0.91735537193907546</v>
       </c>
       <c r="G3" s="6">
-        <v>7.0809984726752109E-2</v>
+        <v>0.31376975172403437</v>
       </c>
       <c r="H3" s="6">
-        <v>12.288786482451039</v>
+        <v>13.598851812193923</v>
       </c>
       <c r="I3" s="33">
         <v>-1.2181303116347046</v>
       </c>
       <c r="J3" s="36">
-        <v>6.2894618195883139</v>
+        <v>8.5510419779700104</v>
       </c>
       <c r="K3" t="s">
         <v>8</v>
@@ -13535,7 +13535,7 @@
         <v>-1.8769230768713843</v>
       </c>
       <c r="J4" s="37">
-        <v>-8.4516910685519395</v>
+        <v>-21.026022976578382</v>
       </c>
       <c r="K4" t="s">
         <v>4</v>
@@ -13546,7 +13546,7 @@
         <v>66.5378514784054</v>
       </c>
       <c r="B5" s="7">
-        <v>27.89762076432757</v>
+        <v>31.587987988378472</v>
       </c>
       <c r="C5" s="7">
         <v>14.993079585090214</v>
@@ -13558,19 +13558,19 @@
         <v>4.1487889273423448</v>
       </c>
       <c r="F5" s="7">
-        <v>0.29757785468469006</v>
+        <v>0.86507378782305955</v>
       </c>
       <c r="G5" s="7">
-        <v>0.14878892734234503</v>
+        <v>0.48137737177886247</v>
       </c>
       <c r="H5" s="7">
-        <v>22.231833910135176</v>
+        <v>21.359803232603017</v>
       </c>
       <c r="I5" s="32">
         <v>0</v>
       </c>
       <c r="J5" s="38">
-        <v>8.2470371951106376</v>
+        <v>18.629430249231707</v>
       </c>
       <c r="K5" t="s">
         <v>3</v>
@@ -13581,7 +13581,7 @@
         <v>63.506946497468597</v>
       </c>
       <c r="B6" s="6">
-        <v>29.189476795789602</v>
+        <v>30.769735045273187</v>
       </c>
       <c r="C6" s="6">
         <v>16.503120499182636</v>
@@ -13593,19 +13593,19 @@
         <v>5.2725420275346382</v>
       </c>
       <c r="F6" s="6">
-        <v>0.4523809523784722</v>
+        <v>0.83210526319337974</v>
       </c>
       <c r="G6" s="6">
-        <v>0</v>
+        <v>0.23361344540395459</v>
       </c>
       <c r="H6" s="6">
-        <v>12.288786482451039</v>
+        <v>13.997608609283898</v>
       </c>
       <c r="I6" s="33">
         <v>-1.3125158669957651</v>
       </c>
       <c r="J6" s="39">
-        <v>-6.1280155961706955</v>
+        <v>-0.97524710273244863</v>
       </c>
       <c r="K6" t="s">
         <v>6</v>
@@ -13616,7 +13616,7 @@
         <v>75.486580691170019</v>
       </c>
       <c r="B7" s="4">
-        <v>45.302197802282329</v>
+        <v>45.736369680975471</v>
       </c>
       <c r="C7" s="4">
         <v>18.248867201492281</v>
@@ -13628,19 +13628,19 @@
         <v>4.9255369928891541</v>
       </c>
       <c r="F7" s="4">
-        <v>0.25584725539327757</v>
+        <v>0.43471337583487168</v>
       </c>
       <c r="G7" s="4">
-        <v>0.41861575179775923</v>
+        <v>0.51512738855189366</v>
       </c>
       <c r="H7" s="4">
-        <v>11.813186813693997</v>
+        <v>13.198417529471161</v>
       </c>
       <c r="I7" s="34">
         <v>-1.4607425440405062</v>
       </c>
       <c r="J7" s="37">
-        <v>4.8925406540189602</v>
+        <v>-0.27444547492562932</v>
       </c>
       <c r="K7" t="s">
         <v>2</v>
@@ -13651,7 +13651,7 @@
         <v>63.861591695991187</v>
       </c>
       <c r="B8" s="7">
-        <v>26.636678200765793</v>
+        <v>29.864811133606942</v>
       </c>
       <c r="C8" s="7">
         <v>14.993079585090214</v>
@@ -13663,19 +13663,19 @@
         <v>4.1487889273423448</v>
       </c>
       <c r="F8" s="7">
-        <v>0.29757785468469006</v>
+        <v>0.71091703061638034</v>
       </c>
       <c r="G8" s="7">
-        <v>0.14878892734234503</v>
+        <v>0.35545851530819017</v>
       </c>
       <c r="H8" s="7">
-        <v>22.231833910135176</v>
+        <v>19.262008733423691</v>
       </c>
       <c r="I8" s="32">
         <v>0</v>
       </c>
       <c r="J8" s="38">
-        <v>6.4882038632626138</v>
+        <v>7.069907056814932</v>
       </c>
       <c r="K8" t="s">
         <v>0</v>
@@ -13710,7 +13710,7 @@
         <v>-2.0357706470673951</v>
       </c>
       <c r="J9" s="39">
-        <v>-17.850949128688761</v>
+        <v>-29.599045216919471</v>
       </c>
       <c r="K9" t="s">
         <v>7</v>
@@ -13721,7 +13721,7 @@
         <v>74.157765501170715</v>
       </c>
       <c r="B10" s="4">
-        <v>42.483808913072558</v>
+        <v>43.098910803677917</v>
       </c>
       <c r="C10" s="4">
         <v>18.410273516043535</v>
@@ -13733,19 +13733,19 @@
         <v>4.8138489209041815</v>
       </c>
       <c r="F10" s="4">
-        <v>0.29901079139096548</v>
+        <v>0.589208633142001</v>
       </c>
       <c r="G10" s="4">
-        <v>0.39433453238027122</v>
+        <v>0.51546762591641748</v>
       </c>
       <c r="H10" s="4">
-        <v>12.408184680466718</v>
+        <v>13.892796849172694</v>
       </c>
       <c r="I10" s="34">
         <v>-1.2585212374635</v>
       </c>
       <c r="J10" s="37">
-        <v>6.9735060261693862</v>
+        <v>5.0204441449465964</v>
       </c>
       <c r="K10" t="s">
         <v>5</v>
@@ -13756,7 +13756,7 @@
         <v>60.403061224736156</v>
       </c>
       <c r="B11" s="5">
-        <v>29.969387755209912</v>
+        <v>33.483382415290627</v>
       </c>
       <c r="C11" s="5">
         <v>17.974522292964096</v>
@@ -13768,19 +13768,19 @@
         <v>5.7441418619976812</v>
       </c>
       <c r="F11" s="5">
-        <v>0.5</v>
+        <v>0.96193353478593313</v>
       </c>
       <c r="G11" s="5">
-        <v>0</v>
+        <v>0.32552693211932282</v>
       </c>
       <c r="H11" s="5">
-        <v>10</v>
+        <v>11.953161592715938</v>
       </c>
       <c r="I11" s="35">
         <v>-0.48964218457233455</v>
       </c>
       <c r="J11" s="40">
-        <v>3.6284132448837005</v>
+        <v>13.635285688913468</v>
       </c>
       <c r="K11" t="s">
         <v>1</v>
@@ -13924,35 +13924,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AJ53"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView topLeftCell="G37" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:36" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="62"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="59"/>
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
       <c r="W1" s="8"/>
@@ -13971,56 +13971,56 @@
       <c r="AJ1" s="8"/>
     </row>
     <row r="2" spans="1:36" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="63" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="64"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="61"/>
     </row>
     <row r="3" spans="1:36" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="60" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="59"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="62"/>
+      <c r="R3" s="62"/>
+      <c r="S3" s="62"/>
+      <c r="T3" s="63"/>
     </row>
     <row r="4" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
@@ -14089,7 +14089,7 @@
         <v>63.657179937203423</v>
       </c>
       <c r="B5" s="12">
-        <v>28.510231355634964</v>
+        <v>30.975084914117708</v>
       </c>
       <c r="C5" s="12">
         <v>17.826608050857388</v>
@@ -14101,19 +14101,19 @@
         <v>5.362722012839134</v>
       </c>
       <c r="F5" s="12">
-        <v>0.5249092894136782</v>
+        <v>0.87473031756622754</v>
       </c>
       <c r="G5" s="12">
-        <v>3.5404992363376055E-2</v>
+        <v>0.2736915985639945</v>
       </c>
       <c r="H5" s="12">
-        <v>12.288786482451039</v>
+        <v>13.798230210738911</v>
       </c>
       <c r="I5" s="12">
         <v>-1.2653230893152347</v>
       </c>
       <c r="J5" s="26">
-        <v>8.0723111708814188E-2</v>
+        <v>3.7878974376187848</v>
       </c>
       <c r="K5" s="22">
         <v>60.236448997221061</v>
@@ -14131,19 +14131,19 @@
         <v>5.2725420275346382</v>
       </c>
       <c r="P5" s="12">
-        <v>0.4523809523784722</v>
+        <v>0.63193588164619208</v>
       </c>
       <c r="Q5" s="12">
-        <v>0</v>
+        <v>0.13225499525916601</v>
       </c>
       <c r="R5" s="12">
-        <v>12.288786482451039</v>
+        <v>13.249663828099127</v>
       </c>
       <c r="S5" s="12">
         <v>-1.4765356734608985</v>
       </c>
       <c r="T5" s="17">
-        <v>-7.8131568023122044</v>
+        <v>-11.355187540147956</v>
       </c>
       <c r="U5" t="s">
         <v>33</v>
@@ -14154,7 +14154,7 @@
         <v>69.646997034054138</v>
       </c>
       <c r="B6" s="13">
-        <v>36.566591858881331</v>
+        <v>38.458402231968847</v>
       </c>
       <c r="C6" s="13">
         <v>18.699481402012211</v>
@@ -14166,25 +14166,25 @@
         <v>5.1892194955163919</v>
       </c>
       <c r="F6" s="13">
-        <v>0.42664244092108089</v>
+        <v>0.67603437388697363</v>
       </c>
       <c r="G6" s="13">
-        <v>0.24471286826225566</v>
+        <v>0.41444857013796399</v>
       </c>
       <c r="H6" s="13">
-        <v>12.050986648072518</v>
+        <v>13.398634670832543</v>
       </c>
       <c r="I6" s="13">
         <v>-1.3394364278376054</v>
       </c>
       <c r="J6" s="27">
-        <v>5.591001236803641</v>
+        <v>4.1382982515221949</v>
       </c>
       <c r="K6" s="23">
         <v>124</v>
       </c>
-      <c r="L6" s="13" t="e">
-        <v>#NUM!</v>
+      <c r="L6" s="13">
+        <v>50</v>
       </c>
       <c r="M6" s="13">
         <v>54</v>
@@ -14196,19 +14196,19 @@
         <v>8</v>
       </c>
       <c r="P6" s="13">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="Q6" s="13">
         <v>1</v>
       </c>
-      <c r="R6" s="13" t="e">
-        <v>#NUM!</v>
+      <c r="R6" s="13">
+        <v>20</v>
       </c>
       <c r="S6" s="13">
         <v>0</v>
       </c>
-      <c r="T6" s="18" t="e">
-        <v>#NUM!</v>
+      <c r="T6" s="18">
+        <v>128.60882549606845</v>
       </c>
       <c r="U6" t="s">
         <v>34</v>
@@ -14219,7 +14219,7 @@
         <v>63.834502536464726</v>
       </c>
       <c r="B7" s="14">
-        <v>27.233832058123063</v>
+        <v>30.522622958284586</v>
       </c>
       <c r="C7" s="14">
         <v>17.071587593811174</v>
@@ -14231,25 +14231,25 @@
         <v>4.8008454627429877</v>
       </c>
       <c r="F7" s="14">
-        <v>0.4475077405667871</v>
+        <v>0.8141362012777279</v>
       </c>
       <c r="G7" s="14">
-        <v>0.10979945603454858</v>
+        <v>0.33461413351611224</v>
       </c>
       <c r="H7" s="14">
-        <v>17.260310196293108</v>
+        <v>16.430430272808806</v>
       </c>
       <c r="I7" s="14">
         <v>-0.60906515581735232</v>
       </c>
       <c r="J7" s="28">
-        <v>6.3888328414254643</v>
+        <v>7.8104745173924686</v>
       </c>
       <c r="K7" s="30" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="L7" s="14" t="e">
-        <v>#NUM!</v>
+      <c r="L7" s="14">
+        <v>50</v>
       </c>
       <c r="M7" s="14" t="e">
         <v>#NUM!</v>
@@ -14260,14 +14260,14 @@
       <c r="O7" s="14" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="P7" s="14" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Q7" s="14" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="R7" s="14" t="e">
-        <v>#NUM!</v>
+      <c r="P7" s="14">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>1</v>
+      </c>
+      <c r="R7" s="14">
+        <v>10</v>
       </c>
       <c r="S7" s="14">
         <v>0</v>
@@ -14284,7 +14284,7 @@
         <v>68.080396325980445</v>
       </c>
       <c r="B8" s="13">
-        <v>36.381661474816156</v>
+        <v>37.171790599557944</v>
       </c>
       <c r="C8" s="13">
         <v>16.410651158763443</v>
@@ -14296,19 +14296,19 @@
         <v>4.9897986211404799</v>
       </c>
       <c r="F8" s="13">
-        <v>0.29214139643858683</v>
+        <v>0.4820035518460406</v>
       </c>
       <c r="G8" s="13">
-        <v>0.18865030674978359</v>
+        <v>0.3054570294517609</v>
       </c>
       <c r="H8" s="13">
-        <v>12.050986648072518</v>
+        <v>12.905397711488948</v>
       </c>
       <c r="I8" s="13">
         <v>-1.5947194719335747</v>
       </c>
       <c r="J8" s="27">
-        <v>-7.2898533323613135</v>
+        <v>-11.000635039655407</v>
       </c>
       <c r="K8" s="23">
         <v>70.750000000000014</v>
@@ -14349,7 +14349,7 @@
         <v>74.070213422831159</v>
       </c>
       <c r="B9" s="13">
-        <v>44.438021978062515</v>
+        <v>44.655107917409083</v>
       </c>
       <c r="C9" s="13">
         <v>17.283524509918266</v>
@@ -14361,19 +14361,19 @@
         <v>4.8162961038177379</v>
       </c>
       <c r="F9" s="13">
-        <v>0.19387454794598952</v>
+        <v>0.28330760816678657</v>
       </c>
       <c r="G9" s="13">
-        <v>0.39795818264866323</v>
+        <v>0.44621400102573039</v>
       </c>
       <c r="H9" s="13">
-        <v>11.813186813693997</v>
+        <v>12.50580217158258</v>
       </c>
       <c r="I9" s="13">
         <v>-1.6688328104559451</v>
       </c>
       <c r="J9" s="27">
-        <v>-1.7795752072664861</v>
+        <v>-10.650234225752001</v>
       </c>
       <c r="K9" s="23">
         <v>73.01648351727134</v>
@@ -14403,7 +14403,7 @@
         <v>-1.7582417581741334</v>
       </c>
       <c r="T9" s="18">
-        <v>-7.2575351682520548</v>
+        <v>-19.83072445294458</v>
       </c>
       <c r="U9" t="s">
         <v>37</v>
@@ -14414,7 +14414,7 @@
         <v>68.257718925241733</v>
       </c>
       <c r="B10" s="13">
-        <v>35.105262177304247</v>
+        <v>36.719328643724822</v>
       </c>
       <c r="C10" s="13">
         <v>15.65563070171723</v>
@@ -14426,19 +14426,19 @@
         <v>4.4279220710443328</v>
       </c>
       <c r="F10" s="13">
-        <v>0.21473984759169579</v>
+        <v>0.4214094355575409</v>
       </c>
       <c r="G10" s="13">
-        <v>0.26304477042095609</v>
+        <v>0.36637956440387864</v>
       </c>
       <c r="H10" s="13">
-        <v>17.022510361914588</v>
+        <v>15.537597773558844</v>
       </c>
       <c r="I10" s="13">
         <v>-0.93846153843569213</v>
       </c>
       <c r="J10" s="27">
-        <v>-0.98174360264466143</v>
+        <v>-6.9780579598817241</v>
       </c>
       <c r="K10" s="23" t="e">
         <v>#NUM!</v>
@@ -14479,7 +14479,7 @@
         <v>65.022398987936995</v>
       </c>
       <c r="B11" s="12">
-        <v>28.543548780058586</v>
+        <v>31.17886151682583</v>
       </c>
       <c r="C11" s="12">
         <v>15.748100042136425</v>
@@ -14491,25 +14491,25 @@
         <v>4.7106654774384911</v>
       </c>
       <c r="F11" s="12">
-        <v>0.3749794035315811</v>
+        <v>0.84858952550821964</v>
       </c>
       <c r="G11" s="12">
-        <v>7.4394463671172514E-2</v>
+        <v>0.35749540859140855</v>
       </c>
       <c r="H11" s="12">
-        <v>17.260310196293108</v>
+        <v>17.678705920943457</v>
       </c>
       <c r="I11" s="12">
         <v>-0.65625793349788253</v>
       </c>
       <c r="J11" s="26">
-        <v>1.0595107994699706</v>
+        <v>8.8270915732496285</v>
       </c>
       <c r="K11" s="22">
         <v>70.999999999999986</v>
       </c>
       <c r="L11" s="12">
-        <v>30</v>
+        <v>36.967418546682488</v>
       </c>
       <c r="M11" s="12" t="e">
         <v>#NUM!</v>
@@ -14520,14 +14520,14 @@
       <c r="O11" s="12" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="P11" s="12" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Q11" s="12" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="R11" s="12" t="e">
-        <v>#NUM!</v>
+      <c r="P11" s="12">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="12">
+        <v>1</v>
+      </c>
+      <c r="R11" s="12">
+        <v>20</v>
       </c>
       <c r="S11" s="12">
         <v>0</v>
@@ -14544,7 +14544,7 @@
         <v>71.01221608478771</v>
       </c>
       <c r="B12" s="13">
-        <v>36.599909283304953</v>
+        <v>38.662178834676972</v>
       </c>
       <c r="C12" s="13">
         <v>16.620973393291248</v>
@@ -14556,19 +14556,19 @@
         <v>4.537162960115749</v>
       </c>
       <c r="F12" s="13">
-        <v>0.27671255503898384</v>
+        <v>0.64989358182896562</v>
       </c>
       <c r="G12" s="13">
-        <v>0.28370233957005214</v>
+        <v>0.49825238016537809</v>
       </c>
       <c r="H12" s="13">
-        <v>17.022510361914588</v>
+        <v>17.279110381037089</v>
       </c>
       <c r="I12" s="13">
         <v>-0.73037127202025309</v>
       </c>
       <c r="J12" s="27">
-        <v>6.5697889245648007</v>
+        <v>9.1774923871530394</v>
       </c>
       <c r="K12" s="23" t="e">
         <v>#NUM!</v>
@@ -14585,14 +14585,14 @@
       <c r="O12" s="13" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="P12" s="13" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Q12" s="13" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="R12" s="13" t="e">
-        <v>#NUM!</v>
+      <c r="P12" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="Q12" s="13">
+        <v>1</v>
+      </c>
+      <c r="R12" s="13">
+        <v>20</v>
       </c>
       <c r="S12" s="13">
         <v>0</v>
@@ -14609,7 +14609,7 @@
         <v>65.199721587198297</v>
       </c>
       <c r="B13" s="25">
-        <v>27.267149482546682</v>
+        <v>30.726399560992707</v>
       </c>
       <c r="C13" s="25">
         <v>14.993079585090214</v>
@@ -14621,19 +14621,19 @@
         <v>4.1487889273423448</v>
       </c>
       <c r="F13" s="25">
-        <v>0.29757785468469006</v>
+        <v>0.78799540921971989</v>
       </c>
       <c r="G13" s="25">
-        <v>0.14878892734234503</v>
+        <v>0.41841794354352635</v>
       </c>
       <c r="H13" s="25">
-        <v>22.231833910135176</v>
+        <v>20.310905983013356</v>
       </c>
       <c r="I13" s="25">
         <v>0</v>
       </c>
       <c r="J13" s="29">
-        <v>7.3676205291866266</v>
+        <v>12.849668653023318</v>
       </c>
       <c r="K13" s="24">
         <v>63.861591695991187</v>
@@ -14663,37 +14663,37 @@
         <v>0</v>
       </c>
       <c r="T13" s="20">
-        <v>4.7061300761323235</v>
+        <v>-7.7843061815675902</v>
       </c>
       <c r="U13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:36" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="60" t="s">
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="58"/>
-      <c r="R14" s="58"/>
-      <c r="S14" s="58"/>
-      <c r="T14" s="59"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="62"/>
+      <c r="O14" s="62"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="62"/>
+      <c r="T14" s="63"/>
     </row>
     <row r="15" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
@@ -14763,7 +14763,7 @@
         <v>64.264723434309744</v>
       </c>
       <c r="B16" s="9">
-        <v>28.517811596887885</v>
+        <v>30.489694443674079</v>
       </c>
       <c r="C16" s="9">
         <v>16.869919534243131</v>
@@ -14775,19 +14775,19 @@
         <v>5.0905341165105664</v>
       </c>
       <c r="F16" s="9">
-        <v>0.46573848322588185</v>
+        <v>0.74559530574792132</v>
       </c>
       <c r="G16" s="9">
-        <v>5.1318646297985396E-2</v>
+        <v>0.24194793125848016</v>
       </c>
       <c r="H16" s="9">
-        <v>13.931748610422067</v>
+        <v>15.139303593052365</v>
       </c>
       <c r="I16" s="9">
         <v>-1.4194126008656667</v>
       </c>
       <c r="J16" s="17">
-        <v>-3.5056113363707073</v>
+        <v>-2.8894910932888722</v>
       </c>
       <c r="K16" s="22">
         <v>65.929125138505597</v>
@@ -14817,7 +14817,7 @@
         <v>-4.2857142857142856</v>
       </c>
       <c r="T16" s="17">
-        <v>-41.005112675470841</v>
+        <v>-52.901939192699373</v>
       </c>
       <c r="U16" t="s">
         <v>33</v>
@@ -14831,7 +14831,7 @@
         <v>69.056577111790318</v>
       </c>
       <c r="B17" s="10">
-        <v>34.962899999484975</v>
+        <v>36.476348297954992</v>
       </c>
       <c r="C17" s="10">
         <v>17.56821821516699</v>
@@ -14843,19 +14843,19 @@
         <v>4.9517321026523735</v>
       </c>
       <c r="F17" s="10">
-        <v>0.38712500443180403</v>
+        <v>0.58663855080451821</v>
       </c>
       <c r="G17" s="10">
-        <v>0.21876494701708907</v>
+        <v>0.35455350851765577</v>
       </c>
       <c r="H17" s="10">
-        <v>13.741508742919251</v>
+        <v>14.819627161127269</v>
       </c>
       <c r="I17" s="10">
         <v>-1.4787032716835633</v>
       </c>
       <c r="J17" s="18">
-        <v>0.90261116370516037</v>
+        <v>-2.609170442166139</v>
       </c>
       <c r="K17" s="23" t="e">
         <v>#NUM!</v>
@@ -14896,7 +14896,7 @@
         <v>64.406581513718791</v>
       </c>
       <c r="B18" s="10">
-        <v>27.496692158878364</v>
+        <v>30.12772487900758</v>
       </c>
       <c r="C18" s="10">
         <v>16.265903168606162</v>
@@ -14908,19 +14908,19 @@
         <v>4.6410328764336501</v>
       </c>
       <c r="F18" s="10">
-        <v>0.403817244148369</v>
+        <v>0.69712001271712165</v>
       </c>
       <c r="G18" s="10">
-        <v>0.11083421723492341</v>
+        <v>0.29068595922017437</v>
       </c>
       <c r="H18" s="10">
-        <v>17.908967581495723</v>
+        <v>17.245063642708281</v>
       </c>
       <c r="I18" s="10">
         <v>-0.89440625406736096</v>
       </c>
       <c r="J18" s="18">
-        <v>1.5408764474026189</v>
+        <v>0.32857057053008187</v>
       </c>
       <c r="K18" s="23" t="e">
         <v>#NUM!</v>
@@ -14961,7 +14961,7 @@
         <v>67.803296545331364</v>
       </c>
       <c r="B19" s="9">
-        <v>34.814955692232836</v>
+        <v>35.447058992026271</v>
       </c>
       <c r="C19" s="9">
         <v>15.737154020567976</v>
@@ -14973,19 +14973,19 @@
         <v>4.7921954031516432</v>
       </c>
       <c r="F19" s="9">
-        <v>0.27952416884580877</v>
+        <v>0.43141389317177181</v>
       </c>
       <c r="G19" s="9">
-        <v>0.17391489780711142</v>
+        <v>0.26736027596869327</v>
       </c>
       <c r="H19" s="9">
-        <v>13.741508742919251</v>
+        <v>14.425037593652394</v>
       </c>
       <c r="I19" s="9">
         <v>-1.6829297069603388</v>
       </c>
       <c r="J19" s="17">
-        <v>-9.4020724916268072</v>
+        <v>-14.720317075108222</v>
       </c>
       <c r="K19" s="22" t="e">
         <v>#NUM!</v>
@@ -15026,7 +15026,7 @@
         <v>72.595150222811938</v>
       </c>
       <c r="B20" s="10">
-        <v>41.260044094829922</v>
+        <v>41.433712846307181</v>
       </c>
       <c r="C20" s="10">
         <v>16.435452701491833</v>
@@ -15038,19 +15038,19 @@
         <v>4.6533933892934503</v>
       </c>
       <c r="F20" s="10">
-        <v>0.20091069005173093</v>
+        <v>0.27245713822836859</v>
       </c>
       <c r="G20" s="10">
-        <v>0.34136119852621516</v>
+        <v>0.37996585322786885</v>
       </c>
       <c r="H20" s="10">
-        <v>13.551268875416435</v>
+        <v>14.105361161727298</v>
       </c>
       <c r="I20" s="10">
         <v>-1.742220377778235</v>
       </c>
       <c r="J20" s="18">
-        <v>-4.99384999155094</v>
+        <v>-14.439996423985498</v>
       </c>
       <c r="K20" s="23" t="e">
         <v>#NUM!</v>
@@ -15091,7 +15091,7 @@
         <v>67.945154624740397</v>
       </c>
       <c r="B21" s="10">
-        <v>33.793836254223308</v>
+        <v>35.085089427359769</v>
       </c>
       <c r="C21" s="10">
         <v>15.133137654931009</v>
@@ -15103,19 +15103,19 @@
         <v>4.342694163074726</v>
       </c>
       <c r="F21" s="10">
-        <v>0.21760292976829593</v>
+        <v>0.38293860014097203</v>
       </c>
       <c r="G21" s="10">
-        <v>0.23343046874404944</v>
+        <v>0.31609830393038746</v>
       </c>
       <c r="H21" s="10">
-        <v>17.718727713992905</v>
+        <v>16.530797643308311</v>
       </c>
       <c r="I21" s="10">
         <v>-1.1579233601620327</v>
       </c>
       <c r="J21" s="18">
-        <v>-4.3555847078534793</v>
+        <v>-11.502255411289271</v>
       </c>
       <c r="K21" s="23" t="e">
         <v>#NUM!</v>
@@ -15156,7 +15156,7 @@
         <v>65.356898674896598</v>
       </c>
       <c r="B22" s="9">
-        <v>28.544465536426781</v>
+        <v>30.652715725840579</v>
       </c>
       <c r="C22" s="9">
         <v>15.207113127266362</v>
@@ -15168,19 +15168,19 @@
         <v>4.5688888881900525</v>
       </c>
       <c r="F22" s="9">
-        <v>0.34579457452020418</v>
+        <v>0.72468267210151505</v>
       </c>
       <c r="G22" s="9">
-        <v>8.2510223344222561E-2</v>
+        <v>0.30899097928041142</v>
       </c>
       <c r="H22" s="9">
-        <v>17.908967581495723</v>
+        <v>18.243684161216002</v>
       </c>
       <c r="I22" s="9">
         <v>-0.93216047621178499</v>
       </c>
       <c r="J22" s="17">
-        <v>-2.7225811861617784</v>
+        <v>1.1418642152158067</v>
       </c>
       <c r="K22" s="22">
         <v>73</v>
@@ -15221,7 +15221,7 @@
         <v>70.148752352377173</v>
       </c>
       <c r="B23" s="10">
-        <v>34.989553939023878</v>
+        <v>36.639369580121489</v>
       </c>
       <c r="C23" s="10">
         <v>15.90541180819022</v>
@@ -15233,19 +15233,19 @@
         <v>4.4300868743318587</v>
       </c>
       <c r="F23" s="10">
-        <v>0.26718109572612636</v>
+        <v>0.56572591715811182</v>
       </c>
       <c r="G23" s="10">
-        <v>0.24995652406332627</v>
+        <v>0.42159655653958705</v>
       </c>
       <c r="H23" s="10">
-        <v>17.718727713992905</v>
+        <v>17.924007729290906</v>
       </c>
       <c r="I23" s="10">
         <v>-0.99145114702968162</v>
       </c>
       <c r="J23" s="18">
-        <v>1.6856413139140811</v>
+        <v>1.4221848663385317</v>
       </c>
       <c r="K23" s="23" t="e">
         <v>#NUM!</v>
@@ -15286,7 +15286,7 @@
         <v>65.498756754305646</v>
       </c>
       <c r="B24" s="19">
-        <v>27.52334609841726</v>
+        <v>30.290746161174081</v>
       </c>
       <c r="C24" s="19">
         <v>14.603096761629393</v>
@@ -15298,19 +15298,19 @@
         <v>4.1193876481131353</v>
       </c>
       <c r="F24" s="19">
-        <v>0.28387333544269133</v>
+        <v>0.67620737907071526</v>
       </c>
       <c r="G24" s="19">
-        <v>0.14202579428116058</v>
+        <v>0.35772900724210566</v>
       </c>
       <c r="H24" s="19">
-        <v>21.886186552569377</v>
+        <v>20.349444210871919</v>
       </c>
       <c r="I24" s="19">
         <v>-0.407154129413479</v>
       </c>
       <c r="J24" s="20">
-        <v>2.3239065976115443</v>
+        <v>4.3599258790347601</v>
       </c>
       <c r="K24" s="24">
         <v>65.410569106348078</v>
@@ -15340,37 +15340,37 @@
         <v>0</v>
       </c>
       <c r="T24" s="20">
-        <v>0.87101847892389195</v>
+        <v>-10.798028350673622</v>
       </c>
       <c r="U24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="58" t="s">
+      <c r="A25" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="58"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="60" t="s">
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="58"/>
-      <c r="S25" s="58"/>
-      <c r="T25" s="59"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="62"/>
+      <c r="N25" s="62"/>
+      <c r="O25" s="62"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="62"/>
+      <c r="R25" s="62"/>
+      <c r="S25" s="62"/>
+      <c r="T25" s="63"/>
     </row>
     <row r="26" spans="1:22" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
@@ -15440,7 +15440,7 @@
         <v>65.757297049996879</v>
       </c>
       <c r="B27" s="12">
-        <v>31.304946867122482</v>
+        <v>33.399850092029752</v>
       </c>
       <c r="C27" s="12">
         <v>17.943341143894617</v>
@@ -15452,19 +15452,19 @@
         <v>5.2529473944521436</v>
       </c>
       <c r="F27" s="12">
-        <v>0.47972958980913571</v>
+        <v>0.81762598068138226</v>
       </c>
       <c r="G27" s="12">
-        <v>0.10719090036675509</v>
+        <v>0.32204680403447911</v>
       </c>
       <c r="H27" s="12">
-        <v>12.312666122054175</v>
+        <v>13.817143538425668</v>
       </c>
       <c r="I27" s="9">
         <v>-1.2639627189448877</v>
       </c>
       <c r="J27" s="17">
-        <v>1.4592796946009319</v>
+        <v>4.0344067790843505</v>
       </c>
       <c r="K27" s="22" t="e">
         <v>#NUM!</v>
@@ -15481,14 +15481,14 @@
       <c r="O27" s="12" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="P27" s="12" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Q27" s="12" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="R27" s="12" t="e">
-        <v>#NUM!</v>
+      <c r="P27" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="12">
+        <v>1</v>
+      </c>
+      <c r="R27" s="12">
+        <v>20</v>
       </c>
       <c r="S27" s="12">
         <v>0</v>
@@ -15508,7 +15508,7 @@
         <v>70.549150727477453</v>
       </c>
       <c r="B28" s="13">
-        <v>37.750035269719575</v>
+        <v>39.386503946310661</v>
       </c>
       <c r="C28" s="13">
         <v>18.641639824818476</v>
@@ -15520,25 +15520,25 @@
         <v>5.1141453805939499</v>
       </c>
       <c r="F28" s="13">
-        <v>0.40111611101505779</v>
+        <v>0.65866922573797915</v>
       </c>
       <c r="G28" s="13">
-        <v>0.27463720108585876</v>
+        <v>0.43465238129365469</v>
       </c>
       <c r="H28" s="13">
-        <v>12.122426254551359</v>
+        <v>13.497467106500574</v>
       </c>
       <c r="I28" s="10">
         <v>-1.3232533897627843</v>
       </c>
       <c r="J28" s="18">
-        <v>5.8675021946767902</v>
+        <v>4.3147274302070793</v>
       </c>
       <c r="K28" s="23">
         <v>124</v>
       </c>
-      <c r="L28" s="13" t="e">
-        <v>#NUM!</v>
+      <c r="L28" s="13">
+        <v>50</v>
       </c>
       <c r="M28" s="13">
         <v>54</v>
@@ -15555,14 +15555,14 @@
       <c r="Q28" s="13">
         <v>1</v>
       </c>
-      <c r="R28" s="13" t="e">
-        <v>#NUM!</v>
+      <c r="R28" s="13">
+        <v>20</v>
       </c>
       <c r="S28" s="13">
         <v>0</v>
       </c>
-      <c r="T28" s="18" t="e">
-        <v>#NUM!</v>
+      <c r="T28" s="18">
+        <v>139.80116925437443</v>
       </c>
       <c r="U28" t="s">
         <v>34</v>
@@ -15573,7 +15573,7 @@
         <v>65.899155129405926</v>
       </c>
       <c r="B29" s="13">
-        <v>30.283827429112961</v>
+        <v>33.037880527363249</v>
       </c>
       <c r="C29" s="13">
         <v>17.339324778257645</v>
@@ -15585,19 +15585,19 @@
         <v>4.8034461543752265</v>
       </c>
       <c r="F29" s="13">
-        <v>0.41780835073162281</v>
+        <v>0.76915068765058248</v>
       </c>
       <c r="G29" s="13">
-        <v>0.16670647130369312</v>
+        <v>0.37078483199617329</v>
       </c>
       <c r="H29" s="13">
-        <v>16.289885093127829</v>
+        <v>15.922903588081585</v>
       </c>
       <c r="I29" s="10">
         <v>-0.73895637214658183</v>
       </c>
       <c r="J29" s="18">
-        <v>6.5057674783742474</v>
+        <v>7.252468442903294</v>
       </c>
       <c r="K29" s="23" t="e">
         <v>#NUM!</v>
@@ -15614,14 +15614,14 @@
       <c r="O29" s="13" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="P29" s="13" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Q29" s="13" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="R29" s="13" t="e">
-        <v>#NUM!</v>
+      <c r="P29" s="13">
+        <v>2</v>
+      </c>
+      <c r="Q29" s="13">
+        <v>1</v>
+      </c>
+      <c r="R29" s="13">
+        <v>20</v>
       </c>
       <c r="S29" s="13">
         <v>0</v>
@@ -15638,7 +15638,7 @@
         <v>69.295870161018499</v>
       </c>
       <c r="B30" s="12">
-        <v>37.602090962467436</v>
+        <v>38.35721464038194</v>
       </c>
       <c r="C30" s="12">
         <v>16.810575630219461</v>
@@ -15650,19 +15650,19 @@
         <v>4.9546086810932204</v>
       </c>
       <c r="F30" s="12">
-        <v>0.29351527542906253</v>
+        <v>0.50344456810523275</v>
       </c>
       <c r="G30" s="12">
-        <v>0.22978715187588111</v>
+        <v>0.34745914874469219</v>
       </c>
       <c r="H30" s="12">
-        <v>12.122426254551359</v>
+        <v>13.102877539025698</v>
       </c>
       <c r="I30" s="9">
         <v>-1.5274798250395598</v>
       </c>
       <c r="J30" s="17">
-        <v>-4.4371814606551769</v>
+        <v>-7.7964192027350085</v>
       </c>
       <c r="K30" s="22" t="e">
         <v>#NUM!</v>
@@ -15703,7 +15703,7 @@
         <v>74.087723838499073</v>
       </c>
       <c r="B31" s="13">
-        <v>44.047179365064522</v>
+        <v>44.34386849466285</v>
       </c>
       <c r="C31" s="13">
         <v>17.50887431114332</v>
@@ -15715,19 +15715,19 @@
         <v>4.8158066672350266</v>
       </c>
       <c r="F31" s="13">
-        <v>0.21490179663498471</v>
+        <v>0.34448781316182947</v>
       </c>
       <c r="G31" s="13">
-        <v>0.39723345259498483</v>
+        <v>0.46006472600386783</v>
       </c>
       <c r="H31" s="13">
-        <v>11.932186387048542</v>
+        <v>12.783201107100604</v>
       </c>
       <c r="I31" s="10">
         <v>-1.586770495857456</v>
       </c>
       <c r="J31" s="18">
-        <v>-2.8958960579311466E-2</v>
+        <v>-7.5160985516122771</v>
       </c>
       <c r="K31" s="23">
         <v>73.01648351727134</v>
@@ -15757,7 +15757,7 @@
         <v>-1.7582417581741334</v>
       </c>
       <c r="T31" s="18">
-        <v>-7.2575351682520548</v>
+        <v>-19.83072445294458</v>
       </c>
       <c r="U31" t="s">
         <v>37</v>
@@ -15768,7 +15768,7 @@
         <v>69.437728240427532</v>
       </c>
       <c r="B32" s="13">
-        <v>36.580971524457908</v>
+        <v>37.995245075715438</v>
       </c>
       <c r="C32" s="13">
         <v>16.206559264582491</v>
@@ -15780,19 +15780,19 @@
         <v>4.5051074410163023</v>
       </c>
       <c r="F32" s="13">
-        <v>0.23159403635154971</v>
+        <v>0.45496927507443291</v>
       </c>
       <c r="G32" s="13">
-        <v>0.2893027228128191</v>
+        <v>0.39619717670638643</v>
       </c>
       <c r="H32" s="13">
-        <v>16.099645225625014</v>
+        <v>15.208637588681615</v>
       </c>
       <c r="I32" s="10">
         <v>-1.0024734782412537</v>
       </c>
       <c r="J32" s="18">
-        <v>0.60930632311814681</v>
+        <v>-4.5783575389160589</v>
       </c>
       <c r="K32" s="23" t="e">
         <v>#NUM!</v>
@@ -15833,7 +15833,7 @@
         <v>66.849472290583748</v>
       </c>
       <c r="B33" s="12">
-        <v>31.331600806661378</v>
+        <v>33.562871374196249</v>
       </c>
       <c r="C33" s="12">
         <v>16.280534736917847</v>
@@ -15845,25 +15845,25 @@
         <v>4.7313021661316288</v>
       </c>
       <c r="F33" s="12">
-        <v>0.35978568110345799</v>
+        <v>0.79671334703497598</v>
       </c>
       <c r="G33" s="12">
-        <v>0.13838247741299226</v>
+        <v>0.38908985205641033</v>
       </c>
       <c r="H33" s="12">
-        <v>16.289885093127829</v>
+        <v>16.921524106589306</v>
       </c>
       <c r="I33" s="9">
         <v>-0.77671059429100597</v>
       </c>
       <c r="J33" s="17">
-        <v>2.2423098448098506</v>
+        <v>8.0657620875890217</v>
       </c>
       <c r="K33" s="22">
         <v>69</v>
       </c>
       <c r="L33" s="12">
-        <v>30</v>
+        <v>36.967418546682495</v>
       </c>
       <c r="M33" s="12" t="e">
         <v>#NUM!</v>
@@ -15874,14 +15874,14 @@
       <c r="O33" s="12" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="P33" s="12" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Q33" s="12" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="R33" s="12" t="e">
-        <v>#NUM!</v>
+      <c r="P33" s="12">
+        <v>2</v>
+      </c>
+      <c r="Q33" s="12">
+        <v>1</v>
+      </c>
+      <c r="R33" s="12">
+        <v>20</v>
       </c>
       <c r="S33" s="12">
         <v>0</v>
@@ -15898,7 +15898,7 @@
         <v>71.641325968064308</v>
       </c>
       <c r="B34" s="13">
-        <v>37.776689209258471</v>
+        <v>39.549525228477158</v>
       </c>
       <c r="C34" s="13">
         <v>16.978833417841706</v>
@@ -15910,19 +15910,19 @@
         <v>4.5925001522734359</v>
       </c>
       <c r="F34" s="13">
-        <v>0.28117220230938017</v>
+        <v>0.63775659209157265</v>
       </c>
       <c r="G34" s="13">
-        <v>0.30582877813209597</v>
+        <v>0.50169542931558597</v>
       </c>
       <c r="H34" s="13">
-        <v>16.099645225625014</v>
+        <v>16.60184767466421</v>
       </c>
       <c r="I34" s="10">
         <v>-0.8360012651089026</v>
       </c>
       <c r="J34" s="18">
-        <v>6.650532344885721</v>
+        <v>8.3460827387117504</v>
       </c>
       <c r="K34" s="23" t="e">
         <v>#NUM!</v>
@@ -15939,14 +15939,14 @@
       <c r="O34" s="13" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="P34" s="13" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Q34" s="13" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="R34" s="13" t="e">
-        <v>#NUM!</v>
+      <c r="P34" s="13">
+        <v>2</v>
+      </c>
+      <c r="Q34" s="13">
+        <v>1</v>
+      </c>
+      <c r="R34" s="13">
+        <v>20</v>
       </c>
       <c r="S34" s="13">
         <v>0</v>
@@ -15963,7 +15963,7 @@
         <v>66.991330369992781</v>
       </c>
       <c r="B35" s="25">
-        <v>30.310481368651857</v>
+        <v>33.200901809529753</v>
       </c>
       <c r="C35" s="25">
         <v>15.676518371280878</v>
@@ -15975,19 +15975,19 @@
         <v>4.2818009260547125</v>
       </c>
       <c r="F35" s="25">
-        <v>0.29786444202594514</v>
+        <v>0.7482380540041762</v>
       </c>
       <c r="G35" s="25">
-        <v>0.19789804834993027</v>
+        <v>0.43782788001810458</v>
       </c>
       <c r="H35" s="25">
-        <v>20.267104064201483</v>
+        <v>19.027284156245223</v>
       </c>
       <c r="I35" s="19">
         <v>-0.25170424749269998</v>
       </c>
       <c r="J35" s="20">
-        <v>7.2887976285831737</v>
+        <v>11.283823751407976</v>
       </c>
       <c r="K35" s="24">
         <v>55</v>
@@ -16017,37 +16017,37 @@
         <v>0</v>
       </c>
       <c r="T35" s="20">
-        <v>26.64653595667486</v>
+        <v>9.4569880872890462</v>
       </c>
       <c r="U35" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="58" t="s">
+      <c r="A36" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="59"/>
-      <c r="K36" s="60" t="s">
+      <c r="B36" s="62"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="63"/>
+      <c r="K36" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="L36" s="58"/>
-      <c r="M36" s="58"/>
-      <c r="N36" s="58"/>
-      <c r="O36" s="58"/>
-      <c r="P36" s="58"/>
-      <c r="Q36" s="58"/>
-      <c r="R36" s="58"/>
-      <c r="S36" s="58"/>
-      <c r="T36" s="59"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="62"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="62"/>
+      <c r="R36" s="62"/>
+      <c r="S36" s="62"/>
+      <c r="T36" s="63"/>
     </row>
     <row r="37" spans="1:22" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
@@ -16117,7 +16117,7 @@
         <v>63.006356194709973</v>
       </c>
       <c r="B38" s="9">
-        <v>28.802062635549952</v>
+        <v>31.476744414352293</v>
       </c>
       <c r="C38" s="9">
         <v>17.856190899278729</v>
@@ -16129,19 +16129,19 @@
         <v>5.4390059826708441</v>
       </c>
       <c r="F38" s="9">
-        <v>0.51992743153094256</v>
+        <v>0.89217096101016868</v>
       </c>
       <c r="G38" s="9">
-        <v>2.8323993890700845E-2</v>
+        <v>0.28405866527506018</v>
       </c>
       <c r="H38" s="9">
-        <v>11.831029185960832</v>
+        <v>13.429216487134317</v>
       </c>
       <c r="I38" s="9">
         <v>-1.1101869083666547</v>
       </c>
       <c r="J38" s="17">
-        <v>0.79026113834379463</v>
+        <v>5.757375087877727</v>
       </c>
       <c r="K38" s="22">
         <v>56.666666666666657</v>
@@ -16159,19 +16159,19 @@
         <v>5.7441418619976812</v>
       </c>
       <c r="P38" s="9">
-        <v>0.5</v>
+        <v>0.68971792541314336</v>
       </c>
       <c r="Q38" s="9">
-        <v>0</v>
+        <v>8.8030398999503059E-2</v>
       </c>
       <c r="R38" s="9">
-        <v>10</v>
+        <v>10.880303989995031</v>
       </c>
       <c r="S38" s="9">
         <v>0</v>
       </c>
       <c r="T38" s="17">
-        <v>6.6115958185113737</v>
+        <v>1.3891790374763895</v>
       </c>
       <c r="U38" t="s">
         <v>33</v>
@@ -16185,7 +16185,7 @@
         <v>67.79820987219054</v>
       </c>
       <c r="B39" s="10">
-        <v>35.247151038147045</v>
+        <v>37.463398268633206</v>
       </c>
       <c r="C39" s="10">
         <v>18.554489580202588</v>
@@ -16197,25 +16197,25 @@
         <v>5.3002039688126503</v>
       </c>
       <c r="F39" s="10">
-        <v>0.44131395273686475</v>
+        <v>0.73321420606676546</v>
       </c>
       <c r="G39" s="10">
-        <v>0.19577029460980452</v>
+        <v>0.39666424253423577</v>
       </c>
       <c r="H39" s="10">
-        <v>11.640789318458015</v>
+        <v>13.109540055209223</v>
       </c>
       <c r="I39" s="10">
         <v>-1.1694775791845511</v>
       </c>
       <c r="J39" s="18">
-        <v>5.1984836384196571</v>
+        <v>6.0376957390004531</v>
       </c>
       <c r="K39" s="23" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="L39" s="10" t="e">
-        <v>#NUM!</v>
+      <c r="L39" s="10">
+        <v>50</v>
       </c>
       <c r="M39" s="10" t="e">
         <v>#NUM!</v>
@@ -16226,14 +16226,14 @@
       <c r="O39" s="10" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="P39" s="10" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Q39" s="10" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="R39" s="10" t="e">
-        <v>#NUM!</v>
+      <c r="P39" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="10">
+        <v>1</v>
+      </c>
+      <c r="R39" s="10">
+        <v>20</v>
       </c>
       <c r="S39" s="10">
         <v>0</v>
@@ -16250,7 +16250,7 @@
         <v>63.148214274119013</v>
       </c>
       <c r="B40" s="10">
-        <v>27.780943197540431</v>
+        <v>31.114774849685794</v>
       </c>
       <c r="C40" s="10">
         <v>17.252174533641757</v>
@@ -16262,25 +16262,25 @@
         <v>4.989504742593927</v>
       </c>
       <c r="F40" s="10">
-        <v>0.45800619245342966</v>
+        <v>0.84369566797936901</v>
       </c>
       <c r="G40" s="10">
-        <v>8.7839564827638855E-2</v>
+        <v>0.33279669323675437</v>
       </c>
       <c r="H40" s="10">
-        <v>15.808248157034487</v>
+        <v>15.534976536790234</v>
       </c>
       <c r="I40" s="10">
         <v>-0.58518056156834874</v>
       </c>
       <c r="J40" s="18">
-        <v>5.8367489221171116</v>
+        <v>8.9754367516966713</v>
       </c>
       <c r="K40" s="23" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="L40" s="10" t="e">
-        <v>#NUM!</v>
+      <c r="L40" s="10">
+        <v>50</v>
       </c>
       <c r="M40" s="10" t="e">
         <v>#NUM!</v>
@@ -16291,14 +16291,14 @@
       <c r="O40" s="10" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="P40" s="10" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Q40" s="10" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="R40" s="10" t="e">
-        <v>#NUM!</v>
+      <c r="P40" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q40" s="10">
+        <v>1</v>
+      </c>
+      <c r="R40" s="10">
+        <v>0</v>
       </c>
       <c r="S40" s="10">
         <v>0</v>
@@ -16315,7 +16315,7 @@
         <v>66.544929305731586</v>
       </c>
       <c r="B41" s="9">
-        <v>35.099206730894906</v>
+        <v>36.434108962704485</v>
       </c>
       <c r="C41" s="9">
         <v>16.723425385603573</v>
@@ -16327,19 +16327,19 @@
         <v>5.1406672693119209</v>
       </c>
       <c r="F41" s="9">
-        <v>0.33371311715086949</v>
+        <v>0.57798954843401906</v>
       </c>
       <c r="G41" s="9">
-        <v>0.15092024539982687</v>
+        <v>0.30947100998527327</v>
       </c>
       <c r="H41" s="9">
-        <v>11.640789318458015</v>
+        <v>12.714950487734345</v>
       </c>
       <c r="I41" s="9">
         <v>-1.3737040144613266</v>
       </c>
       <c r="J41" s="17">
-        <v>-5.1062000169123083</v>
+        <v>-6.0734508939416347</v>
       </c>
       <c r="K41" s="22">
         <v>70.750000000000014</v>
@@ -16380,7 +16380,7 @@
         <v>71.33678298321216</v>
       </c>
       <c r="B42" s="10">
-        <v>41.544295133491993</v>
+        <v>42.420762816985395</v>
       </c>
       <c r="C42" s="10">
         <v>17.421724066527432</v>
@@ -16392,19 +16392,19 @@
         <v>5.0018652554537271</v>
       </c>
       <c r="F42" s="10">
-        <v>0.25509963835679161</v>
+        <v>0.41903279349061584</v>
       </c>
       <c r="G42" s="10">
-        <v>0.31836654611893056</v>
+        <v>0.42207658724444885</v>
       </c>
       <c r="H42" s="10">
-        <v>11.450549450955197</v>
+        <v>12.395274055809251</v>
       </c>
       <c r="I42" s="10">
         <v>-1.432994685279223</v>
       </c>
       <c r="J42" s="18">
-        <v>-0.69797751683644749</v>
+        <v>-5.7931302428189069</v>
       </c>
       <c r="K42" s="23" t="e">
         <v>#NUM!</v>
@@ -16445,7 +16445,7 @@
         <v>66.686787385140619</v>
       </c>
       <c r="B43" s="10">
-        <v>34.078087292885378</v>
+        <v>36.072139398037983</v>
       </c>
       <c r="C43" s="10">
         <v>16.119409019966604</v>
@@ -16457,19 +16457,19 @@
         <v>4.6911660292350019</v>
       </c>
       <c r="F43" s="10">
-        <v>0.27179187807335664</v>
+        <v>0.52951425540321939</v>
       </c>
       <c r="G43" s="10">
-        <v>0.21043581633676486</v>
+        <v>0.35820903794696746</v>
       </c>
       <c r="H43" s="10">
-        <v>15.618008289531669</v>
+        <v>14.820710537390264</v>
       </c>
       <c r="I43" s="10">
         <v>-0.84869766766302068</v>
       </c>
       <c r="J43" s="18">
-        <v>-5.9712233138992314E-2</v>
+        <v>-2.8553892301226864</v>
       </c>
       <c r="K43" s="23" t="e">
         <v>#NUM!</v>
@@ -16510,7 +16510,7 @@
         <v>64.098531435296835</v>
       </c>
       <c r="B44" s="9">
-        <v>28.828716575088851</v>
+        <v>31.639765696518786</v>
       </c>
       <c r="C44" s="9">
         <v>16.193384492301959</v>
@@ -16522,25 +16522,25 @@
         <v>4.9173607543503293</v>
       </c>
       <c r="F44" s="9">
-        <v>0.39998352282526489</v>
+        <v>0.8712583273637623</v>
       </c>
       <c r="G44" s="9">
-        <v>5.951557093693801E-2</v>
+        <v>0.35110171329699141</v>
       </c>
       <c r="H44" s="9">
-        <v>15.808248157034487</v>
+        <v>16.533597055297953</v>
       </c>
       <c r="I44" s="9">
         <v>-0.622934783712773</v>
       </c>
       <c r="J44" s="17">
-        <v>1.5732912885527182</v>
+        <v>9.7887303963823946</v>
       </c>
       <c r="K44" s="22" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="L44" s="9" t="e">
-        <v>#NUM!</v>
+      <c r="L44" s="9">
+        <v>50</v>
       </c>
       <c r="M44" s="9" t="e">
         <v>#NUM!</v>
@@ -16551,14 +16551,14 @@
       <c r="O44" s="9" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="P44" s="9" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Q44" s="9" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="R44" s="9" t="e">
-        <v>#NUM!</v>
+      <c r="P44" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q44" s="9">
+        <v>1</v>
+      </c>
+      <c r="R44" s="9">
+        <v>20</v>
       </c>
       <c r="S44" s="9">
         <v>0</v>
@@ -16575,7 +16575,7 @@
         <v>68.890385112777409</v>
       </c>
       <c r="B45" s="10">
-        <v>35.273804977685941</v>
+        <v>37.626419550799703</v>
       </c>
       <c r="C45" s="10">
         <v>16.891683173225818</v>
@@ -16587,19 +16587,19 @@
         <v>4.7785587404921355</v>
       </c>
       <c r="F45" s="10">
-        <v>0.32137004403118707</v>
+        <v>0.71230157242035907</v>
       </c>
       <c r="G45" s="10">
-        <v>0.2269618716560417</v>
+        <v>0.463707290556167</v>
       </c>
       <c r="H45" s="10">
-        <v>15.618008289531669</v>
+        <v>16.213920623372861</v>
       </c>
       <c r="I45" s="10">
         <v>-0.68222545453066941</v>
       </c>
       <c r="J45" s="18">
-        <v>5.9815137886285816</v>
+        <v>10.069051047505127</v>
       </c>
       <c r="K45" s="23" t="e">
         <v>#NUM!</v>
@@ -16616,14 +16616,14 @@
       <c r="O45" s="10" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="P45" s="10" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Q45" s="10" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="R45" s="10" t="e">
-        <v>#NUM!</v>
+      <c r="P45" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="10">
+        <v>1</v>
+      </c>
+      <c r="R45" s="10">
+        <v>20</v>
       </c>
       <c r="S45" s="10">
         <v>0</v>
@@ -16640,7 +16640,7 @@
         <v>64.240389514705868</v>
       </c>
       <c r="B46" s="19">
-        <v>27.80759713707933</v>
+        <v>31.277796131852291</v>
       </c>
       <c r="C46" s="19">
         <v>15.58936812666499</v>
@@ -16652,19 +16652,19 @@
         <v>4.4678595142734121</v>
       </c>
       <c r="F46" s="19">
-        <v>0.33806228374775205</v>
+        <v>0.82278303433296252</v>
       </c>
       <c r="G46" s="19">
-        <v>0.11903114187387602</v>
+        <v>0.39983974125868565</v>
       </c>
       <c r="H46" s="19">
-        <v>19.785467128108142</v>
+        <v>18.639357104953874</v>
       </c>
       <c r="I46" s="19">
         <v>-9.7928436914466913E-2</v>
       </c>
       <c r="J46" s="20">
-        <v>6.6197790723260415</v>
+        <v>13.00679206020135</v>
       </c>
       <c r="K46" s="24" t="e">
         <v>#NUM!</v>
@@ -16705,7 +16705,7 @@
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J50" t="s">
         <v>5</v>
@@ -16827,125 +16827,125 @@
     <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" s="46">
         <f>J16</f>
-        <v>66.234839164722985</v>
+        <v>-2.8894910932888722</v>
       </c>
       <c r="B52" s="46">
         <f>J17</f>
-        <v>65.742305935746685</v>
+        <v>-2.609170442166139</v>
       </c>
       <c r="C52" s="46">
         <f>J18</f>
-        <v>71.098061417107019</v>
+        <v>0.32857057053008187</v>
       </c>
       <c r="D52" s="46">
         <f>J19</f>
-        <v>64.767198704393138</v>
+        <v>-14.720317075108222</v>
       </c>
       <c r="E52" s="46">
         <f>J20</f>
-        <v>64.274665475416825</v>
+        <v>-14.439996423985498</v>
       </c>
       <c r="F52" s="46">
         <f>J21</f>
-        <v>69.630420956777158</v>
+        <v>-11.502255411289271</v>
       </c>
       <c r="G52" s="46">
         <f>J22</f>
-        <v>70.986913965221305</v>
+        <v>1.1418642152158067</v>
       </c>
       <c r="H52" s="46">
         <f>J23</f>
-        <v>70.494380736244992</v>
+        <v>1.4221848663385317</v>
       </c>
       <c r="I52" s="46">
         <f>J24</f>
-        <v>75.850136217605339</v>
+        <v>4.3599258790347601</v>
       </c>
       <c r="J52" s="46">
         <f>J27</f>
-        <v>69.879595568809521</v>
+        <v>4.0344067790843505</v>
       </c>
       <c r="K52" s="46">
         <f>J28</f>
-        <v>69.387062339833221</v>
+        <v>4.3147274302070793</v>
       </c>
       <c r="L52" s="46">
         <f>J29</f>
-        <v>74.742817821193569</v>
+        <v>7.252468442903294</v>
       </c>
       <c r="M52" s="46">
         <f>J30</f>
-        <v>68.411955108479674</v>
+        <v>-7.7964192027350085</v>
       </c>
       <c r="N52" s="46">
         <f>J31</f>
-        <v>67.919421879503375</v>
+        <v>-7.5160985516122771</v>
       </c>
       <c r="O52" s="46">
         <f>J32</f>
-        <v>73.275177360863708</v>
+        <v>-4.5783575389160589</v>
       </c>
       <c r="P52" s="46">
         <f>J33</f>
-        <v>74.631670369307855</v>
+        <v>8.0657620875890217</v>
       </c>
       <c r="Q52" s="46">
         <f>J34</f>
-        <v>74.139137140331528</v>
+        <v>8.3460827387117504</v>
       </c>
       <c r="R52" s="46">
         <f>J35</f>
-        <v>79.494892621691889</v>
+        <v>11.283823751407976</v>
       </c>
       <c r="S52" s="46">
         <f>J38</f>
-        <v>71.634369636016089</v>
+        <v>5.757375087877727</v>
       </c>
       <c r="T52" s="46">
         <f>J39</f>
-        <v>71.141836407039804</v>
+        <v>6.0376957390004531</v>
       </c>
       <c r="U52" s="46">
         <f>J40</f>
-        <v>76.497591888400137</v>
+        <v>8.9754367516966713</v>
       </c>
       <c r="V52" s="46">
         <f>J41</f>
-        <v>70.166729175686257</v>
+        <v>-6.0734508939416347</v>
       </c>
       <c r="W52" s="46">
         <f>J42</f>
-        <v>69.674195946709958</v>
+        <v>-5.7931302428189069</v>
       </c>
       <c r="X52" s="46">
         <f>J43</f>
-        <v>75.029951428070277</v>
+        <v>-2.8553892301226864</v>
       </c>
       <c r="Y52" s="46">
         <f>J44</f>
-        <v>76.386444436514424</v>
+        <v>9.7887303963823946</v>
       </c>
       <c r="Z52" s="46">
         <f>J45</f>
-        <v>75.893911207538125</v>
+        <v>10.069051047505127</v>
       </c>
       <c r="AA52" s="46">
         <f>J46</f>
-        <v>81.249666688898458</v>
+        <v>13.00679206020135</v>
       </c>
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" s="46">
         <f>T16</f>
-        <v>38.446599589058643</v>
+        <v>-52.901939192699373</v>
       </c>
       <c r="B53" s="46" t="e">
         <f>T17</f>
         <v>#NUM!</v>
       </c>
-      <c r="C53" s="46">
+      <c r="C53" s="46" t="e">
         <f>T18</f>
-        <v>70.906136035185824</v>
+        <v>#NUM!</v>
       </c>
       <c r="D53" s="46" t="e">
         <f>T19</f>
@@ -16969,15 +16969,15 @@
       </c>
       <c r="I53" s="46">
         <f>T24</f>
-        <v>81.809108790439183</v>
+        <v>-10.798028350673622</v>
       </c>
       <c r="J53" s="46" t="e">
         <f>T27</f>
         <v>#NUM!</v>
       </c>
-      <c r="K53" s="46" t="e">
+      <c r="K53" s="46">
         <f>T28</f>
-        <v>#NUM!</v>
+        <v>139.80116925437443</v>
       </c>
       <c r="L53" s="46" t="e">
         <f>T29</f>
@@ -16989,7 +16989,7 @@
       </c>
       <c r="N53" s="46">
         <f>T31</f>
-        <v>77.412540761452632</v>
+        <v>-19.83072445294458</v>
       </c>
       <c r="O53" s="46" t="e">
         <f>T32</f>
@@ -17005,11 +17005,11 @@
       </c>
       <c r="R53" s="46">
         <f>T35</f>
-        <v>77.803502498541008</v>
+        <v>9.4569880872890462</v>
       </c>
       <c r="S53" s="46">
         <f>T38</f>
-        <v>85.267534783374572</v>
+        <v>1.3891790374763895</v>
       </c>
       <c r="T53" s="46" t="e">
         <f>T39</f>
@@ -17019,9 +17019,9 @@
         <f>T40</f>
         <v>#NUM!</v>
       </c>
-      <c r="V53" s="46">
+      <c r="V53" s="46" t="e">
         <f>T41</f>
-        <v>49.617266749077956</v>
+        <v>#NUM!</v>
       </c>
       <c r="W53" s="46" t="e">
         <f>T42</f>
@@ -17039,24 +17039,24 @@
         <f>T45</f>
         <v>#NUM!</v>
       </c>
-      <c r="AA53" s="46">
+      <c r="AA53" s="46" t="e">
         <f>T46</f>
-        <v>67.536211870302736</v>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="K2:T2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="K3:T3"/>
     <mergeCell ref="A14:J14"/>
     <mergeCell ref="K14:T14"/>
     <mergeCell ref="K25:T25"/>
     <mergeCell ref="A25:J25"/>
     <mergeCell ref="A36:J36"/>
     <mergeCell ref="K36:T36"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="K2:T2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="K3:T3"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:A13">
     <cfRule type="colorScale" priority="40">
@@ -17547,8 +17547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6240820C-A703-4D82-AEA4-6398523FBADE}">
   <dimension ref="H1:S42"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" workbookViewId="0">
-      <selection activeCell="AD27" sqref="AD27"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Scores from states matches
</commit_message>
<xml_diff>
--- a/Red Team Data.xlsx
+++ b/Red Team Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\FTCStats\FTCStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E979BB1-5CD0-4ABE-8FC7-668CB454EC5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B30641-E85D-4BBC-A53F-7C71131DCF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{943F8BFE-BB93-4FCB-9D8B-2434F109755A}"/>
   </bookViews>
   <sheets>
     <sheet name="Match Data" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="48">
   <si>
     <t>Cyrus</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>Alan</t>
-  </si>
-  <si>
-    <t>t23</t>
   </si>
 </sst>
 </file>
@@ -1107,13 +1104,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-12.348010303524767</c:v>
+                  <c:v>-10.157226504346077</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.641866177795908</c:v>
+                  <c:v>30.493490997233081</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-9.5064113339223937</c:v>
+                  <c:v>-19.778393870594858</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1498,85 +1495,85 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>-6.7851149468987053</c:v>
+                  <c:v>-6.9826965569050987</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.2108356456295688</c:v>
+                  <c:v>9.2775904437265577</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.6484753590577546</c:v>
+                  <c:v>-10.831163503404618</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8.6755596249879119</c:v>
+                  <c:v>-9.2260667370975291</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.3203909675403533</c:v>
+                  <c:v>7.0342202635341256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-7.5389200371469638</c:v>
+                  <c:v>-13.074533683597044</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-14.773954785520552</c:v>
+                  <c:v>-15.085470332880661</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2219958070077284</c:v>
+                  <c:v>1.1748166677510006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-13.637315197679603</c:v>
+                  <c:v>-18.933937279380167</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.2000110313711669</c:v>
+                  <c:v>0.85868056005839488</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.795939561157107</c:v>
+                  <c:v>17.118967560690056</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-6.3371443530212623E-2</c:v>
+                  <c:v>-2.9897863864411223</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-3.0904557094603726</c:v>
+                  <c:v>-1.3846896201340324</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12.905494883067897</c:v>
+                  <c:v>14.875597380497622</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1.9538161216194201</c:v>
+                  <c:v>-5.2331565666335509</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-9.1888508699930078</c:v>
+                  <c:v>-7.2440932159171663</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.8070997225352698</c:v>
+                  <c:v>9.0161937847144937</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-8.0522112821520615</c:v>
+                  <c:v>-11.092560162416676</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-3.0320308034372618</c:v>
+                  <c:v>-4.0204146574760529</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12.963919789091015</c:v>
+                  <c:v>12.239872343155611</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-1.8953912155963137</c:v>
+                  <c:v>-7.868881603975562</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-4.9224754815264671</c:v>
+                  <c:v>-6.2637848376684717</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.073475111001802</c:v>
+                  <c:v>9.9965021629631785</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-3.7858358936855177</c:v>
+                  <c:v>-10.112251784167992</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-11.02087064205911</c:v>
+                  <c:v>-12.123188433451608</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.9750799504691692</c:v>
+                  <c:v>4.1370985671800575</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-9.8842310542181586</c:v>
+                  <c:v>-15.971655379951114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1966,85 +1963,85 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>-29.36107703225629</c:v>
+                  <c:v>-37.245302929037749</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-14.084834484234207</c:v>
+                  <c:v>-21.46263233107954</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-27.835293021733488</c:v>
+                  <c:v>-37.771610191960512</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>72.548621829143627</c:v>
+                  <c:v>82.962089792477116</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-18.909332536343285</c:v>
+                  <c:v>-26.038442851625394</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-15.957272500652767</c:v>
+                  <c:v>-22.266162823060348</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44.388086307786004</c:v>
+                  <c:v>44.90085788241619</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>72.450260355057594</c:v>
+                  <c:v>76.815697229394232</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30.482168794003105</c:v>
+                  <c:v>34.087806039109523</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-31.276490513430083</c:v>
+                  <c:v>29.213979496051596</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.0222358955907325</c:v>
+                  <c:v>-0.50320210012384692</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>66.834382603178824</c:v>
+                  <c:v>1.9656300570695049</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>79.964241060212345</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.202981131810297</c:v>
+                  <c:v>26.029053396707386</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-51.68363952503455</c:v>
+                  <c:v>-63.227789918018182</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-5.3472030886467099</c:v>
+                  <c:v>-10.357996932071655</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>105.13615859362464</c:v>
+                  <c:v>-8.8419620243753378</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>108.95931681550806</c:v>
+                  <c:v>122.05407406125485</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-23.87743571736819</c:v>
+                  <c:v>-31.003342908411931</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>16.98862533234675</c:v>
+                  <c:v>10.574631553192672</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>46.667293967436805</c:v>
+                  <c:v>42.905511180354353</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>14.31969315047489</c:v>
+                  <c:v>17.954832553354933</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>50.981147973497762</c:v>
+                  <c:v>55.099880467133474</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-23.367744770491132</c:v>
+                  <c:v>-40.316252349407925</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2424,31 +2421,31 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-11.080896307068945</c:v>
+                  <c:v>-16.750069086071726</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108.83425180295959</c:v>
+                  <c:v>80.085604986587541</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.868831158395455</c:v>
+                  <c:v>23.249447117671849</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-24.933494062454223</c:v>
+                  <c:v>-12.576611349104505</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.3636689641393982</c:v>
+                  <c:v>6.4236807473126376</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>56.750838285307822</c:v>
+                  <c:v>8.7889435776169726</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.9373800278804101</c:v>
+                  <c:v>23.642901340758936</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.172881486221605</c:v>
+                  <c:v>40.655119359891494</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-28.409011018688524</c:v>
+                  <c:v>-40.531303528157075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2812,13 +2809,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.2006173886217288</c:v>
+                  <c:v>5.9343572825165669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47450569339870902</c:v>
+                  <c:v>0.32593183203549475</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-14.771482207932882</c:v>
+                  <c:v>-14.322577157422323</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3178,13 +3175,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-19.630788904687449</c:v>
+                  <c:v>-26.467744340866496</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.2947306729502586</c:v>
+                  <c:v>12.739141243950977</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.86536818738022214</c:v>
+                  <c:v>-11.656334843721224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3566,31 +3563,31 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-3.5736964574515202</c:v>
+                  <c:v>-2.1114346109147535</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.421241783208824</c:v>
+                  <c:v>18.213924139874827</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.152896972650332</c:v>
+                  <c:v>-6.9220182940391481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.9367523050630293</c:v>
+                  <c:v>-4.9156473361552866</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.058185935597308</c:v>
+                  <c:v>15.409711414634284</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.5159528202618437</c:v>
+                  <c:v>-9.7262310192796768</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-13.559746255728831</c:v>
+                  <c:v>-12.239901830884202</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.4351919849315209</c:v>
+                  <c:v>8.0854569199053756</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-12.138946770927642</c:v>
+                  <c:v>-17.050485514008589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9873,7 +9870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E71918B-9D42-46BC-B578-CF08432FB725}">
   <dimension ref="A1:Y125"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" zoomScale="120" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="120" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L122" sqref="L122"/>
     </sheetView>
   </sheetViews>
@@ -15468,31 +15465,31 @@
         <v>5</v>
       </c>
       <c r="F119">
-        <v>-1</v>
+        <v>86</v>
       </c>
       <c r="G119">
-        <v>-1</v>
+        <v>50</v>
       </c>
       <c r="H119">
-        <v>-1</v>
+        <v>16</v>
       </c>
       <c r="I119">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="J119">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K119">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L119">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M119">
-        <v>-1</v>
+        <v>20</v>
       </c>
       <c r="N119">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="O119" s="49">
         <v>1</v>
@@ -15515,31 +15512,31 @@
         <v>5</v>
       </c>
       <c r="F120">
-        <v>-1</v>
+        <v>100</v>
       </c>
       <c r="G120">
-        <v>-1</v>
+        <v>50</v>
       </c>
       <c r="H120">
-        <v>-1</v>
+        <v>30</v>
       </c>
       <c r="I120">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="J120">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="K120">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L120">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="M120">
-        <v>-1</v>
+        <v>20</v>
       </c>
       <c r="N120">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="O120" s="49">
         <v>1</v>
@@ -15562,31 +15559,31 @@
         <v>47</v>
       </c>
       <c r="F121">
-        <v>-1</v>
+        <v>116</v>
       </c>
       <c r="G121">
-        <v>-1</v>
+        <v>50</v>
       </c>
       <c r="H121">
-        <v>-1</v>
+        <v>46</v>
       </c>
       <c r="I121">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="J121">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K121">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="L121">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="M121">
-        <v>-1</v>
+        <v>20</v>
       </c>
       <c r="N121">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="O121" s="49">
         <v>1</v>
@@ -15609,31 +15606,31 @@
         <v>1</v>
       </c>
       <c r="F122">
-        <v>-1</v>
+        <v>90</v>
       </c>
       <c r="G122">
-        <v>-1</v>
+        <v>50</v>
       </c>
       <c r="H122">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I122">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="J122">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K122">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L122">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M122">
-        <v>-1</v>
+        <v>40</v>
       </c>
       <c r="N122">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="O122" s="49">
         <v>1</v>
@@ -15656,31 +15653,31 @@
         <v>5</v>
       </c>
       <c r="F123">
-        <v>-1</v>
+        <v>101</v>
       </c>
       <c r="G123">
-        <v>-1</v>
+        <v>28</v>
       </c>
       <c r="H123">
-        <v>-1</v>
+        <v>33</v>
       </c>
       <c r="I123">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="J123">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="K123">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="L123">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M123">
-        <v>-1</v>
+        <v>40</v>
       </c>
       <c r="N123">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="O123" s="49">
         <v>1</v>
@@ -15703,31 +15700,31 @@
         <v>1</v>
       </c>
       <c r="F124">
-        <v>-1</v>
+        <v>56</v>
       </c>
       <c r="G124">
-        <v>-1</v>
+        <v>30</v>
       </c>
       <c r="H124">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="I124">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="J124">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="K124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M124">
-        <v>-1</v>
+        <v>20</v>
       </c>
       <c r="N124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="O124" s="49">
         <v>1</v>
@@ -15847,60 +15844,60 @@
     </row>
     <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="48">
-        <v>75.818181818181813</v>
+        <v>77.7</v>
       </c>
       <c r="B3" s="48">
-        <v>34</v>
+        <v>35.102040816326529</v>
       </c>
       <c r="C3" s="48">
-        <v>17.554140127388536</v>
+        <v>18.121546961325969</v>
       </c>
       <c r="D3" s="48">
-        <v>3.0266666666666668</v>
+        <v>3</v>
       </c>
       <c r="E3" s="48">
-        <v>5.0952380952380949</v>
+        <v>4.9181286549707606</v>
       </c>
       <c r="F3" s="48">
-        <v>0.4370860927152318</v>
+        <v>0.49142857142857144</v>
       </c>
       <c r="G3" s="48">
-        <v>0.22580645161290322</v>
+        <v>0.24022346368715083</v>
       </c>
       <c r="H3" s="48">
-        <v>23.969696969696969</v>
+        <v>24.312169312169313</v>
       </c>
       <c r="I3" s="48">
-        <v>-0.91891891891891897</v>
+        <v>-0.8133971291866029</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="49">
-        <v>49.494577725536743</v>
+        <v>44.124576578101255</v>
       </c>
       <c r="B4" s="49">
-        <v>23.708527515054246</v>
+        <v>21.676619661331717</v>
       </c>
       <c r="C4" s="49">
-        <v>13.481364075608345</v>
+        <v>13.52290210424025</v>
       </c>
       <c r="D4" s="49">
-        <v>2.3682134888572897</v>
+        <v>1.9307841413447502</v>
       </c>
       <c r="E4" s="49">
-        <v>3.7831496401748903</v>
+        <v>3.1558452875974901</v>
       </c>
       <c r="F4" s="49">
-        <v>0.71680260453738576</v>
+        <v>0.64566729663643463</v>
       </c>
       <c r="G4" s="49">
-        <v>0.50980269406935452</v>
+        <v>0.34409285760302832</v>
       </c>
       <c r="H4" s="49">
-        <v>19.072220428127476</v>
+        <v>17.581059177953392</v>
       </c>
       <c r="I4" s="49">
-        <v>2.1511109378774251</v>
+        <v>2.0541666250733197</v>
       </c>
       <c r="J4" s="49"/>
     </row>
@@ -15917,7 +15914,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView zoomScale="167" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15970,34 +15967,34 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
-        <v>73.278481012658233</v>
+        <v>74.448275862068968</v>
       </c>
       <c r="B3" s="6">
-        <v>29.657894736842106</v>
+        <v>30.642857142857142</v>
       </c>
       <c r="C3" s="6">
-        <v>18.887323943661972</v>
+        <v>19.60759493670886</v>
       </c>
       <c r="D3" s="6">
-        <v>3.2714285714285714</v>
+        <v>3.2435897435897436</v>
       </c>
       <c r="E3" s="6">
-        <v>5.535211267605634</v>
+        <v>5.3797468354430382</v>
       </c>
       <c r="F3" s="6">
-        <v>0.53521126760563376</v>
+        <v>0.58227848101265822</v>
       </c>
       <c r="G3" s="6">
-        <v>0.21333333333333335</v>
+        <v>0.24096385542168675</v>
       </c>
       <c r="H3" s="6">
-        <v>23.421052631578949</v>
+        <v>23.095238095238095</v>
       </c>
       <c r="I3" s="33">
-        <v>-0.95238095238095233</v>
+        <v>-0.86956521739130432</v>
       </c>
       <c r="J3" s="36">
-        <v>5.2006173886217288</v>
+        <v>5.9343572825165669</v>
       </c>
       <c r="K3" t="s">
         <v>8</v>
@@ -16005,34 +16002,34 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
-        <v>82.41935483870968</v>
+        <v>83.685714285714283</v>
       </c>
       <c r="B4" s="4">
-        <v>40.225806451612904</v>
+        <v>40.085714285714289</v>
       </c>
       <c r="C4" s="4">
-        <v>18.896551724137932</v>
+        <v>19.575757575757574</v>
       </c>
       <c r="D4" s="4">
-        <v>2.7083333333333335</v>
+        <v>2.75</v>
       </c>
       <c r="E4" s="4">
-        <v>4.916666666666667</v>
+        <v>5</v>
       </c>
       <c r="F4" s="4">
-        <v>0.33333333333333331</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="G4" s="4">
-        <v>0.27083333333333331</v>
+        <v>0.23214285714285715</v>
       </c>
       <c r="H4" s="4">
-        <v>24.035087719298247</v>
+        <v>24.76923076923077</v>
       </c>
       <c r="I4" s="34">
-        <v>-0.967741935483871</v>
+        <v>-0.8571428571428571</v>
       </c>
       <c r="J4" s="37">
-        <v>0.47450569339870902</v>
+        <v>0.32593183203549475</v>
       </c>
       <c r="K4" t="s">
         <v>4</v>
@@ -16040,34 +16037,34 @@
     </row>
     <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
-        <v>69.857142857142861</v>
+        <v>74.534883720930239</v>
       </c>
       <c r="B5" s="7">
-        <v>32.352941176470587</v>
+        <v>35.714285714285715</v>
       </c>
       <c r="C5" s="7">
-        <v>11.392857142857142</v>
+        <v>12.194444444444445</v>
       </c>
       <c r="D5" s="7">
-        <v>2.96875</v>
+        <v>2.875</v>
       </c>
       <c r="E5" s="7">
-        <v>4.2857142857142856</v>
+        <v>3.7777777777777777</v>
       </c>
       <c r="F5" s="7">
-        <v>0.375</v>
+        <v>0.4</v>
       </c>
       <c r="G5" s="7">
-        <v>0.1875</v>
+        <v>0.25</v>
       </c>
       <c r="H5" s="7">
-        <v>25.15625</v>
+        <v>26.125</v>
       </c>
       <c r="I5" s="32">
-        <v>-0.76923076923076927</v>
+        <v>-0.63829787234042556</v>
       </c>
       <c r="J5" s="38">
-        <v>-14.771482207932882</v>
+        <v>-14.322577157422323</v>
       </c>
       <c r="K5" t="s">
         <v>3</v>
@@ -16075,34 +16072,34 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
-        <v>67.27956989247312</v>
+        <v>69.910891089108915</v>
       </c>
       <c r="B6" s="6">
-        <v>28.351063829787233</v>
+        <v>29.186274509803923</v>
       </c>
       <c r="C6" s="6">
-        <v>15.592592592592593</v>
+        <v>17.022471910112358</v>
       </c>
       <c r="D6" s="6">
-        <v>3.0384615384615383</v>
+        <v>3.0348837209302326</v>
       </c>
       <c r="E6" s="6">
-        <v>5.1518987341772151</v>
+        <v>5.0919540229885056</v>
       </c>
       <c r="F6" s="6">
-        <v>0.37179487179487181</v>
+        <v>0.47674418604651164</v>
       </c>
       <c r="G6" s="6">
-        <v>0.12195121951219512</v>
+        <v>0.15555555555555556</v>
       </c>
       <c r="H6" s="6">
-        <v>23.928571428571427</v>
+        <v>24.456521739130434</v>
       </c>
       <c r="I6" s="33">
-        <v>-1.3402061855670102</v>
+        <v>-1.2380952380952381</v>
       </c>
       <c r="J6" s="39">
-        <v>-12.348010303524767</v>
+        <v>-10.157226504346077</v>
       </c>
       <c r="K6" t="s">
         <v>6</v>
@@ -16110,34 +16107,34 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
-        <v>90.888888888888886</v>
+        <v>90.258064516129039</v>
       </c>
       <c r="B7" s="4">
-        <v>45.76</v>
+        <v>44.96551724137931</v>
       </c>
       <c r="C7" s="4">
-        <v>23.775510204081634</v>
+        <v>24.087719298245613</v>
       </c>
       <c r="D7" s="4">
-        <v>3.1162790697674421</v>
+        <v>3.0980392156862746</v>
       </c>
       <c r="E7" s="4">
-        <v>5.4634146341463419</v>
+        <v>5.2244897959183669</v>
       </c>
       <c r="F7" s="4">
-        <v>0.65909090909090906</v>
+        <v>0.71153846153846156</v>
       </c>
       <c r="G7" s="4">
-        <v>0.45454545454545453</v>
+        <v>0.46153846153846156</v>
       </c>
       <c r="H7" s="4">
-        <v>21.346153846153847</v>
+        <v>21.166666666666668</v>
       </c>
       <c r="I7" s="34">
-        <v>-0.70175438596491224</v>
+        <v>-0.61538461538461542</v>
       </c>
       <c r="J7" s="37">
-        <v>27.641866177795908</v>
+        <v>30.493490997233081</v>
       </c>
       <c r="K7" t="s">
         <v>2</v>
@@ -16145,34 +16142,34 @@
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
-        <v>75.137931034482762</v>
+        <v>77.918918918918919</v>
       </c>
       <c r="B8" s="7">
-        <v>31.964285714285715</v>
+        <v>35.972222222222221</v>
       </c>
       <c r="C8" s="7">
-        <v>12.148148148148149</v>
+        <v>11.2</v>
       </c>
       <c r="D8" s="7">
-        <v>2.8620689655172415</v>
+        <v>2.7837837837837838</v>
       </c>
       <c r="E8" s="7">
-        <v>4.3703703703703702</v>
+        <v>4.0571428571428569</v>
       </c>
       <c r="F8" s="7">
-        <v>0.27586206896551724</v>
+        <v>0.21621621621621623</v>
       </c>
       <c r="G8" s="7">
-        <v>0.17241379310344829</v>
+        <v>0.13513513513513514</v>
       </c>
       <c r="H8" s="7">
-        <v>28.793103448275861</v>
+        <v>29.054054054054053</v>
       </c>
       <c r="I8" s="32">
         <v>0</v>
       </c>
       <c r="J8" s="38">
-        <v>-9.5064113339223937</v>
+        <v>-19.778393870594858</v>
       </c>
       <c r="K8" t="s">
         <v>0</v>
@@ -16207,7 +16204,7 @@
         <v>-1.6981132075471699</v>
       </c>
       <c r="J9" s="39">
-        <v>-19.630788904687449</v>
+        <v>-26.467744340866496</v>
       </c>
       <c r="K9" t="s">
         <v>7</v>
@@ -16215,34 +16212,34 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
-        <v>82.648148148148152</v>
+        <v>85.015151515151516</v>
       </c>
       <c r="B10" s="4">
-        <v>41.709090909090911</v>
+        <v>41.880597014925371</v>
       </c>
       <c r="C10" s="4">
-        <v>18.615384615384617</v>
+        <v>20.0625</v>
       </c>
       <c r="D10" s="4">
-        <v>2.82</v>
+        <v>2.8548387096774195</v>
       </c>
       <c r="E10" s="4">
-        <v>5.0434782608695654</v>
+        <v>5.0344827586206895</v>
       </c>
       <c r="F10" s="4">
-        <v>0.52</v>
+        <v>0.61290322580645162</v>
       </c>
       <c r="G10" s="4">
-        <v>0.32</v>
+        <v>0.32258064516129031</v>
       </c>
       <c r="H10" s="4">
-        <v>22.410714285714285</v>
+        <v>23.161764705882351</v>
       </c>
       <c r="I10" s="34">
-        <v>-0.68965517241379315</v>
+        <v>-0.5714285714285714</v>
       </c>
       <c r="J10" s="37">
-        <v>8.2947306729502586</v>
+        <v>12.739141243950977</v>
       </c>
       <c r="K10" t="s">
         <v>5</v>
@@ -16250,34 +16247,34 @@
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
-        <v>71.738461538461536</v>
+        <v>71.876712328767127</v>
       </c>
       <c r="B11" s="5">
-        <v>31.338983050847457</v>
+        <v>32.373134328358212</v>
       </c>
       <c r="C11" s="5">
-        <v>16.075471698113208</v>
+        <v>14.360655737704919</v>
       </c>
       <c r="D11" s="5">
-        <v>3.1960784313725492</v>
+        <v>3.0338983050847457</v>
       </c>
       <c r="E11" s="5">
-        <v>4.8461538461538458</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="F11" s="5">
-        <v>0.44230769230769229</v>
+        <v>0.38333333333333336</v>
       </c>
       <c r="G11" s="5">
-        <v>0.21428571428571427</v>
+        <v>0.1875</v>
       </c>
       <c r="H11" s="5">
-        <v>22.982456140350877</v>
+        <v>23.846153846153847</v>
       </c>
       <c r="I11" s="35">
-        <v>-0.5714285714285714</v>
+        <v>-0.51282051282051277</v>
       </c>
       <c r="J11" s="40">
-        <v>-0.86536818738022214</v>
+        <v>-11.656334843721224</v>
       </c>
       <c r="K11" t="s">
         <v>1</v>
@@ -16421,8 +16418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AJ53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="86" workbookViewId="0">
-      <selection activeCell="T48" sqref="T48"/>
+    <sheetView topLeftCell="A25" zoomScale="86" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16583,34 +16580,34 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
-        <v>70.279025452565676</v>
+        <v>72.179583475588942</v>
       </c>
       <c r="B5" s="12">
-        <v>29.004479283314669</v>
+        <v>29.914565826330531</v>
       </c>
       <c r="C5" s="12">
-        <v>17.239958268127282</v>
+        <v>18.315033423410611</v>
       </c>
       <c r="D5" s="12">
-        <v>3.1549450549450548</v>
+        <v>3.1392367322599881</v>
       </c>
       <c r="E5" s="12">
-        <v>5.3435550008914241</v>
+        <v>5.2358504292157715</v>
       </c>
       <c r="F5" s="12">
-        <v>0.45350306970025278</v>
+        <v>0.5295113335295849</v>
       </c>
       <c r="G5" s="12">
-        <v>0.16764227642276425</v>
+        <v>0.19825970548862115</v>
       </c>
       <c r="H5" s="12">
-        <v>23.674812030075188</v>
+        <v>23.775879917184263</v>
       </c>
       <c r="I5" s="12">
-        <v>-1.1462935689739813</v>
+        <v>-1.0538302277432712</v>
       </c>
       <c r="J5" s="26">
-        <v>-3.5736964574515202</v>
+        <v>-2.1114346109147535</v>
       </c>
       <c r="K5" s="22">
         <v>65.951612903225808</v>
@@ -16640,7 +16637,7 @@
         <v>-1.25</v>
       </c>
       <c r="T5" s="17">
-        <v>-11.080896307068945</v>
+        <v>-16.750069086071726</v>
       </c>
       <c r="U5" t="s">
         <v>33</v>
@@ -16648,64 +16645,64 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
-        <v>82.083684950773559</v>
+        <v>82.353170189099004</v>
       </c>
       <c r="B6" s="13">
-        <v>37.70894736842105</v>
+        <v>37.804187192118228</v>
       </c>
       <c r="C6" s="13">
-        <v>21.331417073871805</v>
+        <v>21.847657117477237</v>
       </c>
       <c r="D6" s="13">
-        <v>3.1938538205980067</v>
+        <v>3.1708144796380093</v>
       </c>
       <c r="E6" s="13">
-        <v>5.4993129508759875</v>
+        <v>5.302118315680703</v>
       </c>
       <c r="F6" s="13">
-        <v>0.59715108834827135</v>
+        <v>0.64690847127555995</v>
       </c>
       <c r="G6" s="13">
-        <v>0.33393939393939392</v>
+        <v>0.35125115848007415</v>
       </c>
       <c r="H6" s="13">
-        <v>22.383603238866399</v>
+        <v>22.13095238095238</v>
       </c>
       <c r="I6" s="13">
-        <v>-0.82706766917293228</v>
+        <v>-0.74247491638795982</v>
       </c>
       <c r="J6" s="27">
-        <v>16.421241783208824</v>
+        <v>18.213924139874827</v>
       </c>
       <c r="K6" s="23">
-        <v>114</v>
+        <v>101.55555555555556</v>
       </c>
       <c r="L6" s="13">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="M6" s="13">
-        <v>43.571428571428569</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="N6" s="13">
-        <v>3.8571428571428572</v>
+        <v>3.4</v>
       </c>
       <c r="O6" s="13">
-        <v>6.7142857142857144</v>
+        <v>5.2666666666666666</v>
       </c>
       <c r="P6" s="13">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="Q6" s="13">
-        <v>0.875</v>
+        <v>0.6875</v>
       </c>
       <c r="R6" s="13">
-        <v>25</v>
+        <v>22.5</v>
       </c>
       <c r="S6" s="13">
         <v>0</v>
       </c>
       <c r="T6" s="18">
-        <v>108.83425180295959</v>
+        <v>80.085604986587541</v>
       </c>
       <c r="U6" t="s">
         <v>34</v>
@@ -16713,34 +16710,34 @@
     </row>
     <row r="7" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
-        <v>74.208206023570497</v>
+        <v>76.183597390493944</v>
       </c>
       <c r="B7" s="14">
-        <v>30.811090225563909</v>
+        <v>33.307539682539684</v>
       </c>
       <c r="C7" s="14">
-        <v>15.51773604590506</v>
+        <v>15.40379746835443</v>
       </c>
       <c r="D7" s="14">
-        <v>3.0667487684729062</v>
+        <v>3.0136867636867635</v>
       </c>
       <c r="E7" s="14">
-        <v>4.9527908189880021</v>
+        <v>4.7184448462929476</v>
       </c>
       <c r="F7" s="14">
-        <v>0.4055366682855755</v>
+        <v>0.39924734861443723</v>
       </c>
       <c r="G7" s="14">
-        <v>0.19287356321839083</v>
+        <v>0.18804949527841094</v>
       </c>
       <c r="H7" s="14">
-        <v>26.107078039927405</v>
+        <v>26.074646074646076</v>
       </c>
       <c r="I7" s="14">
-        <v>-0.47619047619047616</v>
+        <v>-0.43478260869565216</v>
       </c>
       <c r="J7" s="28">
-        <v>-2.152896972650332</v>
+        <v>-6.9220182940391481</v>
       </c>
       <c r="K7" s="30">
         <v>80</v>
@@ -16770,7 +16767,7 @@
         <v>0</v>
       </c>
       <c r="T7" s="31">
-        <v>22.868831158395455</v>
+        <v>23.249447117671849</v>
       </c>
       <c r="U7" t="s">
         <v>35</v>
@@ -16778,64 +16775,64 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
-        <v>74.849462365591393</v>
+        <v>76.798302687411592</v>
       </c>
       <c r="B8" s="13">
-        <v>34.288435140700066</v>
+        <v>34.635994397759106</v>
       </c>
       <c r="C8" s="13">
-        <v>17.244572158365262</v>
+        <v>18.299114742934968</v>
       </c>
       <c r="D8" s="13">
-        <v>2.8733974358974361</v>
+        <v>2.8924418604651163</v>
       </c>
       <c r="E8" s="13">
-        <v>5.034282700421941</v>
+        <v>5.0459770114942533</v>
       </c>
       <c r="F8" s="13">
-        <v>0.35256410256410253</v>
+        <v>0.45265780730897009</v>
       </c>
       <c r="G8" s="13">
-        <v>0.19639227642276422</v>
+        <v>0.19384920634920635</v>
       </c>
       <c r="H8" s="13">
-        <v>23.981829573934839</v>
+        <v>24.612876254180602</v>
       </c>
       <c r="I8" s="13">
-        <v>-1.1539740605254405</v>
+        <v>-1.0476190476190477</v>
       </c>
       <c r="J8" s="27">
-        <v>-5.9367523050630293</v>
+        <v>-4.9156473361552866</v>
       </c>
       <c r="K8" s="23">
-        <v>71.15789473684211</v>
+        <v>76.347826086956516</v>
       </c>
       <c r="L8" s="13">
-        <v>29.3</v>
+        <v>29.083333333333332</v>
       </c>
       <c r="M8" s="13">
-        <v>13.3125</v>
+        <v>17.25</v>
       </c>
       <c r="N8" s="13">
-        <v>2.2142857142857144</v>
+        <v>2.3888888888888888</v>
       </c>
       <c r="O8" s="13">
-        <v>4</v>
+        <v>4.2222222222222223</v>
       </c>
       <c r="P8" s="13">
-        <v>0.14285714285714285</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="Q8" s="13">
-        <v>7.1428571428571425E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="R8" s="13">
-        <v>31.333333333333332</v>
+        <v>33.157894736842103</v>
       </c>
       <c r="S8" s="13">
-        <v>-1.0526315789473684</v>
+        <v>-0.86956521739130432</v>
       </c>
       <c r="T8" s="18">
-        <v>-24.933494062454223</v>
+        <v>-12.576611349104505</v>
       </c>
       <c r="U8" t="s">
         <v>36</v>
@@ -16843,34 +16840,34 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
-        <v>86.654121863799276</v>
+        <v>86.971889400921668</v>
       </c>
       <c r="B9" s="13">
-        <v>42.992903225806451</v>
+        <v>42.525615763546796</v>
       </c>
       <c r="C9" s="13">
-        <v>21.336030964109781</v>
+        <v>21.831738437001594</v>
       </c>
       <c r="D9" s="13">
-        <v>2.912306201550388</v>
+        <v>2.9240196078431371</v>
       </c>
       <c r="E9" s="13">
-        <v>5.1900406504065044</v>
+        <v>5.112244897959183</v>
       </c>
       <c r="F9" s="13">
-        <v>0.49621212121212122</v>
+        <v>0.57005494505494503</v>
       </c>
       <c r="G9" s="13">
-        <v>0.36268939393939392</v>
+        <v>0.34684065934065933</v>
       </c>
       <c r="H9" s="13">
-        <v>22.690620782726047</v>
+        <v>22.967948717948719</v>
       </c>
       <c r="I9" s="13">
-        <v>-0.83474816072439162</v>
+        <v>-0.73626373626373631</v>
       </c>
       <c r="J9" s="27">
-        <v>14.058185935597308</v>
+        <v>15.409711414634284</v>
       </c>
       <c r="K9" s="23">
         <v>85.536585365853654</v>
@@ -16900,7 +16897,7 @@
         <v>-0.97560975609756095</v>
       </c>
       <c r="T9" s="18">
-        <v>8.3636689641393982</v>
+        <v>6.4236807473126376</v>
       </c>
       <c r="U9" t="s">
         <v>37</v>
@@ -16908,64 +16905,64 @@
     </row>
     <row r="10" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
-        <v>78.778642936596214</v>
+        <v>80.802316602316608</v>
       </c>
       <c r="B10" s="13">
-        <v>36.09504608294931</v>
+        <v>38.028968253968259</v>
       </c>
       <c r="C10" s="13">
-        <v>15.522349936143041</v>
+        <v>15.387878787878787</v>
       </c>
       <c r="D10" s="13">
-        <v>2.7852011494252875</v>
+        <v>2.7668918918918921</v>
       </c>
       <c r="E10" s="13">
-        <v>4.643518518518519</v>
+        <v>4.5285714285714285</v>
       </c>
       <c r="F10" s="13">
-        <v>0.3045977011494253</v>
+        <v>0.32239382239382242</v>
       </c>
       <c r="G10" s="13">
-        <v>0.2216235632183908</v>
+        <v>0.18363899613899615</v>
       </c>
       <c r="H10" s="13">
-        <v>26.414095583787052</v>
+        <v>26.911642411642411</v>
       </c>
       <c r="I10" s="13">
-        <v>-0.4838709677419355</v>
+        <v>-0.42857142857142855</v>
       </c>
       <c r="J10" s="27">
-        <v>-4.5159528202618437</v>
+        <v>-9.7262310192796768</v>
       </c>
       <c r="K10" s="23">
-        <v>125.5</v>
+        <v>99.166666666666671</v>
       </c>
       <c r="L10" s="13">
         <v>50</v>
       </c>
       <c r="M10" s="13">
-        <v>30.5</v>
+        <v>20.833333333333332</v>
       </c>
       <c r="N10" s="13">
-        <v>3.5</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="O10" s="13">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="P10" s="13">
-        <v>0.5</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="Q10" s="13">
-        <v>0.5</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="R10" s="13">
-        <v>45</v>
+        <v>28.333333333333332</v>
       </c>
       <c r="S10" s="13">
         <v>0</v>
       </c>
       <c r="T10" s="18">
-        <v>56.750838285307822</v>
+        <v>8.7889435776169726</v>
       </c>
       <c r="U10" t="s">
         <v>38</v>
@@ -16973,64 +16970,64 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
-        <v>68.568356374807991</v>
+        <v>72.222887405019577</v>
       </c>
       <c r="B11" s="12">
-        <v>30.352002503128908</v>
+        <v>32.450280112044823</v>
       </c>
       <c r="C11" s="12">
-        <v>13.492724867724867</v>
+        <v>14.608458177278401</v>
       </c>
       <c r="D11" s="12">
-        <v>3.0036057692307692</v>
+        <v>2.9549418604651163</v>
       </c>
       <c r="E11" s="12">
-        <v>4.7188065099457503</v>
+        <v>4.4348659003831417</v>
       </c>
       <c r="F11" s="12">
-        <v>0.3733974358974359</v>
+        <v>0.43837209302325586</v>
       </c>
       <c r="G11" s="12">
-        <v>0.15472560975609756</v>
+        <v>0.20277777777777778</v>
       </c>
       <c r="H11" s="12">
-        <v>24.542410714285715</v>
+        <v>25.290760869565219</v>
       </c>
       <c r="I11" s="12">
-        <v>-1.0547184773988898</v>
+        <v>-0.93819655521783185</v>
       </c>
       <c r="J11" s="26">
-        <v>-13.559746255728831</v>
+        <v>-12.239901830884202</v>
       </c>
       <c r="K11" s="22">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="L11" s="12">
-        <v>34</v>
+        <v>37.764705882352942</v>
       </c>
       <c r="M11" s="12">
-        <v>18</v>
+        <v>22.363636363636363</v>
       </c>
       <c r="N11" s="12">
-        <v>3.4444444444444446</v>
+        <v>3.3076923076923075</v>
       </c>
       <c r="O11" s="12">
-        <v>6.1428571428571432</v>
+        <v>5.3636363636363633</v>
       </c>
       <c r="P11" s="12">
-        <v>0.66666666666666663</v>
+        <v>0.76923076923076927</v>
       </c>
       <c r="Q11" s="12">
-        <v>0.33333333333333331</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="R11" s="12">
-        <v>21.111111111111111</v>
+        <v>20.76923076923077</v>
       </c>
       <c r="S11" s="12">
-        <v>-2.1428571428571428</v>
+        <v>-1.6666666666666667</v>
       </c>
       <c r="T11" s="17">
-        <v>2.9373800278804101</v>
+        <v>23.642901340758936</v>
       </c>
       <c r="U11" t="s">
         <v>39</v>
@@ -17038,34 +17035,34 @@
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
-        <v>80.373015873015873</v>
+        <v>82.396474118529639</v>
       </c>
       <c r="B12" s="13">
-        <v>39.056470588235292</v>
+        <v>40.339901477832512</v>
       </c>
       <c r="C12" s="13">
-        <v>17.58418367346939</v>
+        <v>18.14108187134503</v>
       </c>
       <c r="D12" s="13">
-        <v>3.042514534883721</v>
+        <v>2.9865196078431371</v>
       </c>
       <c r="E12" s="13">
-        <v>4.8745644599303137</v>
+        <v>4.5011337868480723</v>
       </c>
       <c r="F12" s="13">
-        <v>0.51704545454545459</v>
+        <v>0.55576923076923079</v>
       </c>
       <c r="G12" s="13">
-        <v>0.32102272727272729</v>
+        <v>0.35576923076923078</v>
       </c>
       <c r="H12" s="13">
-        <v>23.251201923076923</v>
+        <v>23.645833333333336</v>
       </c>
       <c r="I12" s="13">
-        <v>-0.7354925775978407</v>
+        <v>-0.62684124386252049</v>
       </c>
       <c r="J12" s="27">
-        <v>6.4351919849315209</v>
+        <v>8.0854569199053756</v>
       </c>
       <c r="K12" s="23">
         <v>87</v>
@@ -17095,7 +17092,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="18">
-        <v>37.172881486221605</v>
+        <v>40.655119359891494</v>
       </c>
       <c r="U12" t="s">
         <v>40</v>
@@ -17103,64 +17100,64 @@
     </row>
     <row r="13" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19">
-        <v>72.497536945812811</v>
+        <v>76.226901319924579</v>
       </c>
       <c r="B13" s="25">
-        <v>32.158613445378151</v>
+        <v>35.843253968253968</v>
       </c>
       <c r="C13" s="25">
-        <v>11.770502645502646</v>
+        <v>11.697222222222223</v>
       </c>
       <c r="D13" s="25">
-        <v>2.915409482758621</v>
+        <v>2.8293918918918921</v>
       </c>
       <c r="E13" s="25">
-        <v>4.3280423280423275</v>
+        <v>3.9174603174603173</v>
       </c>
       <c r="F13" s="25">
-        <v>0.32543103448275862</v>
+        <v>0.30810810810810813</v>
       </c>
       <c r="G13" s="25">
-        <v>0.17995689655172414</v>
+        <v>0.19256756756756757</v>
       </c>
       <c r="H13" s="25">
-        <v>26.974676724137929</v>
+        <v>27.589527027027025</v>
       </c>
       <c r="I13" s="25">
-        <v>-0.38461538461538464</v>
+        <v>-0.31914893617021278</v>
       </c>
       <c r="J13" s="29">
-        <v>-12.138946770927642</v>
+        <v>-17.050485514008589</v>
       </c>
       <c r="K13" s="24">
-        <v>68.400000000000006</v>
+        <v>72</v>
       </c>
       <c r="L13" s="25">
-        <v>30.421052631578949</v>
+        <v>33.826086956521742</v>
       </c>
       <c r="M13" s="25">
-        <v>8.1578947368421044</v>
+        <v>6.7391304347826084</v>
       </c>
       <c r="N13" s="25">
-        <v>2.5789473684210527</v>
+        <v>2.4782608695652173</v>
       </c>
       <c r="O13" s="25">
-        <v>3.4210526315789473</v>
+        <v>2.8260869565217392</v>
       </c>
       <c r="P13" s="25">
-        <v>0.10526315789473684</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="Q13" s="25">
-        <v>5.2631578947368418E-2</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="R13" s="25">
-        <v>27.105263157894736</v>
+        <v>29.347826086956523</v>
       </c>
       <c r="S13" s="25">
         <v>0</v>
       </c>
       <c r="T13" s="20">
-        <v>-28.409011018688524</v>
+        <v>-40.531303528157075</v>
       </c>
       <c r="U13" t="s">
         <v>41</v>
@@ -17257,34 +17254,34 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
-        <v>70.359069418656318</v>
+        <v>71.879515837074933</v>
       </c>
       <c r="B16" s="9">
-        <v>28.777657500725809</v>
+        <v>29.505726735138502</v>
       </c>
       <c r="C16" s="9">
-        <v>16.891966614501825</v>
+        <v>17.752026738728489</v>
       </c>
       <c r="D16" s="9">
-        <v>3.1195115995115996</v>
+        <v>3.1069449413635462</v>
       </c>
       <c r="E16" s="9">
-        <v>5.3459551118242503</v>
+        <v>5.2597914544837279</v>
       </c>
       <c r="F16" s="9">
-        <v>0.40280245576020224</v>
+        <v>0.46360906682366798</v>
       </c>
       <c r="G16" s="9">
-        <v>0.14744715447154472</v>
+        <v>0.17194109772423025</v>
       </c>
       <c r="H16" s="9">
-        <v>24.398182957393484</v>
+        <v>24.479037267080745</v>
       </c>
       <c r="I16" s="9">
-        <v>-1.256657496688619</v>
+        <v>-1.1826868237040509</v>
       </c>
       <c r="J16" s="17">
-        <v>-6.7851149468987053</v>
+        <v>-6.9826965569050987</v>
       </c>
       <c r="K16" s="22">
         <v>68.63333333333334</v>
@@ -17314,7 +17311,7 @@
         <v>-2.3333333333333335</v>
       </c>
       <c r="T16" s="17">
-        <v>-29.36107703225629</v>
+        <v>-37.245302929037749</v>
       </c>
       <c r="U16" t="s">
         <v>33</v>
@@ -17325,34 +17322,34 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
-        <v>79.802797017222616</v>
+        <v>80.018385207882972</v>
       </c>
       <c r="B17" s="10">
-        <v>35.741231968810915</v>
+        <v>35.817423827768657</v>
       </c>
       <c r="C17" s="10">
-        <v>20.165133659097442</v>
+        <v>20.578125693981789</v>
       </c>
       <c r="D17" s="10">
-        <v>3.1506386120339611</v>
+        <v>3.1322071392659629</v>
       </c>
       <c r="E17" s="10">
-        <v>5.4705614718119007</v>
+        <v>5.3128057636556729</v>
       </c>
       <c r="F17" s="10">
-        <v>0.51772087067861716</v>
+        <v>0.55752677702044795</v>
       </c>
       <c r="G17" s="10">
-        <v>0.28048484848484845</v>
+        <v>0.29433426011739267</v>
       </c>
       <c r="H17" s="10">
-        <v>23.365215924426455</v>
+        <v>23.163095238095238</v>
       </c>
       <c r="I17" s="10">
-        <v>-1.0012767768477797</v>
+        <v>-0.93360257461980178</v>
       </c>
       <c r="J17" s="18">
-        <v>9.2108356456295688</v>
+        <v>9.2775904437265577</v>
       </c>
       <c r="K17" s="23" t="e">
         <v>#NUM!</v>
@@ -17390,34 +17387,34 @@
     </row>
     <row r="18" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
-        <v>73.502413875460178</v>
+        <v>75.082726968998927</v>
       </c>
       <c r="B18" s="10">
-        <v>30.222946254525205</v>
+        <v>32.220105820105822</v>
       </c>
       <c r="C18" s="10">
-        <v>15.514188836724049</v>
+        <v>15.423037974683544</v>
       </c>
       <c r="D18" s="10">
-        <v>3.0489545703338807</v>
+        <v>3.0065049665049663</v>
       </c>
       <c r="E18" s="10">
-        <v>5.0333437663015124</v>
+        <v>4.8458669881454686</v>
       </c>
       <c r="F18" s="10">
-        <v>0.36442933462846039</v>
+        <v>0.35939787889154978</v>
       </c>
       <c r="G18" s="10">
-        <v>0.16763218390804599</v>
+        <v>0.1637729295560621</v>
       </c>
       <c r="H18" s="10">
-        <v>26.34399576527526</v>
+        <v>26.31805019305019</v>
       </c>
       <c r="I18" s="10">
-        <v>-0.72057502246181493</v>
+        <v>-0.68744872846595562</v>
       </c>
       <c r="J18" s="18">
-        <v>-5.6484753590577546</v>
+        <v>-10.831163503404618</v>
       </c>
       <c r="K18" s="23">
         <v>72</v>
@@ -17447,7 +17444,7 @@
         <v>0</v>
       </c>
       <c r="T18" s="18">
-        <v>-14.084834484234207</v>
+        <v>-21.46263233107954</v>
       </c>
       <c r="U18" t="s">
         <v>35</v>
@@ -17455,34 +17452,34 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
-        <v>74.015418949076889</v>
+        <v>75.574491206533054</v>
       </c>
       <c r="B19" s="9">
-        <v>33.004822186634129</v>
+        <v>33.282869592281358</v>
       </c>
       <c r="C19" s="9">
-        <v>16.89565772669221</v>
+        <v>17.739291794347974</v>
       </c>
       <c r="D19" s="9">
-        <v>2.8942735042735044</v>
+        <v>2.9095090439276485</v>
       </c>
       <c r="E19" s="9">
-        <v>5.0985372714486639</v>
+        <v>5.1078927203065136</v>
       </c>
       <c r="F19" s="9">
-        <v>0.32205128205128203</v>
+        <v>0.4021262458471761</v>
       </c>
       <c r="G19" s="9">
-        <v>0.17044715447154471</v>
+        <v>0.1684126984126984</v>
       </c>
       <c r="H19" s="9">
-        <v>24.643796992481207</v>
+        <v>25.148634336677816</v>
       </c>
       <c r="I19" s="9">
-        <v>-1.2628018899297864</v>
+        <v>-1.1777178796046721</v>
       </c>
       <c r="J19" s="17">
-        <v>-8.6755596249879119</v>
+        <v>-9.2260667370975291</v>
       </c>
       <c r="K19" s="22">
         <v>77.333333333333329</v>
@@ -17512,7 +17509,7 @@
         <v>-3.3333333333333335</v>
       </c>
       <c r="T19" s="17">
-        <v>-27.835293021733488</v>
+        <v>-37.771610191960512</v>
       </c>
       <c r="U19" t="s">
         <v>36</v>
@@ -17520,34 +17517,34 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
-        <v>83.459146547643201</v>
+        <v>83.713360577341106</v>
       </c>
       <c r="B20" s="10">
-        <v>39.968396654719236</v>
+        <v>39.594566684911513</v>
       </c>
       <c r="C20" s="10">
-        <v>20.168824771287824</v>
+        <v>20.565390749601274</v>
       </c>
       <c r="D20" s="10">
-        <v>2.9254005167958659</v>
+        <v>2.9347712418300653</v>
       </c>
       <c r="E20" s="10">
-        <v>5.2231436314363142</v>
+        <v>5.1609070294784569</v>
       </c>
       <c r="F20" s="10">
-        <v>0.43696969696969701</v>
+        <v>0.49604395604395607</v>
       </c>
       <c r="G20" s="10">
-        <v>0.30348484848484847</v>
+        <v>0.29080586080586079</v>
       </c>
       <c r="H20" s="10">
-        <v>23.61082995951417</v>
+        <v>23.832692307692309</v>
       </c>
       <c r="I20" s="10">
-        <v>-1.0074211700889473</v>
+        <v>-0.92863363052042303</v>
       </c>
       <c r="J20" s="18">
-        <v>7.3203909675403533</v>
+        <v>7.0342202635341256</v>
       </c>
       <c r="K20" s="23">
         <v>94.333333333333329</v>
@@ -17577,7 +17574,7 @@
         <v>0</v>
       </c>
       <c r="T20" s="18">
-        <v>72.548621829143627</v>
+        <v>82.962089792477116</v>
       </c>
       <c r="U20" t="s">
         <v>37</v>
@@ -17585,34 +17582,34 @@
     </row>
     <row r="21" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
-        <v>77.158763405880748</v>
+        <v>78.777702338457061</v>
       </c>
       <c r="B21" s="10">
-        <v>34.450110940433525</v>
+        <v>35.997248677248685</v>
       </c>
       <c r="C21" s="10">
-        <v>15.517879948914432</v>
+        <v>15.41030303030303</v>
       </c>
       <c r="D21" s="10">
-        <v>2.8237164750957855</v>
+        <v>2.8090690690690692</v>
       </c>
       <c r="E21" s="10">
-        <v>4.7859259259259259</v>
+        <v>4.6939682539682535</v>
       </c>
       <c r="F21" s="10">
-        <v>0.28367816091954023</v>
+        <v>0.2979150579150579</v>
       </c>
       <c r="G21" s="10">
-        <v>0.19063218390804598</v>
+        <v>0.16024453024453025</v>
       </c>
       <c r="H21" s="10">
-        <v>26.589609800362972</v>
+        <v>26.987647262647261</v>
       </c>
       <c r="I21" s="10">
-        <v>-0.72671941570298237</v>
+        <v>-0.68247978436657686</v>
       </c>
       <c r="J21" s="18">
-        <v>-7.5389200371469638</v>
+        <v>-13.074533683597044</v>
       </c>
       <c r="K21" s="23" t="e">
         <v>#NUM!</v>
@@ -17650,34 +17647,34 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
-        <v>68.990534156450167</v>
+        <v>71.914158980619433</v>
       </c>
       <c r="B22" s="9">
-        <v>29.855676076577204</v>
+        <v>31.534298163709934</v>
       </c>
       <c r="C22" s="9">
-        <v>13.894179894179894</v>
+        <v>14.78676654182272</v>
       </c>
       <c r="D22" s="9">
-        <v>2.9984401709401709</v>
+        <v>2.9595090439276488</v>
       </c>
       <c r="E22" s="9">
-        <v>4.8461563190677115</v>
+        <v>4.6190038314176238</v>
       </c>
       <c r="F22" s="9">
-        <v>0.33871794871794869</v>
+        <v>0.3906976744186047</v>
       </c>
       <c r="G22" s="9">
-        <v>0.13711382113821138</v>
+        <v>0.17555555555555555</v>
       </c>
       <c r="H22" s="9">
-        <v>25.092261904761905</v>
+        <v>25.690942028985507</v>
       </c>
       <c r="I22" s="9">
-        <v>-1.1833974234285458</v>
+        <v>-1.0901798856836993</v>
       </c>
       <c r="J22" s="17">
-        <v>-14.773954785520552</v>
+        <v>-15.085470332880661</v>
       </c>
       <c r="K22" s="22">
         <v>70.714285714285708</v>
@@ -17707,7 +17704,7 @@
         <v>-1.4285714285714286</v>
       </c>
       <c r="T22" s="17">
-        <v>-18.909332536343285</v>
+        <v>-26.038442851625394</v>
       </c>
       <c r="U22" t="s">
         <v>39</v>
@@ -17715,34 +17712,34 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
-        <v>78.434261755016479</v>
+        <v>80.053028351427486</v>
       </c>
       <c r="B23" s="10">
-        <v>36.81925054466231</v>
+        <v>37.845995256340089</v>
       </c>
       <c r="C23" s="10">
-        <v>17.167346938775513</v>
+        <v>17.612865497076022</v>
       </c>
       <c r="D23" s="10">
-        <v>3.0295671834625324</v>
+        <v>2.9847712418300651</v>
       </c>
       <c r="E23" s="10">
-        <v>4.9707626790553618</v>
+        <v>4.6720181405895689</v>
       </c>
       <c r="F23" s="10">
-        <v>0.45363636363636373</v>
+        <v>0.48461538461538467</v>
       </c>
       <c r="G23" s="10">
-        <v>0.27015151515151514</v>
+        <v>0.29794871794871797</v>
       </c>
       <c r="H23" s="10">
-        <v>24.059294871794872</v>
+        <v>24.375000000000004</v>
       </c>
       <c r="I23" s="10">
-        <v>-0.92801670358770649</v>
+        <v>-0.84109563659945041</v>
       </c>
       <c r="J23" s="18">
-        <v>1.2219958070077284</v>
+        <v>1.1748166677510006</v>
       </c>
       <c r="K23" s="23" t="e">
         <v>#NUM!</v>
@@ -17780,34 +17777,34 @@
     </row>
     <row r="24" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="19">
-        <v>72.133878613254026</v>
+        <v>75.117370112543441</v>
       </c>
       <c r="B24" s="19">
-        <v>31.300964830376596</v>
+        <v>34.248677248677254</v>
       </c>
       <c r="C24" s="19">
-        <v>12.516402116402116</v>
+        <v>12.457777777777778</v>
       </c>
       <c r="D24" s="19">
-        <v>2.9278831417624525</v>
+        <v>2.8590690690690694</v>
       </c>
       <c r="E24" s="19">
-        <v>4.5335449735449727</v>
+        <v>4.2050793650793654</v>
       </c>
       <c r="F24" s="19">
-        <v>0.3003448275862069</v>
+        <v>0.2864864864864865</v>
       </c>
       <c r="G24" s="19">
-        <v>0.15729885057471266</v>
+        <v>0.1673873873873874</v>
       </c>
       <c r="H24" s="19">
-        <v>27.038074712643674</v>
+        <v>27.529954954954952</v>
       </c>
       <c r="I24" s="19">
-        <v>-0.6473149492017416</v>
+        <v>-0.59494179044560425</v>
       </c>
       <c r="J24" s="20">
-        <v>-13.637315197679603</v>
+        <v>-18.933937279380167</v>
       </c>
       <c r="K24" s="24">
         <v>64.833333333333329</v>
@@ -17837,7 +17834,7 @@
         <v>0</v>
       </c>
       <c r="T24" s="20">
-        <v>-15.957272500652767</v>
+        <v>-22.266162823060348</v>
       </c>
       <c r="U24" t="s">
         <v>41</v>
@@ -17934,34 +17931,34 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
-        <v>72.752849991682169</v>
+        <v>74.746697083501459</v>
       </c>
       <c r="B27" s="12">
-        <v>31.545401608469916</v>
+        <v>32.307772064049502</v>
       </c>
       <c r="C27" s="12">
-        <v>17.515043537578748</v>
+        <v>18.66452673872849</v>
       </c>
       <c r="D27" s="12">
-        <v>3.0879560439560438</v>
+        <v>3.0823571277434745</v>
       </c>
       <c r="E27" s="12">
-        <v>5.2835396528870522</v>
+        <v>5.1955768950967549</v>
       </c>
       <c r="F27" s="12">
-        <v>0.46680245576020224</v>
+        <v>0.54618971198495825</v>
       </c>
       <c r="G27" s="12">
-        <v>0.19811382113821141</v>
+        <v>0.22312389342315497</v>
       </c>
       <c r="H27" s="12">
-        <v>23.421992481203006</v>
+        <v>23.65305687492388</v>
       </c>
       <c r="I27" s="9">
-        <v>-1.0549658896619438</v>
+        <v>-0.9573498964803312</v>
       </c>
       <c r="J27" s="17">
-        <v>-1.2000110313711669</v>
+        <v>0.85868056005839488</v>
       </c>
       <c r="K27" s="22">
         <v>99.666666666666671</v>
@@ -17991,7 +17988,7 @@
         <v>0</v>
       </c>
       <c r="T27" s="17">
-        <v>44.388086307786004</v>
+        <v>44.90085788241619</v>
       </c>
       <c r="U27" t="s">
         <v>33</v>
@@ -18002,34 +17999,34 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
-        <v>82.196577590248481</v>
+        <v>82.885566454309497</v>
       </c>
       <c r="B28" s="13">
-        <v>38.508976076555022</v>
+        <v>38.619469156679656</v>
       </c>
       <c r="C28" s="13">
-        <v>20.788210582174365</v>
+        <v>21.490625693981791</v>
       </c>
       <c r="D28" s="13">
-        <v>3.1190830564784053</v>
+        <v>3.1076193256458913</v>
       </c>
       <c r="E28" s="13">
-        <v>5.4081460128747034</v>
+        <v>5.2485912042687008</v>
       </c>
       <c r="F28" s="13">
-        <v>0.58172087067861711</v>
+        <v>0.64010742218173822</v>
       </c>
       <c r="G28" s="13">
-        <v>0.33115151515151514</v>
+        <v>0.34551705581631736</v>
       </c>
       <c r="H28" s="13">
-        <v>22.389025448235977</v>
+        <v>22.337114845938373</v>
       </c>
       <c r="I28" s="10">
-        <v>-0.7995851698211045</v>
+        <v>-0.70826564739608211</v>
       </c>
       <c r="J28" s="18">
-        <v>14.795939561157107</v>
+        <v>17.118967560690056</v>
       </c>
       <c r="K28" s="23">
         <v>119.5</v>
@@ -18059,7 +18056,7 @@
         <v>0</v>
       </c>
       <c r="T28" s="18">
-        <v>72.450260355057594</v>
+        <v>76.815697229394232</v>
       </c>
       <c r="U28" t="s">
         <v>34</v>
@@ -18067,34 +18064,34 @@
     </row>
     <row r="29" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
-        <v>75.896194448486028</v>
+        <v>77.949908215425452</v>
       </c>
       <c r="B29" s="13">
-        <v>32.990690362269312</v>
+        <v>35.022151149016821</v>
       </c>
       <c r="C29" s="13">
-        <v>16.137265759800972</v>
+        <v>16.335537974683543</v>
       </c>
       <c r="D29" s="13">
-        <v>3.017399014778325</v>
+        <v>2.9819171528848947</v>
       </c>
       <c r="E29" s="13">
-        <v>4.9709283073643151</v>
+        <v>4.7816524287584965</v>
       </c>
       <c r="F29" s="13">
-        <v>0.42842933462846045</v>
+        <v>0.4419785240528401</v>
       </c>
       <c r="G29" s="13">
-        <v>0.21829885057471268</v>
+        <v>0.21495572525498682</v>
       </c>
       <c r="H29" s="13">
-        <v>25.367805289084782</v>
+        <v>25.492069800893329</v>
       </c>
       <c r="I29" s="10">
-        <v>-0.51888341543513961</v>
+        <v>-0.462111801242236</v>
       </c>
       <c r="J29" s="18">
-        <v>-6.3371443530212623E-2</v>
+        <v>-2.9897863864411223</v>
       </c>
       <c r="K29" s="23">
         <v>104</v>
@@ -18124,7 +18121,7 @@
         <v>0</v>
       </c>
       <c r="T29" s="18">
-        <v>30.482168794003105</v>
+        <v>34.087806039109523</v>
       </c>
       <c r="U29" t="s">
         <v>35</v>
@@ -18132,64 +18129,64 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
-        <v>76.409199522102739</v>
+        <v>78.44167245295958</v>
       </c>
       <c r="B30" s="12">
-        <v>35.772566294378237</v>
+        <v>36.084914921192357</v>
       </c>
       <c r="C30" s="12">
-        <v>17.518734649769133</v>
+        <v>18.651791794347975</v>
       </c>
       <c r="D30" s="12">
-        <v>2.862717948717949</v>
+        <v>2.8849212303075769</v>
       </c>
       <c r="E30" s="12">
-        <v>5.0361218125114657</v>
+        <v>5.0436781609195407</v>
       </c>
       <c r="F30" s="12">
-        <v>0.38605128205128203</v>
+        <v>0.48470689100846637</v>
       </c>
       <c r="G30" s="12">
-        <v>0.22111382113821137</v>
+        <v>0.21959549411162316</v>
       </c>
       <c r="H30" s="12">
-        <v>23.667606516290725</v>
+        <v>24.322653944520951</v>
       </c>
       <c r="I30" s="9">
-        <v>-1.0611102829031112</v>
+        <v>-0.95238095238095233</v>
       </c>
       <c r="J30" s="17">
-        <v>-3.0904557094603726</v>
+        <v>-1.3846896201340324</v>
       </c>
       <c r="K30" s="22">
-        <v>42</v>
+        <v>81.333333333333329</v>
       </c>
       <c r="L30" s="12">
-        <v>20</v>
+        <v>25.333333333333332</v>
       </c>
       <c r="M30" s="12">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="N30" s="12">
-        <v>2</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="O30" s="12">
         <v>5</v>
       </c>
       <c r="P30" s="12">
-        <v>0</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="Q30" s="12">
         <v>0</v>
       </c>
       <c r="R30" s="12">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="S30" s="12">
         <v>0</v>
       </c>
       <c r="T30" s="17">
-        <v>-31.276490513430083</v>
+        <v>29.213979496051596</v>
       </c>
       <c r="U30" t="s">
         <v>36</v>
@@ -18197,34 +18194,34 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
-        <v>85.852927120669051</v>
+        <v>86.580541823767632</v>
       </c>
       <c r="B31" s="13">
-        <v>42.736140762463343</v>
+        <v>42.396612013822512</v>
       </c>
       <c r="C31" s="13">
-        <v>20.791901694364746</v>
+        <v>21.477890749601276</v>
       </c>
       <c r="D31" s="13">
-        <v>2.8938449612403105</v>
+        <v>2.9101834282099937</v>
       </c>
       <c r="E31" s="13">
-        <v>5.160728172499117</v>
+        <v>5.0966924700914849</v>
       </c>
       <c r="F31" s="13">
-        <v>0.50096969696969695</v>
+        <v>0.57862460120524628</v>
       </c>
       <c r="G31" s="13">
-        <v>0.35415151515151516</v>
+        <v>0.34198865650478549</v>
       </c>
       <c r="H31" s="13">
-        <v>22.634639483323696</v>
+        <v>23.006711915535444</v>
       </c>
       <c r="I31" s="10">
-        <v>-0.80572956306227184</v>
+        <v>-0.70329670329670324</v>
       </c>
       <c r="J31" s="18">
-        <v>12.905494883067897</v>
+        <v>14.875597380497622</v>
       </c>
       <c r="K31" s="23">
         <v>84.441176470588232</v>
@@ -18254,7 +18251,7 @@
         <v>-1.1764705882352942</v>
       </c>
       <c r="T31" s="18">
-        <v>2.0222358955907325</v>
+        <v>-0.50320210012384692</v>
       </c>
       <c r="U31" t="s">
         <v>37</v>
@@ -18262,64 +18259,64 @@
     </row>
     <row r="32" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
-        <v>79.552543978906598</v>
+        <v>81.644883584883587</v>
       </c>
       <c r="B32" s="13">
-        <v>37.217855048177633</v>
+        <v>38.799294006159684</v>
       </c>
       <c r="C32" s="13">
-        <v>16.140956871991357</v>
+        <v>16.322803030303028</v>
       </c>
       <c r="D32" s="13">
-        <v>2.7921609195402302</v>
+        <v>2.7844812554489975</v>
       </c>
       <c r="E32" s="13">
-        <v>4.7235104669887287</v>
+        <v>4.6297536945812805</v>
       </c>
       <c r="F32" s="13">
-        <v>0.34767816091954024</v>
+        <v>0.38049570307634822</v>
       </c>
       <c r="G32" s="13">
-        <v>0.24129885057471262</v>
+        <v>0.21142732594345498</v>
       </c>
       <c r="H32" s="13">
-        <v>25.613419324172497</v>
+        <v>26.1616668704904</v>
       </c>
       <c r="I32" s="10">
-        <v>-0.52502780867630705</v>
+        <v>-0.45714285714285713</v>
       </c>
       <c r="J32" s="18">
-        <v>-1.9538161216194201</v>
+        <v>-5.2331565666335509</v>
       </c>
       <c r="K32" s="23">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="L32" s="13">
         <v>50</v>
       </c>
       <c r="M32" s="13">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="N32" s="13">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="O32" s="13">
-        <v>8</v>
+        <v>6.4</v>
       </c>
       <c r="P32" s="13">
         <v>0</v>
       </c>
       <c r="Q32" s="13">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="R32" s="13">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="S32" s="13">
         <v>0</v>
       </c>
       <c r="T32" s="18">
-        <v>66.834382603178824</v>
+        <v>1.9656300570695049</v>
       </c>
       <c r="U32" t="s">
         <v>38</v>
@@ -18327,52 +18324,52 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
-        <v>71.384314729476017</v>
+        <v>74.781340227045959</v>
       </c>
       <c r="B33" s="12">
-        <v>32.623420184321311</v>
+        <v>34.336343492620934</v>
       </c>
       <c r="C33" s="12">
-        <v>14.517256817256817</v>
+        <v>15.69926654182272</v>
       </c>
       <c r="D33" s="12">
-        <v>2.9668846153846156</v>
+        <v>2.9349212303075771</v>
       </c>
       <c r="E33" s="12">
-        <v>4.7837408601305134</v>
+        <v>4.5547892720306518</v>
       </c>
       <c r="F33" s="12">
-        <v>0.40271794871794875</v>
+        <v>0.47327831957989497</v>
       </c>
       <c r="G33" s="12">
-        <v>0.18778048780487805</v>
+        <v>0.22673835125448027</v>
       </c>
       <c r="H33" s="12">
-        <v>24.116071428571427</v>
+        <v>24.864961636828646</v>
       </c>
       <c r="I33" s="9">
-        <v>-0.98170581640187038</v>
+        <v>-0.86484295845997983</v>
       </c>
       <c r="J33" s="17">
-        <v>-9.1888508699930078</v>
+        <v>-7.2440932159171663</v>
       </c>
       <c r="K33" s="22">
-        <v>69</v>
+        <v>89.666666666666671</v>
       </c>
       <c r="L33" s="12">
-        <v>36.666666666666664</v>
-      </c>
-      <c r="M33" s="12" t="e">
-        <v>#NUM!</v>
+        <v>44.285714285714285</v>
+      </c>
+      <c r="M33" s="12">
+        <v>30</v>
       </c>
       <c r="N33" s="12">
+        <v>3.2</v>
+      </c>
+      <c r="O33" s="12">
         <v>4</v>
       </c>
-      <c r="O33" s="12" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="P33" s="12">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="Q33" s="12">
         <v>1</v>
@@ -18383,8 +18380,8 @@
       <c r="S33" s="12">
         <v>0</v>
       </c>
-      <c r="T33" s="17" t="e">
-        <v>#NUM!</v>
+      <c r="T33" s="17">
+        <v>79.964241060212345</v>
       </c>
       <c r="U33" t="s">
         <v>39</v>
@@ -18392,34 +18389,34 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="10">
-        <v>80.828042328042329</v>
+        <v>82.920209597854011</v>
       </c>
       <c r="B34" s="13">
-        <v>39.586994652406418</v>
+        <v>40.648040585251081</v>
       </c>
       <c r="C34" s="13">
-        <v>17.790423861852435</v>
+        <v>18.525365497076024</v>
       </c>
       <c r="D34" s="13">
-        <v>2.9980116279069771</v>
+        <v>2.9601834282099935</v>
       </c>
       <c r="E34" s="13">
-        <v>4.9083472201181646</v>
+        <v>4.6078035812025959</v>
       </c>
       <c r="F34" s="13">
-        <v>0.51763636363636367</v>
+        <v>0.56719602977667494</v>
       </c>
       <c r="G34" s="13">
-        <v>0.32081818181818184</v>
+        <v>0.34913151364764267</v>
       </c>
       <c r="H34" s="13">
-        <v>23.083104395604398</v>
+        <v>23.549019607843139</v>
       </c>
       <c r="I34" s="10">
-        <v>-0.72632509656103117</v>
+        <v>-0.61575870937573074</v>
       </c>
       <c r="J34" s="18">
-        <v>6.8070997225352698</v>
+        <v>9.0161937847144937</v>
       </c>
       <c r="K34" s="23">
         <v>83</v>
@@ -18449,7 +18446,7 @@
         <v>0</v>
       </c>
       <c r="T34" s="18">
-        <v>23.202981131810297</v>
+        <v>26.029053396707386</v>
       </c>
       <c r="U34" t="s">
         <v>40</v>
@@ -18457,34 +18454,34 @@
     </row>
     <row r="35" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="19">
-        <v>74.527659186279877</v>
+        <v>77.984551358969966</v>
       </c>
       <c r="B35" s="25">
-        <v>34.068708938120707</v>
+        <v>37.050722577588246</v>
       </c>
       <c r="C35" s="25">
-        <v>13.139479039479038</v>
+        <v>13.370277777777778</v>
       </c>
       <c r="D35" s="25">
-        <v>2.8963275862068967</v>
+        <v>2.8344812554489978</v>
       </c>
       <c r="E35" s="25">
-        <v>4.4711295146077754</v>
+        <v>4.1408648056923916</v>
       </c>
       <c r="F35" s="25">
-        <v>0.3643448275862069</v>
+        <v>0.36906713164777682</v>
       </c>
       <c r="G35" s="25">
-        <v>0.20796551724137932</v>
+        <v>0.21857018308631213</v>
       </c>
       <c r="H35" s="25">
-        <v>26.061884236453199</v>
+        <v>26.703974562798088</v>
       </c>
       <c r="I35" s="19">
-        <v>-0.44562334217506638</v>
+        <v>-0.36960486322188452</v>
       </c>
       <c r="J35" s="20">
-        <v>-8.0522112821520615</v>
+        <v>-11.092560162416676</v>
       </c>
       <c r="K35" s="24">
         <v>43</v>
@@ -18514,7 +18511,7 @@
         <v>0</v>
       </c>
       <c r="T35" s="20">
-        <v>-51.68363952503455</v>
+        <v>-63.227789918018182</v>
       </c>
       <c r="U35" t="s">
         <v>41</v>
@@ -18611,34 +18608,34 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="9">
-        <v>70.570912669744843</v>
+        <v>72.119009246224579</v>
       </c>
       <c r="B38" s="9">
-        <v>29.471380036821227</v>
+        <v>30.406279526736068</v>
       </c>
       <c r="C38" s="9">
-        <v>17.007060954124466</v>
+        <v>17.524157886269471</v>
       </c>
       <c r="D38" s="9">
-        <v>3.163171730230554</v>
+        <v>3.1181690468249394</v>
       </c>
       <c r="E38" s="9">
-        <v>5.244074769943909</v>
+        <v>5.0553470100392834</v>
       </c>
       <c r="F38" s="9">
-        <v>0.45126399422174063</v>
+        <v>0.50027573349033461</v>
       </c>
       <c r="G38" s="9">
-        <v>0.17697096399535425</v>
+        <v>0.19610776439089692</v>
       </c>
       <c r="H38" s="9">
-        <v>23.536340852130326</v>
+        <v>23.789934702978179</v>
       </c>
       <c r="I38" s="9">
-        <v>-1.0313205694648993</v>
+        <v>-0.94562828475871952</v>
       </c>
       <c r="J38" s="17">
-        <v>-3.0320308034372618</v>
+        <v>-4.0204146574760529</v>
       </c>
       <c r="K38" s="22">
         <v>55.07692307692308</v>
@@ -18668,7 +18665,7 @@
         <v>-0.37037037037037035</v>
       </c>
       <c r="T38" s="17">
-        <v>-5.3472030886467099</v>
+        <v>-10.357996932071655</v>
       </c>
       <c r="U38" t="s">
         <v>33</v>
@@ -18679,64 +18676,64 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="10">
-        <v>80.014640268311155</v>
+        <v>80.257878617032631</v>
       </c>
       <c r="B39" s="10">
-        <v>36.434954504906329</v>
+        <v>36.717976619366226</v>
       </c>
       <c r="C39" s="10">
-        <v>20.280227998720086</v>
+        <v>20.350256841522771</v>
       </c>
       <c r="D39" s="10">
-        <v>3.1942987427529155</v>
+        <v>3.1434312447273567</v>
       </c>
       <c r="E39" s="10">
-        <v>5.3686811299315593</v>
+        <v>5.1083613192112285</v>
       </c>
       <c r="F39" s="10">
-        <v>0.56618240914015561</v>
+        <v>0.59419344368711458</v>
       </c>
       <c r="G39" s="10">
-        <v>0.31000865800865796</v>
+        <v>0.31850092678405933</v>
       </c>
       <c r="H39" s="10">
-        <v>22.503373819163293</v>
+        <v>22.473992673992672</v>
       </c>
       <c r="I39" s="10">
-        <v>-0.77593984962406015</v>
+        <v>-0.69654403567447043</v>
       </c>
       <c r="J39" s="18">
-        <v>12.963919789091015</v>
+        <v>12.239872343155611</v>
       </c>
       <c r="K39" s="23">
-        <v>107.25</v>
+        <v>81.625</v>
       </c>
       <c r="L39" s="10">
-        <v>50</v>
+        <v>36.666666666666664</v>
       </c>
       <c r="M39" s="10">
-        <v>44</v>
+        <v>13.6</v>
       </c>
       <c r="N39" s="10">
-        <v>4</v>
+        <v>2.4</v>
       </c>
       <c r="O39" s="10">
-        <v>8</v>
+        <v>3.2</v>
       </c>
       <c r="P39" s="10">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="Q39" s="10">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="R39" s="10">
-        <v>25</v>
+        <v>21.666666666666668</v>
       </c>
       <c r="S39" s="10">
         <v>0</v>
       </c>
       <c r="T39" s="18">
-        <v>105.13615859362464</v>
+        <v>-8.8419620243753378</v>
       </c>
       <c r="U39" t="s">
         <v>34</v>
@@ -18744,34 +18741,34 @@
     </row>
     <row r="40" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="10">
-        <v>73.714257126548702</v>
+        <v>75.322220378148586</v>
       </c>
       <c r="B40" s="10">
-        <v>30.916668790620616</v>
+        <v>33.120658611703391</v>
       </c>
       <c r="C40" s="10">
-        <v>15.629283176346689</v>
+        <v>15.195169122224527</v>
       </c>
       <c r="D40" s="10">
-        <v>3.0926147010528346</v>
+        <v>3.0177290719663601</v>
       </c>
       <c r="E40" s="10">
-        <v>4.931463424421171</v>
+        <v>4.6414225437010241</v>
       </c>
       <c r="F40" s="10">
-        <v>0.41289087308999883</v>
+        <v>0.39606454555821646</v>
       </c>
       <c r="G40" s="10">
-        <v>0.19715599343185553</v>
+        <v>0.18793959622272877</v>
       </c>
       <c r="H40" s="10">
-        <v>25.482153660012099</v>
+        <v>25.628947628947628</v>
       </c>
       <c r="I40" s="10">
-        <v>-0.49523809523809526</v>
+        <v>-0.45039018952062426</v>
       </c>
       <c r="J40" s="18">
-        <v>-1.8953912155963137</v>
+        <v>-7.868881603975562</v>
       </c>
       <c r="K40" s="23">
         <v>84</v>
@@ -18801,7 +18798,7 @@
         <v>0</v>
       </c>
       <c r="T40" s="18">
-        <v>108.95931681550806</v>
+        <v>122.05407406125485</v>
       </c>
       <c r="U40" t="s">
         <v>35</v>
@@ -18809,34 +18806,34 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="9">
-        <v>74.227262200165427</v>
+        <v>75.813984615682699</v>
       </c>
       <c r="B41" s="9">
-        <v>33.698544722729544</v>
+        <v>34.183422383878927</v>
       </c>
       <c r="C41" s="9">
-        <v>17.010752066314851</v>
+        <v>17.511422941888959</v>
       </c>
       <c r="D41" s="9">
-        <v>2.9379336349924587</v>
+        <v>2.9207331493890423</v>
       </c>
       <c r="E41" s="9">
-        <v>4.9966569295683225</v>
+        <v>4.9034482758620692</v>
       </c>
       <c r="F41" s="9">
-        <v>0.37051282051282047</v>
+        <v>0.43879291251384273</v>
       </c>
       <c r="G41" s="9">
-        <v>0.19997096399535425</v>
+        <v>0.19257936507936507</v>
       </c>
       <c r="H41" s="9">
-        <v>23.781954887218046</v>
+        <v>24.459531772575254</v>
       </c>
       <c r="I41" s="9">
-        <v>-1.0374649627060666</v>
+        <v>-0.94065934065934065</v>
       </c>
       <c r="J41" s="17">
-        <v>-4.9224754815264671</v>
+        <v>-6.2637848376684717</v>
       </c>
       <c r="K41" s="22">
         <v>74</v>
@@ -18866,7 +18863,7 @@
         <v>-0.7142857142857143</v>
       </c>
       <c r="T41" s="17">
-        <v>-23.87743571736819</v>
+        <v>-31.003342908411931</v>
       </c>
       <c r="U41" t="s">
         <v>36</v>
@@ -18874,34 +18871,34 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="10">
-        <v>83.670989798731725</v>
+        <v>83.952853986490751</v>
       </c>
       <c r="B42" s="10">
-        <v>40.66211919081465</v>
+        <v>40.495119476509082</v>
       </c>
       <c r="C42" s="10">
-        <v>20.283919110910468</v>
+        <v>20.33752189714226</v>
       </c>
       <c r="D42" s="10">
-        <v>2.9690606475148202</v>
+        <v>2.9459953472914586</v>
       </c>
       <c r="E42" s="10">
-        <v>5.1212632895559729</v>
+        <v>4.9564625850340125</v>
       </c>
       <c r="F42" s="10">
-        <v>0.4854312354312354</v>
+        <v>0.53271062271062264</v>
       </c>
       <c r="G42" s="10">
-        <v>0.33300865800865798</v>
+        <v>0.31497252747252746</v>
       </c>
       <c r="H42" s="10">
-        <v>22.748987854251013</v>
+        <v>23.143589743589747</v>
       </c>
       <c r="I42" s="10">
-        <v>-0.78208424286522749</v>
+        <v>-0.69157509157509156</v>
       </c>
       <c r="J42" s="18">
-        <v>11.073475111001802</v>
+        <v>9.9965021629631785</v>
       </c>
       <c r="K42" s="23">
         <v>88.25</v>
@@ -18931,7 +18928,7 @@
         <v>0</v>
       </c>
       <c r="T42" s="18">
-        <v>16.98862533234675</v>
+        <v>10.574631553192672</v>
       </c>
       <c r="U42" t="s">
         <v>37</v>
@@ -18939,34 +18936,34 @@
     </row>
     <row r="43" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="10">
-        <v>77.370606656969272</v>
+        <v>79.017195747606706</v>
       </c>
       <c r="B43" s="10">
-        <v>35.14383347652894</v>
+        <v>36.897801468846254</v>
       </c>
       <c r="C43" s="10">
-        <v>15.632974288537074</v>
+        <v>15.182434177844012</v>
       </c>
       <c r="D43" s="10">
-        <v>2.8673766058147399</v>
+        <v>2.8202931745304629</v>
       </c>
       <c r="E43" s="10">
-        <v>4.6840455840455846</v>
+        <v>4.489523809523809</v>
       </c>
       <c r="F43" s="10">
-        <v>0.33213969938107868</v>
+        <v>0.33458172458172458</v>
       </c>
       <c r="G43" s="10">
-        <v>0.22015599343185549</v>
+        <v>0.18441119691119692</v>
       </c>
       <c r="H43" s="10">
-        <v>25.727767695099818</v>
+        <v>26.298544698544696</v>
       </c>
       <c r="I43" s="10">
-        <v>-0.50138248847926259</v>
+        <v>-0.44542124542124545</v>
       </c>
       <c r="J43" s="18">
-        <v>-3.7858358936855177</v>
+        <v>-10.112251784167992</v>
       </c>
       <c r="K43" s="23">
         <v>120</v>
@@ -18996,7 +18993,7 @@
         <v>0</v>
       </c>
       <c r="T43" s="18">
-        <v>46.667293967436805</v>
+        <v>42.905511180354353</v>
       </c>
       <c r="U43" t="s">
         <v>38</v>
@@ -19004,34 +19001,34 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44" s="9">
-        <v>69.202377407538705</v>
+        <v>72.153652389769078</v>
       </c>
       <c r="B44" s="9">
-        <v>30.549398612672615</v>
+        <v>32.434850955307503</v>
       </c>
       <c r="C44" s="9">
-        <v>14.009274233802534</v>
+        <v>14.558897689363704</v>
       </c>
       <c r="D44" s="9">
-        <v>3.0421003016591248</v>
+        <v>2.9707331493890421</v>
       </c>
       <c r="E44" s="9">
-        <v>4.7442759771873693</v>
+        <v>4.4145593869731794</v>
       </c>
       <c r="F44" s="9">
-        <v>0.38717948717948719</v>
+        <v>0.42736434108527133</v>
       </c>
       <c r="G44" s="9">
-        <v>0.16663763066202092</v>
+        <v>0.19972222222222222</v>
       </c>
       <c r="H44" s="9">
-        <v>24.230419799498748</v>
+        <v>25.001839464882941</v>
       </c>
       <c r="I44" s="9">
-        <v>-0.95806049620482603</v>
+        <v>-0.85312134673836792</v>
       </c>
       <c r="J44" s="17">
-        <v>-11.02087064205911</v>
+        <v>-12.123188433451608</v>
       </c>
       <c r="K44" s="22">
         <v>61</v>
@@ -19061,7 +19058,7 @@
         <v>-5</v>
       </c>
       <c r="T44" s="17">
-        <v>14.31969315047489</v>
+        <v>17.954832553354933</v>
       </c>
       <c r="U44" t="s">
         <v>39</v>
@@ -19069,34 +19066,34 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="10">
-        <v>78.646105006105003</v>
+        <v>80.292521760577145</v>
       </c>
       <c r="B45" s="10">
-        <v>37.512973080757725</v>
+        <v>38.746548047937651</v>
       </c>
       <c r="C45" s="10">
-        <v>17.282441278398153</v>
+        <v>17.384996644617008</v>
       </c>
       <c r="D45" s="10">
-        <v>3.0732273141814863</v>
+        <v>2.9959953472914589</v>
       </c>
       <c r="E45" s="10">
-        <v>4.8688823371750205</v>
+        <v>4.4675736961451245</v>
       </c>
       <c r="F45" s="10">
-        <v>0.50209790209790217</v>
+        <v>0.5212820512820513</v>
       </c>
       <c r="G45" s="10">
-        <v>0.29967532467532465</v>
+        <v>0.32211538461538464</v>
       </c>
       <c r="H45" s="10">
-        <v>23.197452766531715</v>
+        <v>23.685897435897438</v>
       </c>
       <c r="I45" s="10">
-        <v>-0.70267977636398682</v>
+        <v>-0.60403709765411895</v>
       </c>
       <c r="J45" s="18">
-        <v>4.9750799504691692</v>
+        <v>4.1370985671800575</v>
       </c>
       <c r="K45" s="23">
         <v>89</v>
@@ -19126,7 +19123,7 @@
         <v>0</v>
       </c>
       <c r="T45" s="18">
-        <v>50.981147973497762</v>
+        <v>55.099880467133474</v>
       </c>
       <c r="U45" t="s">
         <v>40</v>
@@ -19134,49 +19131,49 @@
     </row>
     <row r="46" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="19">
-        <v>72.345721864342551</v>
+        <v>75.3568635216931</v>
       </c>
       <c r="B46" s="19">
-        <v>31.994687366472011</v>
+        <v>35.149230040274816</v>
       </c>
       <c r="C46" s="19">
-        <v>12.631496456024758</v>
+        <v>12.229908925318762</v>
       </c>
       <c r="D46" s="19">
-        <v>2.9715432724814064</v>
+        <v>2.8702931745304627</v>
       </c>
       <c r="E46" s="19">
-        <v>4.4316646316646313</v>
+        <v>4.000634920634921</v>
       </c>
       <c r="F46" s="19">
-        <v>0.34880636604774534</v>
+        <v>0.32315315315315318</v>
       </c>
       <c r="G46" s="19">
-        <v>0.18682266009852216</v>
+        <v>0.19155405405405407</v>
       </c>
       <c r="H46" s="19">
-        <v>26.17623260738052</v>
+        <v>26.840852390852387</v>
       </c>
       <c r="I46" s="19">
-        <v>-0.42197802197802198</v>
+        <v>-0.35788325150027278</v>
       </c>
       <c r="J46" s="20">
-        <v>-9.8842310542181586</v>
+        <v>-15.971655379951114</v>
       </c>
       <c r="K46" s="24">
-        <v>84.888888888888886</v>
+        <v>86.461538461538467</v>
       </c>
       <c r="L46" s="19">
-        <v>39</v>
+        <v>42.666666666666664</v>
       </c>
       <c r="M46" s="19">
-        <v>6.5</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="N46" s="19">
-        <v>4</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="O46" s="19">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="P46" s="19">
         <v>0</v>
@@ -19185,13 +19182,13 @@
         <v>0</v>
       </c>
       <c r="R46" s="19">
-        <v>35</v>
+        <v>36.666666666666664</v>
       </c>
       <c r="S46" s="19">
         <v>0</v>
       </c>
       <c r="T46" s="20">
-        <v>-23.367744770491132</v>
+        <v>-40.316252349407925</v>
       </c>
       <c r="U46" t="s">
         <v>41</v>
@@ -19324,117 +19321,117 @@
     <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" s="46">
         <f>J16</f>
-        <v>-6.7851149468987053</v>
+        <v>-6.9826965569050987</v>
       </c>
       <c r="B52" s="46">
         <f>J17</f>
-        <v>9.2108356456295688</v>
+        <v>9.2775904437265577</v>
       </c>
       <c r="C52" s="46">
         <f>J18</f>
-        <v>-5.6484753590577546</v>
+        <v>-10.831163503404618</v>
       </c>
       <c r="D52" s="46">
         <f>J19</f>
-        <v>-8.6755596249879119</v>
+        <v>-9.2260667370975291</v>
       </c>
       <c r="E52" s="46">
         <f>J20</f>
-        <v>7.3203909675403533</v>
+        <v>7.0342202635341256</v>
       </c>
       <c r="F52" s="46">
         <f>J21</f>
-        <v>-7.5389200371469638</v>
+        <v>-13.074533683597044</v>
       </c>
       <c r="G52" s="46">
         <f>J22</f>
-        <v>-14.773954785520552</v>
+        <v>-15.085470332880661</v>
       </c>
       <c r="H52" s="46">
         <f>J23</f>
-        <v>1.2219958070077284</v>
+        <v>1.1748166677510006</v>
       </c>
       <c r="I52" s="46">
         <f>J24</f>
-        <v>-13.637315197679603</v>
+        <v>-18.933937279380167</v>
       </c>
       <c r="J52" s="46">
         <f>J27</f>
-        <v>-1.2000110313711669</v>
+        <v>0.85868056005839488</v>
       </c>
       <c r="K52" s="46">
         <f>J28</f>
-        <v>14.795939561157107</v>
+        <v>17.118967560690056</v>
       </c>
       <c r="L52" s="46">
         <f>J29</f>
-        <v>-6.3371443530212623E-2</v>
+        <v>-2.9897863864411223</v>
       </c>
       <c r="M52" s="46">
         <f>J30</f>
-        <v>-3.0904557094603726</v>
+        <v>-1.3846896201340324</v>
       </c>
       <c r="N52" s="46">
         <f>J31</f>
-        <v>12.905494883067897</v>
+        <v>14.875597380497622</v>
       </c>
       <c r="O52" s="46">
         <f>J32</f>
-        <v>-1.9538161216194201</v>
+        <v>-5.2331565666335509</v>
       </c>
       <c r="P52" s="46">
         <f>J33</f>
-        <v>-9.1888508699930078</v>
+        <v>-7.2440932159171663</v>
       </c>
       <c r="Q52" s="46">
         <f>J34</f>
-        <v>6.8070997225352698</v>
+        <v>9.0161937847144937</v>
       </c>
       <c r="R52" s="46">
         <f>J35</f>
-        <v>-8.0522112821520615</v>
+        <v>-11.092560162416676</v>
       </c>
       <c r="S52" s="46">
         <f>J38</f>
-        <v>-3.0320308034372618</v>
+        <v>-4.0204146574760529</v>
       </c>
       <c r="T52" s="46">
         <f>J39</f>
-        <v>12.963919789091015</v>
+        <v>12.239872343155611</v>
       </c>
       <c r="U52" s="46">
         <f>J40</f>
-        <v>-1.8953912155963137</v>
+        <v>-7.868881603975562</v>
       </c>
       <c r="V52" s="46">
         <f>J41</f>
-        <v>-4.9224754815264671</v>
+        <v>-6.2637848376684717</v>
       </c>
       <c r="W52" s="46">
         <f>J42</f>
-        <v>11.073475111001802</v>
+        <v>9.9965021629631785</v>
       </c>
       <c r="X52" s="46">
         <f>J43</f>
-        <v>-3.7858358936855177</v>
+        <v>-10.112251784167992</v>
       </c>
       <c r="Y52" s="46">
         <f>J44</f>
-        <v>-11.02087064205911</v>
+        <v>-12.123188433451608</v>
       </c>
       <c r="Z52" s="46">
         <f>J45</f>
-        <v>4.9750799504691692</v>
+        <v>4.1370985671800575</v>
       </c>
       <c r="AA52" s="46">
         <f>J46</f>
-        <v>-9.8842310542181586</v>
+        <v>-15.971655379951114</v>
       </c>
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" s="46">
         <f>T16</f>
-        <v>-29.36107703225629</v>
+        <v>-37.245302929037749</v>
       </c>
       <c r="B53" s="46" t="e">
         <f>T17</f>
@@ -19442,15 +19439,15 @@
       </c>
       <c r="C53" s="46">
         <f>T18</f>
-        <v>-14.084834484234207</v>
+        <v>-21.46263233107954</v>
       </c>
       <c r="D53" s="46">
         <f>T19</f>
-        <v>-27.835293021733488</v>
+        <v>-37.771610191960512</v>
       </c>
       <c r="E53" s="46">
         <f>T20</f>
-        <v>72.548621829143627</v>
+        <v>82.962089792477116</v>
       </c>
       <c r="F53" s="46" t="e">
         <f>T21</f>
@@ -19458,86 +19455,87 @@
       </c>
       <c r="G53" s="46">
         <f>T22</f>
-        <v>-18.909332536343285</v>
-      </c>
-      <c r="H53" s="46" t="s">
-        <v>48</v>
+        <v>-26.038442851625394</v>
+      </c>
+      <c r="H53" s="46" t="e">
+        <f>T23</f>
+        <v>#NUM!</v>
       </c>
       <c r="I53" s="46">
         <f>T24</f>
-        <v>-15.957272500652767</v>
+        <v>-22.266162823060348</v>
       </c>
       <c r="J53" s="46">
         <f>T27</f>
-        <v>44.388086307786004</v>
+        <v>44.90085788241619</v>
       </c>
       <c r="K53" s="46">
         <f>T28</f>
-        <v>72.450260355057594</v>
+        <v>76.815697229394232</v>
       </c>
       <c r="L53" s="46">
         <f>T29</f>
-        <v>30.482168794003105</v>
+        <v>34.087806039109523</v>
       </c>
       <c r="M53" s="46">
         <f>T30</f>
-        <v>-31.276490513430083</v>
+        <v>29.213979496051596</v>
       </c>
       <c r="N53" s="46">
         <f>T31</f>
-        <v>2.0222358955907325</v>
+        <v>-0.50320210012384692</v>
       </c>
       <c r="O53" s="46">
         <f>T32</f>
-        <v>66.834382603178824</v>
-      </c>
-      <c r="P53" s="46" t="e">
+        <v>1.9656300570695049</v>
+      </c>
+      <c r="P53" s="46">
         <f>T33</f>
-        <v>#NUM!</v>
+        <v>79.964241060212345</v>
       </c>
       <c r="Q53" s="46">
         <f>T34</f>
-        <v>23.202981131810297</v>
+        <v>26.029053396707386</v>
       </c>
       <c r="R53" s="46">
         <f>T35</f>
-        <v>-51.68363952503455</v>
+        <v>-63.227789918018182</v>
       </c>
       <c r="S53" s="46">
         <f>T38</f>
-        <v>-5.3472030886467099</v>
+        <v>-10.357996932071655</v>
       </c>
       <c r="T53" s="46">
         <f>T39</f>
-        <v>105.13615859362464</v>
+        <v>-8.8419620243753378</v>
       </c>
       <c r="U53" s="46">
         <f>T40</f>
-        <v>108.95931681550806</v>
+        <v>122.05407406125485</v>
       </c>
       <c r="V53" s="46">
         <f>T41</f>
-        <v>-23.87743571736819</v>
+        <v>-31.003342908411931</v>
       </c>
       <c r="W53" s="46">
         <f>T42</f>
-        <v>16.98862533234675</v>
+        <v>10.574631553192672</v>
       </c>
       <c r="X53" s="46">
         <f>T43</f>
-        <v>46.667293967436805</v>
+        <v>42.905511180354353</v>
       </c>
       <c r="Y53" s="46">
         <f>T44</f>
-        <v>14.31969315047489</v>
+        <v>17.954832553354933</v>
       </c>
       <c r="Z53" s="46">
         <f>T45</f>
-        <v>50.981147973497762</v>
+        <v>55.099880467133474</v>
       </c>
       <c r="AA53" s="46">
         <f>T46</f>
-        <v>-23.367744770491132</v>
+        <v>-40.316252349407925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>